<commit_message>
added 2 second shift before grabbing image
</commit_message>
<xml_diff>
--- a/RDO.xlsx
+++ b/RDO.xlsx
@@ -445,6 +445,7 @@
           <t>6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 13HP, 15HP, 16HP, 20 Trailer, 27C ZTS, 30 Trailer, 35C, 42, 50C, 76F, 131, 204, 204K, 204L, 205, 206, 206C, 210C, 210R, 212R, 244 P, 244E, 244J, 244K, 244K-II, 244L, 304H, 304J, 304K, 304L, 312, 314, 316, 319, 323, 324, 324 P, 324A, 324H, 324J, 324K, 324L, 325, 328, 328A, 331, 344H, 344J, 344K, 430, 450E, 450M, 458, 459, 459E, 460M, 469, 488, 500, 531, 540A, 540E, 540G-II, 545, 548E, 548G-II, 550, 550M, 551, 558, 559, 560M, 565, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 600L HIGH DUMP, 605C, 614R, 615R, 616, 616R, 618PF, 618R, 620PF, 620R, 622PF, 622R, 622X, 625D, 625PF, 625R, 625X, 630D, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 631, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 640, 640E, 640G, 640X, 644, 648E, 648G, 651, 655C, 661, 670, 678, 690E, 722X, 725D, 725X, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730X, 731, 735FD, 735FD PERFORMANCE UPGRADES, 735X, 740A, 740G, 740PF, 740X, 744, 744K, 744K-II, 748, 748E, 748G-III, 751, 755C, 755D, 770B, 770BH, 772B, 772BH, 805, 824K, 842, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 850D, 852, 854, 862, 864, 918, 920, 920R, 922, 922R, 925, 925D, 925R, 930D, 936D, 950C, 950J, 995, 1010, 1015, 1025, 1030, 1035, 1050C, 1050J, 1107, 1109, 1111, 1113, 1165, 1170, 1175, 1185, 1340, 1350, 1424, 1424C, 1433, 1433C, 1434, 1434C, 1438GS, 1438HS, 1450, 1470, 1504, 1505, 1515, 1520, 1530, 1535, 1538HR, 1550, 1560, 1570, 1590, 1640, 1646, 1646HS, 1700, 1705, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725NT, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1850, 1903, 1905, 1950, 1950N, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2140, 2155, 2250, 2254, 2256, 2258, 2264, 2266, 2266E, 2350, 2355, 2355N, 2400 PRECISIONCUT, 2450, 2500B, 2500E, 2550, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2555, 2650, 2720, 2750, 2755, 2850, 2950, 2955, 3033R, 3038R, 3039R, 3040, 3045R, 3046R, 3050, 3140, 3155, 3316, 3350, 3520, 3522, 3640, 3650, 3950, 3970, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 5070M, 5080M, 5080R, 5090M, 5090R, 5100M, 5100R, 5200, 5300, 5310N, 5320N, 5400, 5420N, 5500, 5500N, 5510N, 5520N, 5600, 5620, 5700, 5720, 5820, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100J, 6100M, 6105 MC, 6105 RC, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115J, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125E MONTENEGRO, 6125J, 6125M, 6125R, 6130, 6130J, 6130M, 6130R, 6135J, 6135M, 6135R, 6140J, 6140M, 6145J, 6145M, 6150M, 6155J, 6165J, 6170R, 6180J, 6190R, 6200, 6200L, 6210, 6210L, 6210R, 6215, 6220, 6220L, 6225, 6230, 6230 Premium, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500L, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7205J, 7210J, 7215J, 7220, 7225J, 7230, 7230 Premium, 7230J, 7250, 7280, 7300, 7320, 7330 Premium, 7350, 7380, 7400, 7405, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7505, 7515, 7520, 7525, 7530E, 7550, 7580, 7630, 7700, 7715, 7730, 7750, 7780, 7800, 7810, 7815, 7830, 7850, 7930, 7950, 7980, 8000, 8100, 8200, 8230T, 8300, 8330T, 8400, 8430T, 8500, 8600, 8700, 8800, 9209, 9211, 9213, 9215, 9218, 9230, 9330, 9430, 9500, 9600, 9670, 9700, 9800, 9880 STS, 9900, C1 200, C2 300, C2 400, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C670, CH570, CP770, CS770, CX15, CX20, DB37, DB40, DB44, DB50, DB55, DB58, DB60, DB66, DB74, DB80, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, E12, E15, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, HX15, HX20, L50, L60, L70, L330, L624, L633, L634, L1524, L1533, L1534, M15, M20, MaxEmerge XP, MX15, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R2 300, R10, R15, R20, R230, R310R, R350R, R930R, S160, S180, S200, S430, S440, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W50, W70, W80, W100, W110, W155, W170, W210, W230, W235, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, Y110, Y115, Y210, Y215, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -457,6 +458,7 @@
           <t>1030, 1035, 1700, 1705, 1715, 1735, 1740, 1745, 1750, 1755, 1765, 1770, 1775, 1775NT, 1780, 1785, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, MaxEmerge XP, PLANTER PERFORMANCE UPGRADES, Pro-Series XP</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -469,6 +471,7 @@
           <t>1520 - Drill, Grain, 1520 Integral Grain Drill - PC2513, , 450 - Drill, Grain, 450 Series End-Wheel and Folding Grain Drills (North American Edition) - PC2250, , 455 - Drill, Grain, 455 Series Folding Grain Drills (North American Edition) - PC2333, , 515 - Drill, Soybean and Grain, 515 Series Integral Soybean and Grain Drills - PC1912, , 520 - Drill, Soybean and Grain, 520 Series Integral Soybean and Grain Drills - PC1893, , 730 - Drill, Air, 730 Air Disk Drill - PC2392, , 730 LL - Drill, Air, 730 LL Air Disk Drill - PC9901, , 740A - Drill, Grain, 740A Mulch Grain Drill (Worldwide Edition) - PC4293, , 9400 - Drill, Grain, 9400 Series Grain Drills and Multiple Hitches (North American Edition) - PC2222, , 9450 - Drill, Grain, 9400 Series Grain Drills and Multiple Hitches (North American Edition) - PC2222</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -481,6 +484,7 @@
           <t>8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9500, 9600, 9700, 9800, 9900, CH570, CH670, CH950, CH960, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W235, W260, W540, W550, W650, W660</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -510,6 +514,7 @@
           <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 2304, 8R 2704, 8R 3004, 7200R, 7210R, 7215R, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 8100, 8110, 8120, 8130, 8200, 8210, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310, 8320, 8330, 8400, 8410, 8420, 8430, 8520</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -553,6 +558,7 @@
           <t>9670 STS, 9770 STS, 9870 STS, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -565,6 +571,7 @@
           <t>7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 260 P, 260E, 310 P, 310E, 350 P, 380 P, 400R, 408R, 410R, 412R, 600R, 612R, 616R, 644K, 670G, 672G, 724 P, 724K, 724L, 744 P, 744K-II, 744L, 768L-II, 770G, 772G, 800R, 824 P, 824L, 848L, 848L-II, 870G, 872G, 948L, 948L-II, 1110E, 1210E, 4940, 6090CB450, 6090CB451, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 8100, 8200, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8310R, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400R, 9360R, 9370R, CH570, CH670, F4365, R4038, R4044, R4045, R4060, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T560, T660, T670, W650, W660</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -618,6 +625,7 @@
           <t>9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9550, 9560, 9560 STS, 9570 STS, 9600, 9610, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, CTS, CTS II, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -665,6 +673,11 @@
           <t>AXE12904</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -686,6 +699,11 @@
           <t>AH170291</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>6103, 9410, 9450, 9500, 9510, 9540, 9550, 9560, 9580, 9600, 9610, 9640, 9650, 9660, 9670, 9680, 9780, C670, CTS, CTS II, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -700,6 +718,11 @@
           <t>AN276545</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>7455, 9935, 9970, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -714,6 +737,11 @@
           <t>AXE79102</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>615F, 616, 616F, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 625D, 625F, 625R, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 645FD, 645FD PERFORMANCE UPGRADES, 725D, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 745FD, 745FD PERFORMANCE UPGRADES, D625, D630, D636, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -721,6 +749,11 @@
           <t>AXE13829</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9550, 9560, 9560 STS, 9570 STS, 9600, 9610, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, CTS, CTS II, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -728,6 +761,16 @@
           <t>KXE10059</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2054, 2056, 2058, 2064, 2066, 6103, 9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9880 STS, C670, CTS, CTS II, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -742,6 +785,11 @@
           <t>DZ108095</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>460DC, 540H, 548H, 640G, 640H, 648G, 648H, 648HT, 748H, 748HT, 848H, 848HT, 1450, 1550, 1570, 2704, 2904, 3004, 3204, 3520, 4930, 6068HF252, 6068HF254, 6068HF485, 6068HFC28, 6068HFC48, 6068HFG85, 6068HFS89, 6068TF252, 6068TF254, 6090HF485, 6090HFC47, 6090HFC48, 6135HF485, 6630 Premium, 6830 Premium, 6930, 7180, 7250, 7330 Premium, 7350, 7380, 7450, 7480, 7550, 7580, 7660, 7750, 7760, 7780, 8130, 8200, 8225R, 8230, 8230T, 8245R, 8270R, 8295R, 8295RT, 8300, 8320R, 8320RT, 8330, 8330T, 8345R, 8345RT, 8400, 8430, 8430T, 8500, 8530, 8600, 9230, 9330, 9420R, 9430, 9430T, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9560, 9560 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9630, 9630 SCRAPER, 9630T, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9870 STS, 9970, C670, CH570, CH670, CP690, S440, S560, S660, S670, S680, S690, S760, S770, S780, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -756,6 +804,11 @@
           <t>AH161392</t>
         </is>
       </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>7660, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -763,6 +816,11 @@
           <t>AH161392</t>
         </is>
       </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>7660, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -770,6 +828,11 @@
           <t>AH128597</t>
         </is>
       </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -784,6 +847,11 @@
           <t>AH216122</t>
         </is>
       </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -791,6 +859,11 @@
           <t>AH154566</t>
         </is>
       </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>335C, 435C, 437C, 630FD, 635FD, 640FD, 700M, 3510, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9450, 9470 STS, 9500, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, A400, C670, CP770, CS770, CT322, H340, H360, H380, H480, R450, S7 600, S7 700, S7 800, S7 850, S7 900, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -798,6 +871,11 @@
           <t>PFA10260</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -805,6 +883,11 @@
           <t>AR75693</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 4055, 4250, 4255, 4450, 4455, 4555, 4560, 4650, 4755, 4760, 4850, 4955, 4960, 7715, 7720, 7815, 7820, 7920, 8100, 8100T, 8110, 8120, 8130, 8200, 8200T, 8210, 8220, 8230, 8270R, 8295R, 8300, 8300T, 8310, 8320, 8320R, 8330, 8345R, 8370R, 8400, 8400R, 8400T, 8410, 8420, 8430, 8520, 8530, 8560, 8570, 8760, 8770, 8850, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9370R, 9400, 9400T, 9410, 9420, 9420R, 9420RX, 9420T, 9430T, 9450, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530T, 9540, 9550, 9560, 9560RT, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630T, 9640, 9650, 9650 STS, 9660, 9680, 9750 STS, 9780, 9880 STS, C850, CTS, CTS II</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -819,6 +902,11 @@
           <t>HXE46664</t>
         </is>
       </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>S7 600, S7 700, S7 800, S7 850, S7 900, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -826,6 +914,11 @@
           <t>R128694</t>
         </is>
       </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>250D, 300D, 300DW, 330C, 370, 370C, 530B, 535, 540G-II, 548G-II, 640G, 644G, 644H, 644HMH, 644J, 648G, 653E, 724J, 740G, 748G-II, 748G-III, 750C, 750J, 762B, 770C, 770C II, 770CH, 770CH II, 770D, 772CH, 772CH II, 772D, 848G, 850C, 850J, 870D, 872D, 1185, 1450, 1550, 1570, 2254, 2256, 2258, 2264, 2266, 2266E, 3510, 3554, 6081AF001, 6081AFM01, 6081HF001, 6081HF070, 6081HFN01, 6081HFN02, 6081HFN03, 6081HFN04, 6081TF001, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7610, 7710, 7810, 8100, 8100T, 8110, 8110T, 8200, 8200T, 8210, 8210T, 8300, 8300T, 8310, 8310T, 8400, 8400T, 8410, 8410T, 9100, 9200, 9300, 9400, 9510, 9550, 9610, 9650, 9650 STS, 9750 STS, 9780, 9970, 9976, 9986, CTS, CTS II</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -840,6 +933,11 @@
           <t>AH232736</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -847,6 +945,11 @@
           <t>RE504819</t>
         </is>
       </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>450C, 744H, 744J, 824J, 6105AF001, 6105HF001, 6125AF001, 6125AFM01, 6125AFM75, 6125HF001, 6125HF070, 6125SFM75, 6135HF485, 6135HFC48, 6650, 6750, 6850, 6950, 7700, 7800, 9750 STS, 9860 STS, 9880 STS</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -854,6 +957,11 @@
           <t>RE508282</t>
         </is>
       </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>9400 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 9100 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 9300 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 9200 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6125HRW02 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6125HRW07 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6125HRW05 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6081HRW05 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6125HRW01 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6125HRW09 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 6105HRW01 - Tractor, 9100, 9200, 9300 and 9400 Tractors (Worldwide Edition) - PC2500, , 9620 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 9420 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 9120 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 9220 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 9520 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 9320 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 6125HRW17 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 6125HRW16 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 6125HRW13 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 6081HRW30 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 6125HRW15 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 6125HRW18 - Tractor, 9120, 9220, 9320, 9420, 9520 and 9620 Tractors (Worldwide Edition) - PC2852, , 9300T - Tractor, 9300T, 9400T Tractors (Worldwide Edition) - PC2663, , 9400T - Tractor, 9300T, 9400T Tractors (Worldwide Edition) - PC2663, , 6125HRW08 - Tractor, 9300T, 9400T Tractors (Worldwide Edition) - PC2663, , 6125HRW04 - Tractor, 9300T, 9400T Tractors (Worldwide Edition) - PC2663, , 6125HRW06 - Tractor, 9300T, 9400T Tractors (Worldwide Edition) - PC2663, , 6125HRW03 - Tractor, 9300T, 9400T Tractors (Worldwide Edition) - PC2663, , 9420T - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 9520T - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 9620T - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 9320T - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 6125HRW15 - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 6125HRW16 - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 6125HRW13 - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 6125HRW17 - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854, , 6125HRW18 - Tractor, 9320T, 9420T, 9520T, 9620T Tractors (Worldwide Edition) - PC2854</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -861,6 +969,16 @@
           <t>RE516346</t>
         </is>
       </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>250D, 300D, 300DW, 330C, 370C, 608BH, 608L, 608LH, 608SH, 644H, 644HMH, 644J, 703G, 703GH, 703JH, 748G-III, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 853G, 900, 903G, 953G, 3554, 6081HF070, 7200, 7300, 7400, 7500, 7710, 7810, 9540, 9560, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9680, 9750 STS, 9760 STS, 9780</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -868,6 +986,11 @@
           <t>RE507011</t>
         </is>
       </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>330C, 370C, 608BH, 608L, 608LH, 608SH, 644H, 644HMH, 644J, 703G, 703GH, 703JH, 724J, 748G-III, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 853G, 900, 903G, 953G, 3554, 6081HF070, 7200, 7300, 7400, 7500, 7720, 7820, 7920, 8120, 8120T, 8220, 8220T, 8320, 8320T, 8420, 8420T, 8520, 8520T, 9540, 9560, 9560 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9680, 9750 STS, 9760 STS, 9780</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -896,6 +1019,16 @@
           <t>L78422</t>
         </is>
       </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>240 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 250 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029DKV50 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029DKV51 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029DKV53 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029DKV54 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029DKV55 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029TKV50 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 3029TKV51 - Loader, Skid-Steer, 240 and 250 Skid-Steer Loaders - PC2690, , 270 - Loader, Skid-Steer, 260 and 270 Skid-Steer Loaders - PC2691, , 260 - Loader, Skid-Steer, 260 and 270 Skid-Steer Loaders - PC2691, , 3029TKV52 - Loader, Skid-Steer, 260 and 270 Skid-Steer Loaders - PC2691, , 3029TKV53 - Loader, Skid-Steer, 260 and 270 Skid-Steer Loaders - PC2691, , 4045DKV50 - Loader, Skid-Steer, 260 and 270 Skid-Steer Loaders - PC2691, , 4045DKV51 - Loader, Skid-Steer, 260 and 270 Skid-Steer Loaders - PC2691, , 280 - Loader, Skid-Steer, 280 Skid Steer - PC2688, , 317 - Loader, Skid-Steer, 317 and 320 Skid-Steers - PC9347, , 320 - Loader, Skid-Steer, 317 and 320 Skid-Steers - PC9347, , 4024TT001 - Loader, Skid-Steer, 317 and 320 Skid-Steers - PC9347, , 4024TT002 - Loader, Skid-Steer, 317 and 320 Skid-Steers - PC9347, , 328 - Loader, Skid-Steer, 325 and 328 Skid Steers - PC9348, , 325 - Loader, Skid-Steer, 325 and 328 Skid Steers - PC9348, , 5030TT002 - Loader, Skid-Steer, 325 and 328 Skid Steers - PC9348, , 5030TT001 - Loader, Skid-Steer, 325 and 328 Skid Steers - PC9348, , 332 - Loader, Skid-Steer, 332 Skid Steer - PC9349, , 5030HT001 - Loader, Skid-Steer, 332 Skid Steer - PC9349, , CT322 - Loader, Skid-Steer, CT322 Compact Track Loader - PC9492, , 4024TT002 - Loader, Skid-Steer, CT322 Compact Track Loader - PC9492, , CT332 - Loader, Skid-Steer, CT332 Compact Track Loader - PC9493, , 5030TT002 - Loader, Skid-Steer, CT332 Compact Track Loader - PC9493</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -903,6 +1036,11 @@
           <t>AT368739</t>
         </is>
       </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>8100, 8200, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -910,6 +1048,11 @@
           <t>R240361</t>
         </is>
       </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>9330 - Tractor, 9330 Tractors (Worldwide Edition) - PC10590, , 6135HRW04 - Tractor, 9330 Tractors (Worldwide Edition) - PC10590, , 6135HRW02 - Tractor, 9330 Tractors (Worldwide Edition) - PC10590, , 9430 - Tractor, 9430 Tractor (6135HRW Engine)(Russian Edition) - PC10533, , 6135HRW02 - Tractor, 9430 Tractor (6135HRW Engine)(Russian Edition) - PC10533, , 6135HRW04 - Tractor, 9430 Tractor (6135HRW Engine)(Russian Edition) - PC10533, , 9430 - Tractor, 9430 Tractors (Worldwide Edition) - PC10591, , 6135HRW04 - Tractor, 9430 Tractors (Worldwide Edition) - PC10591, , 6135HRW02 - Tractor, 9430 Tractors (Worldwide Edition) - PC10591, , 9430T - Tractor, 9430T Tractors (Worldwide Edition) - PC10594, , 6135HRW04 - Tractor, 9430T Tractors (Worldwide Edition) - PC10594, , 6135HRW02 - Tractor, 9430T Tractors (Worldwide Edition) - PC10594, , 9530 - Tractor, 9530 Tractors (Worldwide) - PC10592, , 6135HRW01 - Tractor, 9530 Tractors (Worldwide) - PC10592, , 6135HRW04 - Tractor, 9530 Tractors (Worldwide) - PC10592, , 9530T - Tractor, 9530T Tractors (Worldwide Edition) - PC10595, , 6135HRW04 - Tractor, 9530T Tractors (Worldwide Edition) - PC10595, , 6135HRW01 - Tractor, 9530T Tractors (Worldwide Edition) - PC10595, , 9630 - Tractor, 9630 Tractors (Worldwide Edition) - PC10593, , 6135HRW04 - Tractor, 9630 Tractors (Worldwide Edition) - PC10593, , 6135HRW01 - Tractor, 9630 Tractors (Worldwide Edition) - PC10593, , 9630T - Tractor, 9630T Tractors (Worldwide Edition) - PC10596, , 6135HRW04 - Tractor, 9630T Tractors (Worldwide Edition) - PC10596, , 6135HRW01 - Tractor, 9630T Tractors (Worldwide Edition) - PC10596</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -917,6 +1060,11 @@
           <t>AL205624</t>
         </is>
       </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>6J-1704, 6J-1904, 210K, 210K EP, 210L, 210L EP, 210LJ, 1470, 1570, 1854, 1854J, 2054, 2056, 2058, 2064, 2066, 2204, 2254, 2256, 2258, 2264, 2266, 2266E, 2854, 4044R, 4049R, 4052R, 4066R, 4320, 4520, 4720, 4730, 4830, 4940, 5075M, 5076E, 5076EN, 5082E, 5083E, 5085M, 5090E, 5090EH, 5090EN, 5093E, 5100M, 5101E, 5115M, 5200, 5210, 5220, 5225, 5300, 5310, 5310N, 5320, 5320N, 5325, 5325N, 5400, 5410, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5510, 5510N, 5520, 5520N, 5525, 5525N, 5603, 5625, 6010, 6020, 6090 MC, 6100 MC, 6100D, 6100E SALTILLO, 6105E, 6105J, 6110, 6110 MC, 6110D, 6110E SALTILLO, 6115D, 6115E, 6120, 6120E, 6125E SALTILLO, 6130D, 6130E SALTILLO, 6135E, 6140J, 6140JH, 6155J, 6155JH, 6165J, 6185J, 6200, 6205J, 6210, 6210J, 6215, 6220, 6230, 6300, 6310, 6320, 6330, 6400, 6403, 6405, 6410, 6415, 6420, 6420S, 6430, 6500, 6500L, 6510, 6510S, 6520, 6600, 6605, 6610, 6615, 6620, 6715, 6800, 6810, 6820, 6900, 6910, 6910S, 6920, 6920S, 6930, 7180, 7200, 7200J, 7215J, 7220, 7230J, 7250, 7280, 7300, 7320, 7350, 7380, 7400, 7420, 7425, 7450, 7480, 7500, 7520, 7525, 7550, 7580, 7630, 7700, 7715, 7720, 7730, 7750, 7780, 7800, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8520, 8520T, 8530, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9400, 9400T, 9410R, 9420, 9420T, 9430, 9430T, 9460R, 9460RT, 9470 STS, 9510R, 9510RT, 9520, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9560, 9560R, 9560RT, 9570 STS, 9580, 9620, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9660, 9670, 9670 STS, 9680, 9770 STS, 9780, C670, F4365, R4023, R4030, R4038, R4044, R4045, R4060, T550, T560, T660, T670, W330, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -938,6 +1086,16 @@
           <t>H86911</t>
         </is>
       </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>220 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 215 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 224 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 222 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 218 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 213 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 216 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 230 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 200 - Combine, Platform (Flex Cutterbar/Rigid), 200 Series (200,213,215,216,218,220,222,224,230) Combine Cutting Platforms - PC1558, , 218 - Combine, Platform (Cutting), 218 Draper Platform - PC1664, , 810 - Cutting Platform, 810, 812, 814, 816, 818, 820 Cutting Platforms (-017623) (European Edition) - PC4219, , 816 - Cutting Platform, 810, 812, 814, 816, 818, 820 Cutting Platforms (-017623) (European Edition) - PC4219, , 818 - Cutting Platform, 810, 812, 814, 816, 818, 820 Cutting Platforms (-017623) (European Edition) - PC4219, , 820 - Cutting Platform, 810, 812, 814, 816, 818, 820 Cutting Platforms (-017623) (European Edition) - PC4219, , 812 - Cutting Platform, 810, 812, 814, 816, 818, 820 Cutting Platforms (-017623) (European Edition) - PC4219, , 814 - Cutting Platform, 810, 812, 814, 816, 818, 820 Cutting Platforms (-017623) (European Edition) - PC4219, , 814 - Cutting Platform, 814, 816, 818, 820 Cutting Platforms (017624-) (European Edition) - PC4303, , 816 - Cutting Platform, 814, 816, 818, 820 Cutting Platforms (017624-) (European Edition) - PC4303, , 820 - Cutting Platform, 814, 816, 818, 820 Cutting Platforms (017624-) (European Edition) - PC4303, , 818 - Cutting Platform, 814, 816, 818, 820 Cutting Platforms (017624-) (European Edition) - PC4303</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -952,6 +1110,11 @@
           <t>R108457</t>
         </is>
       </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>8400 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8100 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8200 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8300 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW07 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW34 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW06 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW35 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW08 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW33 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW01 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -959,6 +1122,11 @@
           <t>R162192</t>
         </is>
       </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>8400 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8100 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8200 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8300 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW07 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW34 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW06 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW35 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW08 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW33 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW01 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8300T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8200T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8100T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8400T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW09 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW03 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW10 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW02 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8410 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8310 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8110 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8210 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW40 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW15 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW11 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW17 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW13 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8110T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 8210T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 8410T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 8310T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW12 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW16 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW18 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW14 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -973,6 +1141,11 @@
           <t>R162192</t>
         </is>
       </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>8400 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8100 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8200 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8300 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW07 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW34 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW06 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW35 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW08 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6076HRW33 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 6081HRW01 - Tractor, 8100, 8200, 8300 and 8400 Tractors (Worldwide Edition) - PC2389, , 8300T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8200T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8100T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8400T - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW09 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW03 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW10 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 6081HRW02 - Tractor, 8100T, 8200T, 8300T and 8400T Tractors (Worldwide Edition) - PC2501, , 8410 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8310 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8110 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8210 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW40 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW15 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW11 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW17 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 6081HRW13 - Tractor, 8110, 8210, 8310 and 8410 Tractors (Worldwide Edition) - PC2733, , 8110T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 8210T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 8410T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 8310T - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW12 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW16 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW18 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770, , 6081HRW14 - Tractor, 8110T, 8210T, 8310T and 8410T Tractors (Worldwide Edition) - PC2770</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -980,6 +1153,11 @@
           <t>H218818</t>
         </is>
       </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>9770 STS, 9870 STS, S7 700, S7 800, S7 850, S7 900, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -987,6 +1165,11 @@
           <t>H218817</t>
         </is>
       </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>9770 STS, 9870 STS, S7 700, S7 800, S7 850, S7 900, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -994,6 +1177,11 @@
           <t>AH218323</t>
         </is>
       </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>9580WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9540WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9560WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ017 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6068HZ060 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ008 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6068HZ470 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ009 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9560SH - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9560 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH054 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH055 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9660CTS - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 6081HH017 - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9780i CTS - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 9780CTS - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 6081HZ019 - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 6090HZ003 - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -1001,6 +1189,11 @@
           <t>AH218323</t>
         </is>
       </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>9580WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9540WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9560WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ017 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6068HZ060 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ008 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6068HZ470 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ009 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9560SH - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9560 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH054 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH055 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9660CTS - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 6081HH017 - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9780i CTS - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 9780CTS - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 6081HZ019 - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 6090HZ003 - Combine, 9780CTS, 9780i CTS Combines (S.N. 072800- )Worldwide Edition - PC4389, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -1008,6 +1201,11 @@
           <t>AH142394</t>
         </is>
       </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>9400 - Combine, 9400 Maximizer Combine - PC2180, , 6068HH001 - Combine, 9400 Maximizer Combine - PC2180, , 6359AH001 - Combine, 9400 Maximizer Combine - PC2180, , 6068HH050 - Combine, 9400 Maximizer Combine - PC2180, , 9410 - Combine, 9410 Maximizer Combine - PC2700, , 6068HH051 - Combine, 9410 Maximizer Combine - PC2700, , 9450 - Combine, 9450 Self-Propelled Combine - PC2800, , 6068HH052 - Combine, 9450 Self-Propelled Combine - PC2800, , 9500 - Combine, 9500 Maximizer and 9500 SideHill Combines - PC2179, , 9500SH - Combine, 9500 Maximizer and 9500 SideHill Combines - PC2179, , 9501 - Combine, 9501 Pull-Type Combine - PC2310, , 9510 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , SH9510 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , 6081HH001 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , 6081HH002 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , TRACK - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550SH - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH054 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH055 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH020 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH009 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH021 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH008 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9560SH - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9560 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH054 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH055 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , TRACK - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 9650CTS - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH017 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH010 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9780 - Combine, 9780 CTS Combine (S.N. 071443-072697)(Europe Edition) - PC4373, , CTS - Combine, CTS Combine (670101-674000) (European Edition) - PC2605, , CTS - Combine, CTS Combine (North American Version) - PC2341, , CTS - Combine, CTS Combine (S.N. 070231-071384) (Europe Edition) - PC4318, , CTS - Combine, CTS Combines (S.N. 068887-070122) (Europe Edition) - PC4304, , CTSII - Combine, CTSII Combine (North American Edition) - PC2752, , 6081HH003 - Combine, CTSII Combine (North American Edition) - PC2752, , CTSII - Combine, CTSII Combine (S.N. 675000- ) (European Edition) - PC2753</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -1015,6 +1213,11 @@
           <t>CE17886</t>
         </is>
       </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>9470 STS, 9540, 9560, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, S7 600, S7 700, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S690, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -1022,6 +1225,11 @@
           <t>H174618</t>
         </is>
       </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>600 - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 625R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 635F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 622R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 625F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 630R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 620R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 630F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 622F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 620F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 618R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 618F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 615F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 635R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 615R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 600 - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 630R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 630F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 618R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 620F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 622R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 616R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 635F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 618F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 625F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 616F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 620R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 625R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 622F - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 635R - Combine, Platform (Cutting), 600 Series (Rigid and Flex) Cutting Platforms (Brasil) - PC9284, , 616F - Combine, Platform (Cutting), 616F Cutting Platform (PIN: 1CQ616FXXXX145100- )(Worldwide Edition) - PC16232, , 618F - Combine, Platform (Cutting), 618F Cutting Platform (PIN: 1CQ618FXXXX145100- )(Worldwide Edition) - PC16233, , 620F - Combine, Platform (Cutting), 620F Cutting Platform (PIN: 1CQ620FXXXX145100- )(Worldwide Edition) - PC16234, , 622F - Combine, Platform (Cutting), 622F Cutting Platform (PIN: 1CQ622FXXXX145100- )(Worldwide Edition) - PC16235, , 625F - Combine, Platform (Cutting), 625F Cutting Platform (PIN: 1CQ625FXXXX145100- )(Worldwide Edition) - PC16236, , 630F - Combine, Platform (Cutting), 630F Cutting Platform (PIN: 1CQ630FXXXX145100- )(Worldwide Edition) - PC16237, , 630FD - Combine, Platform (Cutting), 630FD Flex Draper Platform (North American Edition) - PC11904, , 635F - Combine, Platform (Cutting), 635F Cutting Platform (PIN: 1CQ635FXXXX145100- )(Worldwide Edition) - PC16238, , 635FD - Combine, Platform (Cutting), 635FD Flex Draper Platform (North America Edition) - PC10309, , 640FD - Combine, Platform (Cutting), 640FD Flex Draper Platform (North American Edition) - PC10310</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -1050,6 +1258,11 @@
           <t>hxe19072</t>
         </is>
       </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>S7 800, S7 850, S7 900, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -1057,6 +1270,11 @@
           <t>HXE19072</t>
         </is>
       </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>S7 800, S7 850, S7 900, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -1064,6 +1282,11 @@
           <t>AZ10691</t>
         </is>
       </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1032 - Combine, 1032, 1042, 1052 Combines - PC4197, , 1042 - Combine, 1032, 1042, 1052 Combines - PC4197, , 1052 - Combine, 1032, 1042, 1052 Combines - PC4197, , 1055 - Combine, 1055 Combine - PC4198, , 1065 - Combine, 1065, 1068H (-041200) Combines - PC4191, , 1068H - Combine, 1065, 1068H (-041200) Combines - PC4191, , 1065 - Combine, 1065, 1068H (041201-) Combines - PC4201, , 1068H - Combine, 1065, 1068H (041201-) Combines - PC4201, , 1133 - Combine, 1133, 1144 Combines - PC4235, , 1144 - Combine, 1133, 1144 Combines - PC4235, , 1157 - Combine, 1155, 1157, 1158 Combines - PC4236, , 1155 - Combine, 1155, 1157, 1158 Combines - PC4236, , 1158 - Combine, 1155, 1157, 1158 Combines - PC4236, , 1165 - Combine, 1165 Combine (s.n. -060006) - PC9184, , 6059TJ02 - Combine, 1165 Combine (s.n. -060006) - PC9184, , 6068T414 - Combine, 1165 Combine (s.n. -060006) - PC9184, , 1175AH - Combine, 1165, 1175A e 1175AH Combine - PCCQ28973, , 1165 - Combine, 1165, 1175A e 1175AH Combine - PCCQ28973, , 1175A - Combine, 1165, 1175A e 1175AH Combine - PCCQ28973, , 1175 - Combine, 1165,1175 and 1175 Hydro Walker Combine (s.n. 060155-091543)(South American Edition) - PC9609, , 1165 - Combine, 1165,1175 and 1175 Hydro Walker Combine (s.n. 060155-091543)(South American Edition) - PC9609, , 1175H - Combine, 1165,1175 and 1175 Hydro Walker Combine (s.n. 060155-091543)(South American Edition) - PC9609, , 6068TJ04 - Combine, 1165,1175 and 1175 Hydro Walker Combine (s.n. 060155-091543)(South American Edition) - PC9609, , 1175A - Combine, 1165A, 1175A e 1175H4 Combine - PCCQ20662, , 1165A - Combine, 1165A, 1175A e 1175H4 Combine - PCCQ20662, , 1175H4 - Combine, 1165A, 1175A e 1175H4 Combine - PCCQ20662, , 1166HY/4 - Combine, 1166, 1166HY/4 Combines - PC4240, , 1166 - Combine, 1166, 1166HY/4 Combines - PC4240, , 1169HY/4 - Combine, 1169, 1169HY/4 Combines - PC4241, , 1169 - Combine, 1169, 1169HY/4 Combines - PC4241, , 7200 - Combine, 6200, 7100 e 7200 Combine - PCCQ17359, , 6200 - Combine, 6200, 7100 e 7200 Combine - PCCQ17359, , 7100 - Combine, 6200, 7100 e 7200 Combine - PCCQ17359, , 6300 - Combine, 6300, 7300, 7500 Turbo, 7700 Combine - PCCQ19925, , 7500 - Combine, 6300, 7300, 7500 Turbo, 7700 Combine - PCCQ19925, , 7300 - Combine, 6300, 7300, 7500 Turbo, 7700 Combine - PCCQ19925, , 7700 - Combine, 6300, 7300, 7500 Turbo, 7700 Combine - PCCQ19925, , 7700H4 - Combine, 6300, 7300, 7500, 7700H4 e 7700 Combine - PCCQ20663, , 7500 - Combine, 6300, 7300, 7500, 7700H4 e 7700 Combine - PCCQ20663, , 7700 - Combine, 6300, 7300, 7500, 7700H4 e 7700 Combine - PCCQ20663, , 6300 - Combine, 6300, 7300, 7500, 7700H4 e 7700 Combine - PCCQ20663, , 7300 - Combine, 6300, 7300, 7500, 7700H4 e 7700 Combine - PCCQ20663, , 952 - Combine, 952 Combine - PC4162, , 955 - Combine, 955 Combine - PC4146, , 968H - Combine, 965, 965H, 968H Combines - PC4179, , 965 - Combine, 965, 965H, 968H Combines - PC4179, , 965H - Combine, 965, 965H, 968H Combines - PC4179, , 970 - Combine, Combines 950, 960, 970 - PC4125, , 950 - Combine, Combines 950, 960, 970 - PC4125, , 960 - Combine, Combines 950, 960, 970 - PC4125</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -1106,6 +1329,11 @@
           <t>AZ58905</t>
         </is>
       </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>9640, 9660, 9670, 9680, T660, T670, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -1113,6 +1341,16 @@
           <t>AH216678</t>
         </is>
       </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -1120,6 +1358,11 @@
           <t>AH216675</t>
         </is>
       </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -1127,6 +1370,11 @@
           <t>AH167739</t>
         </is>
       </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
@@ -1134,6 +1382,16 @@
           <t>AH216678</t>
         </is>
       </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
@@ -1141,6 +1399,11 @@
           <t>AH167739</t>
         </is>
       </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
@@ -1148,6 +1411,11 @@
           <t>AH216674</t>
         </is>
       </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
@@ -1155,6 +1423,11 @@
           <t>AH216675</t>
         </is>
       </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -1169,6 +1442,11 @@
           <t>AH216677</t>
         </is>
       </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -1176,6 +1454,11 @@
           <t>H236279</t>
         </is>
       </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9670 STS - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH006 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH008 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 9770 STS - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH006 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH008 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
@@ -1211,6 +1494,11 @@
           <t>H158386</t>
         </is>
       </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
@@ -1288,11 +1576,31 @@
           <t>AH160003</t>
         </is>
       </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7480, 7500, 7550, 7580, 7700, 7750, 7780, 7800, 7850, 7950, 7980, 9470 STS, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, S560, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W235, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
           <t>AH160003</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7480, 7500, 7550, 7580, 7700, 7750, 7780, 7800, 7850, 7950, 7980, 9470 STS, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, S560, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W235, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Пусто</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added from 3 to 4 second shift before grabbing image
</commit_message>
<xml_diff>
--- a/RDO.xlsx
+++ b/RDO.xlsx
@@ -445,7 +445,6 @@
           <t>6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 13HP, 15HP, 16HP, 20 Trailer, 27C ZTS, 30 Trailer, 35C, 42, 50C, 76F, 131, 204, 204K, 204L, 205, 206, 206C, 210C, 210R, 212R, 244 P, 244E, 244J, 244K, 244K-II, 244L, 304H, 304J, 304K, 304L, 312, 314, 316, 319, 323, 324, 324 P, 324A, 324H, 324J, 324K, 324L, 325, 328, 328A, 331, 344H, 344J, 344K, 430, 450E, 450M, 458, 459, 459E, 460M, 469, 488, 500, 531, 540A, 540E, 540G-II, 545, 548E, 548G-II, 550, 550M, 551, 558, 559, 560M, 565, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 600L HIGH DUMP, 605C, 614R, 615R, 616, 616R, 618PF, 618R, 620PF, 620R, 622PF, 622R, 622X, 625D, 625PF, 625R, 625X, 630D, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 631, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 640, 640E, 640G, 640X, 644, 648E, 648G, 651, 655C, 661, 670, 678, 690E, 722X, 725D, 725X, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730X, 731, 735FD, 735FD PERFORMANCE UPGRADES, 735X, 740A, 740G, 740PF, 740X, 744, 744K, 744K-II, 748, 748E, 748G-III, 751, 755C, 755D, 770B, 770BH, 772B, 772BH, 805, 824K, 842, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 850D, 852, 854, 862, 864, 918, 920, 920R, 922, 922R, 925, 925D, 925R, 930D, 936D, 950C, 950J, 995, 1010, 1015, 1025, 1030, 1035, 1050C, 1050J, 1107, 1109, 1111, 1113, 1165, 1170, 1175, 1185, 1340, 1350, 1424, 1424C, 1433, 1433C, 1434, 1434C, 1438GS, 1438HS, 1450, 1470, 1504, 1505, 1515, 1520, 1530, 1535, 1538HR, 1550, 1560, 1570, 1590, 1640, 1646, 1646HS, 1700, 1705, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725NT, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1850, 1903, 1905, 1950, 1950N, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2140, 2155, 2250, 2254, 2256, 2258, 2264, 2266, 2266E, 2350, 2355, 2355N, 2400 PRECISIONCUT, 2450, 2500B, 2500E, 2550, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2555, 2650, 2720, 2750, 2755, 2850, 2950, 2955, 3033R, 3038R, 3039R, 3040, 3045R, 3046R, 3050, 3140, 3155, 3316, 3350, 3520, 3522, 3640, 3650, 3950, 3970, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 5070M, 5080M, 5080R, 5090M, 5090R, 5100M, 5100R, 5200, 5300, 5310N, 5320N, 5400, 5420N, 5500, 5500N, 5510N, 5520N, 5600, 5620, 5700, 5720, 5820, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100J, 6100M, 6105 MC, 6105 RC, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115J, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125E MONTENEGRO, 6125J, 6125M, 6125R, 6130, 6130J, 6130M, 6130R, 6135J, 6135M, 6135R, 6140J, 6140M, 6145J, 6145M, 6150M, 6155J, 6165J, 6170R, 6180J, 6190R, 6200, 6200L, 6210, 6210L, 6210R, 6215, 6220, 6220L, 6225, 6230, 6230 Premium, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500L, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7205J, 7210J, 7215J, 7220, 7225J, 7230, 7230 Premium, 7230J, 7250, 7280, 7300, 7320, 7330 Premium, 7350, 7380, 7400, 7405, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7505, 7515, 7520, 7525, 7530E, 7550, 7580, 7630, 7700, 7715, 7730, 7750, 7780, 7800, 7810, 7815, 7830, 7850, 7930, 7950, 7980, 8000, 8100, 8200, 8230T, 8300, 8330T, 8400, 8430T, 8500, 8600, 8700, 8800, 9209, 9211, 9213, 9215, 9218, 9230, 9330, 9430, 9500, 9600, 9670, 9700, 9800, 9880 STS, 9900, C1 200, C2 300, C2 400, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C670, CH570, CP770, CS770, CX15, CX20, DB37, DB40, DB44, DB50, DB55, DB58, DB60, DB66, DB74, DB80, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, E12, E15, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, HX15, HX20, L50, L60, L70, L330, L624, L633, L634, L1524, L1533, L1534, M15, M20, MaxEmerge XP, MX15, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R2 300, R10, R15, R20, R230, R310R, R350R, R930R, S160, S180, S200, S430, S440, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W50, W70, W80, W100, W110, W155, W170, W210, W230, W235, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, Y110, Y115, Y210, Y215, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -458,7 +457,6 @@
           <t>1030, 1035, 1700, 1705, 1715, 1735, 1740, 1745, 1750, 1755, 1765, 1770, 1775, 1775NT, 1780, 1785, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, MaxEmerge XP, PLANTER PERFORMANCE UPGRADES, Pro-Series XP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -471,7 +469,6 @@
           <t>1520 - Drill, Grain, 1520 Integral Grain Drill - PC2513, , 450 - Drill, Grain, 450 Series End-Wheel and Folding Grain Drills (North American Edition) - PC2250, , 455 - Drill, Grain, 455 Series Folding Grain Drills (North American Edition) - PC2333, , 515 - Drill, Soybean and Grain, 515 Series Integral Soybean and Grain Drills - PC1912, , 520 - Drill, Soybean and Grain, 520 Series Integral Soybean and Grain Drills - PC1893, , 730 - Drill, Air, 730 Air Disk Drill - PC2392, , 730 LL - Drill, Air, 730 LL Air Disk Drill - PC9901, , 740A - Drill, Grain, 740A Mulch Grain Drill (Worldwide Edition) - PC4293, , 9400 - Drill, Grain, 9400 Series Grain Drills and Multiple Hitches (North American Edition) - PC2222, , 9450 - Drill, Grain, 9400 Series Grain Drills and Multiple Hitches (North American Edition) - PC2222</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -484,7 +481,6 @@
           <t>8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9500, 9600, 9700, 9800, 9900, CH570, CH670, CH950, CH960, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W235, W260, W540, W550, W650, W660</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -514,7 +510,6 @@
           <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 2304, 8R 2704, 8R 3004, 7200R, 7210R, 7215R, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 8100, 8110, 8120, 8130, 8200, 8210, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310, 8320, 8330, 8400, 8410, 8420, 8430, 8520</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -558,7 +553,6 @@
           <t>9670 STS, 9770 STS, 9870 STS, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -571,7 +565,6 @@
           <t>7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 260 P, 260E, 310 P, 310E, 350 P, 380 P, 400R, 408R, 410R, 412R, 600R, 612R, 616R, 644K, 670G, 672G, 724 P, 724K, 724L, 744 P, 744K-II, 744L, 768L-II, 770G, 772G, 800R, 824 P, 824L, 848L, 848L-II, 870G, 872G, 948L, 948L-II, 1110E, 1210E, 4940, 6090CB450, 6090CB451, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 8100, 8200, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8310R, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400R, 9360R, 9370R, CH570, CH670, F4365, R4038, R4044, R4045, R4060, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T560, T660, T670, W650, W660</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -625,7 +618,6 @@
           <t>9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9550, 9560, 9560 STS, 9570 STS, 9600, 9610, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, CTS, CTS II, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -638,7 +630,6 @@
           <t>9470 STS, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W540, W550, W650, W660</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -658,7 +649,6 @@
           <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S690</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1638,6 +1628,11 @@
           <t>AH220593</t>
         </is>
       </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670, 9670 STS, 9770 STS, 9870 STS, A400, C670, S560, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
@@ -1645,6 +1640,11 @@
           <t>AXE20524</t>
         </is>
       </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
@@ -1652,6 +1652,11 @@
           <t>AH220593</t>
         </is>
       </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670, 9670 STS, 9770 STS, 9870 STS, A400, C670, S560, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
@@ -1659,6 +1664,11 @@
           <t>AXE20524</t>
         </is>
       </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
@@ -1666,6 +1676,11 @@
           <t>AH235610</t>
         </is>
       </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>S660 - Combine, S660 Combine (Europe Edition, MY 2012-2013) - PC4745, , 6090HH015 - Combine, S660 Combine (Europe Edition, MY 2012-2013) - PC4745, , S660 - Combine, S660 Combine (Worldwide Edition, S.N. 745100-765171) - PC10716, , 6090HH006 - Combine, S660 Combine (Worldwide Edition, S.N. 745100-765171) - PC10716, , 6090HH015 - Combine, S660 Combine (Worldwide Edition, S.N. 745100-765171) - PC10716, , S670 - Combine, S670 Combine (Europe Edition, MY 2012-2013) - PC4746, , 6090HH015 - Combine, S670 Combine (Europe Edition, MY 2012-2013) - PC4746, , S670 - Combine, S670 Combine (Worldwide Edition, S.N. 745100-765252) - PC10717, , 6090HH006 - Combine, S670 Combine (Worldwide Edition, S.N. 745100-765252) - PC10717, , 6090HH015 - Combine, S670 Combine (Worldwide Edition, S.N. 745100-765252) - PC10717, , S670HM - Combine, S670HM Combine (Europe Edition, MY 2012-2013) - PC4747, , 6090HH015 - Combine, S670HM Combine (Europe Edition, MY 2012-2013) - PC4747, , 6090HH006 - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , 6090HH015 - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , S670HM - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , HILLMASTER - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , S680 - Combine, S680 Combine (Worldwide Edition, S.N. 745100-766006) - PC10718, , 6135HH003 - Combine, S680 Combine (Worldwide Edition, S.N. 745100-766006) - PC10718, , 6135HH004 - Combine, S680 Combine (Worldwide Edition, S.N. 745100-766006) - PC10718, , 6135HH004 - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , HILLMASTER - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , S680HM - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , 6135HH003 - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , S685 - Combine, S685 Combine (Europe Edition) - PC11902, , 6135HH003 - Combine, S685 Combine (Europe Edition) - PC11902, , 6135HH003 - Combine, S685HM Combine (Europe Edition) - PC11903, , S685HM - Combine, S685HM Combine (Europe Edition) - PC11903, , S690 - Combine, S690 Combine (Worldwide Edition, S.N. 745100-765249) - PC10719, , 6135HH003 - Combine, S690 Combine (Worldwide Edition, S.N. 745100-765249) - PC10719, , 6135HH004 - Combine, S690 Combine (Worldwide Edition, S.N. 745100-765249) - PC10719, , 6135HH003 - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722, , 6135HH004 - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722, , HILLMASTER - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722, , S690HM - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
@@ -1673,6 +1688,11 @@
           <t>AXE25728</t>
         </is>
       </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>S550 - Combine, S550 Combine (Worldwide Edition, S.N. 745100-764999) - PC10715, , 6068HH062 - Combine, S550 Combine (Worldwide Edition, S.N. 745100-764999) - PC10715, , 6068HH061 - Combine, S550 Combine (Worldwide Edition, S.N. 745100-764999) - PC10715, , S660 - Combine, S660 Combine (Europe Edition, MY 2012-2013) - PC4745, , 6090HH015 - Combine, S660 Combine (Europe Edition, MY 2012-2013) - PC4745, , S660 - Combine, S660 Combine (Worldwide Edition, S.N. 745100-765171) - PC10716, , 6090HH006 - Combine, S660 Combine (Worldwide Edition, S.N. 745100-765171) - PC10716, , 6090HH015 - Combine, S660 Combine (Worldwide Edition, S.N. 745100-765171) - PC10716, , S670 - Combine, S670 Combine (Europe Edition, MY 2012-2013) - PC4746, , 6090HH015 - Combine, S670 Combine (Europe Edition, MY 2012-2013) - PC4746, , S670 - Combine, S670 Combine (Worldwide Edition, S.N. 745100-765252) - PC10717, , 6090HH006 - Combine, S670 Combine (Worldwide Edition, S.N. 745100-765252) - PC10717, , 6090HH015 - Combine, S670 Combine (Worldwide Edition, S.N. 745100-765252) - PC10717, , S670HM - Combine, S670HM Combine (Europe Edition, MY 2012-2013) - PC4747, , 6090HH015 - Combine, S670HM Combine (Europe Edition, MY 2012-2013) - PC4747, , 6090HH006 - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , 6090HH015 - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , S670HM - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , HILLMASTER - Combine, S670HM Combine (Worldwide Edition, S.N. -765000) - PC10720, , S680 - Combine, S680 Combine (Worldwide Edition, S.N. 745100-766006) - PC10718, , 6135HH003 - Combine, S680 Combine (Worldwide Edition, S.N. 745100-766006) - PC10718, , 6135HH004 - Combine, S680 Combine (Worldwide Edition, S.N. 745100-766006) - PC10718, , 6135HH004 - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , HILLMASTER - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , S680HM - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , 6135HH003 - Combine, S680HM Combine (Worldwide Edition, S.N. -765000) - PC10721, , S685 - Combine, S685 Combine (Europe Edition) - PC11902, , 6135HH003 - Combine, S685 Combine (Europe Edition) - PC11902, , 6135HH003 - Combine, S685HM Combine (Europe Edition) - PC11903, , S685HM - Combine, S685HM Combine (Europe Edition) - PC11903, , S690 - Combine, S690 Combine (Worldwide Edition, S.N. 745100-765249) - PC10719, , 6135HH003 - Combine, S690 Combine (Worldwide Edition, S.N. 745100-765249) - PC10719, , 6135HH004 - Combine, S690 Combine (Worldwide Edition, S.N. 745100-765249) - PC10719, , 6135HH003 - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722, , 6135HH004 - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722, , HILLMASTER - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722, , S690HM - Combine, S690HM Combine (Worldwide Edition, S.N. 745101 - 765000) - PC10722</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
@@ -1680,6 +1700,11 @@
           <t>AH232851</t>
         </is>
       </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>9560 STS, 9570 STS, 9660, 9660 STS, 9670, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S550, S560, S660, S670, S680, S690, S760, S770, S780, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
@@ -1687,6 +1712,11 @@
           <t>AH203076</t>
         </is>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
@@ -1694,6 +1724,11 @@
           <t>AH217952</t>
         </is>
       </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, S550, S560, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
@@ -1715,6 +1750,11 @@
           <t>AH201582</t>
         </is>
       </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>9450 - Combine, 9450 Self-Propelled Combine - PC2800, , 6068HH052 - Combine, 9450 Self-Propelled Combine - PC2800, , TRACK - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550SH - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH054 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH055 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH020 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH009 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH021 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH008 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , TRACK - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 9650CTS - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH017 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH010 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , TRACK - Combine, 9650 Self-Propelled Combine - PC2802, , 9650 - Combine, 9650 Self-Propelled Combine - PC2802, , 6081HH017 - Combine, 9650 Self-Propelled Combine - PC2802, , 6081HH010 - Combine, 9650 Self-Propelled Combine - PC2802, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9780 - Combine, 9780 CTS Combine (S.N. 071443-072697)(Europe Edition) - PC4373</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
@@ -1736,6 +1776,11 @@
           <t>RE520953</t>
         </is>
       </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>210G, 240D, 250D, 250D-II, 270D, 300D-II, 300DW, 300WW, 350D, 350G, 380G, 460DC, 624J, 640G, 640H, 644J, 648G, 648H, 748H, 810D, 810E, 848H, 1010D, 1450, 1550, 1570, 3154G, 3156G, 3510, 3520, 3522, 3754G, 3756G, 4045HF485, 4045HFG85, 4045HFJ85, 4930, 6068HF485, 6068SFM75, 6068SFM85, 6090HF485, 6090HFC47, 6090HFC48, 6090HFG84, 6090HFG86, 6230 Premium, 6330 Premium, 6430 Premium, 6530 Premium, 6630 Premium, 6830 Premium, 6930, 7130 Premium, 7230 Premium, 7330 Premium, 7630, 7730, 7830, 7930, 8130, 8230, 8230T, 8330, 8330T, 8430, 8430T, 8530, 9230, 9430, 9560 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, C670, CH570, CH670</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
@@ -1750,6 +1795,11 @@
           <t>RE522515</t>
         </is>
       </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>250D, 300D, 300DW, 330C, 370C, 608BH, 608L, 608LH, 608SH, 644H, 644HMH, 644J, 703G, 703GH, 703JH, 724J, 748G-III, 750J, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 850J, 853G, 853J, 853JH, 900, 903G, 903J, 903JH, 909J, 909JH, 953G, 953J, 959J, 3554, 4920, 6081AFH75, 6081AFM75, 6081HF070, 6081HFH70, 7710, 7720, 7810, 7820, 7920, 8120, 8120T, 8220, 8220T, 8320, 8320T, 8420, 8420T, 8520, 8520T, 9560 STS, 9650, 9650 STS, 9660, 9660 STS, 9750 STS, 9760 STS, 9996</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
@@ -1757,6 +1807,11 @@
           <t>SE502812</t>
         </is>
       </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>6105AF001, 6125ADW01, 6125AF001, 6125AFM01, 6125AFM75, 6125HF070, 6125SFM75, 7200, 7300, 7400, 7500, 7700, 7800, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9400, 9400T, 9420, 9420T, 9520, 9520T, 9520T SCRAPER, 9620, 9620T, 9750 STS, 9860 STS, 9880 STS</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
@@ -1764,6 +1819,11 @@
           <t>RE531808</t>
         </is>
       </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>210G, 240D, 250G, 270D, 290G, 310K, 310L, 310SK, 310SL, 350D, 350G, 380G, 524K-II, 544K-II, 624K, 624K-II, 624KR, 644K, 670G, 672G, 703JH, 724K, 744K, 744K-II, 748H, 753J, 753JH, 755D, 759J, 759JH, 764, 770G, 772G, 810D, 810E, 850J, 850J-II, 850JR, 870G, 872G, 903K, 903KH, 909K, 909KH, 953K, 959K, 1010D, 1010E, 1070D, 1070E, 1110D, 1110E, 1110G, 1170E, 1210E, 1210G, 1270D, 1270E, 1270G, 1410D, 1450, 1470D, 1470E, 1470G, 1490D, 1510E, 1510G, 1550, 1570, 1710D, 1711D, 1910E, 2144G, 2154G, 2156G, 2204, 2454D, 2654G, 2656G, 2954D, 3154G, 3156G, 3520, 3522, 3754D, 3754G, 3756G, 4045AFM85, 4045HF485, 4045HFG85, 4045HFJ85, 4045SFM85, 4730, 4830, 5430I, 6068AFM75, 6068AFM85, 6068HF252, 6068HF254, 6068HF485, 6068HFC28, 6068HFC48, 6068HFG25, 6068HFG85, 6068HFL84, 6068HFS89, 6068HRT81, 6068SFM75, 6068SFM85, 6068TF252, 6068TF254, 6090AFM75, 6090AFM85, 6090HF475, 6090HF484, 6090HF485, 6090HFC47, 6090HFC48, 6090HFG84, 6090HFG86, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090SFM75, 6090SFM85, 6103, 6230 Premium, 6330 Premium, 6430 Premium, 6530 Premium, 6534 Premium, 6630 Premium, 6830 Premium, 6930, 7130 Premium, 7180, 7195J, 7200J, 7210J, 7215J, 7225J, 7230 Premium, 7230J, 7250, 7330 Premium, 7430E, 7530E, 7630, 7660, 7730, 7830, 7930, 8100, 8130, 8200, 8225R, 8230, 8230T, 8245R, 8270R, 8295R, 8295RT, 8320R, 8320RT, 8330, 8330T, 8345R, 8345RT, 8430, 8430T, 8530, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9970, C670, CH570, CH670, E210, E210LC, E230, E240, E240LC, E260, E300LC, E330, E360, E400, M4030, M4040, S440, S540, S550, S560, S660, S670, S670H, S760, S770, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
@@ -1771,6 +1831,11 @@
           <t>RE507980</t>
         </is>
       </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>6105AF001, 6105HF001, 6125ADW01, 6125AF001, 6125AFM01, 6125AFM75, 6125HF001, 6125HF070, 6125SFM75, 7200, 7300, 7400, 7500, 7700, 7800, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9400, 9400T, 9420, 9420T, 9520, 9520T, 9520T SCRAPER, 9620, 9620T, 9750 STS, 9860 STS, 9880 STS</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
@@ -1785,6 +1850,16 @@
           <t>AH228828</t>
         </is>
       </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, S550, S660, S670, S670H, S680H, S690</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
@@ -1799,6 +1874,16 @@
           <t>AH228828</t>
         </is>
       </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, S550, S660, S670, S670H, S680H, S690</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
@@ -1806,6 +1891,16 @@
           <t>AH219055</t>
         </is>
       </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9870 STS, 9880 STS, C670, S550, S560, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
@@ -1841,6 +1936,11 @@
           <t>AH169693</t>
         </is>
       </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>9540, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9880 STS, C670, S560, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
@@ -1862,6 +1962,11 @@
           <t>DZ114431</t>
         </is>
       </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>370E, 410E, 460E, 824K, 844K, 1050K, 6135AFM75, 6135AFM85, 6135HF475, 6135HF485, 6135HFC48, 6135HFG75, 6135HFG84, 6135HFM85, 6135SFM75, 6135SFM85, 7350, 7380, 7450, 7480, 7550, 7580, 7750, 7760, 7780, 8200, 8300, 8400, 8500, 8600, 9330, 9410R, 9420R, 9420RX, 9430, 9430T, 9460R, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9560R, 9560RT, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9630, 9630 SCRAPER, 9630T, 9870 STS, CP690, S680, S680H, S685, S685H, S690, S690H, S780, S790</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
@@ -1869,6 +1974,11 @@
           <t>DZ112023</t>
         </is>
       </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>370E, 370E-II, 410 P, 410E, 410E-II, 460 P, 460E, 460E-II, 470 P, 470G, 824K, 844 P, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 904 P, 944K, 1050K, 1050K PL, 6135CI550, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 7280, 7380, 7480, 7580, 7760, 7780, 8200, 8300, 8400, 8500, 8600, 9410R, 9420R, 9420RX, 9460R, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9560R, 9560RT, 9600, CP690, CS690, S680, S680H, S685, S685H, S690, S690H, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
@@ -1911,6 +2021,11 @@
           <t>AXE24395</t>
         </is>
       </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
@@ -1918,6 +2033,11 @@
           <t>AXE24394</t>
         </is>
       </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
@@ -1939,6 +2059,11 @@
           <t>H168433</t>
         </is>
       </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
@@ -1946,6 +2071,11 @@
           <t>19M7785</t>
         </is>
       </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>2C-280, 2C-284, 2C-300, 2C-304, 2C-324, 2C-350, 2C-354, 3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17HP, 20, 20 Trailer, 26, 30 IN., 30 Trailer, 38 IN., 42 IN., 46, 47, 47 IN., 48, 48 IN., 50 in., 52 IN., 54, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 62 IN. DECKS, 72, 72 IN., 107, 110, 110 TLB, 112R, 120C, 120D, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180A, 180G, 200, 200 G, 200C, 200D, 200G, 204L, 205C, 206C, 207C, 208C, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 220A, 222F, 222R, 230C, 240, 240D, 244J, 244K, 244K-II, 244L, 245, 246, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270C, 270D, 280, 285, 290G, 300, 300C, 300D-II, 300DW, 300F, 300G, 300WW, 304, 304J, 304L, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324E, 324G, 324H, 324J, 324K, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330C, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 338, 339, 344H, 344J, 344K, 344L, 345, 348, 349, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 355, 359, 360, 360DC, 365, 370, 370B, 370C, 370E, 370E-II, 375, 375A, 380 P, 380G, 385A, 390, 400C, 400D, 400D-II, 400F, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 420, 425, 430, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 482C, 485, 485A, 485E, 486E, 488E, 490, 493, 494, 500, 524 P, 524K, 524K-II, 524L, 530, 530B, 533, 540E, 540G-II, 540G-III, 540H, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 553, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 595D, 600R, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620I, 620R, 622, 622F, 622G, 622R, 622X, 623, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625R, 625X, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 639, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643G, 643H, 643J, 643K, 643L, 643L-II, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 649, 650, 650G, 650H, 650J, 650K, 652E, 653, 653E, 653G, 654, 655, 655K, 659, 660R, 663, 663R, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 678, 680R, 683, 683R, 690, 690E, 692, 693, 694, 696, 698, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 700M, 702, 703G, 703GH, 703JH, 704, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 721, 722X, 724 P, 724J, 724K, 724L, 725D, 725X, 726, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735X, 737, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740X, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 762B, 764, 768L-II, 770, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772B, 772BH, 772CH, 772CH II, 772D, 772G, 777, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 995, 997, 1010, 1010D, 1010E, 1010G, 1015, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050J, 1050K, 1050K PL, 1070D, 1070E, 1070G, 1092, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1185, 1210E, 1210G, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1295, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1505, 1510DC, 1510E, 1510G, 1512FX, 1516FX, 1524FX, 1530, 1535, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1800, 1810, 1810DC, 1812DC, 1814DC, 1820, 1830, 1835, 1840, 1846, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1903, 1905, 1910, 1910E, 1910G, 1990, 2010DE, 2014DE, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2054, 2056, 2058, 2064, 2066, 2104, 2112DC, 2144G, 2154D, 2154G, 2156G, 2204, 2210, 2230FH, 2230LL, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2330, 2400 PRECISIONCUT, 2412DE, 2430, 2430C, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510S, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2630, 2633, 2633VT, 2635, 2653, 2653A, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029DFG20, 3029DFS29, 3029DFU20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG80, 3029HFG89, 3029HFU20, 3029HFU80, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG80, 3029TFG89, 3029TFU20, 3029TFU29, 3029TFU80, 3029TFU89, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3316, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4120, 4200, 4210, 4239TF001, 4250, 4300, 4310, 4320, 4400, 4410, 4450, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081HF001, 6081HF070, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, B25C, B30C, B35C, B40C, B350, BP15, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E12, E15, E100, E110, E120, E130, E140, E150, E160, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, FD45, G15, GROUPER, GS25, GS30, GS45, GS75, GT225, GT245, GX85, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX15, HX20, L60, L70, L330, L331, L340, L341, L1524, L1533, L1534, LT150, LT160, LT170, LT180, LT190, LTR180, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M15, M20, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MX15, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R15, R20, R40, R230, R450, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S140, S160, S170, S180, S220, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2546, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, TX 4X2, V451R, V461R, W50, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X105, X106, X107, X115R, X116R, X117R, X125, X126, X127, X135R, X145, X146R, X147R, X155R, X165, X166, X166R, X167, X167R, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z510A, Z520A, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
@@ -1953,6 +2083,11 @@
           <t>R528387</t>
         </is>
       </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>5B-700, 5B-704, 5B-750, 5B-754, 120D, 130G, 160D, 160G, 180G, 200G, 210G, 240D, 250G, 270D, 290G, 310J, 310K, 310L, 310SJ, 310SK, 310SL, 310TJ, 315J, 315SK, 315SL, 410J, 410K, 410L, 444K, 460DC, 524K, 524K-II, 540H, 544K, 544K-II, 548H, 550, 554, 605K, 620G, 624J, 624K, 624K-II, 624KR, 640G, 640H, 640L, 640L-II, 643J, 643K, 643L, 643L-II, 644J, 644K, 648G, 648H, 648HT, 648L, 648L-II, 650, 654, 670C II, 670CH II, 670D, 670G, 672D, 672G, 700J-II, 748H, 748HT, 748L, 748L-II, 750J-II, 755D, 764, 843J, 843K, 848H, 848HT, 850J, 850J-II, 1070E, 1110D, 1110E, 1110G, 1170E, 1210E, 1210G, 1410D, 1450, 1490D, 1510E, 1510G, 1550, 1570, 1654, 1854, 2144G, 2154G, 2156G, 2204, 2454D, 2654G, 2656G, 2954D, 3029DF120, 3029DF124, 3029DF129, 3029DF150, 3029DF151, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HF270, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG80, 3029HFG89, 3029HFU20, 3029HFU80, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF152, 3029TF270, 3029TFG20, 3029TFG80, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU80, 3029TFU89, 3029TSG20, 4045HFC93, 4045HFC95, 4045HFG81, 4045HFG93, 4045HFL93, 4045HFS73, 4045HFS85, 4045HFU81, 4045TF285, 4045TFM85, 4630, 4720, 4730, 4830, 5005, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5067E, 5070E, 5075E, 5075EF, 5075M, 5080E, 5080EN, 5080R, 5090R, 5100R, 5103, 5103E, 5103S, 5104, 5105, 5203, 5203S, 5204, 5205, 5210, 5303, 5305, 5310, 5403, 5405, 5410, 5430I, 5503, 5610, 6068AFM75, 6068AFM85, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF252, 6068HF254, 6068HF275, 6068HF475, 6068HF485, 6068HFC28, 6068HFC48, 6068HFG25, 6068HFG82, 6068HFG85, 6068HFL84, 6068HFS77, 6068HFS89, 6068HFU82, 6068HT087, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF252, 6068TF254, 6068TF275, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6105M, 6105R, 6110M, 6115J, 6115M, 6115R, 6125E MONTENEGRO, 6125J, 6125M, 6125R, 6130, 6130M, 6130R, 6140M, 6165J, 6185J, 6230, 6230 Premium, 6320, 6330, 6330 Premium, 6420, 6420S, 6430, 6430 Premium, 6530 Premium, 6534, 6630 Premium, 6830 Premium, 6930, 7130, 7130 Premium, 7195J, 7200J, 7210J, 7215J, 7225J, 7230 Premium, 7230J, 7330 Premium, 7430E, 7455, 7530E, 7630, 7720, 7730, 7820, 7830, 7920, 7930, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9935, 9970, C230, E240, E240LC, E260, E300LC, L60, M4025, M4030, M4040, M4040DN, R40, S440, S550, T550, W50, W70, W540, W550, W650, WL56</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
@@ -1960,6 +2095,11 @@
           <t>19M7786</t>
         </is>
       </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-454, 3B-484, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 22B, 30 IN., 30 Trailer, 30G, 35G, 42 IN., 46, 47, 47 IN., 48, 48 IN., 50 in., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 62 IN. DECKS, 72 IN., 80, 108, 110, 110 TLB, 112R, 120C, 120D, 120R, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180G, 200, 200 G, 200C, 200D, 200G, 203C, 204K, 204L, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 220R, 230C, 240, 240D, 244E, 244L, 245, 250, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270A, 270B, 270C, 270D, 280, 285, 290G, 300D, 300D-II, 300DW, 300E, 300G, 300WW, 304K, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 344G, 344H, 344J, 344K, 344L, 345, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 355, 360DC, 370, 370B, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400C, 400D, 400D-II, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 420, 430, 435, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444G, 444H, 444J, 444K, 444L, 446, 447, 448, 449, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455G, 456, 457, 458, 459, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 485, 485A, 485E, 486E, 488E, 490, 500R, 520M, 521, 522, 524 P, 524K, 524K-II, 524L, 530B, 531, 533, 535, 540A, 540E, 540G-II, 540G-III, 540H, 540M, 541, 542, 543M, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 553, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 595D, 600R, 603M, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620R, 622, 622F, 622G, 622R, 623, 623M, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625R, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650, 650G, 650H, 650J, 650K, 651, 653, 653E, 653G, 654, 655, 655K, 660R, 661, 663, 663R, 667A, 670, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 678, 680R, 683, 683R, 690E, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 700M, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 725D, 727A, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 731, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755C, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 762B, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772CH, 772CH II, 772D, 772G, 777, 778, 790, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 835 SHORT CHASSIS, 842, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 856, 859M, 859MH, 862, 862B, 864, 870, 870D, 870G, 872D, 872G, 890, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 946, 948L, 948L-II, 950, 950C, 950J, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1050, 1050C, 1050J, 1050K, 1050K PL, 1070, 1070D, 1070E, 1070G, 1107, 1109, 1110D, 1110E, 1110G, 1111, 1113, 1165, 1170, 1170E, 1170G, 1175, 1185, 1200, 1210E, 1210G, 1270D, 1270E, 1270G, 1312C, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1442, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1510C, 1510DC, 1510E, 1510G, 1512C, 1512E, 1517, 1518, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1590, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1654, 1690, 1700, 1705, 1710D, 1711D, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1742HS, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1820, 1830, 1835, 1840, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 1948GV, 1948HV, 1990, 2010DE, 2014DE, 2018, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2104, 2109, 2111, 2112C, 2112DC, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2148HV, 2154D, 2154G, 2156G, 2204, 2210, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2412DE, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500E, 2510C, 2510H, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF120, 3029DF128, 3029DF129, 3029DF150, 3029DF160, 3029DF180, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF158, 3029TF160, 3029TF180, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3316, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4010, 4020DF101, 4020TF006, 4020TF105, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4560, 4600, 4610, 4630, 4650, 4700, 4710, 4720, 4730, 4760, 4830, 4850, 4890, 4895, 4920, 4930, 4940, 4960, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030TF220, 5030TF270, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6059DF001, 6059DF092, 6059T, 6059TF001, 6059TF002, 6059TF003, 6059TF004, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068D, 6068DF, 6068DF001, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081HF001, 6081HF070, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6359DF001, 6359TF001, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, B35C, B40C, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP12C, CP12D, CP18C, CP18D, CP20, CP24C, CP24D, CP30C, CP30D, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DF500, DR12, DR12T, DR16, DR18, DR24, E12, E15, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F510, F525, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, FD45, FD55, FL100, FR50, FS50, G15, GROUPER, GS25, GS30, GS45, GS75, GX85, GX255, GX325, GX355, H240, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2 D, HPX 4X4 D, HX6, HX7, HX10, HX14, HX15, HX20, L17.542, L60, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L1742, L2048, L2548, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX280, LX289, M-GATOR A1, M-GATOR A3, M15, M20, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MH60, MH60C, MX8, MX10, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P556, P576, P660, P670, P680, P690, PC4, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R15, R20, R40, R230, R450, R500, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RC6R, RC7R, RC8M, RC10M, RC10R, RC14R, RC60B, RC60L, RC72, RC72B, RC72L, RC78, RC78B, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, RS72, RSX 850I, RSX860E, RSX860I, RSX860M, RT52, RT66, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SA60, SA72, SB60, SB60B, SB72, SB72B, SB72H, SB78, SB78B, SB78H, SB84, SB84B, SB84H, SD72, SD84, SH12F, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, VR66C, VR73C, VR84C, W50, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X300, X300R, X304, X305R, X310, X320, X324, X340, X354, X360, X384, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
@@ -1974,6 +2114,11 @@
           <t>H116861</t>
         </is>
       </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9580, 9600, 9610, 9640, 9650, 9660, 9670, 9680, 9780, C670, CTS, CTS II, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
@@ -1981,6 +2126,11 @@
           <t>19M7827</t>
         </is>
       </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 46, 47, 48, 260, 270A, 270B, 300, 300CX, 300X, 325, 335, 345, 355, 370B, 375, 375A, 385A, 410, 419, 420, 430, 447, 448, 449, 450M, 459, 460, 460M, 460R, 469, 470 P, 470G, 485, 485A, 520M, 540M, 540R, 543M, 543R, 550M, 553, 559, 560M, 560R, 563, 565, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 600R, 603M, 603R, 615F, 618F, 618R, 620F, 620R, 622F, 622R, 625D, 625F, 625R, 630D, 630F, 630R, 635D, 635F, 640D, 640L, 640L-II, 648L, 648L-II, 673, 722PF, 725D, 725PF, 730, 730D, 730PF, 735, 735D, 735PF, 740D, 740PF, 748, 748L, 748L-II, 764, 803M, 803MH, 848G, 848L, 848L-II, 853M, 853MH, 859M, 859MH, 890, 895, 896, 903M, 903MH, 909M, 909MH, 948L, 948L-II, 953M, 953MH, 953ML, 959M, 959MH, 959ML, 1107, 1109, 1111, 1113, 1450, 1470, 1550, 1570, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1780, 2025R, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2510H, 2660VT, 3025E, 3032E, 3038E, 3200, 3215, 3220, 3400, 3420, 3800, 4044M, 4052M, 4710, 4720, 4730, 4830, 4890, 4895, 5036C, 5039C, 5041C, 5042C, 5075M, 5076EL, 5076EN, 5083EN, 5085E, 5085M, 5090E, 5090EL, 5090EN, 5090M, 5090R, 5093EN, 5095M, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101EN, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5215F, 5215V, 5225, 5300N, 5310N, 5315F, 5315V, 5320N, 5325, 5325N, 5400, 5410N, 5420N, 5500N, 5510N, 5515F, 5515V, 5520N, 5615, 5615V, 6020, 6105D, 6105E, 6105M, 6115D, 6115M, 6120, 6120E, 6120L, 6125M, 6130, 6130D, 6130M, 6135E, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140D, 6140M, 6150M, 6170M, 6170R, 6190R, 6210J, 6210R, 6215, 6220, 6220L, 6225, 6230, 6320, 6320L, 6325, 6330, 6415, 6420, 6420L, 6420S, 6425, 6430, 6488, 6515, 6520, 6520L, 6525, 6530, 6534, 6610, 6615, 6620, 6630, 6650, 6710, 6715, 6750, 6810, 6850, 6910, 6950, 7130, 7180, 7200, 7200A, 7230, 7250, 7280, 7300, 7330, 7350, 7380, 7400, 7400A, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, C440R, C441R, C670, CH950, CH960, CP20, CP770, CS690, CS770, CTS, CTS II, DB90, F440M, F440R, F441M, F441R, GROUPER, H240, H260, H310, H480, HD35F, HD35R, HD40F, HD40R, HD40X, HD45F, HD45R, HD50F, HD50R, L331, L341, R230, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W330, W540, W550, W650, W660, X9 1000, X9 1100, Y210, Y215</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
@@ -1988,6 +2138,16 @@
           <t>19M7185</t>
         </is>
       </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>6B-1204/6120B, 6B-1404, 6E-1204, 6E-1204P, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 17 ZTS, 20 Trailer, 22 in., 27 ZTS, 27D, 30 Trailer, 35D, 35ZTS, 42 IN., 50D, 50ZTS, 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 75 P, 85 P, 100, 110 TLB, 135D, 180A, 210 G, 210 P, 210L, 210L EP, 220A, 244L, 250C, 250D, 300C, 300D, 300DW, 310 G, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 315J, 315SE, 315SG, 315SK, 315SL, 320 P, 324L, 325J, 325SL, 350C, 350D, 350DW, 360DC, 400, 400C, 400D, 410 P, 410E, 410G, 410J, 410K, 410L, 445, 446, 447, 448, 449, 456, 457, 458, 459, 460DC, 466, 467, 468, 469, 500, 540A, 540G-III, 540H, 544E, 544G, 546, 547, 548G-III, 548H, 556, 557, 558, 559, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 620I, 623, 624E, 624G, 625I, 640, 640G, 640H, 643D, 643G, 644, 644E, 648G, 648H, 648HT, 650, 655C, 670, 676, 678, 710 P, 710L, 717, 717A, 727A, 740A, 748G-III, 748H, 748HT, 750, 750A, 752, 754, 755C, 755D, 756, 764, 770, 790, 805, 825 SHORT CHASSIS, 842, 843G, 848H, 850, 852, 854, 855 SHORT CHASSIS, 856, 862, 864, 870, 886, 900, 916, 926, 936, 940, 946, 950, 950C, 950J, 956, 970, 990, 994, 995, 1010, 1015, 1023E, 1025, 1025R, 1026R, 1040, 1050, 1050C, 1050E, 1050J, 1070, 1107, 1109, 1111, 1113, 1140, 1165, 1170, 1175, 1185, 1350, 1354, 1404, 1420, 1424, 1424C, 1433, 1433C, 1434, 1434C, 1435, 1445, 1450, 1550, 1560, 1565, 1570, 1590, 1640, 1690, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1840, 1850, 1854, 1854J, 1860, 1890, 1895, 1900, 1903, 1905, 1910, 1950, 1950N, 1990, 2025R, 2026R, 2040, 2040S, 2054, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2140, 2155, 2250, 2355, 2355N, 2450, 2555, 2650, 2653, 2755, 2850, 2955, 3004, 3033R, 3038R, 3039R, 3040, 3045B, 3045R, 3046R, 3050, 3050B, 3055, 3120, 3140, 3150, 3155, 3204, 3255, 3320, 3325, 3350, 3365, 3520, 3522, 3640, 3650, 3710, 3720, 4700, 4720, 4730, 4830, 5060EN, 5075EF, 5076E, 5076EL, 5080EN, 5082E, 5083E, 5090E, 5090EH, 5090EL, 5093E, 5220, 5320, 5420, 5425, 5520, 5615, 5625, 5715, 5725, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100D, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E SALTILLO, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E SALTILLO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130M, 6130R, 6135B, 6135E, 6135M, 6135R, 6140B, 6140D, 6140E, 6140J, 6140JH, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155R, 6155RH, 6165J, 6170M, 6170R, 6175M, 6175R, 6185J, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6700, 6800, 6810, 6830, 6830 Premium, 6900, 6910, 6910S, 6930, 7130, 7130 Premium, 7185J, 7195J, 7200, 7200J, 7205J, 7210, 7210J, 7215J, 7220, 7225J, 7230, 7230 Premium, 7230J, 7270R, 7320, 7330, 7330 Premium, 7400, 7410, 7425, 7430E, 7510, 7525, 7530E, 7600, 7610, 7630, 7700, 7710, 7715, 7720, 7730, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 7950, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8450, 8500, 8520, 8520T, 8530, 8560, 8570, 8650, 8760, 8770, 8870, 8960, 8970, 9209, 9211, 9300T, 9320T, 9400, 9400T, 9410, 9420T, 9430T, 9450, 9460RT, 9470RT, 9500, 9501, 9510, 9510RT, 9520RT, 9520T, 9520T SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620RX, 9620T, 9630T, 9640, 9650, 9660, 9670, 9680, 9780, 9880 STS, A2, B25C, B30C, B35C, B40C, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C1 200, C120, C230, C440R, C441R, C450, C451R, C461R, C500, C670, CH570, CH670, CH950, CH960, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DF180G, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, F440M, F440R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L70, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, M-GATOR A3T, M944, M944I, M952, M952I, M962, M962I, M4030, M4040, M4040DN, N530C, N536C, N540C, N542C, R240, R280, R310, R310R, R350R, R944I, R952I, R962I, S160, S180, S200, S430, S440, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, STRAIGHT BLADE, T550, T560, T660, T670, TRAIL BUCK 500, TRAIL BUCK 650, V451R, V461R, W235, W540, W550, W650, W660, X710, X730, X734, X738, X739, X750, X754, X758, X940, X948, X949, XUV825E, XUV825M, XUV855E, XUV855M</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
@@ -1995,6 +2155,11 @@
           <t>19M7791</t>
         </is>
       </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>3B-504, 3B-554, 3B-604, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20, 26, 30 IN., 31C, 38 IN., 42 IN., 46, 47, 47 IN., 48, 52 IN., 54 in., 54 IN. FRONT BLADE, 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 70, 72 IN., 112R, 120D, 130 P, 130G, 146, 160 P, 160D, 160G, 180G, 200 G, 200D, 200G, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 240, 240D, 245, 246, 250, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270D, 280, 285, 290G, 300, 300CX, 300D-II, 300E, 300G, 300X, 305, 310 P, 310E, 310TK TMC, 312GR, 313, 314G, 314R, 315, 316GR, 317, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 326D, 326E, 328, 328D, 328E, 329D, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333G, 335C, 335D, 337E, 344K, 344L, 350G, 360DC, 370B, 370E, 370E-II, 375, 375A, 380G, 385, 385A, 410, 410 P, 410E, 410E-II, 410K, 410TK TMC, 415, 419, 420, 425, 430, 435, 435C, 437C, 437D, 437E, 440E, 440R, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450, 450K, 450M, 455, 456, 457, 458, 459, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 485, 485A, 500R, 524 P, 524K, 524K-II, 524L, 530, 533, 535, 540A, 540E, 540G-II, 540M, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 546, 547, 548E, 548G-II, 548H, 550, 550K, 550M, 554, 556, 557, 558, 559, 560M, 560R, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 605K, 606C, 606SH, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608L, 608LH, 608SH, 612C, 614R, 615F, 615R, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643D, 643G, 643J, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648E, 648G, 648H, 648L, 648L-II, 650, 650K, 653G, 654, 655, 655K, 660, 663R, 665, 670, 670C II, 670CH II, 670D, 670G, 672D, 672G, 673, 678, 680, 681, 683R, 692, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 710K, 710L, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 741, 744, 744H, 744J, 744K, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-III, 748L, 748L-II, 750K, 750L, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770C II, 770CH II, 770D, 770G, 772CH II, 772D, 772G, 777, 790, 797, 800R, 803M, 803MH, 824J, 824K, 830, 835, 842, 843G, 843J, 843K, 843L, 843L-II, 844J, 844K, 848G, 848L, 848L-II, 850, 850JR, 850K, 850L, 850L PL, 852, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 856, 859M, 859MH, 862, 870D, 870G, 872D, 872G, 892, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 909J, 909JH, 909K, 909KH, 909M, 909MH, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 990, 994, 995, 997, 1010, 1015, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050K, 1107, 1109, 1111, 1113, 1175, 1354, 1404, 1420, 1424, 1424C, 1435, 1445, 1450, 1470, 1512E, 1512FX, 1516FX, 1524FX, 1530, 1535, 1550, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1640, 1690, 1700, 1700T, 1705, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810, 1810E, 1814E, 1820, 1830, 1835, 1840, 1850, 1860, 1870, 1890, 1895, 1900, 1910, 1950, 1950N, 1990, 2010DE, 2014DE, 2020A, 2025R, 2026R, 2027R, 2030A, 2032R, 2036R, 2038R, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2140, 2144G, 2154D, 2154G, 2155, 2156G, 2204, 2243, 2250, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2350, 2355, 2355N, 2412DE, 2450, 2454D, 2510H, 2520, 2530L, 2550, 2555, 2630, 2633, 2633VT, 2635, 2650, 2654G, 2656G, 2704, 2720, 2730, 2750, 2755, 2850, 2854, 2904, 2950, 2954D, 2955, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029HFC03, 3029HFG03, 3029HG530, 3029HI530, 3029TF158, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3040, 3043D, 3045B, 3045R, 3046R, 3050, 3050B, 3055, 3110, 3120, 3140, 3150, 3154G, 3155, 3156G, 3200, 3203, 3204, 3210, 3215, 3220, 3255, 3310, 3316, 3320, 3325, 3350, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3640, 3650, 3720, 3754G, 3756G, 3800, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF158, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF158, 4045HF275, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFU72, 4045HFU79, 4045HFU82, 4045HI550, 4045HLC07, 4045HLC09, 4045HN056, 4045HRT90, 4045T, 4045TF120, 4045TF150, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF271, 4045TF275, 4045TFM50, 4045TFM75, 4045TFU20, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4990, 4995, 5005, 5036D, 5038D, 5039D, 5040D, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080M, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5203S, 5205, 5210, 5220, 5225, 5303, 5305, 5310, 5310N, 5320, 5320N, 5325, 5325N, 5403, 5405, 5410, 5415, 5420, 5420N, 5425, 5425N, 5500N, 5510N, 5520, 5520N, 5525, 5525N, 5600, 5603, 5605, 5610, 5615, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068DF150, 6068HB551, 6068HF120, 6068HF150, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC93, 6068HFG85, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HI550, 6068HT087, 6068SFM50, 6068SFM75, 6068SFM85, 6068TF120, 6068TF150, 6068TF158, 6068TF220, 6068TF250, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFG06, 6090HFG09, 6090HFL75, 6090HFL85, 6090HFM85, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6140B, 6140D, 6140J, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175R, 6180CI510, 6180J, 6190J, 6190M, 6190R, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7200, 7200R, 7205J, 7210, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 9009A, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, BP15, C2 400, C100, C230, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F620, F680, F687, F710, F725, F735, F1145, F4365, FL100, FR21B, FR50, FS20, FS22B, FS50, GROUPER, H160, H240, H260, H310, H340, H360, H380, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, L70, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, M4030, M4040, M4040DN, MaxEmerge XP, N530C, N530F, N536C, N540C, N540F, N542C, N543F, N560F, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R230, R450, R500, R4023, R4030, R4038, R4044, R4045, R4060, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, RSX 850I, RSX860E, RSX860I, RSX860M, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SPRAYER PERFORMANCE UPGRADES, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, V451G, V451M, V461M, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X495, X595, X700, X710, X730, X738, X739, X740, X748, X750, X754, X758, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV590I, XUV590I S4, Y110, Y115, Y210, Y215, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
@@ -2002,6 +2167,11 @@
           <t>03H1499</t>
         </is>
       </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>11, 26, 40, 42, 46, 47, 48, 215, 216, 218, 220, 222R, 224, 225, 230, 246, 328, 338, 342T, 346T, 348, 350, 370, 370B, 375, 375A, 385A, 425, 447, 448, 450, 454, 456, 456T, 456W, 459, 466, 468, 485, 485A, 509, 512, 525D, 530D, 536D, 550, 570, 608BH, 608L, 608LH, 608SH, 609, 610, 627, 630, 637, 650, 653, 654, 655, 660, 670, 680, 703G, 703GH, 703JH, 709, 714, 717, 726, 730, 730LL, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 812, 853, 853G, 853J, 856, 886, 900, 903G, 903J, 903K, 903KH, 903M, 903MH, 909J, 909K, 909KH, 909M, 909MH, 911, 913, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 953G, 953J, 953K, 953M, 959J, 959K, 959M, 960, 980, 985, 1008, 1018, 1408, 1418, 1508, 1517, 1518, 1520, 1530, 1535, 1570, 1745, 1840, 2018, 2100, 2200, 2210, 2210LL, 2254, 2310, 2330, 2400, 2410, 2410C, 2430, 2430C, 2510C, 2510L, 2510S, 2620, 2623, 2625, 2630, 2633, 2635, 2680H, 2730, 3235C, 3245C, 3510, 3520, 3522, 3950, 3955, 3970, 3975, 5200, 5400, 5440, 5460, 5720, 5730, 5820, 5830, 6080A E-CUT, 6500A E-CUT, 6620, 7200A, 7400A, 7500, 7500A E-CUT, 7700, 7720, 7721, 8000A E-CUT, 8500, 8700, 8800, 8800A, 8820, 8900A, 9009A, AD07, AD11, AH80, AT14, BA72C, BA84C, BA96C, BH7, BH8, BH9, BH11, BP72C, BP84C, BR60C, BR72C, BR84C, CH570, CH670, CP12C, CP12D, CP18C, CP18D, CP24C, CP24D, CP30C, CP30D, CP48, D625, D630, D636, HH20C, HH40C, HH60C, HH80C, HX6, HX7, HX10, HX14, MH60, MH60C, MX5, MX6, MX7, MX8, MX10, MX225, MX425, P660, P670, P680, P690, RC6R, RC7M, RC7R, RC8M, RC10M, RC10R, RC14R, RC60B, RC60L, RC72, RC72B, RC72L, RC78, RC78B, RS72, RT52, RT66, RX72, RX84, SA60, SA72, SB60, SB60B, SB72, SB72B, SB72H, SB78, SB78B, SB78H, SB84, SB84B, SB84H, SD72, SD84, TC125, VR66C, VR73C, VR84C, X710, X730, X734, X738, X739, X750, X940, X948, X949</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
@@ -2009,6 +2179,11 @@
           <t>19M7789</t>
         </is>
       </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-454, 3B-484, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 30 IN., 38 IN., 42 IN., 46, 47, 47 IN., 48, 48 IN., 52 IN., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 110 TLB, 112R, 160G, 180G, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 225C, 230C, 240, 240D, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260E, 270, 270D, 280, 290G, 300D-II, 300DW, 300G, 300WW, 310 P, 310E, 310K, 310K EP, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 312GR, 313, 314G, 315, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330C, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335D, 337E, 344J, 350 P, 350D, 350DW, 350G, 360DC, 370, 370B, 370C, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400D, 400R, 408R, 410 P, 410E, 410E-II, 410K, 410L, 410R, 410TK TMC, 412R, 415, 425, 435, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450C, 450D, 450E, 450H, 450J, 450K, 450M, 455, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 485, 485A, 493, 494, 500R, 521, 522, 524 P, 524K, 524K-II, 524L, 525, 530, 531, 535, 540E, 540G-II, 540G-III, 540H, 541, 542, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550H, 550J, 550K, 550M, 551, 553, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 600C, 600R, 603M, 603R, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608L, 608LH, 608SH, 612C, 612C PERFORMANCE UPGRADES, 612R, 616C, 616C PERFORMANCE UPGRADES, 616R, 618C, 618C PERFORMANCE UPGRADES, 618PF, 620G, 620I, 620PF, 622G, 622PF, 622X, 623, 623M, 623R, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625D, 625I, 625PF, 625X, 630, 630C, 630D, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630X, 631, 635, 635D, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635X, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643D, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650D, 650H, 650J, 650K, 651, 653E, 655K, 661, 670C II, 670CH II, 670D, 670G, 672D, 672G, 673, 678, 690E, 692, 693, 694, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 710D, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740PF, 740X, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 754, 755K, 756, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770C II, 770CH II, 770D, 770G, 772CH II, 772D, 772G, 790, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853G, 853J, 853JH, 853M, 853MH, 854, 855 LONG CHASSIS, 855 SHORT CHASSIS, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 890, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 911, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 994, 995, 997, 1010, 1018, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050K, 1050K PL, 1092, 1175, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1350, 1360, 1404, 1418, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1512FX, 1516FX, 1524FX, 1530, 1535, 1550, 1570, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1785, 1790, 1795, 1830, 1835, 1842GV, 1842HV, 1848GV, 1848HV, 1850, 1854, 1854J, 1870, 1900, 1910, 1910E, 1910G, 1990, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2104, 2154G, 2156G, 2204, 2210, 2254, 2256, 2258, 2264, 2266, 2266E, 2454D, 2510S, 2653, 2654G, 2656G, 2660VT, 2704, 2730, 2854, 2904, 2954D, 3004, 3005, 3025D, 3025E, 3028EN, 3029DF128, 3029DF129, 3029DFG20, 3029DFU20, 3029DFU29, 3029DFU29R, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFU20, 3029TFU29, 3029TFU89, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3120, 3154G, 3156G, 3200, 3203, 3204, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3316, 3320, 3325, 3365, 3400, 3420, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF158, 4045DF271, 4045DFM50, 4045DFM70, 4045HF120, 4045HF150, 4045HF158, 4045HF285, 4045HF286, 4045HF287, 4045HF289, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG93, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045SFM85, 4045T, 4045TF150, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFU20, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5055D, 5055E, 5060E, 5065E, 5065M, 5070E, 5075E, 5075M, 5076E, 5076EL, 5076EN, 5078E, 5080E, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5204, 5205, 5210, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5320, 5325, 5325N, 5400, 5405, 5410, 5415, 5420, 5425, 5430I, 5440, 5460, 5500, 5500N, 5510, 5510N, 5520, 5525, 5603, 5615, 5620, 5625, 5715, 5720, 5730, 5820, 5830, 6010, 6020, 6068AFM75, 6068AFM85, 6068CI550, 6068DF150, 6068HF120, 6068HF150, 6068HF157, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF475, 6068HFC08, 6068HFC09, 6068HFC94, 6068HFC95, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG55, 6068HFG82, 6068HFG94, 6068HFG95, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HI550, 6068HN075, 6068SFM50, 6068SFM75, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF250, 6068TF258, 6068TFM50, 6068TFM75, 6080A E-CUT, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7410, 7420, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7510, 7515, 7520, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, B25C, BH7, BH8, BH9, BH11, C2 400, C6R, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, DB37, DB41, DB44, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E330, E360, E380, E400, F440R, F441M, F441R, F620, F680, F687, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, G15, GROUPER, GS25, GS30, GS45, GS75, GT242, GT262, GT275, GX255, GX325, GX335, GX345, GX355, H260, H310, H340, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX14, JX75, L330, L331, L340, L341, LX172, LX173, LX176, LX178, LX186, LX188, M-GATOR A3, M-GATOR A3T, MaxEmerge XP, N530C, N536C, N540C, N542C, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R400, R450, R500, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W70, W80, W100, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W440, W540, W550, W650, W660, WE80, WE85, WL53, WL56, X9 1000, X9 1100, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z510A, Z520A, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
@@ -2016,6 +2191,11 @@
           <t>03H1764</t>
         </is>
       </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>38 IN., 42 IN., 46, 47, 48, 218, 260, 270A, 270B, 328, 338, 348, 370B, 375, 375A, 385A, 447, 448, 456, 456T, 456W, 466, 468, 485, 485A, 544G, 595, 624G, 627, 637, 644E, 644G, 650, 900, 911, 918, 920D, 960, 1065A, 1520, 1530, 1535, 2310, 3765, 4055, 4250, 4255, 4450, 4455, 4475, 4555, 4650, 4755, 4850, 4955, 5050E, 5060E, 5067E, 5075E, 5575, 5720, 5820, 6620, 7720, 7721, 7722, 8820, BH7, BH8, BH9, BH11, CP12C, CP12D, CP18C, CP18D, CP24C, CP24D, CP30C, CP30D, CP48, MH60, MH60C, RC60B, RC60L, RC72, RC72B, RC72L, RC78, RC78B, RS72, RT52, RT66, SA60, SA72, SB60, SB60B, SB72, SB72B, SB72H, SB78, SB78B, SB78H, SB84, SB84B, SB84H, SD72, SD84, VR66C, VR73C, VR84C</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
@@ -2023,6 +2203,16 @@
           <t>H207542</t>
         </is>
       </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>525D, 530D, 536D, 614R, 615F, 615R, 616, 616R, 618F, 618PF, 618R, 620F, 620PF, 620R, 622F, 622PF, 622R, 622X, 625F, 625PF, 625R, 625X, 630F, 630PF, 630R, 630X, 635F, 635PF, 635R, 635X, 640X, 722PF, 722X, 725PF, 725X, 730PF, 730X, 735PF, 735X, 740PF, 740X, 918, 920, 920R, 922, 922R, 925, 925R, 1450, 1550, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
@@ -2030,6 +2220,11 @@
           <t>19H1919</t>
         </is>
       </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>75C, 75D, 80, 80C, 85D, 85G, 100, 108, 110, 111, 112L, 115, 120C, 120D, 130G, 135C, 135D, 135G, 140A, 160, 160A, 160C, 160D, 160G, 170, 175, 180, 180A, 180G, 185, 190DW, 190E, 200, 200C, 200D, 200G, 210C, 210G, 210LE, 215, 216, 218, 220, 220DW, 222R, 224, 225C, 225D, 230, 230C, 240, 240D, 245, 245G, 260, 265, 270, 270C, 270D, 285, 290D, 290G, 300D, 310D, 315D, 318, 320, 330C, 335, 350, 350D, 350G, 370, 370C, 375, 380G, 385, 410D, 415D, 420, 420D, 425, 425D, 430, 430D, 435, 435D, 440D, 445, 446, 447, 448, 450, 450C, 450D, 450G, 454, 455, 455G, 456, 457, 458, 466, 467, 468, 470G, 490E, 510D, 512, 524D, 535, 544E, 546, 547, 550, 550G, 555G, 556, 557, 558, 566, 567, 568, 570, 570B, 590D, 595D, 624E, 625I, 636M, 637, 643D, 643G, 644E, 648M, 648R, 650G, 652B, 652E, 652M, 652R, 653, 653E, 653G, 654, 661R, 670B, 670C, 670C II, 670CH, 670CH II, 672B, 672CH, 690E, 710D, 717, 717A, 724D, 727A, 730LL, 737, 757, 762B, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 772B, 772BH, 772CH, 772CH II, 777, 790E, 792D, 797, 826D, 828D, 840, 843G, 853, 862B, 892E, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920D, 920F, 920R, 922F, 922R, 924, 924DE, 925, 925F, 925R, 930, 930F, 930R, 940, 997, 1010, 1015, 1030, 1032D, 1040, 1128DDE, 1128DE, 1140, 1160A, 1180A, 1332DDE, 1350, 1415D, 1420D, 1425D, 1430D, 1435D, 1440D, 1445D, 1508, 1517, 1518, 1550, 1640, 1750, 1800, 1840, 1850, 1905, 1950, 1950N, 2018, 2020, 2030, 2040, 2040S, 2140, 2150, 2155, 2210, 2210LL, 2250, 2255, 2310, 2350, 2355, 2355N, 2410, 2410C, 2430C, 2450, 2510C, 2510H, 2510S, 2550, 2555, 2620, 2623, 2623VT, 2625, 2650, 2700, 2720, 2750, 2755, 2850, 2950, 2955, 3040, 3050, 3055, 3140, 3150, 3155, 3179DF, 3179T, 3255, 3350, 3510, 3520, 3522, 3640, 3650, 3950, 3955, 3970, 3975, 4039D, 4039DF001, 4039DF092, 4039T, 4039TF001, 4045D, 4045DF001, 4045TF001, 4055, 4219DF01, 4239A, 4239D, 4239DF001, 4239DT004, 4250, 4255, 4276DF01, 4276T, 4276TF01, 4450, 4455, 4555, 4560, 4650, 4700, 4755, 4760, 4850, 4955, 4960, 5200, 5400, 5440, 5460, 5720, 5730, 5820, 5830, 6068DFM01, 6068HF275, 6068HF475, 6068TF275, 6068TFM01, 6076AFN, 6076HF030, 6076TF, 6081AF001, 6081AFM01, 6081HF001, 6081HF070, 6081HFN01, 6081HFN02, 6081HFN03, 6081HFN04, 6081TF001, 6101HF010, 6101HF011, 6125HF070, 6329DF01, 6414D, 6414T, 6414TDW14, 6414TDW16, 6466A, 6466D, 6466T, 6610, 6619A, 6619A Engine SE500219, 6619A Engine SE500493, 6619A Engine SE500087, 6619A Engine SE500089, 6619A Engine SE500090, 6619A Engine SE500091, 6619TF-01, 6620, 6650, 6700, 6710, 6750, 6810, 6850, 6910, 6950, 7020, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7480, 7500, 7520, 7550, 7580, 7700, 7720, 7721, 7722, 7750, 7780, 7800, 7850, 7950, 7980, 8430, 8440, 8450, 8560, 8570, 8630, 8640, 8650, 8760, 8770, 8820, 8850, 8870, 8960, 8970, AMT600, CH570, CH670, F910, F930, HX10, HX14, L100, L105, L107, L108, LA105, LA115, LX172, LX173, LX176, LX178, LX186, LX188, M653, M655, M665, MX8, MX10, S80, S82, S92, STRAIGHT BLADE, TH 6X4, TH 6X4 D, TRS22, TRS24, TRS26, TRS27, TRS32, TRX24, TRX26, TURF TX 4X2, TX 4X2, W110, W150, W155, WH36A, WH48A, WH52A, X110, X120, X145, X330, X465, X475, X485, X495, X575, X585, X595, X700, X720, X724, X728, X729, X740, X744, X748, X749, Z225, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
@@ -2037,6 +2232,11 @@
           <t>HXE72751</t>
         </is>
       </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
@@ -2044,6 +2244,11 @@
           <t>HXE72751</t>
         </is>
       </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
@@ -2051,6 +2256,11 @@
           <t>AXE12269</t>
         </is>
       </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
@@ -2058,6 +2268,11 @@
           <t>H218588</t>
         </is>
       </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
@@ -2065,6 +2280,11 @@
           <t>AXE12269</t>
         </is>
       </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
@@ -2072,6 +2292,11 @@
           <t>H218588</t>
         </is>
       </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
@@ -2079,6 +2304,11 @@
           <t>R521323</t>
         </is>
       </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 250D, 250D-II, 260 P, 260E, 300D-II, 300DW, 300WW, 310 P, 310E, 350 P, 350D, 350G, 380 P, 380G, 400R, 410R, 412R, 600R, 612R, 616R, 644K, 670G, 672G, 703JH, 724 P, 724K, 724L, 744 P, 744K, 744K-II, 744L, 753J, 753JH, 759J, 759JH, 768L-II, 770G, 772G, 800R, 803M, 803MH, 824 P, 824L, 848L, 848L-II, 850J, 850J-II, 850JR, 850L, 850L PL, 853M, 853MH, 859M, 859MH, 870G, 872G, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1270D, 1270E, 1270G, 1470D, 1470E, 1470G, 1710D, 1711D, 1910E, 1910G, 2704, 2854, 2904, 3004, 3154G, 3156G, 3204, 3520, 3522, 3754D, 3754G, 3756G, 4930, 4940, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFS85, 6090HFS86, 6090HFU84, 7180, 7230R, 7250, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7660, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400R, 8430, 8430T, 8530, 9230, 9360R, 9370R, 9540, 9560, 9560 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, C670, CH570, CH670, E330, E360, E380, E400, F4365, R4038, R4044, R4045, R4060, S560, S650, S660, S670, S670H, S760, S770, T560, T660, T670, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
@@ -2086,6 +2316,11 @@
           <t>19M7826</t>
         </is>
       </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 46, 47, 47 IN., 48, 54D IN., 60 IN. DECKS, 60D IN., 62 IN., 260, 270, 280, 313, 315, 318D, 318E, 319D, 319E, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325G, 326D, 326E, 328D, 328E, 329D, 329E, 330G, 331G, 332D, 332E, 332G, 333D, 333E, 333G, 370B, 375, 375A, 385A, 447, 448, 450M, 460M, 460R, 485, 485A, 520M, 525, 530, 535, 540M, 553, 560M, 560R, 563, 565, 568, 572, 575, 578, 582, 592, 614R, 615F, 615P, 615R, 616, 616F, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 622X, 625, 625F, 625R, 625X, 630, 630F, 630R, 630X, 635, 635F, 635R, 635X, 640X, 648L, 648L-II, 673, 700M, 722X, 725X, 730, 730X, 735, 735PF, 735X, 740PF, 740X, 748, 748L, 748L-II, 768L-II, 803M, 803MH, 830, 835, 848L, 848L-II, 853M, 853MH, 859M, 859MH, 890, 895, 896, 903K, 903KH, 909K, 909KH, 909M, 909MH, 913, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 946, 948L, 948L-II, 953K, 956, 959K, 959M, 959MH, 959ML, 1510C, 1510DC, 1512C, 1512E, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1870, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2112C, 2112DC, 2112E, 2254, 2256, 2258, 2264, 2266, 2266E, 2510C, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2956G, 3025E, 3032E, 3033R, 3038E, 3038R, 3039R, 3045R, 3046R, 4044M, 4044R, 4045CC550, 4045HRT83, 4045HRT90, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4890, 4895, 4990, 4995, 5050E, 5060E, 5065M, 5067E, 5070M, 5075E, 5075M, 5080M, 5085E, 5085M, 5090M, 5090R, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 6068HC550, 6180CI510, 7180, 7200, 7210R, 7230R, 7250, 7250R, 7270R, 7280, 7290R, 7300, 7310R, 7350, 7380, 7400, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8500, 8600, 8700, 8800, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9986, 9996, BP15, C300, C350, C400, C670, CP690, CP770, CS690, CT315, CTS, CTS II, DF150, DF250, FR50, FS50, GROUPER, H240, H260, H310, H360, H380, H480, HD35F, HD35R, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, L330, L331, L340, L341, P576, R400, R450, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W235, W260, W540, W550, W650, W660, X9 1000, X9 1100, X300, X304, X310, X320, X324, X340, X360, X500, X520, X530, X534, X540, X590</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
@@ -2100,6 +2335,11 @@
           <t>19M7789</t>
         </is>
       </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-454, 3B-484, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 30 IN., 38 IN., 42 IN., 46, 47, 47 IN., 48, 48 IN., 52 IN., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 110 TLB, 112R, 160G, 180G, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 225C, 230C, 240, 240D, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260E, 270, 270D, 280, 290G, 300D-II, 300DW, 300G, 300WW, 310 P, 310E, 310K, 310K EP, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 312GR, 313, 314G, 315, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330C, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335D, 337E, 344J, 350 P, 350D, 350DW, 350G, 360DC, 370, 370B, 370C, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400D, 400R, 408R, 410 P, 410E, 410E-II, 410K, 410L, 410R, 410TK TMC, 412R, 415, 425, 435, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450C, 450D, 450E, 450H, 450J, 450K, 450M, 455, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 485, 485A, 493, 494, 500R, 521, 522, 524 P, 524K, 524K-II, 524L, 525, 530, 531, 535, 540E, 540G-II, 540G-III, 540H, 541, 542, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550H, 550J, 550K, 550M, 551, 553, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 600C, 600R, 603M, 603R, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608L, 608LH, 608SH, 612C, 612C PERFORMANCE UPGRADES, 612R, 616C, 616C PERFORMANCE UPGRADES, 616R, 618C, 618C PERFORMANCE UPGRADES, 618PF, 620G, 620I, 620PF, 622G, 622PF, 622X, 623, 623M, 623R, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625D, 625I, 625PF, 625X, 630, 630C, 630D, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630X, 631, 635, 635D, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635X, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643D, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650D, 650H, 650J, 650K, 651, 653E, 655K, 661, 670C II, 670CH II, 670D, 670G, 672D, 672G, 673, 678, 690E, 692, 693, 694, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 710D, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740PF, 740X, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 754, 755K, 756, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770C II, 770CH II, 770D, 770G, 772CH II, 772D, 772G, 790, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853G, 853J, 853JH, 853M, 853MH, 854, 855 LONG CHASSIS, 855 SHORT CHASSIS, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 890, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 911, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 994, 995, 997, 1010, 1018, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050K, 1050K PL, 1092, 1175, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1350, 1360, 1404, 1418, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1512FX, 1516FX, 1524FX, 1530, 1535, 1550, 1570, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1785, 1790, 1795, 1830, 1835, 1842GV, 1842HV, 1848GV, 1848HV, 1850, 1854, 1854J, 1870, 1900, 1910, 1910E, 1910G, 1990, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2104, 2154G, 2156G, 2204, 2210, 2254, 2256, 2258, 2264, 2266, 2266E, 2454D, 2510S, 2653, 2654G, 2656G, 2660VT, 2704, 2730, 2854, 2904, 2954D, 3004, 3005, 3025D, 3025E, 3028EN, 3029DF128, 3029DF129, 3029DFG20, 3029DFU20, 3029DFU29, 3029DFU29R, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFU20, 3029TFU29, 3029TFU89, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3120, 3154G, 3156G, 3200, 3203, 3204, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3316, 3320, 3325, 3365, 3400, 3420, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF158, 4045DF271, 4045DFM50, 4045DFM70, 4045HF120, 4045HF150, 4045HF158, 4045HF285, 4045HF286, 4045HF287, 4045HF289, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG93, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045SFM85, 4045T, 4045TF150, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFU20, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5055D, 5055E, 5060E, 5065E, 5065M, 5070E, 5075E, 5075M, 5076E, 5076EL, 5076EN, 5078E, 5080E, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5204, 5205, 5210, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5320, 5325, 5325N, 5400, 5405, 5410, 5415, 5420, 5425, 5430I, 5440, 5460, 5500, 5500N, 5510, 5510N, 5520, 5525, 5603, 5615, 5620, 5625, 5715, 5720, 5730, 5820, 5830, 6010, 6020, 6068AFM75, 6068AFM85, 6068CI550, 6068DF150, 6068HF120, 6068HF150, 6068HF157, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF475, 6068HFC08, 6068HFC09, 6068HFC94, 6068HFC95, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG55, 6068HFG82, 6068HFG94, 6068HFG95, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HI550, 6068HN075, 6068SFM50, 6068SFM75, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF250, 6068TF258, 6068TFM50, 6068TFM75, 6080A E-CUT, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7410, 7420, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7510, 7515, 7520, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, B25C, BH7, BH8, BH9, BH11, C2 400, C6R, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, DB37, DB41, DB44, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E330, E360, E380, E400, F440R, F441M, F441R, F620, F680, F687, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, G15, GROUPER, GS25, GS30, GS45, GS75, GT242, GT262, GT275, GX255, GX325, GX335, GX345, GX355, H260, H310, H340, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX14, JX75, L330, L331, L340, L341, LX172, LX173, LX176, LX178, LX186, LX188, M-GATOR A3, M-GATOR A3T, MaxEmerge XP, N530C, N536C, N540C, N542C, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R400, R450, R500, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W70, W80, W100, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W440, W540, W550, W650, W660, WE80, WE85, WL53, WL56, X9 1000, X9 1100, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z510A, Z520A, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
@@ -2107,6 +2347,11 @@
           <t>Z55241</t>
         </is>
       </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S560, S690</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
@@ -2114,6 +2359,11 @@
           <t>19M7785</t>
         </is>
       </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>2C-280, 2C-284, 2C-300, 2C-304, 2C-324, 2C-350, 2C-354, 3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17HP, 20, 20 Trailer, 26, 30 IN., 30 Trailer, 38 IN., 42 IN., 46, 47, 47 IN., 48, 48 IN., 50 in., 52 IN., 54, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 62 IN. DECKS, 72, 72 IN., 107, 110, 110 TLB, 112R, 120C, 120D, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180A, 180G, 200, 200 G, 200C, 200D, 200G, 204L, 205C, 206C, 207C, 208C, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 220A, 222F, 222R, 230C, 240, 240D, 244J, 244K, 244K-II, 244L, 245, 246, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270C, 270D, 280, 285, 290G, 300, 300C, 300D-II, 300DW, 300F, 300G, 300WW, 304, 304J, 304L, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324E, 324G, 324H, 324J, 324K, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330C, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 338, 339, 344H, 344J, 344K, 344L, 345, 348, 349, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 355, 359, 360, 360DC, 365, 370, 370B, 370C, 370E, 370E-II, 375, 375A, 380 P, 380G, 385A, 390, 400C, 400D, 400D-II, 400F, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 420, 425, 430, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 482C, 485, 485A, 485E, 486E, 488E, 490, 493, 494, 500, 524 P, 524K, 524K-II, 524L, 530, 530B, 533, 540E, 540G-II, 540G-III, 540H, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 553, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 595D, 600R, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620I, 620R, 622, 622F, 622G, 622R, 622X, 623, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625R, 625X, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 639, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643G, 643H, 643J, 643K, 643L, 643L-II, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 649, 650, 650G, 650H, 650J, 650K, 652E, 653, 653E, 653G, 654, 655, 655K, 659, 660R, 663, 663R, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 678, 680R, 683, 683R, 690, 690E, 692, 693, 694, 696, 698, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 700M, 702, 703G, 703GH, 703JH, 704, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 721, 722X, 724 P, 724J, 724K, 724L, 725D, 725X, 726, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735X, 737, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740X, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 762B, 764, 768L-II, 770, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772B, 772BH, 772CH, 772CH II, 772D, 772G, 777, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 995, 997, 1010, 1010D, 1010E, 1010G, 1015, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050J, 1050K, 1050K PL, 1070D, 1070E, 1070G, 1092, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1185, 1210E, 1210G, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1295, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1505, 1510DC, 1510E, 1510G, 1512FX, 1516FX, 1524FX, 1530, 1535, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1800, 1810, 1810DC, 1812DC, 1814DC, 1820, 1830, 1835, 1840, 1846, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1903, 1905, 1910, 1910E, 1910G, 1990, 2010DE, 2014DE, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2054, 2056, 2058, 2064, 2066, 2104, 2112DC, 2144G, 2154D, 2154G, 2156G, 2204, 2210, 2230FH, 2230LL, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2330, 2400 PRECISIONCUT, 2412DE, 2430, 2430C, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510S, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2630, 2633, 2633VT, 2635, 2653, 2653A, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029DFG20, 3029DFS29, 3029DFU20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG80, 3029HFG89, 3029HFU20, 3029HFU80, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG80, 3029TFG89, 3029TFU20, 3029TFU29, 3029TFU80, 3029TFU89, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3316, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4120, 4200, 4210, 4239TF001, 4250, 4300, 4310, 4320, 4400, 4410, 4450, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081HF001, 6081HF070, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, B25C, B30C, B35C, B40C, B350, BP15, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E12, E15, E100, E110, E120, E130, E140, E150, E160, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, FD45, G15, GROUPER, GS25, GS30, GS45, GS75, GT225, GT245, GX85, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX15, HX20, L60, L70, L330, L331, L340, L341, L1524, L1533, L1534, LT150, LT160, LT170, LT180, LT190, LTR180, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M15, M20, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MX15, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R15, R20, R40, R230, R450, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S140, S160, S170, S180, S220, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2546, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, TX 4X2, V451R, V461R, W50, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X105, X106, X107, X115R, X116R, X117R, X125, X126, X127, X135R, X145, X146R, X147R, X155R, X165, X166, X166R, X167, X167R, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z510A, Z520A, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
@@ -2128,6 +2378,11 @@
           <t>R522160</t>
         </is>
       </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 250D, 250D-II, 260 P, 260E, 300D-II, 300DW, 300WW, 310 P, 310E, 318D, 318E, 319D, 319E, 320D, 320E, 323D, 323E, 326D, 326E, 328D, 328E, 329D, 329E, 332D, 332E, 333D, 333E, 350 P, 350D, 350G, 370E, 380 P, 380G, 400R, 408R, 410E, 410R, 412R, 460E, 600R, 612R, 616R, 644K, 670G, 672G, 703JH, 724 P, 724K, 724L, 744 P, 744K, 744K-II, 744L, 753J, 753JH, 759J, 759JH, 768L-II, 770G, 772G, 800R, 803M, 803MH, 824 P, 824K, 824L, 844K, 848L, 848L-II, 850J, 850J-II, 850JR, 850L, 850L PL, 853M, 853MH, 859M, 859MH, 870G, 872G, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1050K, 1270D, 1270E, 1270G, 1470D, 1470E, 1470G, 1710D, 1711D, 1910E, 1910G, 2704, 2854, 2904, 3004, 3154G, 3156G, 3204, 3520, 3522, 3754D, 3754G, 3756G, 4930, 4940, 5075M, 5090M, 5095M, 5100M, 5100ML, 5105M, 5105ML, 5115M, 5115ML, 5120M, 5120ML, 5125ML, 5130M, 5130ML, 6081HF070, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFS85, 6090HFS86, 6090HFU84, 6105AF001, 6105HF001, 6125AF001, 6125AFM01, 6125AFM75, 6125HF001, 6125HF070, 6125SFM75, 6135AFM75, 6135AFM85, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135SFM75, 6135SFM85, 7180, 7200, 7230R, 7250, 7250R, 7260R, 7270R, 7280R, 7290R, 7300, 7310R, 7350, 7380, 7400, 7450, 7480, 7500, 7550, 7580, 7660, 7750, 7760, 7780, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8430, 8430T, 8500, 8530, 8600, 9120, 9220, 9230, 9320, 9320T, 9330, 9360R, 9370R, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9460R, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9560, 9560 STS, 9560R, 9560RT, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9620, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CH570, CH670, CP690, E330, E360, E400, F4365, R4038, R4044, R4045, R4060, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S790, T560, T660, T670, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
@@ -2149,6 +2404,11 @@
           <t>19M7786</t>
         </is>
       </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-454, 3B-484, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 22B, 30 IN., 30 Trailer, 30G, 35G, 42 IN., 46, 47, 47 IN., 48, 48 IN., 50 in., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 62 IN. DECKS, 72 IN., 80, 108, 110, 110 TLB, 112R, 120C, 120D, 120R, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180G, 200, 200 G, 200C, 200D, 200G, 203C, 204K, 204L, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 220R, 230C, 240, 240D, 244E, 244L, 245, 250, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270A, 270B, 270C, 270D, 280, 285, 290G, 300D, 300D-II, 300DW, 300E, 300G, 300WW, 304K, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 344G, 344H, 344J, 344K, 344L, 345, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 355, 360DC, 370, 370B, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400C, 400D, 400D-II, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 420, 430, 435, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444G, 444H, 444J, 444K, 444L, 446, 447, 448, 449, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455G, 456, 457, 458, 459, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 485, 485A, 485E, 486E, 488E, 490, 500R, 520M, 521, 522, 524 P, 524K, 524K-II, 524L, 530B, 531, 533, 535, 540A, 540E, 540G-II, 540G-III, 540H, 540M, 541, 542, 543M, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 553, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 595D, 600R, 603M, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620R, 622, 622F, 622G, 622R, 623, 623M, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625R, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650, 650G, 650H, 650J, 650K, 651, 653, 653E, 653G, 654, 655, 655K, 660R, 661, 663, 663R, 667A, 670, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 678, 680R, 683, 683R, 690E, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 700M, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 725D, 727A, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 731, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755C, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 762B, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772CH, 772CH II, 772D, 772G, 777, 778, 790, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 835 SHORT CHASSIS, 842, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 856, 859M, 859MH, 862, 862B, 864, 870, 870D, 870G, 872D, 872G, 890, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 946, 948L, 948L-II, 950, 950C, 950J, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1050, 1050C, 1050J, 1050K, 1050K PL, 1070, 1070D, 1070E, 1070G, 1107, 1109, 1110D, 1110E, 1110G, 1111, 1113, 1165, 1170, 1170E, 1170G, 1175, 1185, 1200, 1210E, 1210G, 1270D, 1270E, 1270G, 1312C, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1442, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1510C, 1510DC, 1510E, 1510G, 1512C, 1512E, 1517, 1518, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1590, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1654, 1690, 1700, 1705, 1710D, 1711D, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1742HS, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1820, 1830, 1835, 1840, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 1948GV, 1948HV, 1990, 2010DE, 2014DE, 2018, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2104, 2109, 2111, 2112C, 2112DC, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2148HV, 2154D, 2154G, 2156G, 2204, 2210, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2412DE, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500E, 2510C, 2510H, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF120, 3029DF128, 3029DF129, 3029DF150, 3029DF160, 3029DF180, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF158, 3029TF160, 3029TF180, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3316, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4010, 4020DF101, 4020TF006, 4020TF105, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4560, 4600, 4610, 4630, 4650, 4700, 4710, 4720, 4730, 4760, 4830, 4850, 4890, 4895, 4920, 4930, 4940, 4960, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030TF220, 5030TF270, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6059DF001, 6059DF092, 6059T, 6059TF001, 6059TF002, 6059TF003, 6059TF004, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068D, 6068DF, 6068DF001, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081HF001, 6081HF070, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6359DF001, 6359TF001, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, B35C, B40C, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP12C, CP12D, CP18C, CP18D, CP20, CP24C, CP24D, CP30C, CP30D, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DF500, DR12, DR12T, DR16, DR18, DR24, E12, E15, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F510, F525, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, FD45, FD55, FL100, FR50, FS50, G15, GROUPER, GS25, GS30, GS45, GS75, GX85, GX255, GX325, GX355, H240, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2 D, HPX 4X4 D, HX6, HX7, HX10, HX14, HX15, HX20, L17.542, L60, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L1742, L2048, L2548, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX280, LX289, M-GATOR A1, M-GATOR A3, M15, M20, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MH60, MH60C, MX8, MX10, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P556, P576, P660, P670, P680, P690, PC4, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R15, R20, R40, R230, R450, R500, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RC6R, RC7R, RC8M, RC10M, RC10R, RC14R, RC60B, RC60L, RC72, RC72B, RC72L, RC78, RC78B, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, RS72, RSX 850I, RSX860E, RSX860I, RSX860M, RT52, RT66, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SA60, SA72, SB60, SB60B, SB72, SB72B, SB72H, SB78, SB78B, SB78H, SB84, SB84B, SB84H, SD72, SD84, SH12F, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, VR66C, VR73C, VR84C, W50, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X300, X300R, X304, X305R, X310, X320, X324, X340, X354, X360, X384, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
@@ -2156,6 +2416,11 @@
           <t>19M8166</t>
         </is>
       </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>6J-1704, 6J-1904, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 40I, 50I, 200C, 225C, 230C, 250D, 250D-II, 270, 270C, 300D, 300D-II, 300DW, 300WW, 304H, 310 G, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 312GR, 314G, 315 P, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317G, 318G, 320 P, 324H, 325J, 325SK, 325SL, 326D, 326E, 328D, 328E, 329D, 329E, 330C, 330G, 331G, 332D, 332E, 332G, 333D, 333E, 333G, 344H, 344J, 344K, 344L, 350D, 350DW, 360DC, 370, 370C, 400D, 410 P, 410D, 410E, 410G, 410J, 410K, 410L, 450C, 450G, 450H, 450J, 455G, 460DC, 510D, 540E, 540G-II, 540G-III, 540H, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 555G, 600C, 604C, 605C, 606C, 607C, 608C, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 613C, 614C, 615C, 616C, 617C, 620G, 622G, 640E, 640G, 640H, 640L, 640L-II, 644G, 644H, 644HMH, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650D, 650G, 650H, 650J, 655C, 670C, 670CH, 670G, 672CH, 672G, 700H, 700J, 710 P, 710D, 710G, 710J, 710K, 710L, 740G, 744H, 748E, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755C, 759J, 759JH, 764, 770C, 770CH, 770G, 772CH, 772G, 800C, 848H, 848HT, 850, 850C, 850D, 850J, 850J-II, 850JR, 853G, 870G, 872G, 950C, 953G, 1050C, 1100/1150, 1512E, 1810E, 1814E, 1854, 1854J, 2010DE, 2014DE, 2054, 2112E, 2154D, 2154G, 2156G, 2412DE, 2454D, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2654G, 2656G, 2954D, 3154G, 3156G, 3554, 3754D, 3754G, 3756G, 3800, 5060E, 5070E, 5078E, 5080E, 5090E, 5215, 5215F, 5215V, 5300, 5310, 5315, 5315F, 5315V, 5400, 5410, 5415, 5500, 5510, 5515, 5515 HIGH CROP, 5515F, 5515V, 5615, 5615V, 6010, 6020, 6076AFN, 6076HF030, 6081AF001, 6081AFM01, 6081HF001, 6081HF070, 6081HFN02, 6081HFN03, 6081HFN04, 6081TF001, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105HF001, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110M, 6110R, 6115 MC, 6115 RC, 6115J, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125AF001, 6125HF001, 6125J, 6125M, 6125R, 6130, 6130M, 6130R, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140M, 6140R, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205J, 6210, 6210J, 6210M, 6210R, 6215R, 6220, 6220L, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6320, 6320L, 6330, 6330 Premium, 6400, 6400L, 6410, 6420, 6420L, 6420S, 6430, 6430 Premium, 6500L, 6506, 6510, 6510S, 6520, 6520L, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6610, 6620, 6630, 6630 Premium, 6800, 6810, 6820, 6830, 6830 Premium, 6900, 6910, 6910S, 6920, 6920S, 6930, 7130, 7130 Premium, 7200, 7210, 7220, 7230, 7230 Premium, 7320, 7330, 7330 Premium, 7400, 7410, 7430E, 7510, 7530E, 7600, 7610, 7660, 7700, 7710, 7760, 7800, 7810, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, 9986, 9996, BUCK 500, BUCK 650, C670, CP690, CP770, CTS, CTS II, E130, E140, F710, F725, F735, R4040i, R4050i, R4140i, R4150i, S160, S180, S200, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, TRAIL BUCK 500, TRAIL BUCK 650, W110, W150, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
@@ -2163,6 +2428,11 @@
           <t>H152450</t>
         </is>
       </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>614R, 615F, 615P, 615R, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 625F, 625PF, 625R, 630, 630F, 630PF, 630R, 635, 635F, 635PF, 635R, 913, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 1720 CCS, 1725, 1725 CCS, 1725NT, 1765, 1770, 1775, 7760, BP15, CP690, CS690, DR12, DR12T, DR16, DR18, DR24, PLANTER PERFORMANCE UPGRADES, X9 1000, X9 1100, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
@@ -2170,6 +2440,11 @@
           <t>19M7791</t>
         </is>
       </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>3B-504, 3B-554, 3B-604, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20, 26, 30 IN., 31C, 38 IN., 42 IN., 46, 47, 47 IN., 48, 52 IN., 54 in., 54 IN. FRONT BLADE, 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 70, 72 IN., 112R, 120D, 130 P, 130G, 146, 160 P, 160D, 160G, 180G, 200 G, 200D, 200G, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 240, 240D, 245, 246, 250, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270D, 280, 285, 290G, 300, 300CX, 300D-II, 300E, 300G, 300X, 305, 310 P, 310E, 310TK TMC, 312GR, 313, 314G, 314R, 315, 316GR, 317, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 326D, 326E, 328, 328D, 328E, 329D, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333G, 335C, 335D, 337E, 344K, 344L, 350G, 360DC, 370B, 370E, 370E-II, 375, 375A, 380G, 385, 385A, 410, 410 P, 410E, 410E-II, 410K, 410TK TMC, 415, 419, 420, 425, 430, 435, 435C, 437C, 437D, 437E, 440E, 440R, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450, 450K, 450M, 455, 456, 457, 458, 459, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 485, 485A, 500R, 524 P, 524K, 524K-II, 524L, 530, 533, 535, 540A, 540E, 540G-II, 540M, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 546, 547, 548E, 548G-II, 548H, 550, 550K, 550M, 554, 556, 557, 558, 559, 560M, 560R, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 605K, 606C, 606SH, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608L, 608LH, 608SH, 612C, 614R, 615F, 615R, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643D, 643G, 643J, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648E, 648G, 648H, 648L, 648L-II, 650, 650K, 653G, 654, 655, 655K, 660, 663R, 665, 670, 670C II, 670CH II, 670D, 670G, 672D, 672G, 673, 678, 680, 681, 683R, 692, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 710K, 710L, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 741, 744, 744H, 744J, 744K, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-III, 748L, 748L-II, 750K, 750L, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770C II, 770CH II, 770D, 770G, 772CH II, 772D, 772G, 777, 790, 797, 800R, 803M, 803MH, 824J, 824K, 830, 835, 842, 843G, 843J, 843K, 843L, 843L-II, 844J, 844K, 848G, 848L, 848L-II, 850, 850JR, 850K, 850L, 850L PL, 852, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 856, 859M, 859MH, 862, 870D, 870G, 872D, 872G, 892, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 909J, 909JH, 909K, 909KH, 909M, 909MH, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 990, 994, 995, 997, 1010, 1015, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050K, 1107, 1109, 1111, 1113, 1175, 1354, 1404, 1420, 1424, 1424C, 1435, 1445, 1450, 1470, 1512E, 1512FX, 1516FX, 1524FX, 1530, 1535, 1550, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1640, 1690, 1700, 1700T, 1705, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810, 1810E, 1814E, 1820, 1830, 1835, 1840, 1850, 1860, 1870, 1890, 1895, 1900, 1910, 1950, 1950N, 1990, 2010DE, 2014DE, 2020A, 2025R, 2026R, 2027R, 2030A, 2032R, 2036R, 2038R, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2140, 2144G, 2154D, 2154G, 2155, 2156G, 2204, 2243, 2250, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2350, 2355, 2355N, 2412DE, 2450, 2454D, 2510H, 2520, 2530L, 2550, 2555, 2630, 2633, 2633VT, 2635, 2650, 2654G, 2656G, 2704, 2720, 2730, 2750, 2755, 2850, 2854, 2904, 2950, 2954D, 2955, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029HFC03, 3029HFG03, 3029HG530, 3029HI530, 3029TF158, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3040, 3043D, 3045B, 3045R, 3046R, 3050, 3050B, 3055, 3110, 3120, 3140, 3150, 3154G, 3155, 3156G, 3200, 3203, 3204, 3210, 3215, 3220, 3255, 3310, 3316, 3320, 3325, 3350, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3640, 3650, 3720, 3754G, 3756G, 3800, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF158, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF158, 4045HF275, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFU72, 4045HFU79, 4045HFU82, 4045HI550, 4045HLC07, 4045HLC09, 4045HN056, 4045HRT90, 4045T, 4045TF120, 4045TF150, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF271, 4045TF275, 4045TFM50, 4045TFM75, 4045TFU20, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4990, 4995, 5005, 5036D, 5038D, 5039D, 5040D, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080M, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5203S, 5205, 5210, 5220, 5225, 5303, 5305, 5310, 5310N, 5320, 5320N, 5325, 5325N, 5403, 5405, 5410, 5415, 5420, 5420N, 5425, 5425N, 5500N, 5510N, 5520, 5520N, 5525, 5525N, 5600, 5603, 5605, 5610, 5615, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068DF150, 6068HB551, 6068HF120, 6068HF150, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC93, 6068HFG85, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HI550, 6068HT087, 6068SFM50, 6068SFM75, 6068SFM85, 6068TF120, 6068TF150, 6068TF158, 6068TF220, 6068TF250, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFG06, 6090HFG09, 6090HFL75, 6090HFL85, 6090HFM85, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6140B, 6140D, 6140J, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175R, 6180CI510, 6180J, 6190J, 6190M, 6190R, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7200, 7200R, 7205J, 7210, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 9009A, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, BP15, C2 400, C100, C230, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F620, F680, F687, F710, F725, F735, F1145, F4365, FL100, FR21B, FR50, FS20, FS22B, FS50, GROUPER, H160, H240, H260, H310, H340, H360, H380, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, L70, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, M4030, M4040, M4040DN, MaxEmerge XP, N530C, N530F, N536C, N540C, N540F, N542C, N543F, N560F, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R230, R450, R500, R4023, R4030, R4038, R4044, R4045, R4060, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, RSX 850I, RSX860E, RSX860I, RSX860M, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SPRAYER PERFORMANCE UPGRADES, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, V451G, V451M, V461M, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X495, X595, X700, X710, X730, X738, X739, X740, X748, X750, X754, X758, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV590I, XUV590I S4, Y110, Y115, Y210, Y215, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
@@ -2177,6 +2452,11 @@
           <t>19M7889</t>
         </is>
       </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>8RT 310, 8RT 340, 8RT 370, 8RT 410, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 370E, 370E-II, 410 P, 410E, 410E-II, 444J, 444K, 460 P, 460E, 460E-II, 524K, 544H, 544J, 544K, 644J, 644K, 644K HYBRID, 655C, 670C, 670C II, 670CH, 670CH II, 670D, 672CH, 672D, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 724K, 744K, 753J, 753JH, 755C, 759J, 759JH, 770C, 770C II, 770CH, 770CH II, 770D, 772CH, 772CH II, 772D, 824K, 850JR, 859M, 859MH, 870D, 872D, 909J, 909JH, 909K, 909KH, 909M, 909MH, 950C, 950J, 950K, 959J, 959K, 959M, 959MH, 959ML, 1050C, 1050J, 1770, 1775, 1790, 1795, 1830, 1835, 1870, 2730, 3800, 4930, 5065M, 5075M, 5085M, 5090M, 5095M, 5095MH, 5100M, 5100MH, 5100ML, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5120M, 5120ML, 5125ML, 5130ML, 6095B, 6100D, 6100E SALTILLO, 6105D, 6105E, 6105EH, 6110B, 6110D, 6110E SALTILLO, 6115D, 6115E, 6120B, 6120E, 6120EH, 6125D, 6125E SALTILLO, 6130D, 6130E SALTILLO, 6135B, 6140D, 6140E, 6403, 6603, 6803, 7660, 7760, 8100, 8200, 8295RT, 8300, 8310RT, 8320RT, 8335RT, 8345RT, 8360RT, 8370RT, 8400, 8500, 8600, 8700, 8800, 9120, 9220, 9320, 9400, 9410, 9420, 9450, 9470 STS, 9470RT, 9500, 9510, 9520, 9520R, 9520RT, 9540, 9550, 9560, 9560 STS, 9570 STS, 9570RT, 9580, 9600, 9610, 9620, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, C670, CP690, CP770, CS690, CTS, CTS II, E130, E140, E300, E300LC, E330, E360, E380, E400, H540F, H541, H550, H550F, H560F, H561, L1524, L1534, P576, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, TC54H, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
@@ -2184,6 +2464,11 @@
           <t>R248720</t>
         </is>
       </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>9330 - Tractor, 9330 Tractors (Worldwide Edition) - PC10590, , 6135HRW04 - Tractor, 9330 Tractors (Worldwide Edition) - PC10590, , 6135HRW02 - Tractor, 9330 Tractors (Worldwide Edition) - PC10590, , 9430 - Tractor, 9430 Tractor (6135HRW Engine)(Russian Edition) - PC10533, , 6135HRW02 - Tractor, 9430 Tractor (6135HRW Engine)(Russian Edition) - PC10533, , 6135HRW04 - Tractor, 9430 Tractor (6135HRW Engine)(Russian Edition) - PC10533, , 9430 - Tractor, 9430 Tractors (Worldwide Edition) - PC10591, , 6135HRW04 - Tractor, 9430 Tractors (Worldwide Edition) - PC10591, , 6135HRW02 - Tractor, 9430 Tractors (Worldwide Edition) - PC10591, , 9430T - Tractor, 9430T Tractors (Worldwide Edition) - PC10594, , 6135HRW04 - Tractor, 9430T Tractors (Worldwide Edition) - PC10594, , 6135HRW02 - Tractor, 9430T Tractors (Worldwide Edition) - PC10594, , 9530 - Tractor, 9530 Tractors (Worldwide) - PC10592, , 6135HRW01 - Tractor, 9530 Tractors (Worldwide) - PC10592, , 6135HRW04 - Tractor, 9530 Tractors (Worldwide) - PC10592, , 9530T - Tractor, 9530T Tractors (Worldwide Edition) - PC10595, , 6135HRW04 - Tractor, 9530T Tractors (Worldwide Edition) - PC10595, , 6135HRW01 - Tractor, 9530T Tractors (Worldwide Edition) - PC10595, , 9630 - Tractor, 9630 Tractors (Worldwide Edition) - PC10593, , 6135HRW04 - Tractor, 9630 Tractors (Worldwide Edition) - PC10593, , 6135HRW01 - Tractor, 9630 Tractors (Worldwide Edition) - PC10593, , 9630T - Tractor, 9630T Tractors (Worldwide Edition) - PC10596, , 6135HRW04 - Tractor, 9630T Tractors (Worldwide Edition) - PC10596, , 6135HRW01 - Tractor, 9630T Tractors (Worldwide Edition) - PC10596, , 6136NX401 - Picker, Cotton, CP770 Cotton Picker - PC13734, , CP770 - Picker, Cotton, CP770 Cotton Picker - PC13734, , CS770 - Stripper, Cotton, CS770 Cotton Stripper - PC13735, , 6136NX401 - Stripper, Cotton, CS770 Cotton Stripper - PC13735, , 6136HX404 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , 6136HX504 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , X9 1000 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , 1000 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , 6136HX304 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , X9 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , X91000 - Combine, X9 1000 Combine (Worldwide Edition) - PC13708, , 6136HX403 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709, , X9 1100 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709, , 6136HX503 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709, , 1100 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709, , X91100 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709, , X9 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709, , 6136HX303 - Combine, X9 1100 Combine (Worldwide Edition) - PC13709</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
@@ -2191,6 +2476,11 @@
           <t>19M7835</t>
         </is>
       </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 5B-700, 5B-750, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 IN., 30 Trailer, 31C, 42 IN., 46, 47, 47 IN., 48, 48 IN., 50 in., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 80, 102, 105, 108, 110, 110 TLB, 115, 120C, 120D, 125, 130G, 135, 135C, 145, 155C, 160, 160 P, 160C, 160D, 160G, 180B, 180C, 180E, 180G, 180SL, 190C, 200, 200 G, 200C, 200D, 200G, 210 G, 210 P, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 220, 220B, 220C, 220SL, 225C, 230C, 240, 240D, 250, 250 P, 250C, 250D, 250D-II, 250G, 260, 260 P, 260B, 260C, 260E, 260SL, 270, 270C, 270D, 280, 290G, 300 P, 300D, 300D-II, 300DW, 300G, 300WW, 310 G, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315 P, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320 P, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 344 P, 344L, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 360DC, 370B, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400C, 400D, 400D-II, 400R, 408R, 410, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 419, 420, 430, 435, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 446, 447, 448, 449, 450, 450 P, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455G, 456, 457, 458, 459, 459E, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 475, 485, 485A, 485E, 486E, 488E, 490, 490 PRO, 520M, 524 P, 524K, 524K-II, 524L, 530B, 531, 533, 535, 540E, 540G-II, 540G-III, 540H, 543R, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550 P, 550G, 550H, 550J, 550K, 550M, 551, 555G, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 600R, 603R, 604C, 605C, 605K, 606C, 606SH, 607C, 608BH, 608C, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616F, 616R, 617C, 618, 618F, 618R, 620, 620F, 620G, 620I, 620R, 622, 622F, 622G, 622R, 623, 623R, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625F, 625I, 625R, 630, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 631, 633, 635, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 639, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643G, 643H, 643J, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648E, 648G, 648H, 648HT, 648L, 648L-II, 649, 650, 650 P, 650G, 650H, 650J, 650K, 651, 653, 653E, 653G, 654, 655, 655K, 659, 660, 661, 663, 665, 670, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 678, 680, 681, 683, 690E, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 710 P, 710G, 710J, 710K, 710L, 712FC, 712FC PERFORMANCE UPGRADES, 717, 717A, 724 P, 724J, 724K, 724L, 725D, 727, 727A, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 731, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 737, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 755D, 755K, 757, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772B, 772BH, 772CH, 772CH II, 772D, 772G, 777, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 835 SHORT CHASSIS, 842, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855 LONG CHASSIS, 855 SHORT CHASSIS, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 911, 913, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944 X, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 997, 1010E, 1010G, 1023E, 1025R, 1026R, 1050K, 1050K PL, 1070E, 1070G, 1107, 1109, 1110E, 1110G, 1111, 1113, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1270D, 1270E, 1270G, 1312C, 1354, 1404, 1420, 1435, 1442, 1445, 1450, 1470, 1470D, 1470E, 1470G, 1505, 1510C, 1510DC, 1510E, 1510G, 1512C, 1512E, 1515, 1545, 1550, 1565, 1570, 1575, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1690, 1700, 1705, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1742HS, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1820, 1830, 1835, 1840, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 1990, 2010DE, 2014DE, 2020A, 2025R, 2026R, 2027R, 2030A, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2112C, 2112DC, 2112E, 2144G, 2154D, 2154G, 2156G, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2412DE, 2454D, 2500B, 2500E, 2510H, 2510S, 2520, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653B, 2654G, 2656G, 2660VT, 2704, 2720, 2730, 2854, 2904, 2954D, 2956G, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029HFC03, 3029HFG03, 3029HFG89, 3029HFU89, 3029HG530, 3029HI530, 3029TF158, 3029WG401, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3400, 3410, 3420, 3510, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF158, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFS72, 4045HFS80, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4210, 4239TF001, 4310, 4320, 4410, 4520, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5042D, 5045D, 5045E, 5047D, 5050D, 5055D, 5055E, 5060E, 5060EN, 5065E, 5065M, 5070E, 5070M, 5075E, 5075EF, 5075EN, 5075M, 5076E, 5076EF, 5076EN, 5078E, 5080E, 5080EN, 5080M, 5080R, 5082E, 5083E, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5200, 5210, 5220, 5225, 5300, 5310, 5310N, 5320, 5320N, 5325, 5400, 5403, 5410, 5415, 5420, 5420N, 5425, 5430I, 5500, 5500N, 5510, 5510N, 5520, 5520N, 5525, 5600, 5603, 5615, 5620, 5625, 5700, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS77, 6068HFS85, 6068HFS86, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6080A PRECISIONCUT, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6466A, 6466D, 6466T, 6488, 6500, 6500A E-CUT, 6500A PRECISIONCUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6700A PRECISIONCUT, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7505, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, A420R, A520R, B25C, B35C, B40C, BH7, BH8, BH9, BH11, BL6, BL7, BL8, BL9, BL10, BP15, C1 200, C2 300, C2 400, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB84, DB88, DB90, DB96, DB120, DR12, DR12T, DR16, DR18, DR24, E100, E110, E120, E130, E140, E150, E160, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F620, F680, F687, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F4365, FS22B, G15, G110, GS66, GS72, GS78, GS84, GS88, GT72, GT80, GU60, GU66, GU72, GU78, GX255, H240, H260, H540F, H541, H550, H550F, H560F, H561, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HD300, HH30, HH50, HH75, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX815E, HX6, HX7, HX10, HX14, HX15, HX20, L17.542, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L1742, L2048, L2548, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LP72, LP78, LP84, LT150, LT155, LT160, LT170, LT180, LT190, LTR180, LX280, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M4030, M4040, M4040DN, MaxEmerge XP, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, MX5, MX6, MX7, MX8, MX10, MX15, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, P660, P670, P680, P690, PLANTER PERFORMANCE UPGRADES, R2 300, R40, R230, R450, R944I, R952I, R962I, R975I, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RB72, RB84, RB96, RC8M, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S140, S160, S170, S180, S220, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TE 4X2, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X105, X106, X107, X110, X115R, X116R, X117R, X120, X125, X126, X127, X130R, X135R, X140, X145, X146R, X147R, X155R, X165, X166, X166R, X167, X167R, X330, X350, X354, X370, X500, X520, X530, X540, X570, X580, X590, X710, X729, X730, X734, X738, X739, X749, X750, X754, X758, X940, X948, X949, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z245, Z255, Z355E, Z445, Z510A, Z520A, Z625, Z645, Z655, Z665, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
@@ -2198,6 +2488,11 @@
           <t>H125890</t>
         </is>
       </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>215, 216, 218, 220, 222R, 224, 230, 615F, 616, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 625F, 625R, 630, 630F, 630R, 635, 635F, 913, 915F, 915R, 918, 918F, 918R, 920D, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, DB60, DB60T, DB66, DB80, DB120</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
@@ -2205,6 +2500,11 @@
           <t>03H1593</t>
         </is>
       </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>26, 72, 160, 246, 359, 415D, 420D, 425D, 430D, 525D, 530D, 536D, 717, 727, 800, 1415D, 1420D, 1425D, 3950, 3955, 3970, 3975, 5200, 5400, 5440, 5460, 5720, 5730, 5820, 5830, 7722, 8875, D625, D630, D636, W110, W150, W155, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
@@ -2212,6 +2512,11 @@
           <t>19H2898</t>
         </is>
       </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>13HP, 15HP, 16HP, 20 Trailer, 27C ZTS, 30 Trailer, 35C, 40, 42, 47 IN., 50C, 72, 100, 115, 118, 120, 127, 135, 140A, 150, 152, 160A, 180A, 210C, 210LE, 220, 240, 245, 250C, 260, 265, 285, 300, 300C, 300CX, 300D, 300X, 310D, 315D, 320, 328, 330B, 335C, 335D, 337E, 338, 344E, 344G, 348, 350, 360DC, 370E, 400CX, 400X, 410, 410D, 410E, 415D, 419, 420, 420D, 425D, 430, 430D, 435C, 435D, 437C, 437D, 437E, 440D, 444E, 444G, 450, 450G, 450H, 450J, 450K, 455, 455G, 460, 460DC, 460E, 468, 482C, 485E, 486E, 488E, 510D, 520, 530B, 535, 540E, 540G-II, 540G-III, 540H, 544E, 544G, 548E, 548G-II, 548G-III, 548H, 550G, 550H, 550J, 550K, 555G, 570B, 590D, 595D, 605C, 605K, 608BH, 608L, 608LH, 608SH, 620G, 622G, 624E, 624G, 640E, 640G, 640H, 640L, 640L-II, 643D, 643G, 643H, 644E, 644G, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650G, 650H, 650J, 650K, 653E, 653G, 670, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 680, 690E, 700, 703G, 703GH, 703JH, 705, 710D, 726, 740, 740G, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 762B, 764, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772B, 772BH, 772CH, 772CH II, 772D, 772G, 800, 840, 843G, 843H, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 853G, 853J, 853JH, 856, 862B, 870D, 870G, 872D, 872G, 886, 900, 903G, 903J, 903JH, 903K, 903KH, 909J, 909JH, 909K, 913, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 940, 948L, 948L-II, 953G, 953J, 953K, 959J, 959K, 972, 975, 980, 985, 995, 1040, 1140, 1160A, 1165, 1170, 1175, 1180A, 1350, 1415D, 1420D, 1425D, 1430D, 1435D, 1440D, 1445D, 1450, 1538HR, 1550, 1640, 1646, 1646HS, 1720, 1725, 1750, 1800, 1840, 1850, 1870, 1950, 1950N, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2140, 2150, 2154D, 2155, 2200, 2210, 2210LL, 2250, 2254, 2255, 2256, 2258, 2264, 2266, 2266E, 2350, 2355, 2355N, 2400, 2410, 2410C, 2450, 2454D, 2510C, 2510H, 2510S, 2550, 2555, 2650, 2750, 2755, 2850, 2950, 2954D, 2955, 3040, 3050, 3055, 3140, 3150, 3155, 3215, 3215B, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3255, 3325, 3350, 3365, 3510, 3520, 3522, 3640, 3650, 3754D, 3950, 3955, 3970, 3975, 4039D, 4039DF001, 4039DF092, 4039T, 4039TF001, 4045D, 4045DF001, 4045TF001, 4045TF092, 4055, 4219DF01, 4239DF001, 4239DT004, 4250, 4255, 4276DF01, 4276T, 4276TF01, 4450, 4455, 4475, 4555, 4630, 4650, 4700, 4710, 4720, 4730, 4755, 4830, 4850, 4890, 4895, 4920, 4930, 4955, 4990, 4995, 5200, 5400, 5430I, 5575, 5720, 5730, 5820, 5830, 6059DF001, 6059DF092, 6059T, 6059TF001, 6059TF002, 6059TF003, 6059TF004, 6068D, 6068DF, 6068DF001, 6329DF01, 6359DF001, 6359TF001, 6414D, 6414T, 6414TDW14, 6414TDW16, 6610, 6650, 6675, 6700, 6710, 6750, 6810, 6850, 6910, 6950, 7455, 7460, 7600, 7610, 7700, 7710, 7775, 7800, 7810, 8875, 9650 STS, 9750 STS, 9996, AB21, AB31, AB32, AB42, AB43, B25C, B30C, BA72, BA84, BL6, BL6B, BL7, BL7B, BL8, BL8B, BL9, BL9B, BL10, BP72, BP84, BV6, BV8, BV9, CA15, CH330, CH530, CH570, CH670, DB84, DB96, G100, GS66, GS72, GS78, GS84, GS88, GT72, GT80, GU60, GU66, GU72, GU78, H160, H165, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HH30, HH50, HH75, LP72, LP78, LP84, MC519, MCS, ME36, ME50, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, NF44, PA15, PA15B, PA30, PA30B, PLANTER PERFORMANCE UPGRADES, PR60, PR72B, PR72S, PR84B, PR96B, R4023, RB72, RB84, RB96, RL66, RL84, ROW-CROP HARVESTING UNITS, RT55, RT73, SP8, SP8C, SP10, SP10C, TC125, TR36B, TR48B, TR60B, W110, W150, W155, W170, X500, X520, X530, X534, X540</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
@@ -2219,6 +2524,16 @@
           <t>03H1810</t>
         </is>
       </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>15, 44 IN. SNOW BLOWERS, 47 IN., 54 IN., 60 IN., 215, 216, 218, 220, 222R, 224, 230, 918, 920D, 1640, 2040, 2040S, 2140, 2250, 2350, 2355, 2450, 2550, 2555, 2650, 2750, 2755, 2850, 2950, 2955, 3040, 3050, 3055, 3140, 3150, 3155, 3255, 3350, 3640, 3650, 4055, 4250, 4255, 4450, 4455, 4555, 4560, 4650, 4755, 4760, 4850, 4955, 4960, 7260, 7660, 7760, 8430, 8440, 8450, 8630, 8640, 8650, 8850, 9935, 9970, 9996, CP690, MC519, X500, X520, X530, X534, X540</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
@@ -2226,6 +2541,11 @@
           <t>19M7829</t>
         </is>
       </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>210 G, 210 P, 210K, 210K EP, 210L, 210L EP, 210LJ, 312GR, 316GR, 454, 520M, 540M, 543M, 553, 563, 568, 578, 603M, 615F, 616, 616F, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 623, 623M, 625D, 625F, 625R, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 643M, 644, 645FD, 645FD PERFORMANCE UPGRADES, 653, 654, 673, 678, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 735FD PERFORMANCE UPGRADES, 740FD, 740FD PERFORMANCE UPGRADES, 744, 745FD, 745FD PERFORMANCE UPGRADES, 748, 853, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1175, 1470, 1570, 2510H, 2510S, 4320, 4500, 4520, 4600, 4610, 4700, 4710, 4720, 4890, 4895, 6090AFM75, 6090AFM85, 6090SFM75, 6090SFM85, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7460, 7660, 8100, 8200, 8300, 8320RT, 8345RT, 8370RT, 8400, 8500, 8600, 8700, 8800, 9470 STS, 9500, 9560 STS, 9570 STS, 9600, 9650 STS, 9660 STS, 9670 STS, 9700, 9750 STS, 9760 STS, 9770 STS, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9976, 9986, 9996, C850, CP20, CP690, CP770, CS690, CS770, DB37, DB44, H240, H260, H310, H340, H360, H380, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S690, S760, S770, S780, S785, S790, T550, T560, T660, T670, W330, W540, W550, W650, W660, X9 1000, X9 1100</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
@@ -2233,6 +2553,16 @@
           <t>19H1801</t>
         </is>
       </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 25A, 31C, 72, 108, 111, 112L, 160, 215, 216, 218, 220, 222R, 224, 224T, 224WS, 230, 300D, 310D, 315D, 318, 332, 332T, 336T, 336WS, 339, 342T, 346T, 349, 350, 359, 370, 410, 410D, 420, 450, 450G, 455G, 456, 456T, 456W, 459, 466, 485E, 486E, 488E, 510, 510D, 520M, 522, 525D, 530D, 536D, 540M, 540R, 542, 544E, 544G, 550, 550G, 553, 555G, 563, 570, 570B, 624, 624E, 624G, 635, 643H, 645, 647, 650G, 655, 660, 665, 670, 670B, 672B, 673, 680, 681, 703JH, 740, 753J, 753JH, 759J, 759JH, 800, 840, 843, 843H, 862B, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920D, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 940, 1040, 1140, 1200, 1200A, 1200H, 1640, 1835, 1840, 1870, 1890, 1895, 2040, 2040S, 2054, 2056, 2058, 2140, 2150, 2243, 2255, 2350, 2550, 2680H, 2750, 2950, 3040, 3055, 3140, 3150, 3179DF, 3179T, 3215, 3215B, 3225B, 3235, 3235B, 3255, 3635, 3640, 3645, 3760, 3765, 4055, 4219DF01, 4239A, 4239D, 4250, 4255, 4450, 4455, 4555, 4560, 4650, 4730, 4755, 4760, 4830, 4850, 4920, 4955, 4960, 5200, 5300, 5400, 5440, 5460, 5500, 5720, 5730, 5820, 5830, 6081HFN01, 6081HFN02, 6081HFN03, 6081HFN04, 6090 MC, 6095 MC, 6095 RC, 6100 MC, 6101HF010, 6101HF011, 6105 MC, 6105 RC, 6105M, 6105R, 6110 MC, 6110M, 6110R, 6115 MC, 6115 RC, 6115M, 6115R, 6120M, 6120R, 6125M, 6125R, 6130M, 6130R, 6135M, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155M, 6155R, 6155RH, 6170M, 6175M, 6195M, 6359A, 6359T, 6400, 6414D, 6414T, 6414TDW14, 6414TDW16, 6610, 6619A, 6619A Engine SE500219, 6619A Engine SE500493, 6619A Engine SE500087, 6619A Engine SE500089, 6619A Engine SE500090, 6619A Engine SE500091, 6619TF-01, 6620, 6700, 6710, 6810, 6910, 7020, 7520, 7600, 7610, 7700, 7710, 7720, 7721, 7722, 7800, 7810, 7820, 7920, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8300, 8300T, 8310, 8310T, 8320, 8320T, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8440, 8450, 8520, 8520T, 8560, 8570, 8630, 8640, 8650, 8760, 8770, 8820, 8850, 8870, 8960, 8970, 9501, 9570 STS, 9935, 9970, A420R, A520R, BA72, BA84, BP72, BP84, CA15, CP12C, CP12D, CP18C, CP18D, CP24C, CP24D, CP30C, CP30D, D625, D630, D636, F910, F911, F930, LP72, LP78, LP84, MH60, MH60C, PA15, PA15B, PA30, PA30B, PR60, PR72B, PR72S, PR84B, PR96B, RC60B, RC60L, RC72, RC72B, RC72L, RC78, RC78B, RL66, RL84, RS72, RT52, RT55, RT66, RT73, S80, S82, S92, SA60, SA72, SB60, SB60B, SB72, SB72B, SB72H, SB78, SB78B, SB78H, SB84, SB84B, SB84H, SD72, SD84, TR36B, TR48B, TR60B, VR66C, VR73C, VR84C, W36M, W48M, WG32A, WG36A, WG48A, WH61A, WHP36A, WHP48A, WHP52A, WHP61A, Z915E, Z920M, Z925M, Z930M, Z930R, Z945M, Z950M, Z950R, Z955M, Z955R, Z960M, Z970R</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
@@ -2240,6 +2570,11 @@
           <t>03H1512</t>
         </is>
       </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>7H17, 7H19, 47 IN., 54 IN. HEAVY DUTY SNOWBLOWER, 59 IN., 60, 60 IN. HEAVY DUTY SNOWBLOWER, 100, 140A, 150, 160A, 180A, 359, 415D, 420D, 425D, 430D, 435D, 440D, 1023E, 1025R, 1160A, 1180A, 1520, 1530, 1535, 2025R, 2032R, 2038R, 2410C, 2430, 2430C, 2680H, 3025E, 3032E, 3033R, 3038E, 3038R, 3039R, 3045R, 3046R, 4044M, 4044R, 4052M, 4052R, 4250, 4450, 8450, 8650, 8850, BA96, GS88, HH75, HH80, HH100, PA40, PC10, SP10B, SP12B, W110, W150, W155</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
@@ -2247,6 +2582,11 @@
           <t>03H1463</t>
         </is>
       </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>30, 31C, 37, 46, 47, 48, 72, 100, 102, 105, 115, 125, 135, 140A, 145, 150, 155C, 160, 160A, 180A, 190C, 224T, 224WS, 240, 245, 260, 265, 285, 320, 328, 332, 332T, 336T, 336WS, 338, 339, 342T, 346T, 348, 349, 350, 359, 370, 370B, 375, 375A, 385A, 410, 415D, 420D, 425D, 430D, 435D, 440D, 447, 448, 450, 456, 456T, 456W, 459, 466, 468, 485, 485A, 510, 524D, 550, 570, 647, 655, 660, 665, 670, 673, 680, 681, 724D, 826D, 828D, 872, 874, 876, 924DE, 972, 1032D, 1128DDE, 1128DE, 1160A, 1180A, 1332DDE, 1415D, 1420D, 1425D, 1430D, 1435D, 1440D, 1445D, 2950, 2955, 3040, 3050, 3140, 3350, 3950, 3970, 3975, 4475, 5200, 5400, 5440, 5460, 5575, 5720, 5730, 5820, 5830, 6620, 6675, 7720, 7721, 7722, 7775, 8820, 8875, BD1108, BD1110, BD1113, D130, G110, L100, L105, L107, L108, L110, L111, L118, L120, L130, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA140, LA145, LA150, LA155, MCS, ROW-CROP HARVESTING UNITS, W110, W150, W155, WH36A, WH48A, WH52A, WH61A, X110, X120, X140</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
@@ -2254,6 +2594,11 @@
           <t>19H1813</t>
         </is>
       </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>13HP, 15HP, 16HP, 72, 107, 108, 111, 112L, 148, 158, 168, 170, 175, 180, 185, 190E, 210LE, 215, 216, 218, 220, 222R, 224, 230, 240, 243, 244, 250, 260, 270, 280, 290D, 310G, 310SG, 313, 315, 315SG, 317, 318E, 319E, 320, 320E, 323E, 324E, 325, 326E, 328, 328E, 329E, 332, 332E, 333E, 338, 342T, 343, 344, 344E, 344G, 346T, 348, 349, 350, 359, 360, 370, 390, 410, 410G, 443, 444, 444E, 444G, 450, 450G, 450H, 450J, 455, 455G, 456, 456T, 456W, 459, 466, 468, 482C, 490E, 510, 524D, 540E, 540G-II, 540G-III, 540H, 543, 546, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 555G, 570, 570B, 590D, 595D, 640E, 640G, 640H, 643, 644, 645, 648E, 648G, 648H, 648HT, 650G, 650H, 650J, 653E, 655, 655K, 670B, 670C, 670C II, 670CH, 670CH II, 672B, 672CH, 700H, 710G, 724D, 740G, 748E, 748G-II, 748G-III, 748H, 748HT, 750A, 750C, 750J, 755, 755K, 756, 762B, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 772B, 772BH, 772CH, 772CH II, 772D, 800, 826D, 828D, 840, 843, 844, 848H, 848HT, 850C, 850J, 855, 856, 862B, 870D, 872D, 886, 940, 955, 960, 980, 985, 1032D, 1040, 1140, 1243, 1350, 1408, 1438GS, 1438HS, 1520, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1550, 1560, 1590, 1640, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1700, 1720, 1725, 1725 CCS, 1725C, 1750, 1775NT, 1790, 1795, 1840, 1850, 1860, 1890, 1895, 1950, 1950N, 1990, 2000 SERIES, 2020A, 2030A, 2040, 2040S, 2054, 2056, 2058, 2140, 2150, 2155, 2243, 2250, 2254, 2255, 2256, 2258, 2350, 2355, 2355N, 2400 PRECISIONCUT, 2450, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2510S, 2550, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2555, 2650, 2653, 2653A, 2653B, 2700, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2750, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2755, 2850, 2950, 2955, 3029D, 3029DF120, 3029DF128, 3029DF129, 3029DF150, 3029T, 3029TF120, 3029TF150, 3029TF158, 3040, 3050, 3055, 3140, 3150, 3155, 3179DF, 3179T, 3215, 3235, 3255, 3300, 3310, 3350, 3400, 3410, 3640, 3650, 3760, 3765, 3950, 3970, 4039D, 4039DF001, 4039DF004, 4039DF005, 4039DF006, 4039DF008, 4039DF031, 4039DF032, 4039DF092, 4039T, 4039TF001, 4039TF007, 4039TF008, 4045D, 4045DF001, 4045DF120, 4045DF150, 4045DF158, 4045DF271, 4045HF120, 4045HF150, 4045HF158, 4045TF001, 4045TF120, 4045TF150, 4045TF151, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF271, 4055, 4239A, 4239D, 4239TF001, 4250, 4255, 4276DF01, 4276T, 4276TF01, 4450, 4455, 4555, 4560, 4650, 4700, 4710, 4755, 4760, 4850, 4955, 4960, 5200, 5300, 5310N, 5320N, 5400, 5420N, 5440, 5460, 5500, 5500N, 5510N, 5520N, 5720, 5730, 5820, 5830, 6059DF092, 6059T, 6059TF, 6059TF003, 6068DF150, 6068HF150, 6068HF157, 6068HF158, 6068HF250, 6068HF258, 6068TF092, 6068TF120, 6068TF150, 6068TF157, 6068TF158, 6068TF220, 6068TF250, 6068TF258, 6076AFM00, 6076AFM30, 6076AFN, 6076HF030, 6076TF, 6081HFN01, 6081HFN02, 6081HFN03, 6101HF010, 6101HF011, 6359A, 6359T, 6414D, 6414T, 6414TDW14, 6414TDW16, 6466A, 6466D, 6466T, 6610, 6619A, 6619A Engine SE500219, 6619A Engine SE500493, 6619A Engine SE500087, 6619A Engine SE500089, 6619A Engine SE500090, 6619A Engine SE500091, 6619TF-01, 6620, 6710, 6810, 6910, 7020, 7520, 7600, 7700, 7720, 7721, 7722, 7800, 8100, 8100T, 8200, 8200T, 8300, 8300T, 8400, 8400T, 8430, 8440, 8450, 8560, 8570, 8630, 8640, 8650, 8760, 8770, 8820, 8850, 8870, 8875, 8960, 8970, 9100, 9200, 9300, 9400, 15538, AB21, AB31, AB32, AB42, AB43, BD1108, BD1110, BD1113, BL6B, BL7B, BL8B, BL9B, BV6, BV8, BV9, CT315, CT322, CT332, DB37, DB44, DB60, DB66, DB80, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, F510, F525, F910, F911, F912, F915, F925, F930, F932, F935, F1145, G100, GX255, HD200, HD300, MCS, NF44, PLANTER PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S80, S82, S92, SP8, SP8C, SP10, SP10C, STX30, STX38, TRS22, TRS24, TRS26, TRS27, TRS32, TRX24, TRX26</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
@@ -2261,6 +2606,11 @@
           <t>19H2969</t>
         </is>
       </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>17 ZTS, 27 ZTS, 27C ZTS, 35C, 35ZTS, 110 TLB, 175, 240, 245, 300D, 310D, 315D, 335, 375, 440E, 446, 447, 449, 450E, 458, 459, 459E, 468, 520, 521, 522, 531, 540, 540A, 540E, 540G-II, 541, 542, 546, 547, 548E, 548G-II, 551, 608L, 608LH, 608SH, 610, 620, 631, 636M, 640, 640E, 640G, 648E, 648G, 648M, 650, 651, 652M, 661, 670B, 672B, 680, 714, 726, 730, 730LL, 735, 740A, 740G, 748E, 748G-III, 750C, 753G, 753GH, 753GL, 770B, 770BH, 772B, 772BH, 850C, 872, 874, 876, 900, 911, 913V, 915V, 960, 980, 995, 1200, 1550, 1750, 1850, 1950, 1950N, 2200, 2210, 2210LL, 2250, 2254, 2310, 2400, 2410, 2410C, 2430, 2430C, 2450, 2510C, 2510H, 2510S, 2650, 2700, 2850, 3510, 3520, 3522, 3760, 3765, 3950, 3955, 3970, 3975, 4039D, 4039DF001, 4039DF092, 4039T, 4039TF001, 4045D, 4045DF001, 4045TF001, 4055, 4250, 4255, 4450, 4455, 4555, 4560, 4650, 4755, 4760, 4850, 4955, 4960, 5045D, 5045E, 5050E, 5055D, 5055E, 5065E, 5065M, 5075E, 5075M, 5083E, 5083EN, 5085E, 5085M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100R, 5101E, 5101EN, 5105M, 5105ML, 5115M, 5115R, 5125R, 5210, 5225, 5305, 5310, 5325, 5325N, 5425, 5425N, 5525, 5525N, 5603, 5625, 6068TF092, 6359DF001, 6359TF001, 6700, 7200, 7210, 7220, 7320, 7400, 7410, 7420, 7510, 7520, 7600, 7610, 7700, 7710, 7800, 7810, 8100, 8200, 8300, 8400, BH7, BH8, BH9, BH11, CH570, CH670, ROW-CROP HARVESTING UNITS</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
@@ -2268,6 +2618,11 @@
           <t>19H2233</t>
         </is>
       </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>11, 140A, 160A, 180A, 342T, 346T, 350, 370, 410, 415D, 420D, 425, 425D, 430D, 435D, 440D, 450, 455, 456, 456T, 456W, 459, 466, 509, 510, 550, 570, 609, 610, 680, 709, 726, 735, 856, 886, 913V, 915V, 940, 955, 985, 1040, 1140, 1160A, 1180A, 1415D, 1420D, 1425D, 1430D, 1435D, 1440D, 1445D, 1550, 1750, 1810, 1850, 1950, 1950N, 2200, 2210, 2400, 2410, 2430, 2950, 2955, 3040, 3050, 3055, 3140, 3150, 3155, 3255, 3350, 3640, 3650, 3760, 4055, 4250, 4255, 4450, 4455, 4650, 4850, 5038D, 5050E, 5103, 5103E, 5103S, 5104, 5200, 5203, 5203S, 5204, 5210, 5310, 5400, 5440, 5460, 5610, 5720, 5820, 6359A, 6359T, 7520, BA72, BA84, BP72, BP84, CA15, LP72, LP78, LP84, MP25, MX425, PA15, PA15B, PA30, PA30B, PR60, PR72B, PR72S, PR84B, PR96B, RL66, RL84, RT55, RT73, TR36B, TR48B, TR60B, W110, W150, W155</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
@@ -2275,6 +2630,11 @@
           <t>19H2641</t>
         </is>
       </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>22B, 100, 112, 115, 118, 120, 140A, 160A, 180A, 210C, 210LE, 220, 300D, 310D, 315D, 328, 338, 348, 350C, 350D, 350D-II, 350DW, 400C, 400D, 400D-II, 410D, 450, 456, 456T, 456W, 466, 468, 509, 510D, 512, 520, 520M, 521, 522, 541, 542, 553, 563, 570B, 609, 610, 620G, 622G, 643D, 643G, 643H, 644H, 644HMH, 644J, 653G, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 680, 709, 714, 724J, 726, 730, 730LL, 740, 740A, 762B, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772B, 772BH, 772CH, 772CH II, 772D, 772G, 780, 785, 790, 843G, 843H, 850, 856, 870D, 870G, 872, 872D, 872G, 874, 876, 886, 940, 950, 955, 960, 980, 985, 1010, 1015, 1023E, 1025R, 1026R, 1030, 1035, 1040, 1050, 1140, 1160A, 1180A, 1550, 1560, 1590, 1640, 1750, 1850, 1950, 1950N, 2025R, 2026R, 2032R, 2038R, 2040, 2040S, 2140, 2150, 2200, 2210, 2210LL, 2250, 2254, 2255, 2300, 2310, 2320, 2350, 2355, 2400, 2410, 2410C, 2430, 2430C, 2450, 2520, 2550, 2555, 2650, 2720, 2750, 2755, 2850, 3025D, 3025E, 3032E, 3033R, 3035D, 3036E, 3038E, 3038R, 3039R, 3040, 3043D, 3045R, 3046R, 3050, 3120, 3140, 3320, 3350, 3510, 3520, 3522, 3650, 3720, 3950, 3955, 3970, 3975, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4120, 4320, 4520, 4720, 4730, 4830, 5065M, 5075M, 5076EN, 5083EN, 5085E, 5085M, 5090EN, 5090M, 5090R, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101EN, 5105M, 5115M, 5115ML, 5115R, 5125M, 5125R, 5200, 5210, 5225, 5300, 5310, 5325, 5325N, 5400, 5410, 5415, 5425, 5425N, 5500, 5510, 5525, 5525N, 5615, 5625, 5715, 5725, 6100, 6200, 6200L, 6300, 6300L, 6400, 6400L, 6500, 6500L, 6600, AB21, AB31, AB32, AB42, AB43, B35C, B40C, BA72, BA84, BL6B, BL7B, BL8B, BL9B, BP72, BP84, BV6, BV8, BV9, CA15, CH570, CH670, H240, LP72, LP78, LP84, MP25, MX225, NF44, PA15, PA15B, PA30, PA30B, PR60, PR72B, PR72S, PR84B, PR96B, RL66, RL84, RT55, RT73, SP8, SP8C, SP10, SP10C, TR36B, TR48B, TR60B, W150, W155</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
@@ -2282,6 +2642,11 @@
           <t>19M7812</t>
         </is>
       </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>3-Bag, 5E-850, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 6R 155, 6R 165, 6R 175, 6R 195, 6R 215, 7R 210, 7R 230, 7R 250, 7R 270, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20, 20 Trailer, 30 Trailer, 47 IN., 54, 54 in., 60 in., 72 IN., 112R, 120C, 120D, 160, 160C, 200, 200C, 210 G, 210 P, 210L, 210L EP, 210LJ, 230C, 240, 240D, 250, 250 P, 250C, 250D, 250D-II, 250G, 260, 260E, 270, 270C, 270D, 280, 290G, 300 P, 300D-II, 300DW, 300WW, 310 P, 310E, 310L, 310L EP, 310SE, 310SL, 310SL HL, 312GR, 314G, 315SE, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320 P, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 325, 325SL, 326E, 330B, 335, 335C, 337E, 344 P, 344H, 344J, 344K, 344L, 345, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 360DC, 370E, 380 P, 380G, 400C, 400D, 400D-II, 408R, 410 P, 410E, 410L, 435C, 437C, 437E, 440E, 444 G, 444J, 444K, 450 P, 450C, 450E, 450M, 454, 460DC, 460E, 460M, 460R, 470 P, 470G, 524 P, 524K, 524K-II, 524L, 540G-II, 540G-III, 540H, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 548G-II, 548G-III, 548H, 550, 550K, 550M, 560M, 560R, 600C, 605C, 605K, 620G, 622G, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 640G, 640H, 640L, 640L-II, 643G, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 648G, 648H, 648HT, 648L, 648L-II, 650K, 653, 654, 655K, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 690E, 692, 700K, 703JH, 710 P, 710L, 717, 724J, 724K, 727, 730LL, 737, 740G, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750J, 750J-II, 750K, 753J, 753JH, 755K, 757, 759J, 759JH, 768L-II, 770G, 772G, 777, 797, 803M, 803MH, 824J, 824K, 843G, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853, 853M, 853MH, 859M, 859MH, 870G, 872G, 891, 892, 894, 903K, 903KH, 903M, 903MH, 904 P, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 944 X, 944K, 948L, 948L-II, 950K, 953K, 953M, 953MH, 959K, 959M, 959MH, 959ML, 995, 1010G, 1035, 1050K, 1050K PL, 1070E, 1070G, 1092, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1270D, 1270E, 1270G, 1290, 1293, 1295, 1354, 1404, 1450, 1470, 1470D, 1470E, 1470G, 1510DC, 1510E, 1510G, 1512E, 1550, 1570, 1600 TURBO SERIES III, 1612DE, 1690, 1700, 1700T, 1705, 1705T, 1710D, 1711D, 1715, 1720 CCS, 1725T, 1745, 1755, 1770NT, 1775, 1775NT, 1785, 1790, 1795, 1810DC, 1810E, 1812DC, 1814DC, 1814E, 1830, 1835, 1850, 1854, 1854J, 1870, 1890, 1895, 1910, 1910E, 2010DE, 2014DE, 2025R, 2032R, 2036R, 2038R, 2054, 2112DC, 2112E, 2154G, 2156G, 2204, 2230FH, 2254, 2256, 2258, 2264, 2266, 2266E, 2300, 2310, 2400, 2412DE, 2454D, 2654G, 2656G, 2704, 2854, 2904, 2954D, 3004, 3029DF128, 3029TF158, 3110, 3154G, 3156G, 3200, 3204, 3210, 3215, 3220, 3310, 3400, 3410, 3420, 3520, 3522, 3754D, 3754G, 3756G, 3800, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HSG20, 4045HSG21, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF250, 4045TF253, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4239TF001, 4510, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4930, 4940, 4990, 4995, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5060E, 5070E, 5078E, 5080E, 5085E, 5090E, 5200, 5210, 5300, 5310, 5400, 5410, 5415, 5420, 5500, 5510, 5520, 5615, 5715, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HSG22, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6081AF001, 6081AFM75, 6081HF001, 6081HF070, 6081TF001, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6095B, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110M, 6110R, 6115D, 6115E, 6115J, 6120B, 6120E, 6120EH, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125SFM75, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6205J, 6210J, 6210M, 6210R, 6215R, 6320, 6400, 6403, 6415, 6420, 6420S, 6520, 6603, 6620, 6650, 6700, 6750, 6810, 6820, 6830, 6850, 6910, 6910S, 6920, 6920S, 6930, 6950, 7180, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210J, 7210R, 7215J, 7215R, 7225J, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7420, 7425, 7450, 7455, 7460, 7480, 7500, 7505, 7515, 7520, 7525, 7550, 7580, 7630, 7660, 7700, 7720, 7730, 7750, 7760, 7780, 7800, 7820, 7830, 7850, 7920, 7930, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8430, 8430T, 8500, 8530, 8600, 8800, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, 9986, 9996, A400, B25C, B35C, B40C, C1 200, C2 300, C2 400, C100, C110, C120, C230, C240, C440, C670, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CTS, CTS II, DB37, DB44, DB55, DB58, DB60, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F710, F725, F735, FC20M, FC20R, G15, GS25, GS30, GS45, GS75, GT225, GT242, GT245, GT262, GT275, GX255, GX325, GX335, GX345, GX355, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, L70, LT190, LX172, LX173, LX176, LX178, LX186, LX188, M20, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, R2 300, R20, R230, R450, R500, R4023, R4030, R4038, R4044, R4045, R4060, RSX 850I, RSX860E, RSX860I, RSX860M, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, STX38, STX46, T550, T560, T660, T670, TC54H, TC62H, TURF TX 4X2, TX 4X2, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, X950R, Y110, Y115, Y210, Y215, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
@@ -2289,6 +2654,11 @@
           <t>R521323</t>
         </is>
       </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 250D, 250D-II, 260 P, 260E, 300D-II, 300DW, 300WW, 310 P, 310E, 350 P, 350D, 350G, 380 P, 380G, 400R, 410R, 412R, 600R, 612R, 616R, 644K, 670G, 672G, 703JH, 724 P, 724K, 724L, 744 P, 744K, 744K-II, 744L, 753J, 753JH, 759J, 759JH, 768L-II, 770G, 772G, 800R, 803M, 803MH, 824 P, 824L, 848L, 848L-II, 850J, 850J-II, 850JR, 850L, 850L PL, 853M, 853MH, 859M, 859MH, 870G, 872G, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1270D, 1270E, 1270G, 1470D, 1470E, 1470G, 1710D, 1711D, 1910E, 1910G, 2704, 2854, 2904, 3004, 3154G, 3156G, 3204, 3520, 3522, 3754D, 3754G, 3756G, 4930, 4940, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFS85, 6090HFS86, 6090HFU84, 7180, 7230R, 7250, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7660, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400R, 8430, 8430T, 8530, 9230, 9360R, 9370R, 9540, 9560, 9560 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, C670, CH570, CH670, E330, E360, E380, E400, F4365, R4038, R4044, R4045, R4060, S560, S650, S660, S670, S670H, S760, S770, T560, T660, T670, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
@@ -2296,6 +2666,11 @@
           <t>19M7836</t>
         </is>
       </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>6R 230, 6R 250, 6R 2304, 7G18, 7H17, 7H19, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 75D, 120D, 130 P, 130G, 135G, 160 P, 160G, 180G, 200, 200 G, 200C, 200D, 200G, 210 P, 210G, 210K, 210L, 225D, 230C, 240D, 245G, 250 P, 250D-II, 250G, 260 P, 260E, 270, 270C, 270D, 290G, 300 P, 300D-II, 300G, 310 P, 310E, 310K, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 315 P, 315SL, 318E, 319E, 320 P, 320E, 323E, 324E, 325SL, 326E, 328E, 329E, 332E, 333E, 337E, 344 P, 344K, 344L, 350 P, 350G, 360DC, 370E, 370E-II, 380 P, 380G, 410 P, 410E, 410E-II, 410K, 410L, 410TK TMC, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 450 P, 450C, 450D, 450K, 460 P, 460E, 460E-II, 460M, 460R, 468, 469, 524 P, 524K, 524K-II, 524L, 540G-III, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 548G-III, 550 P, 550K, 560M, 560R, 568, 569, 605K, 606SH, 608SH, 616, 616R, 618, 620, 620G, 622, 622G, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625F, 630, 630D, 635, 635D, 635F, 640D, 640G, 640L, 640L-II, 643H, 643L, 643L-II, 644 G, 644 P, 644 X, 644J, 644K, 644K HYBRID, 644L, 644LH, 648G, 648L, 648L-II, 650 P, 650D, 650K, 653E, 653G, 655K, 670G, 672G, 700K, 700L, 700L PL, 710 P, 710K, 710L, 724 P, 724K, 724L, 730D, 735D, 740, 740D, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748L, 748L-II, 750K, 750L, 753J, 753JH, 755K, 759J, 759JH, 764, 768L-II, 770G, 772G, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 843H, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848L, 848L-II, 850K, 850L, 853M, 853MH, 859M, 859MH, 870G, 872G, 903M, 904 P, 910G, 944 X, 944K, 948L, 948L-II, 950K, 953M, 953MH, 953ML, 959M, 959MH, 959ML, 1010G, 1050K, 1050K PL, 1070E, 1070G, 1110E, 1110G, 1170E, 1170G, 1210E, 1210G, 1270E, 1270G, 1450, 1470, 1470E, 1470G, 1510E, 1510G, 1550, 1570, 1590, 1770NT, 1775NT, 1830, 1835, 1840, 1870, 1890, 1895, 1910, 1910G, 1990, 2054, 2056, 2058, 2064, 2066, 2144G, 2154G, 2156G, 2204, 2454D, 2654G, 2656G, 2704, 2854, 2904, 2954D, 2956G, 3004, 3033R, 3038R, 3039R, 3045R, 3046R, 3120, 3154G, 3156G, 3203, 3204, 3310, 3320, 3410, 3520, 3720, 3754G, 3756G, 4044R, 4045CA550, 4045CB551, 4045CI550, 4045CI551, 4045DF271, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF275, 4045HF285, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG92, 4045HFG93, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HN055, 4045HN056, 4045TF150, 4045TF250, 4045TF271, 4045TF275, 4045TFG20, 4049M, 4049R, 4052R, 4066R, 4105, 4210, 4310, 4320, 4400, 4410, 4520, 4710, 4720, 4730, 4830, 4930, 5030HF270, 5045E, 5050E, 5055E, 5058E, 5065E, 5067E, 5075E, 5075EN, 5075M, 5085M, 5100M, 5100MH, 5100ML, 5105, 5115M, 5115ML, 5205, 5220, 5320, 5420, 5430I, 5520, 6068CG550, 6068CI550, 6068CP550, 6068HB551, 6068HF285, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFS01, 6068HFS55, 6068HFU55, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HT087, 6068SFM75, 6068TF275, 6090AFM75, 6090AFM85, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG94, 6090HFG95, 6090HFM85, 6090HFS86, 6090SFM75, 6090SFM85, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6105AF001, 6105D, 6105EH, 6105HF001, 6105J, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6115D, 6120EH, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125SFM75, 6130D, 6135AFM75, 6135AFM85, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140D, 6140R, 6150M, 6150R, 6150RH, 6170M, 6170R, 6175R, 6190R, 6195R, 6210R, 6215R, 6230R, 6250R, 6403, 6425, 6530 Premium, 6603, 6610, 6630 Premium, 6650, 6710, 6750, 6810, 6830 Premium, 6850, 6910, 6930, 6950, 7130 Premium, 7200, 7200R, 7210R, 7215R, 7220, 7230 Premium, 7230R, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330 Premium, 7350, 7380, 7400, 7400A, 7420, 7430E, 7450, 7480, 7500, 7520, 7530E, 7550, 7580, 7630, 7660, 7700, 7730, 7750, 7760, 7780, 7800, 7830, 7930, 8100, 8110, 8120, 8130, 8200, 8210, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310, 8310R, 8310RT, 8320, 8320R, 8320RT, 8330, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370RT, 8400, 8410, 8420, 8430, 8500, 8520, 8530, 8600, 8800A, 9009A, 9100, 9120, 9200, 9220, 9300, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9970, 9976, 9986, 9996, A2, C2 400, C230, C440, C650, C670, CH570, CH670, CP690, CP770, CS690, CS770, E210, E210LC, E230, E240, E240LC, E260, E300LC, E330, E360, E380, E400, F4365, GT242, GT262, GT275, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD40F, HD40R, HD40X, HD45F, HD45R, HD50F, HD50R, M-GATOR A3, M4030, M4040, M4040DN, N530F, N540F, N543F, N550, N560, N560F, P540, P556, R2 300, R230, R4023, R4030, R4038, R4044, R4045, R4060, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SPRAYER PERFORMANCE UPGRADES, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, W100, W155, W170, W200M, W230, W235, W235M, W235R, W260, W260R, W330, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X584</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
@@ -2303,6 +2678,11 @@
           <t>19M7898</t>
         </is>
       </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 40I, 50I, 62 IN. DECKS, 107, 210L, 210LJ, 260E, 310 P, 310E, 310J, 310L, 310SJ, 310SL, 310SL HL, 310TJ, 315J, 315SL, 337E, 408R, 410J, 410L, 437E, 444 P, 444H, 444J, 450K, 524K, 524K-II, 544G, 544H, 544J, 544K, 544K-II, 550K, 620G, 622G, 624G, 624H, 624J, 624K, 624K-II, 624KR, 625D, 630D, 630FD, 635D, 635FD, 640D, 640FD, 643H, 643L, 643L-II, 644 G, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 645FD, 650K, 653G, 670C, 670CH, 670G, 672CH, 672G, 700J-II, 700L, 703JH, 710J, 724J, 724K, 725D, 730D, 730FD, 730LL, 735D, 735FD, 740, 740D, 740FD, 744H, 744J, 744K, 744K-II, 745FD, 750J-II, 753J, 753JH, 757, 759J, 759JH, 770C, 770CH, 770G, 772CH, 772G, 777, 803M, 803MH, 824J, 824K, 843H, 843L, 843L-II, 844J, 844K, 850J-II, 850JR, 850L, 853M, 853MH, 859M, 859MH, 870G, 872G, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 925D, 930D, 936D, 944 X, 944K, 953K, 953M, 953MH, 959K, 959M, 959MH, 959ML, 1420, 1435, 1438GS, 1438HS, 1445, 1538GS, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1642HS, 1642HV, 1646HV, 1690, 1720 CCS, 1725C, 1725T, 1742GS, 1742HS, 1742PR, 1770NT, 1775NT, 1790, 1795, 1820, 1830, 1835, 1846, 1870, 1890, 1895, 1910, 1990, 2025R, 2026R, 2032R, 2036R, 2038R, 2046HV, 2254, 2400 PRECISIONCUT, 2510S, 2630, 2633, 2633VT, 2635, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 3025E, 3032E, 3036E, 3038E, 3510, 3520, 3522, 4045HF285, 4045HF485, 4045HFG85, 4045TF285, 4045TFC03, 4045TI530, 5045D, 5045E, 5055D, 5055E, 5065E, 5075E, 5083E, 5083EN, 5085E, 5090E, 5090EL, 5093E, 5093EN, 5100E, 5101E, 5101EN, 5103, 5203, 5203S, 5204, 5225, 5303, 5310, 5325, 5325N, 5403, 5410, 5425, 5425N, 5430I, 5503, 5525, 5525N, 5610, 5625, 5725, 6010, 6020, 6068HF285, 6068HF475, 6068HF485, 6068HFG85, 6068HFS55, 6068HN075, 6090 MC, 6090 RC, 6090HF475, 6090HF485, 6090HFL75, 6090HFL85, 6090HFU84, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115J, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125E MONTENEGRO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6130, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135J, 6135M, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140M, 6145M, 6150M, 6180CI510, 6200, 6200L, 6205, 6210, 6210L, 6215, 6220, 6220L, 6225, 6230, 6230 Premium, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6715, 7130, 7130 Premium, 7200, 7210R, 7230, 7230 Premium, 7230R, 7250R, 7270R, 7290R, 7300, 7310R, 7350, 7380, 7400, 7400A, 7450, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7950, 7980, 8310RT, 8320RT, 8335RT, 8345RT, 8360RT, 8370RT, 8700, 8800, 9100, 9120, 9200, 9220, 9300, 9320, 9320T, 9330, 9360R, 9400, 9410, 9410R, 9420, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470RT, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570RT, 9580, 9600, 9610, 9620, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9976, 9986, 9996, 15538, A420R, A520R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CTS, CTS II, DB37, DB44, DB60, DB66, DB80, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, F4365, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, N530, N530F, N536, N540, N540F, N542, N543F, N550, N560, P576, R4030, R4040i, R4050i, R4140i, R4150i, RD30F, RD35F, RD40F, RD45F, S430, S440, S560, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, S1642, S1742, S2046, S2546, SST15, SST16, SST18, T550, T560, T660, T670, TC44H, TC54H, TC62H, W70, W200M, W235, W235M, W235R, W260, W260R, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
@@ -2310,6 +2690,16 @@
           <t>19M8896</t>
         </is>
       </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 240, 250, 250D-II, 260, 260 P, 260E, 270, 300D-II, 310 P, 310E, 313, 315, 335D, 337E, 437D, 437E, 444 G, 444 P, 444K, 444L, 450 P, 450J, 450K, 524 P, 524K, 524K-II, 524L, 544 G, 544 P, 544K, 544K-II, 544L, 550 P, 550J, 550K, 615F, 618F, 618R, 620F, 620G, 620R, 622F, 622G, 622R, 624 P, 624K, 624K-II, 625F, 625R, 630F, 630R, 635F, 643L, 643L-II, 644 G, 644 P, 644 X, 644K, 644K HYBRID, 644L, 644LH, 650 P, 650J, 650K, 700K, 703JH, 724 P, 724K, 724L, 740A, 741, 750A, 750L, 753J, 753JH, 759J, 759JH, 803M, 803MH, 843L, 843L-II, 844K-III, 844K-III AGGREGATE HANDLER, 850J-II, 850L, 850L PL, 853M, 853MH, 859M, 859MH, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 944 X, 944K, 950K, 953K, 953M, 953MH, 959K, 959M, 959MH, 959ML, 1050K, 1050K PL, 1070G, 1110G, 1170G, 1210G, 1270D, 1270E, 1270G, 1354, 1404, 1470D, 1470E, 1470G, 1510G, 1710D, 1711D, 1870, 1890, 1895, 1910E, 3033R, 3038R, 3039R, 3045R, 3046R, 3320, 3520, 3522, 3720, 4045HF280, 4045HF285, 4045HF485, 4045HFG85, 5070M, 5075EN, 5075M, 5076EN, 5080M, 5085M, 5090EN, 5090M, 5090R, 5095M, 5100M, 5100MH, 5100ML, 5100R, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125ML, 5125R, 5130M, 5130ML, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068HB551, 6068HF285, 6068HFC08, 6068HFC09, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HG550, 6068HI550, 6068HN075, 6068HP550, 6068SFM75, 6068SFM85, 6090HF475, 6090HF485, 6090HFC09, 6090HFG84, 6090HFL75, 6090HFL85, 6095B, 6100, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6105D, 6105E, 6105EH, 6105M, 6110, 6110B, 6110D, 6110E SALTILLO, 6110L, 6110M, 6115D, 6115E, 6115M, 6120, 6120B, 6120E, 6120EH, 6120L, 6125AFM01, 6125AFM75, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125M, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130M, 6135B, 6135E, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140E, 6180CI510, 6200, 6205, 6210, 6210L, 6215, 6220, 6220L, 6225, 6230, 6300, 6310, 6310L, 6320, 6320L, 6325, 6330, 6400, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6534, 6603, 6605, 6610, 6615, 6620, 6630, 6715, 6803, 7130, 7180, 7230, 7250, 7660, 8320RT, 8345RT, 8370RT, 9360R, 9370R, 9410R, 9420R, 9460R, 9470R, 9500, 9510R, 9520R, 9560 STS, 9560R, 9570R, 9600, 9620R, 9660 STS, 9670 STS, 9700, 9760 STS, 9770 STS, A420R, A520R, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C850, CH570, CH670, CH950, CH960, CP770, CS690, CS770, E330, E360, E400, N530C, N536C, N540C, N540F, N542C, N543F, N550, N560, N560F, P540, P556, P576, R4023, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, TRAIL BUCK 500, TRAIL BUCK 650, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
@@ -2317,6 +2707,11 @@
           <t>03M7190</t>
         </is>
       </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-854, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 26, 30 IN., 30 Trailer, 38 IN., 42 IN., 47 IN., 52 IN., 54 IN. HEAVY DUTY SNOWBLOWER, 60 in., 60 IN. HEAVY DUTY SNOWBLOWER, 100, 120C, 160, 160C, 180C, 180E, 180SL, 203C, 204C, 205C, 206C, 207C, 208C, 209F, 210F, 213F, 215F, 215R, 218F, 218R, 220, 220C, 220F, 220SL, 222F, 222R, 228, 228A, 240, 243, 244, 245, 246, 260, 260C, 260SL, 265, 275, 285, 310SL, 310SL HL, 312GR, 313, 314G, 314R, 315, 316GR, 317, 317G, 318, 318G, 320, 320 P, 324, 324A, 325, 326E, 328, 328A, 328E, 329E, 330, 332, 332E, 333E, 335, 343, 344, 345, 349, 355, 359, 360, 365, 375, 381, 385, 388, 410 P, 410L, 415, 420, 425, 430, 435, 440E, 443, 444, 445, 446, 447, 448, 449, 450, 450 P, 450E, 450G, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460M, 460R, 466, 467, 468, 469, 493, 494, 500R, 508, 510, 512, 525, 530, 535, 543, 545, 546, 547, 550, 550 P, 550G, 550J, 550K, 550M, 554, 555G, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608C, 608C PERFORMANCE UPGRADES, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 622X, 623, 625, 625D, 625F, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 640C, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640X, 643, 644, 645, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647A, 650, 650 P, 650G, 650J, 650K, 653, 654, 655, 655K, 657A, 667A, 676, 678, 684, 686, 688, 692, 693, 694, 700J, 700J-II, 700K, 700L, 700L PL, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 710, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724, 724i, 725D, 725PF, 725X, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 732, 732i, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740i, 740PF, 740X, 744, 745FD, 745FD PERFORMANCE UPGRADES, 748, 750J, 750J-II, 750K, 750L, 755, 755K, 756, 780, 785, 824, 830, 832, 832I, 835, 835 SHORT CHASSIS, 840, 840i, 842, 843, 844, 850J, 850J-II, 850K, 852, 853, 854, 855, 856, 862, 864, 891, 892, 893, 894, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 946, 950K, 955, 956, 960, 990, 995, 1023E, 1026R, 1050K, 1050K PL, 1092, 1165, 1175, 1243, 1290, 1291, 1293, 1295, 1320, 1326, 1327, 1350, 1355, 1360, 1365, 1450, 1460, 1465, 1470, 1550, 1570, 1700, 1705, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1730, 1735, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1850, 1905, 1950, 1950N, 2054, 2056, 2058, 2064, 2066, 2200, 2230FH, 2230LL, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2330, 2400, 2510C, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653, 2653A, 2653B, 3215, 3215B, 3225B, 3225C, 3235, 3235B, 3235C, 3316, 3325, 3365, 3640, 3650, 4115, 4200, 4300, 4400, 4500, 4600, 4700, 4710, 4720, 4730, 4830, 4920, 4930, 5055E, 5065E, 5075E, 5075EN, 5078E, 5082E, 5083E, 5085E, 5090E, 5100E, 5100MH, 5101E, 5103, 5105MH, 5203, 5210, 5220, 5225, 5303, 5310, 5320, 5325, 5403, 5410, 5415, 5420, 5425, 5503, 5510, 5520, 5525, 5615, 5625, 5715, 5725, 6080A E-CUT, 6080A PRECISIONCUT, 6100E ROSARIO, 6100E SALTILLO, 6105EH, 6110E ROSARIO, 6110E SALTILLO, 6115E, 6120EH, 6125E ROSARIO, 6125E SALTILLO, 6130E SALTILLO, 6230R, 6250R, 6415, 6500A E-CUT, 6500A PRECISIONCUT, 6506, 6510, 6510S, 6600, 6610, 6615, 6650, 6700A PRECISIONCUT, 6710, 6750, 6800, 6810, 6850, 6900, 6910, 6910S, 6950, 7180, 7200, 7200A, 7200R, 7210R, 7215R, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7350, 7380, 7400, 7400A, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7550, 7580, 7660, 7700, 7700A PRECISIONCUT, 7720, 7750, 7760, 7780, 7800, 7820, 7850, 7920, 7950, 7980, 8000, 8000A E-CUT, 8100, 8110T, 8120, 8120T, 8130, 8200, 8210T, 8220, 8220T, 8230, 8230T, 8295RT, 8300, 8310RT, 8310T, 8320, 8320RT, 8320T, 8330, 8330T, 8335RT, 8345RT, 8360RT, 8370RT, 8400, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8700A PRECISIONCUT, 8760, 8770, 8800, 8800A, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9370R, 9400, 9400T, 9410, 9420, 9420R, 9420RX, 9420T, 9450, 9470 STS, 9470R, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9520, 9520R, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9540, 9550, 9560, 9560 STS, 9570 STS, 9570R, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, C1 200, C2 300, C2 400, C6R, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, DR12, DR16, DR18, DR24, E120, E130, E140, E150, E160, E170, E180, F440M, F440R, F441M, F441R, F725, GROUPER, GX325, GX335, GX345, GX355, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X4, HPX 4X4 TRAIL, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, M724, M732, M732i, M740, M740i, M944, M944I, M952, M952I, M962, M962I, MaxEmerge XP, PLANTER PERFORMANCE UPGRADES, R2 300, R40, R230, R400, R500, R732I, R740I, R944I, R952I, R962I, R975I, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, STRAIGHT BLADE, T550, T560, T660, T670, TE 4X2, TURF TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W70, W80, W100, W170, W210, W230, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, X146R, X166, X166R, X320, X340, X465, X475, X485, X495, X500, X520, X530, X534, X540, X575, X585, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Z235, Z255, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z515E, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
@@ -2324,6 +2719,11 @@
           <t>19M7784</t>
         </is>
       </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>2C-280, 2C-284, 2C-300, 2C-304, 2C-324, 2C-350, 2C-354, 3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 04, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 47 IN., 50 in., 54, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72, 72 IN., 80, 80C, 100, 108, 110, 110 TLB, 111, 112L, 112R, 120C, 120D, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 170, 175, 180, 180A, 180G, 185, 200, 200 G, 200C, 200D, 200G, 203C, 204C, 205C, 206C, 207C, 208C, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 215, 216, 218, 220, 220A, 222R, 224, 230, 230C, 240, 240D, 243, 244, 244J, 244K-II, 245, 250, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270C, 270D, 275, 280, 285, 290G, 300, 300D, 300D-II, 300DW, 300G, 300WW, 304, 304J, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324E, 324G, 324H, 324J, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330C, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 343, 344, 344H, 344J, 344K, 344L, 345, 350 P, 350D, 350D-II, 350DW, 350G, 360, 360DC, 370, 370C, 370E, 370E-II, 375, 380 P, 380G, 385, 390, 400D, 400D-II, 400F, 408R, 410 P, 410D, 410E, 410E-II, 410G, 410J, 410K, 410L, 410TK TMC, 415, 425, 430, 435, 435C, 437C, 437D, 437E, 440E, 443, 444, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 450, 450C, 450D, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 482C, 485E, 486E, 488E, 490, 490E, 493, 494, 509, 510D, 520, 524 P, 524K, 524K-II, 524L, 530, 530B, 535, 540E, 540G-II, 540G-III, 540H, 543, 543M, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 554, 555G, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 590D, 592, 594, 595D, 600, 600C, 603M, 603R, 604, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 623M, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650, 650D, 650G, 650H, 650J, 650K, 653, 653E, 653G, 654, 655K, 663R, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 676, 678, 683R, 690, 690E, 692, 693, 694, 698, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 709, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755D, 755K, 757, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772CH, 772CH II, 772D, 772G, 777, 778, 790E, 792D, 797, 800C, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843, 843G, 843H, 843J, 843K, 843L, 843L-II, 844, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855 LONG CHASSIS, 855 SHORT CHASSIS, 859M, 859MH, 862, 864, 870, 870D, 870G, 872D, 872G, 891, 892, 892E, 893, 894, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 995, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1050K, 1050K PL, 1054, 1070, 1070D, 1070E, 1070G, 1092, 1107, 1109, 1110D, 1110E, 1110G, 1111, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1243, 1270E, 1270G, 1290, 1291, 1293, 1295, 1312C, 1354, 1355, 1365, 1404, 1410D, 1420, 1424, 1424C, 1435, 1445, 1450, 1465, 1470, 1470E, 1470G, 1490D, 1510C, 1510DC, 1510E, 1510G, 1512C, 1512E, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1790, 1795, 1810, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1820, 1830, 1835, 1840, 1842GV, 1842HV, 1848GV, 1848HV, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1903, 1905, 1910, 1910E, 1910G, 1948GV, 1948HV, 1990, 2010DE, 2014DE, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2036R, 2038R, 2048HV, 2054, 2056, 2058, 2064, 2066, 2104, 2112C, 2112DC, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2148HV, 2154G, 2156G, 2204, 2230FH, 2230LL, 2243, 2254, 2254HV, 2256, 2258, 2264, 2266, 2310, 2330, 2354, 2400 PRECISIONCUT, 2412DE, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2510S, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2653, 2653A, 2653B, 2654G, 2656G, 2700 PRECISIONCUT, 2704, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3220, 3225C, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 3950, 3955, 3970, 3975, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045CA550, 4045CB551, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055B, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075GL, 5075GN, 5075GV, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085GN, 5085GV, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GL, 5090GN, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GL, 5100GN, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105GF, 5105GN, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081AFH75, 6081AFM01, 6081AFM75, 6081HFH70, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8820, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, B350, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, DB37, DB40, DB44, DB50, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DR8T, DR12, DR12T, DR16, DR18, DR24, E12, E15, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F620, F680, F687, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, FL100, G100, GROUPER, GT242, GT262, GT275, GX255, GX325, GX335, GX345, GX355, H540F, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX6, HX7, HX10, HX14, HX15, HX20, L70, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, L2554, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX280, LX289, M-GATOR A3, M-GATOR A3T, M15, M20, M4025, M4030, M4040, M4040DN, MX5, MX6, MX7, MX8, MX10, MX15, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, R10, R15, R20, R40, R160, R200, R230, R240, R280, R310, R450, R732I, R740I, R944I, R952I, R962I, R975I, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RC5M, RC6M, RC6R, RC7M, RC7R, RC8M, RC10M, RC10R, RC14R, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S2048, S2348, S2554, SH8R, SPRAYER PERFORMANCE UPGRADES, SST16, SST18, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X115R, X116R, X117R, X130R, X135R, X146R, X147R, X155R, X166R, X167R, X324, X465, X475, X485, X495, X575, X585, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z245, Z510A, Z520A, Z915B, Z925M, Z930M, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
@@ -2331,6 +2731,11 @@
           <t>R112772</t>
         </is>
       </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 350 P, 380 P, 540R, 600R, 620R, 640R, 660R, 680R, 1690, 1745, 1870, 1890, 1895, 1910, 1990, 2230FH, 2230LL, 6810, 6910, 6910S, 7210R, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7600, 7610, 7700, 7710, 7800, 7810, 9470 STS, 9560 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, C350L, C350T, C400L, C400T, C500L, C500T, C550L, C550T, C650, C650L, C850, C850T, CP690, CP770, CS690, CS770, N530C, N536C, N540C, N542C, N550, N560, N560F, P540, P556, P576, S7 600, S7 700, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S690, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
@@ -2338,6 +2743,11 @@
           <t>03M7191</t>
         </is>
       </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>3-Bag, 04, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 26, 30 IN., 30R, 46R, 47 IN., 48 IN., 52 IN., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 110 TLB, 112R, 180E, 203C, 205C, 206C, 208C, 209F, 209R, 210F, 210R, 212P, 213F, 215F, 215R, 218F, 218R, 220, 220F, 222F, 222R, 228, 228A, 240, 245, 246, 250, 260, 270, 280, 312GR, 314G, 314R, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324A, 324E, 324G, 325, 325G, 326D, 326E, 328, 328A, 328D, 328E, 329D, 329E, 330, 330G, 331G, 332, 332D, 332E, 332G, 332T, 333D, 333E, 333G, 337E, 338, 339, 345, 349, 359, 360, 360DC, 375, 381, 388, 390, 420, 430, 437E, 440E, 440R, 447, 448, 449, 450, 450E, 450M, 454, 455, 457, 458, 459, 459E, 460, 460M, 460R, 467, 468, 469, 475, 493, 494, 500R, 512, 516, 520M, 530, 533, 540A, 540E, 540G-II, 540G-III, 540M, 540R, 545, 547, 548E, 548G-II, 548G-III, 550, 550M, 553, 557, 558, 559, 560M, 560R, 562, 563, 565, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 600L HIGH DUMP, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 622X, 623, 625D, 625F, 625I, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 639, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640X, 644, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648E, 648G, 649, 653, 654, 657, 659, 663, 667, 667A, 670C II, 670CH II, 673, 678, 683, 684, 686, 688, 690, 692, 693, 694, 696, 698, 700M, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724, 724i, 725D, 725PF, 725X, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 732, 732i, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740i, 740PF, 740X, 741, 744, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 750K, 753, 757, 770, 770C II, 770CH II, 772CH II, 777, 778, 780, 785, 797, 800R, 824, 830, 832, 832I, 835, 835 SHORT CHASSIS, 840, 840i, 842, 850K, 852, 853, 854, 862, 864, 890, 891, 892, 893, 894, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 940, 946, 956, 960, 990, 995, 997, 1008, 1010, 1015, 1018, 1023E, 1025R, 1026R, 1030, 1035, 1040, 1092, 1107, 1109, 1111, 1113, 1140, 1290, 1291, 1293, 1295, 1320, 1326, 1327, 1340, 1350, 1355, 1360, 1365, 1418, 1424, 1424C, 1434, 1434C, 1450, 1460, 1465, 1470, 1504, 1505, 1515, 1550, 1570, 1575, 1580, 1585, 1640, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725T, 1730, 1735, 1745, 1750, 1755, 1770, 1770NT, 1775NT, 1780, 1785, 1790, 1795, 1820, 1830, 1835, 1840, 1850, 1854, 1870, 1905, 1910, 1950, 1950N, 1990, 2025R, 2026R, 2032R, 2040, 2040S, 2054, 2104, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2140, 2200, 2204, 2210, 2230FH, 2230LL, 2243, 2250, 2320, 2330, 2350, 2355, 2400, 2400 PRECISIONCUT, 2410, 2410C, 2450, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2520, 2550, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2555, 2650, 2653A, 2653B, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2720, 2730, 2750, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2755, 2850, 2950, 2955, 3025E, 3032E, 3033R, 3038E, 3038R, 3039R, 3040, 3045R, 3046R, 3050, 3120, 3140, 3150, 3155, 3200, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3316, 3320, 3325, 3350, 3365, 3400, 3420, 3510, 3520, 3522, 3640, 3650, 3720, 3800, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4055, 4066M, 4066R, 4120, 4210, 4250, 4255, 4310, 4320, 4410, 4450, 4455, 4500, 4520, 4555, 4560, 4600, 4630, 4650, 4700, 4710, 4720, 4730, 4755, 4760, 4830, 4850, 4920, 4930, 4940, 4955, 4960, 5045D, 5045E, 5050E, 5055D, 5055E, 5060E, 5065E, 5065M, 5070E, 5075E, 5075M, 5076E, 5076EL, 5076EN, 5078E, 5080E, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5105M, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125R, 5200, 5203, 5210, 5220, 5225, 5300, 5303, 5310, 5320, 5325, 5325N, 5400, 5403, 5410, 5415, 5420, 5425, 5425N, 5430I, 5500, 5503, 5510, 5520, 5525, 5525N, 5603, 5615, 5625, 5715, 5725, 6020, 6080A E-CUT, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105EH, 6105J, 6105M, 6105R, 6110 MC, 6110 RC, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120EH, 6120M, 6120R, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6205J, 6210J, 6210M, 6210R, 6215, 6215R, 6220, 6230, 6230 Premium, 6230R, 6250R, 6320, 6320L, 6330, 6330 Premium, 6403, 6415, 6420, 6420L, 6420S, 6430, 6430 Premium, 6488, 6500A E-CUT, 6520, 6520L, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6810, 6820, 6830, 6830 Premium, 6850, 6910, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7195J, 7200, 7200A, 7200J, 7200R, 7210, 7210J, 7210R, 7215J, 7215R, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7330, 7330 Premium, 7350, 7380, 7400, 7410, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7510, 7515, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8440, 8450, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8630, 8640, 8650, 8700, 8760, 8770, 8800, 8800A, 8850, 8870, 8900A, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, A420R, A520R, AMT600, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C670, C850, CH330, CH530, CP20, CP690, CP770, CS690, CS770, CT322, CT332, CTS, CTS II, D105, D125, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, F440M, F440R, F441M, F441R, F620, F680, F687, F4365, GROUPER, H180, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX615E, HPX815E, HX10, HX14, L60, L70, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, LT150, LT155, LT160, LT180, LT190, M724, M732, M732i, M740, M740i, M944, M944I, M952, M952I, M962, M962I, M4025, M4030, M4040, MaxEmerge XP, N530C, N536C, N540C, N542C, PLANTER PERFORMANCE UPGRADES, R40, R230, R400, R450, R500, R732I, R740I, R944I, R952I, R962I, R975I, R4023, R4040i, R4050i, RC10R, RC14R, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, RSX 850I, S160, S180, S200, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SST15, SST16, SST18, STRAIGHT BLADE, T550, T560, T660, T670, V451G, V451M, V451R, V461M, V461R, W36R, W48R, W50, W52R, W61R, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X465, X475, X485, X495, X500, X520, X530, X540, X570, X575, X580, X585, X590, X595, X710, X730, X734, X738, X739, X750, X754, X758, X950R, XUV 550, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z425, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
@@ -2345,6 +2755,11 @@
           <t>03M7192</t>
         </is>
       </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-954, 5E-1004, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 30 IN., 30R, 46R, 47 IN., 48 IN., 54 in., 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 62 IN. DECKS, 72, 72 IN., 102, 105, 115, 125, 135, 145, 155C, 175, 180, 180B, 180C, 180E, 180SL, 190C, 209F, 210F, 210K, 210K EP, 210L, 210L EP, 210LJ, 213F, 215F, 215R, 218F, 218R, 220, 220B, 220C, 220F, 220SL, 222F, 222R, 228, 228A, 240, 245, 250D-II, 260, 260B, 260C, 260SL, 265, 270, 285, 300D, 300D-II, 300F, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 314G, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318G, 320, 324, 325, 325J, 325SK, 325SL, 326E, 328, 328E, 329E, 330G, 331G, 332, 332E, 332G, 333E, 333G, 335, 335D, 337E, 338, 348, 349, 350D-II, 359, 360, 370E, 375, 381, 385, 388, 390, 400D-II, 400F, 410, 410D, 410E, 410G, 410J, 410K, 410L, 410TK TMC, 419, 420, 430, 435, 437D, 437E, 440, 440E, 444J, 444K, 446, 447, 448, 449, 450, 450E, 450J, 450M, 454, 455, 456, 457, 458, 459, 459E, 460, 460E, 460M, 460R, 466, 467, 468, 469, 475, 493, 494, 510D, 524K, 524K-II, 530, 535, 540A, 540G-III, 540H, 543M, 543R, 544J, 544K, 544K-II, 545, 546, 547, 548G-III, 548H, 550, 550J, 550M, 554, 556, 557, 558, 559, 560M, 560R, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 600, 603M, 603R, 604, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 615C, 615F, 615P, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620R, 622, 622F, 622G, 622R, 622X, 623, 624J, 624K, 624KR, 625D, 625F, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 639, 640, 640C, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640H, 640X, 643K, 644, 644J, 644K, 644K HYBRID, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 647A, 648H, 648HT, 650, 650J, 653, 654, 657, 657A, 667, 667A, 670D, 670G, 672D, 672G, 673, 678, 680, 690, 692, 693, 694, 698, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710J, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 722X, 724J, 724K, 725D, 725X, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 730X, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735X, 737, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740X, 744, 744J, 744K, 744K-II, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748H, 748HT, 757, 764, 770, 770D, 770G, 772D, 772G, 777, 780, 785, 797, 803M, 803MH, 824J, 824K, 830, 835, 842, 843K, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 848H, 848HT, 852, 853, 853M, 853MH, 854, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 904, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 960, 990, 995, 997, 1023E, 1025R, 1026R, 1054, 1092, 1107, 1109, 1111, 1113, 1165, 1290, 1291, 1293, 1295, 1320, 1326, 1327, 1350, 1354, 1355, 1360, 1365, 1404, 1424, 1424C, 1433, 1433C, 1460, 1465, 1470, 1520, 1550, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1654, 1700, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1745, 1750, 1755, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1854, 1854J, 1870, 1895, 1910, 2025R, 2026R, 2032R, 2036R, 2038R, 2054, 2104, 2154G, 2156G, 2204, 2230FH, 2230LL, 2310, 2330, 2430, 2510H, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653, 2653A, 2653B, 2654G, 2656G, 2660VT, 2704, 2730, 2854, 2904, 3004, 3033R, 3038R, 3039R, 3045B, 3045R, 3046R, 3050B, 3120, 3154G, 3156G, 3200, 3204, 3215, 3220, 3225C, 3235C, 3245C, 3316, 3320, 3400, 3420, 3510, 3520, 3522, 3720, 3754G, 3756G, 3800, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4055, 4066M, 4066R, 4120, 4255, 4320, 4455, 4520, 4630, 4700, 4710, 4720, 4730, 4830, 4920, 4930, 4940, 5045E, 5050E, 5055B, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075M, 5076E, 5078E, 5080E, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5105M, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5220, 5225, 5320, 5325, 5400, 5405, 5420, 5425, 5430I, 5440, 5460, 5520, 5525, 5603, 5620, 5625, 5720, 5725, 5730, 5820, 5830, 6010, 6020, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068TBM01, 6068TBM02, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120E, 6120EH, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135E, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6205J, 6210, 6210J, 6210M, 6210R, 6215, 6215R, 6220, 6230, 6230 Premium, 6300, 6310, 6320, 6330, 6330 Premium, 6400, 6403, 6405, 6410, 6415, 6420, 6420S, 6430, 6430 Premium, 6500A E-CUT, 6500L, 6506, 6510, 6510S, 6520, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH330, CH530, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT322, CT332, CTS, CTS II, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, E100, E110, E120, E130, E140, E150, E160, E170, E180, F440M, F440R, F441M, F441R, F725, F4365, G110, GROUPER, H240, H260, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LX277, LX279, LX280, M-GATOR A1, M-GATOR A3, M4025, M4030, M4040, M4040DN, MaxEmerge XP, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R450, R4023, R4030, R4038, R4040i, R4044, R4045, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S160, S180, S200, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, T550, T560, T660, T670, TD100, V451G, V451M, V451R, V461M, V461R, W36M, W36R, W48M, W48R, W50, W52R, W61R, W70, W80, W100, W150, W155, W170, W200M, W230, W235, W235M, W235R, W260, W260R, W430, W540, W550, W650, W660, X9 1000, X9 1100, X110, X120, X125, X135R, X140, X145, X155R, X165, X500, X520, X530, X540, X570, X580, X590, X710, X730, X734, X738, X739, X750, X754, X758, X950R, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Y110, Y115, Z510A, Z520A, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
@@ -2352,6 +2767,11 @@
           <t>03M7193</t>
         </is>
       </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>3-Bag, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6X4, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 30 IN., 42 IN., 47 IN., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 62 IN. DECKS, 72 IN., 80, 110, 112R, 120C, 120D, 160, 160C, 160D, 180E, 190E, 200, 200C, 200D, 209F, 210F, 210K, 210L EP, 213F, 215F, 215R, 218F, 218R, 220, 220F, 222F, 222R, 228, 228A, 230C, 240D, 270, 270C, 270D, 290D, 310J, 310K, 310K EP, 310L, 310L EP, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315SL, 316GR, 317, 317G, 318D, 318G, 319D, 320, 320D, 320G, 323D, 324G, 325, 325G, 325J, 325SL, 326D, 328, 328D, 329D, 330C, 330G, 331G, 332, 332D, 332G, 333D, 333G, 335, 345, 350D, 355, 370, 370C, 375, 385, 410J, 410K, 410L, 410TK TMC, 435, 440E, 446, 447, 448, 449, 450, 450E, 450M, 456, 457, 458, 459, 459E, 460M, 460R, 466, 467, 468, 469, 490E, 493, 494, 525, 530, 531, 533, 535, 546, 547, 550M, 551, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 590D, 592, 594, 595D, 604C, 605C, 606C, 606SH, 607C, 608C, 608SH, 609C, 610C, 611C, 612C, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616F, 616R, 617C, 618, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 623, 625, 625D, 625F, 625PF, 625R, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 644, 645FD, 645FD PERFORMANCE UPGRADES, 651, 653, 661, 663, 678, 680, 683, 692, 693, 694, 710G, 710J, 710K, 710L, 712FC, 712FC PERFORMANCE UPGRADES, 717, 725D, 727, 730, 730FD, 730FD PERFORMANCE UPGRADES, 735, 735FD, 735FD PERFORMANCE UPGRADES, 740FD, 740FD PERFORMANCE UPGRADES, 744, 745FD, 745FD PERFORMANCE UPGRADES, 748, 780, 785, 790E, 792D, 803M, 803MH, 830, 835, 842, 852, 853M, 853MH, 854, 859M, 859MH, 862, 864, 891, 892, 893, 894, 913, 915F, 915R, 916, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 950K, 960, 990, 995, 997, 1023E, 1025R, 1026R, 1030, 1035, 1092, 1107, 1109, 1111, 1113, 1290, 1291, 1293, 1295, 1350, 1355, 1360, 1365, 1445, 1450, 1460, 1465, 1470, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1870, 1890, 1895, 1900, 1910, 2025R, 2026R, 2027R, 2032R, 2036R, 2038R, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2154D, 2230FH, 2230LL, 2310, 2330, 2454D, 2510H, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653A, 2653B, 2660VT, 2704, 2720, 2730, 2904, 2954D, 3004, 3025E, 3032E, 3033R, 3036E, 3038E, 3038R, 3039R, 3045R, 3046R, 3200, 3204, 3215, 3215B, 3220, 3225B, 3235, 3235B, 3235C, 3245C, 3316, 3320, 3400, 3420, 3520, 3720, 3754D, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4300, 4320, 4400, 4520, 4600, 4700, 4710, 4720, 4730, 4830, 4920, 4930, 4940, 5055E, 5065E, 5065M, 5075E, 5075M, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5105M, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125R, 5320N, 5325N, 5420N, 5425, 5425N, 5520N, 5525, 5525N, 5603, 5625, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100M, 6105 MC, 6105 RC, 6110 MC, 6110 RC, 6110M, 6115 MC, 6115 RC, 6120, 6120M, 6125M, 6130M, 6140M, 6145M, 6155M, 6155MH, 6175M, 6195M, 6200, 6210M, 6220, 6230 Premium, 6300, 6320, 6330 Premium, 6400, 6420, 6420S, 6430 Premium, 6488, 6500L, 6520, 6530, 6530 Premium, 6534, 6534 Premium, 6620, 6630, 6630 Premium, 6820, 6830, 6830 Premium, 6920, 6920S, 6930, 7130, 7130 Premium, 7180, 7200, 7200R, 7210, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7310R, 7320, 7330 Premium, 7350, 7380, 7400, 7410, 7420, 7430E, 7450, 7455, 7460, 7480, 7500, 7510, 7520, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7730, 7750, 7760, 7780, 7800, 7810, 7830, 7850, 7930, 7950, 7980, 8100, 8110, 8200, 8210, 8225R, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310, 8310R, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8410, 8500, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8870, 8960, 8970, 9009A, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, BP15, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DR8T, DR12, DR12T, DR16, DR18, DR24, E12, E15, F440M, F440R, F441M, F441R, F620, F680, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, GROUPER, GX325, GX335, GX345, GX355, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HX6, HX7, HX10, HX14, HX15, HX20, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M15, M20, M4025, M4030, M4040, M4040DN, MX15, N540F, N543F, N550, N560, P556, P576, PLANTER PERFORMANCE UPGRADES, R10, R15, R20, R40, R230, R4023, R4040i, R4050i, RC6R, RC7R, RC10R, RC14R, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S160, S180, S200, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, T550, T560, T660, T670, V451G, V451M, V451R, V461M, V461R, W36M, W36R, W48M, W48R, W50, W52R, W61R, W70, W100, W170, W210, W230, W540, W550, W650, W660, X9 1000, X9 1100, X530, X540, X580, X590, X710, X730, X734, X738, X739, X750, X754, X758, X940, X948, X949, Y110, Y115, Y210, Y215, Z225, Z245, Z315E, Z320M, Z320R, Z335E, Z335M, Z345M, Z345R, Z425, Z445, Z465, Z915B, Z920M, Z920R, Z925M, Z930R, Z960R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
@@ -2359,6 +2779,11 @@
           <t>19M8637</t>
         </is>
       </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>3B-400, 3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 5E-1000, 5E-1004, 5E-1104, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1404, 6R 110, 6R 120, 6R 130, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 17 ZTS, 38 IN., 100, 110 TLB, 120D, 160, 160 P, 160D, 160G, 180E, 180G, 185 E-CUT, 200 G, 200C, 200D, 200G, 210 G, 210 P, 210K, 210K EP, 210L, 210L EP, 210LJ, 220, 220C, 220SL, 225 E-CUT, 230C, 240, 240D, 250, 250C, 250D, 250D-II, 270C, 270D, 280, 300C, 300D, 300D-II, 300DW, 300WW, 310 G, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315 P, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 318D, 318E, 318G, 320, 320 P, 320D, 320E, 320G, 324E, 324G, 325, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 330C, 332, 332D, 332E, 335C, 335D, 337E, 338, 348, 350C, 350D, 350D-II, 350DW, 350G, 360DC, 365, 370C, 370E, 380G, 400C, 400D, 400D-II, 410 P, 410D, 410E, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 425, 435C, 437C, 437D, 437E, 444 G, 444 P, 444H, 444K, 444L, 445, 450 P, 450C, 450G, 450H, 450J, 450K, 455, 455G, 456, 457, 460, 460DC, 460E, 460S, 466, 467, 468, 510D, 524 P, 524K, 524K-II, 524L, 530B, 540G-III, 544 G, 544 P, 544H, 544K, 544K-II, 544L, 548G-III, 548H, 550, 550 P, 550G, 550H, 550J, 550K, 555G, 556, 557, 566, 567, 600L HIGH DUMP, 605K, 612R, 620G, 622G, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 640G, 640H, 644 G, 644 P, 644 X, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 648G, 648H, 648HT, 650 P, 650G, 650H, 650J, 650K, 655, 655K, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 676, 678, 700H, 700J, 700J-II, 700K, 703JH, 710 P, 710G, 710J, 710K, 710L, 724 P, 724J, 724K, 724L, 744 P, 744H, 744J, 744K, 744K-II, 748G-III, 748H, 748HT, 750C, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755, 755K, 756, 759J, 759JH, 768L-II, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 800R, 803M, 803MH, 824 P, 824J, 824K, 843K, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853M, 853MH, 855, 856, 859M, 859MH, 870D, 870G, 872D, 872G, 903K, 903KH, 903M, 903MH, 904, 904 P, 909K, 909KH, 909M, 909MH, 948L, 948L-II, 950, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1023E, 1025R, 1026R, 1050C, 1050E, 1050K, 1054, 1270D, 1270E, 1270G, 1354, 1404, 1470D, 1470E, 1470G, 1600 TURBO SERIES II, 1710D, 1711D, 1720, 1720 CCS, 1770NT, 1775NT, 1790, 1795, 1910E, 1910G, 2032R, 2054, 2154D, 2230LL, 2454D, 2720, 2954D, 3033R, 3038R, 3039R, 3045B, 3045R, 3046R, 3050B, 3120, 3154G, 3156G, 3200, 3203, 3215, 3220, 3320, 3400, 3420, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4039DF004, 4039DF005, 4039DF006, 4039DF031, 4039DF032, 4039DF092, 4100, 4105, 4110, 4115, 4200, 4210, 4300, 4310, 4400, 4410, 4500, 4510, 4600, 4610, 4700, 4710, 4895, 4920, 4930, 4990, 4995, 5090E, 5100E, 5105, 5205, 5620, 5720, 5820, 6059TF, 6090 MC, 6090 RC, 6090HF475, 6090HF485, 6090HFG84, 6090HFL75, 6090HFL85, 6095 MC, 6095 RC, 6095B, 6100 MC, 6100 RC, 6100B, 6100D, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105HF001, 6110 MC, 6110 RC, 6110B, 6110D, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6120B, 6120M, 6120R, 6125AF001, 6125AFM01, 6125D, 6125HF001, 6125HF070, 6130D, 6130M, 6130R, 6135B, 6135M, 6135R, 6140D, 6145M, 6145R, 6155M, 6155R, 6155RH, 6175M, 6175R, 6195M, 6195R, 6215R, 6403, 6603, 6650, 6675, 6750, 6803, 6850, 6950, 7180, 7200, 7210, 7250, 7300, 7400, 7410, 7500, 7510, 7600, 7610, 7630, 7660, 7700, 7710, 7720, 7730, 7775, 7800, 7810, 7820, 7830, 7920, 7930, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8300T, 8310, 8310R, 8310T, 8320, 8320R, 8320T, 8330, 8330T, 8335R, 8345R, 8360R, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8520, 8520T, 8530, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9460R, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9560 STS, 9560R, 9560RT, 9570RT, 9620, 9620T, 9630, 9630 SCRAPER, 9660 STS, 9670, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9880 STS, A400, B25C, B30C, B35C, B40C, BA72, BA84, BP72, BP84, CA15, CH330, CH530, CP690, CS690, CT315, E330, E360, E380, E400, F4365, FL100, L330, L340, LP72, LP78, LP84, PA15, PA15B, PA30, PA30B, PR60, PR72B, PR72S, PR84B, PR96B, R450, R4030, R4038, R4040i, R4044, R4045, R4060, RL66, RL84, RT55, RT73, S160, S180, S200, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T550, T560, T660, T670, TC44H, TC54H, TC62H, TR36B, TR48B, TR60B, W170, W540, W550, W650, W660, WL53, WL56, X724, X728, X729, X734, X739, X744, X748, X749, X754, X949</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
@@ -2366,6 +2791,11 @@
           <t>19M7804</t>
         </is>
       </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>3-Bag, 04, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 30 IN., 35G, 38 IN., 42 IN., 46, 47, 47 IN., 48, 48 IN., 54, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 110 TLB, 130 P, 130G, 160 P, 160G, 170, 175, 180, 180E, 180G, 185, 190C, 200 G, 200G, 210 G, 210 P, 210K, 210K EP, 210L, 210L EP, 220, 240, 240D, 245, 250 P, 250C, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270D, 285, 290G, 300 P, 300C, 300D-II, 300DW, 300WW, 305, 310 G, 310 P, 310E, 310K, 310K EP, 310L, 310L EP, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 314G, 315 P, 315J, 315SK, 315SL, 316GR, 318D, 318E, 318G, 319D, 319E, 320, 320 P, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328D, 328E, 329D, 329E, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 344 P, 344K, 344L, 345, 350C, 350D, 350D-II, 350DW, 350G, 360DC, 370B, 370E, 370E-II, 375, 375A, 380G, 385A, 400C, 400D, 400D-II, 410 P, 410E, 410E-II, 410J, 410K, 410L, 410TK TMC, 415, 425, 435, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450 P, 450H, 450J, 450K, 450M, 455, 456, 457, 458, 459, 460 P, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 485, 485A, 524 P, 524K, 524K-II, 524L, 535, 540G-II, 540G-III, 540M, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548G-II, 548G-III, 550, 550 P, 550H, 550J, 550K, 550M, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 600R, 605K, 606SH, 608SH, 612R, 615F, 616R, 618F, 618R, 620F, 620G, 620I, 620R, 622F, 622G, 622R, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625R, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640L, 640L-II, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 648G, 648L, 648L-II, 650 P, 650H, 650J, 650K, 655K, 670, 670C II, 670CH II, 670D, 670G, 672D, 672G, 673, 678, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 710 P, 710K, 710L, 724 P, 724J, 724K, 724L, 725D, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 741, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748G-II, 748L, 748L-II, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755K, 759J, 759JH, 764, 768L-II, 770, 770D, 770G, 772D, 772G, 777, 797, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 835 SHORT CHASSIS, 842, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848L, 848L-II, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870D, 870G, 872D, 872G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909JH, 909K, 909KH, 909M, 909MH, 910G, 916, 944 X, 944K, 948L, 948L-II, 950K, 953J, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1010G, 1023E, 1025R, 1026R, 1050K, 1050K PL, 1165, 1175, 1270D, 1270E, 1270G, 1350, 1355, 1360, 1365, 1420, 1435, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1700, 1705, 1710D, 1711D, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1730, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1830, 1835, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 2010DE, 2014DE, 2018, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2154G, 2156G, 2204, 2210, 2243, 2264, 2266, 2266E, 2400 PRECISIONCUT, 2412DE, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2653A, 2653B, 2654G, 2656G, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3005, 3025D, 3025E, 3029DF128, 3029TF158, 3032E, 3033R, 3035D, 3036E, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3120, 3154G, 3156G, 3200, 3203, 3204, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3320, 3325, 3365, 3375, 3400, 3420, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3765, 3800, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CB551, 4045CI550, 4045CI551, 4045DF150, 4045DF158, 4045HAC04, 4045HB551, 4045HF158, 4045HF285, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HI550, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HRT90, 4045TF158, 4045TF258, 4045TF285, 4045TFC03, 4045TFG03, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5210, 5215, 5215F, 5215V, 5310, 5310N, 5315, 5315F, 5315V, 5320N, 5403, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5615, 5615V, 5625, 5705, 5715, 5725, 6068AFM75, 6068AFM85, 6068HF158, 6068HF258, 6068HF285, 6068HF485, 6068HFC93, 6068HFG85, 6068HFL84, 6068HFU82, 6068SFM75, 6068SFM85, 6068TF158, 6068TF258, 6080A E-CUT, 6080A PRECISIONCUT, 6090AFM75, 6090AFM85, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105HF001, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6120E, 6120EH, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125HF001, 6125HF070, 6125SFM75, 6130D, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135M, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140M, 6145M, 6150R, 6150RH, 6155R, 6155RH, 6180CI510, 6500A E-CUT, 6500A PRECISIONCUT, 6700, 6700A PRECISIONCUT, 7180, 7195J, 7200, 7200A, 7200J, 7200R, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7350, 7380, 7400, 7400A, 7420, 7450, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7520, 7550, 7580, 7630, 7660, 7700, 7700A PRECISIONCUT, 7730, 7750, 7760, 7780, 7800, 7830, 7850, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, A400, B25C, B30C, B35C, B40C, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT322, CT332, CTS, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DF500, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E130, E140, E210, E210-II, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F510, F525, F4365, G110, GROUPER, GT242, GT262, GT275, GX325, GX335, GX345, GX355, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, L330, L331, L340, L341, L624, L634, L1524, L1534, LT133, LT150, LT155, LT160, LT166, LT180, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, MaxEmerge XP, N530, N530C, N536, N536C, N540, N540C, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, P660, P670, P680, P690, PC4, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R450, R4038, R4044, R4045, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, V451G, V451M, V461M, W36R, W48R, W52R, W61R, W100, W155, W170, W200M, W235, W235M, W235R, W260, W260R, W330, W540, W550, W650, W660, X9 1000, X9 1100, X300, X304, X320, X324, X340, X495, X520, X595, X700, X740, X744, X748, X750, X754, X758, X940, X948, X949, X950R, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Z225, Z235, Z425, Z435, Z445, Z535M, Z540M, Z720E, Z730M, Z735E, Z735M, Z740R, Z760R, Z860A, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
@@ -2373,6 +2803,11 @@
           <t>19M8292</t>
         </is>
       </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>5B-700, 5B-704, 5B-750, 5B-754, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 20 Trailer, 30 IN., 30 Trailer, 48 IN., 54D IN., 60, 60 IN. DECKS, 60D IN., 62 IN., 120D, 130 P, 130G, 160D, 160G, 180G, 200D, 200G, 203C, 204C, 205C, 206C, 207C, 208C, 210 P, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 250C, 250D-II, 250G, 260, 260 P, 260E, 270, 280, 300D-II, 300G, 310 G, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 313, 315, 315 P, 315J, 315SE, 315SG, 315SK, 315SL, 317, 318D, 319D, 320, 320 P, 320D, 323D, 324H, 325, 325J, 325SK, 325SL, 326D, 328, 328D, 329D, 330B, 330G, 331G, 332, 332D, 332G, 333D, 333G, 335D, 337E, 344H, 344J, 350G, 360, 360DC, 370E, 370E-II, 375, 380G, 390, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410TK TMC, 415, 425, 437D, 440E, 444 G, 444H, 444J, 444K, 445, 446, 447, 448, 449, 450 P, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 475, 485E, 486E, 488E, 490, 524K, 524K-II, 540E, 540G-II, 540G-III, 540H, 544 G, 544G, 544H, 544J, 544K, 544K-II, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550 P, 550G, 550H, 550J, 550K, 550M, 554, 555G, 556, 557, 558, 559, 560M, 566, 567, 568, 569, 600R, 605C, 612R, 616R, 620, 620I, 624G, 624H, 624J, 625I, 639, 640, 640E, 640G, 640H, 643L, 644 G, 644G, 644K, 648E, 648G, 648H, 648HT, 649, 650, 650 P, 650G, 650H, 650J, 650K, 653, 653G, 654, 655, 655K, 659, 670C, 670C II, 670CH, 670CH II, 670G, 672CH, 672G, 690, 690E, 692, 698, 700H, 700J, 700J-II, 700K, 700L PL, 703JH, 710 P, 710D, 710G, 710J, 710K, 710L, 724 P, 724K, 724L, 737, 740, 740G, 741, 744 P, 744J, 744K, 744K-II, 744L, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 750C, 750J, 750J-II, 750K, 753J, 753JH, 755, 755K, 756, 757, 759J, 759JH, 764, 768L-II, 770, 770D, 770G, 772, 772D, 772G, 777, 778, 797, 800R, 803M, 803MH, 810D, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 835 SHORT CHASSIS, 843L, 844 P, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850C, 850J, 850L, 850L PL, 853, 853J, 853M, 853MH, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 870D, 870G, 872D, 872G, 903J, 903K, 903KH, 903M, 903MH, 904 P, 909K, 909KH, 909M, 909MH, 910G, 913, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944 X, 944K, 946, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 955, 956, 959K, 959M, 959MH, 959ML, 1010G, 1023E, 1026R, 1050K, 1050K PL, 1165, 1170, 1175, 1270D, 1270E, 1270G, 1312C, 1354, 1404, 1420, 1435, 1445, 1450, 1470, 1470D, 1470E, 1470G, 1510C, 1512C, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1710D, 1711D, 1725T, 1810C, 1812C, 1814C, 1850, 1854, 1854J, 1900, 1910, 1910E, 1910G, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2038R, 2054, 2056, 2058, 2064, 2066, 2112C, 2154D, 2154G, 2156G, 2230FH, 2230LL, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2400 PRECISIONCUT, 2500B, 2500E, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2654G, 2656G, 2854, 2956G, 3025D, 3025E, 3028EN, 3029DF128, 3029HFC03, 3029HFG03, 3029HG530, 3029HI530, 3029TF158, 3029WG401, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3154G, 3156G, 3200, 3203, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3316, 3400, 3410, 3420, 3754G, 3756G, 3800, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4045CA550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG92, 4045HFG93, 4045HFK80, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HSG20, 4045HSG21, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4105, 4239TF001, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4940, 4990, 4995, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5039D, 5042D, 5045D, 5045E, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5065E, 5067E, 5070M, 5075E, 5075EN, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5100GV, 5100M, 5100R, 5101E, 5101EN, 5210, 5215, 5215F, 5215V, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320N, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5615, 5615V, 5620, 5625, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF150, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN078, 6068HP550, 6068HSG22, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6080A PRECISIONCUT, 6090 MC, 6090 RC, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL85, 6090HFM85, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF070, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135B, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500A PRECISIONCUT, 6500L, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6700A PRECISIONCUT, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7200, 7200A, 7200R, 7205J, 7210, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7850, 7920, 7950, 7980, 8000, 8000A E-CUT, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8430, 8430T, 8500, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9100, 9200, 9300, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, B25C, BA96, C1 200, C2 300, C2 400, C100, C110, C120, C230, C240, C440, C670, CH330, CH530, CH570, CH670, CP20, CP690, CP770, CS690, CS770, CT315, CT332, CTS, CTS II, E130, E140, E210, E210-II, E210LC, E230, E230-II, E330, E360, E400, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, GS88, HD35R, HD40R, HD45R, HD50R, HD200, HD300, HH75, HH80, HH100, L330, L331, L340, L341, M4040DN, PA40, PC10, R2 300, R40, R230, R450, R4038, R4044, R4045, R4060, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SP10B, SP12B, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TE 4X2, TH 6X4, TH 6X4 D, TURF TX 4X2, TX 4X2, W50, W70, W80, W100, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z425, Z445, Z465, Z510A, Z520A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
@@ -2380,6 +2815,11 @@
           <t>19M7807</t>
         </is>
       </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>04, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 145, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 13HP, 15HP, 16HP, 22B, 26, 30 IN., 38 IN., 47 IN., 50 in., 50G, 52 IN., 54 IN. FRONT BLADE, 60 in., 130G, 160, 160G, 180G, 203C, 204C, 204L, 205C, 206C, 207C, 208C, 210 G, 210 P, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 240, 246, 250, 250 P, 250C, 250D-II, 250G, 260, 260 P, 260E, 270, 280, 290G, 300 P, 300D, 300D-II, 300G, 304L, 310 G, 310 P, 310D, 310E, 310K, 310K EP, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 313, 315, 315 P, 315D, 315SK, 315SL, 316GR, 317, 317G, 318E, 318G, 319E, 320, 320 P, 320E, 320G, 323E, 324E, 324G, 325, 325G, 325SK, 325SL, 326E, 328, 328E, 329E, 330G, 331G, 332, 332E, 332G, 333E, 333G, 335, 335D, 337E, 345, 350C, 350D, 350D-II, 350DW, 350G, 355, 360DC, 370E, 370E-II, 380G, 400C, 400D, 400D-II, 408R, 410 P, 410E, 410E-II, 410K, 410L, 410TK TMC, 415, 425, 437D, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 450, 450 P, 450J, 450K, 454, 455, 460 P, 460DC, 460E, 460E-II, 470 P, 470G, 475, 490, 490 PRO, 524 P, 524K, 524K-II, 524L, 540G-II, 540G-III, 540H, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 548G-II, 548G-III, 548H, 550, 550 P, 550J, 550K, 553, 554, 562, 563, 565, 575, 600R, 605C, 605K, 612R, 615F, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620G, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625PF, 625R, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 648G, 648H, 648HT, 648L, 648L-II, 650, 650 P, 650J, 650K, 653, 654, 655, 655K, 670C II, 670CH II, 670D, 670G, 672D, 672G, 673, 690E, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 710 P, 710K, 710L, 724 P, 724J, 724K, 724L, 725D, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 737, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 741, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755, 755K, 756, 757, 759J, 759JH, 764, 768L-II, 770, 770C II, 770CH II, 770D, 770G, 772, 772CH II, 772D, 772G, 777, 780, 785, 797, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 840, 843, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853, 853M, 853MH, 855, 856, 859M, 859MH, 870D, 870G, 872D, 872G, 903K, 903KH, 903M, 903MH, 904 P, 909K, 909KH, 909M, 909MH, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944 X, 944K, 948L, 948L-II, 950J, 950K, 953K, 953M, 953MH, 953ML, 955, 959K, 959M, 959MH, 959ML, 960, 990, 1023E, 1025R, 1026R, 1050J, 1050K, 1050K PL, 1070E, 1070G, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1210E, 1210G, 1270E, 1270G, 1354, 1404, 1420, 1435, 1445, 1470, 1470E, 1470G, 1510E, 1510G, 1538HR, 1545, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES III, 1646, 1646HS, 1700, 1700T, 1705T, 1725, 1725 CCS, 1725C, 1725NT, 1760, 1770, 1770NT, 1775, 1775NT, 1790, 1795, 1830, 1842GV, 1842HV, 1848GV, 1848HV, 1870, 1890, 1895, 1900, 1910, 1910E, 2020A, 2025R, 2026R, 2030A, 2032R, 2036R, 2038R, 2048HV, 2054, 2056, 2058, 2064, 2066, 2154G, 2156G, 2230FH, 2230LL, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2330, 2400 PRECISIONCUT, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510C, 2510S, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2654G, 2656G, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2956G, 3025D, 3025E, 3028EN, 3029DF128, 3029TF158, 3029TFG80, 3029TFU80, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3043D, 3045B, 3046R, 3050B, 3110, 3120, 3200, 3210, 3215, 3215B, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3510, 3520, 3522, 3720, 4020DF101, 4020TF006, 4020TF105, 4024HF285, 4024HF295, 4024TF270, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045DF154, 4045DF158, 4045DF270, 4045DF271, 4045HF152, 4045HF157, 4045HF158, 4045HF289, 4045HF475, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFU72, 4045HFU79, 4045SFM85, 4045T, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF253, 4045TF258, 4045TF270, 4045TF271, 4045TF277, 4045TF281, 4045TFS70, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4120, 4239TF001, 4320, 4520, 4700, 4710, 4720, 4730, 4830, 4920, 5030HF270, 5030TF270, 5036C, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5045D, 5045E, 5047D, 5050D, 5050E, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EN, 5075M, 5076E, 5076EF, 5076EL, 5078E, 5080E, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5120M, 5120ML, 5125M, 5125ML, 5130M, 5130ML, 5203, 5203S, 5204, 5210, 5220, 5225, 5303, 5305, 5310, 5310N, 5320, 5320N, 5325, 5325N, 5403, 5405, 5410, 5415, 5420, 5420N, 5425, 5425N, 5503, 5510, 5510N, 5520, 5520N, 5525, 5525N, 5603, 5610, 5615, 5620, 5625, 5715, 5720, 5725, 5820, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF158, 6068HF258, 6068HF279, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG55, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS83, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HP550, 6068HSG22, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF151, 6068TF158, 6068TF258, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6080A PRECISIONCUT, 6090 MC, 6090 RC, 6090HF475, 6090HF485, 6090HFC95, 6090HFL85, 6090M, 6095 MC, 6095 RC, 6095B, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135M, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140M, 6140R, 6145M, 6145R, 6150J, 6150M, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170R, 6175M, 6175R, 6180J, 6190J, 6190R, 6195M, 6195R, 6210R, 6215, 6215R, 6220, 6220L, 6230, 6230 Premium, 6230R, 6250R, 6320, 6320L, 6330, 6330 Premium, 6403, 6405, 6415, 6420, 6420L, 6420S, 6430, 6430 Premium, 6488, 6500A E-CUT, 6500A PRECISIONCUT, 6510, 6510S, 6520, 6520L, 6603, 6605, 6610, 6615, 6620, 6650, 6700A PRECISIONCUT, 6710, 6715, 6750, 6810, 6850, 6910, 6920, 6950, 7180, 7185J, 7200, 7200A, 7200R, 7205J, 7210, 7210R, 7215R, 7220, 7230R, 7250, 7250R, 7270R, 7280, 7290R, 7300, 7310R, 7320, 7350, 7380, 7400, 7400A, 7410, 7420, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7505, 7510, 7520, 7550, 7580, 7610, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7850, 7920, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8300T, 8310, 8310R, 8310T, 8320, 8320R, 8320T, 8330, 8330T, 8335R, 8345R, 8360R, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, B25C, B35C, B40C, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C1 200, C2 300, C2 400, C230, C240, C440, C440R, C441R, C451R, C461R, C650, C670, C850, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, DB44, DB60, DB66, DF180G, DF230, DR12, DR12T, DR16, DR18, DR24, E210, E210LC, E230, E240, E240LC, E260, E300LC, E330, E360, E400, F440M, F440R, F441M, F441R, F510, F525, F725, F910, F930, F1145, F4365, GT242, GT262, GT275, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX815E, LX172, LX173, LX176, LX178, LX186, LX188, M4030, M4040, M4040DN, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, P660, P670, P680, P690, PC7, PLANTER PERFORMANCE UPGRADES, R2 300, R40, R230, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, RSX860E, RSX860M, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SPRAYER PERFORMANCE UPGRADES, STRAIGHT BLADE, STX38, STX46, T550, T560, T660, T670, TC44H, TC54H, TC62H, TH 6X4, TRAIL BUCK 500, TRAIL BUCK 650, V451G, V451M, V451R, V461M, V461R, W200M, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, X300, X304, X324, X330, X350, X354, X370, X465, X475, X485, X495, X500, X520, X530, X540, X570, X575, X580, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z365R, Z525E, Z535M, Z535R, Z540M, Z540R, Z720E, Z730M, Z735E, Z735M, Z740R, Z760R, Z930R, Z950R, Z955R, Z970R, Z994R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
@@ -2387,6 +2827,16 @@
           <t>19M8499</t>
         </is>
       </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6X4, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 50 in., 52 IN., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 75G, 85G, 120C, 160C, 160G, 180G, 190E, 200D, 200G, 210C, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 240, 244E, 244H, 245, 250C, 250D, 250D-II, 260, 265, 285, 290D, 300C, 300D, 300D-II, 300DW, 300WW, 304H, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 315D, 315J, 315SE, 315SG, 315SL, 320, 324H, 325J, 325SL, 330B, 335C, 344H, 350 P, 350D, 350D-II, 350DW, 350G, 370E, 380G, 400D, 400D-II, 410D, 410E, 410G, 410J, 410K, 410L, 410TK TMC, 435C, 437C, 450, 450D, 450G, 450H, 450J, 450K, 455G, 460E, 470G, 482C, 485E, 486E, 488E, 490E, 510D, 540G-II, 544 G, 544E, 548G-II, 550, 550G, 550H, 550J, 550K, 555G, 590D, 595D, 600C, 605C, 608L, 608LH, 620G, 624E, 640G, 643G, 643J, 643K, 643L, 643L-II, 644 G, 644E, 644G, 648G, 650D, 650G, 650H, 650J, 650K, 655, 655C, 655K, 670C, 670CH, 670G, 672CH, 672G, 690E, 700H, 700J, 700J-II, 700K, 700L PL, 710D, 710G, 710J, 710K, 710L, 740G, 748, 748G-III, 750, 750J, 750J-II, 753GL, 755, 755C, 756, 759G, 759GH, 759J, 759JH, 770G, 772G, 790E, 792D, 843G, 843J, 843K, 843L, 843L-II, 848G, 850, 850D, 850J, 850J-II, 850JR, 850L, 850L PL, 853G, 855, 856, 870G, 872G, 892E, 903K, 903KH, 903M, 903MH, 904, 909K, 909KH, 909M, 909MH, 944K, 950C, 950K, 953G, 953K, 953M, 953MH, 955, 959K, 959M, 959MH, 959ML, 1050K, 1050K PL, 1054, 1354, 1404, 1433, 1433C, 1530, 1535, 1570, 1580, 1585, 1700, 1725, 2032R, 2054, 2310, 2510S, 2653, 2653B, 2704, 2854, 2904, 3004, 3033R, 3038R, 3039R, 3045R, 3046R, 3120, 3204, 3215B, 3225B, 3235B, 3320, 3520, 3554, 3710, 3720, 4730, 4830, 5090E, 5090R, 5100E, 5100R, 5115R, 5125R, 6095B, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6105D, 6105E, 6105EH, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6115D, 6115E, 6120B, 6120E, 6120EH, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6130, 6130D, 6130E SALTILLO, 6135B, 6135E, 6140B, 6140D, 6230, 6230 Premium, 6330, 6330 Premium, 6403, 6415, 6430, 6430 Premium, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6630, 6630 Premium, 6830, 6830 Premium, 6930, 7130 Premium, 7200R, 7210R, 7215R, 7230 Premium, 7230R, 7250R, 7260, 7260R, 7270R, 7280R, 7290R, 7310R, 7330 Premium, 7430E, 7455, 7460, 7530E, 7610, 7700, 7710, 7810, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8300T, 8310, 8310R, 8310T, 8320, 8320R, 8320T, 8330, 8330T, 8335R, 8345R, 8360R, 8370R, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8520, 8520T, 8530, 8560, 8570, 8700, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9400, 9400T, 9410R, 9420, 9420T, 9430, 9460R, 9470 STS, 9500, 9510, 9510R, 9520, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9550, 9560, 9560 STS, 9560R, 9570 STS, 9600, 9610, 9620, 9620T, 9630, 9630 SCRAPER, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, B25C, B30C, CS770, CTS, CTS II, L330, L1533, PLANTER PERFORMANCE UPGRADES, S160, S180, S200, S540, S550, S560, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W170, W650, W660, WL53, WL56</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
@@ -2394,6 +2844,16 @@
           <t>19M8499</t>
         </is>
       </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6X4, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 50 in., 52 IN., 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 72 IN., 75G, 85G, 120C, 160C, 160G, 180G, 190E, 200D, 200G, 210C, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 240, 244E, 244H, 245, 250C, 250D, 250D-II, 260, 265, 285, 290D, 300C, 300D, 300D-II, 300DW, 300WW, 304H, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 315D, 315J, 315SE, 315SG, 315SL, 320, 324H, 325J, 325SL, 330B, 335C, 344H, 350 P, 350D, 350D-II, 350DW, 350G, 370E, 380G, 400D, 400D-II, 410D, 410E, 410G, 410J, 410K, 410L, 410TK TMC, 435C, 437C, 450, 450D, 450G, 450H, 450J, 450K, 455G, 460E, 470G, 482C, 485E, 486E, 488E, 490E, 510D, 540G-II, 544 G, 544E, 548G-II, 550, 550G, 550H, 550J, 550K, 555G, 590D, 595D, 600C, 605C, 608L, 608LH, 620G, 624E, 640G, 643G, 643J, 643K, 643L, 643L-II, 644 G, 644E, 644G, 648G, 650D, 650G, 650H, 650J, 650K, 655, 655C, 655K, 670C, 670CH, 670G, 672CH, 672G, 690E, 700H, 700J, 700J-II, 700K, 700L PL, 710D, 710G, 710J, 710K, 710L, 740G, 748, 748G-III, 750, 750J, 750J-II, 753GL, 755, 755C, 756, 759G, 759GH, 759J, 759JH, 770G, 772G, 790E, 792D, 843G, 843J, 843K, 843L, 843L-II, 848G, 850, 850D, 850J, 850J-II, 850JR, 850L, 850L PL, 853G, 855, 856, 870G, 872G, 892E, 903K, 903KH, 903M, 903MH, 904, 909K, 909KH, 909M, 909MH, 944K, 950C, 950K, 953G, 953K, 953M, 953MH, 955, 959K, 959M, 959MH, 959ML, 1050K, 1050K PL, 1054, 1354, 1404, 1433, 1433C, 1530, 1535, 1570, 1580, 1585, 1700, 1725, 2032R, 2054, 2310, 2510S, 2653, 2653B, 2704, 2854, 2904, 3004, 3033R, 3038R, 3039R, 3045R, 3046R, 3120, 3204, 3215B, 3225B, 3235B, 3320, 3520, 3554, 3710, 3720, 4730, 4830, 5090E, 5090R, 5100E, 5100R, 5115R, 5125R, 6095B, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6105D, 6105E, 6105EH, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6115D, 6115E, 6120B, 6120E, 6120EH, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6130, 6130D, 6130E SALTILLO, 6135B, 6135E, 6140B, 6140D, 6230, 6230 Premium, 6330, 6330 Premium, 6403, 6415, 6430, 6430 Premium, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6630, 6630 Premium, 6830, 6830 Premium, 6930, 7130 Premium, 7200R, 7210R, 7215R, 7230 Premium, 7230R, 7250R, 7260, 7260R, 7270R, 7280R, 7290R, 7310R, 7330 Premium, 7430E, 7455, 7460, 7530E, 7610, 7700, 7710, 7810, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8300T, 8310, 8310R, 8310T, 8320, 8320R, 8320T, 8330, 8330T, 8335R, 8345R, 8360R, 8370R, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8520, 8520T, 8530, 8560, 8570, 8700, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9400, 9400T, 9410R, 9420, 9420T, 9430, 9460R, 9470 STS, 9500, 9510, 9510R, 9520, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9550, 9560, 9560 STS, 9560R, 9570 STS, 9600, 9610, 9620, 9620T, 9630, 9630 SCRAPER, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, B25C, B30C, CS770, CTS, CTS II, L330, L1533, PLANTER PERFORMANCE UPGRADES, S160, S180, S200, S540, S550, S560, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W170, W650, W660, WL53, WL56</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
@@ -2401,6 +2861,11 @@
           <t>19M7809</t>
         </is>
       </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 5B-700, 5B-704, 5B-750, 5B-754, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 6B-954, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 13HP, 15HP, 16HP, 60 in., 107, 108, 110, 120C, 120D, 160, 160C, 200 G, 200C, 200G, 204C, 205C, 206C, 207C, 208C, 210 G, 210 P, 210L, 210L EP, 230C, 240, 250, 250D-II, 260, 260 P, 260E, 270, 270C, 280, 300D-II, 310 G, 310 P, 310E, 310K, 310L, 310L EP, 310SE, 310SK, 310SL, 310SL HL, 312GR, 314G, 314R, 315 P, 315SE, 315SK, 315SL, 316GR, 317, 318D, 318E, 318G, 319D, 319E, 320, 320 P, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 332, 332D, 332E, 333D, 333E, 335C, 335D, 337E, 350G, 360DC, 370E, 370E-II, 380G, 400R, 410 P, 410E, 410E-II, 410K, 410L, 410R, 412R, 435C, 437C, 437D, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 446, 447, 448, 450 P, 450K, 454, 456, 457, 458, 460 P, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 493, 494, 500R, 524 P, 524K, 524K-II, 524L, 540G-II, 540G-III, 540H, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 546, 547, 548G-II, 548G-III, 548H, 550, 550 P, 550K, 554, 556, 557, 558, 560M, 560R, 566, 567, 568, 569, 594, 600R, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 615C, 615F, 615P, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620R, 622, 622F, 622G, 622R, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625R, 630, 630D, 630F, 630R, 635, 635D, 635F, 640D, 640G, 640H, 640L, 640L-II, 643G, 643H, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 648G, 648H, 648HT, 648L, 648L-II, 650, 650 P, 650K, 653, 653E, 653G, 654, 655K, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 692, 693, 694, 700K, 700L, 700L PL, 700M, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710 P, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 725D, 730D, 735D, 737, 740, 740A, 740D, 740G, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750K, 750L, 753J, 753JH, 755K, 757, 759J, 759JH, 768L-II, 770C II, 770CH II, 770D, 770G, 772CH II, 772D, 772G, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850J-II, 850K, 850L, 850L PL, 853, 853M, 853MH, 859M, 859MH, 870D, 870G, 872D, 872G, 892, 893, 894, 903K, 903KH, 903M, 903MH, 904 P, 909K, 909KH, 909M, 909MH, 912, 913, 914, 915F, 915R, 918, 918F, 918R, 920D, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944 X, 944K, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 960, 990, 1010D, 1010E, 1023E, 1025R, 1026R, 1050K, 1050K PL, 1070E, 1070G, 1092, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1270E, 1270G, 1290, 1291, 1293, 1312C, 1420, 1435, 1438GS, 1438HS, 1442, 1445, 1470, 1470E, 1470G, 1510C, 1510DC, 1510E, 1510G, 1512C, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1690, 1720 CCS, 1725NT, 1725T, 1742GS, 1742HS, 1742PR, 1770NT, 1775NT, 1790, 1795, 1810C, 1810DC, 1812C, 1812DC, 1814C, 1814DC, 1846, 1870, 1895, 1900, 1910, 1910G, 2030A, 2046HV, 2054, 2056, 2058, 2064, 2066, 2112C, 2112DC, 2230FH, 2254, 2256, 2258, 2264, 2266, 2266E, 2400 PRECISIONCUT, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2653A, 2653B, 2704, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2904, 3004, 3029D, 3029DF128, 3029DF129, 3029DF160, 3029DF180, 3029HFC03, 3029HFG03, 3029HFG89, 3029T, 3029TF158, 3029TF160, 3029TF180, 3029TF270, 3033R, 3038R, 3039R, 3045R, 3046R, 3100, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3300, 3310, 3320, 3400, 3410, 3420, 3520, 3720, 3754G, 3756G, 3800, 4024HF285, 4024HF295, 4024TF270, 4024TF280, 4024TF281, 4039D, 4039DF001, 4039DF008, 4039DF092, 4039T, 4039TF001, 4039TF008, 4044M, 4044R, 4045D, 4045DF001, 4045DF120, 4045DF120R02, 4045DF150, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045HF120, 4045HF120R02, 4045HF150, 4045HF158, 4045HF275, 4045HF280, 4045HF475, 4045HF485, 4045HFC28, 4045HFG20, 4045HFG85, 4045HFJ85, 4045HFK80, 4045HFS85, 4045TF001, 4045TF092, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF280, 4045TF290, 4045TFG20, 4045TFU20, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4940, 4990, 4995, 5030HF270, 5030HF285, 5030TF270, 5038D, 5039C, 5039D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5065E, 5065M, 5070M, 5075E, 5075EF, 5075M, 5080G, 5080GF, 5080GV, 5080M, 5090E, 5090G, 5090GH, 5090GV, 5090M, 5100E, 5100GV, 5100M, 5103, 5203, 5210, 5215, 5215F, 5215V, 5300, 5300N, 5303, 5310, 5310N, 5315, 5315F, 5315V, 5400, 5403, 5410, 5410N, 5415, 5425, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5615, 5615V, 5620, 5625, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068CI550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF157, 6068HF158, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG20, 6068HFG85, 6068HFS01, 6068HI550, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6080A PRECISIONCUT, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG94, 6090HFG95, 6090HFM85, 6090M, 6090SFM75, 6095B, 6100J, 6100M, 6105EH, 6105J, 6110, 6110J, 6110L, 6110M, 6115J, 6120, 6120EH, 6120L, 6120M, 6125J, 6130J, 6135AFM75, 6135AFM85, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140J, 6140JH, 6145J, 6150J, 6155J, 6155JH, 6165J, 6170J, 6180CI510, 6180J, 6190J, 6205, 6210, 6210L, 6215, 6220, 6220L, 6310, 6310L, 6320, 6320L, 6400, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6500A E-CUT, 6500A PRECISIONCUT, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6605, 6610, 6615, 6620, 6700A PRECISIONCUT, 6715, 6810, 6820, 6910, 6910S, 6920, 6920S, 7180, 7200, 7200A, 7200R, 7210, 7210R, 7215R, 7220, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7450, 7455, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7505, 7510, 7515, 7520, 7525, 7550, 7580, 7610, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7850, 7920, 7950, 7980, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9320, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9630, 9630 SCRAPER, 9630T, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, 15538, BP15, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C230, C440, C451R, C461R, C500, C650, C670, C850, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT322, CT332, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, E12, E15, E210, E210-II, E210LC, E230, E230-II, E330, E360, E380, E400, F510, F525, F620, F680, F687, F910, F911, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, GS25, GS30, GS45, GS75, H480, L17.542, L60, L331, L341, L1742, L2048, L2548, M-GATOR A1, M15, M20, N530C, N540, N540C, N542, N542C, N560F, P576, R10, R15, R20, R40, R500, R4038, R4044, R4045, R4060, RSX 850I, RSX860E, RSX860I, RSX860M, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2546, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, V451R, V461R, W330, W430, W540, W550, W650, W660, WL56, X9 1000, X9 1100, X300R, X305R, X330, X350, X350R, X354, X370, X380, X384, X390, X394, X570, X580, X584, X590, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, Z245, Z425, Z435, Z445, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z910A, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z960A, Z960M, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
@@ -2408,6 +2873,11 @@
           <t>19M7810</t>
         </is>
       </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>3-Bag, 6R 120, 6R 130, 6R 140, 6R 145, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 20 Trailer, 30 Trailer, 47 IN., 50 in., 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 110, 110 TLB, 120C, 120D, 130G, 160, 160C, 200, 200C, 204C, 205C, 206C, 207C, 208C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 230C, 240, 240D, 250D-II, 250G, 260, 260 P, 260E, 270, 270C, 270D, 280, 290G, 300D-II, 300G, 310 P, 310E, 310G, 310J, 310K, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 314G, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 318D, 318G, 319D, 320, 320D, 323D, 324H, 325, 325J, 325SK, 328, 330B, 330C, 332, 335, 335C, 335D, 337E, 344H, 344J, 344K, 350 P, 350D, 350G, 360DC, 370, 370C, 370E, 370E-II, 375, 380 P, 380G, 381, 385, 388, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 435, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 446, 447, 448, 449, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 482C, 485E, 486E, 488, 488E, 524 P, 524K, 524K-II, 524L, 530B, 531, 535, 540E, 540G-II, 540G-III, 540H, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 555G, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 575, 578, 600R, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608L, 608LH, 608SH, 612C, 612C PERFORMANCE UPGRADES, 612R, 615F, 615P, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620F, 620G, 620I, 620R, 622F, 622G, 622R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625R, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 631, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643G, 643H, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650, 650G, 650H, 650J, 650K, 651, 653, 653E, 653G, 654, 655K, 661, 670, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 690E, 700H, 700J, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 718C, 718C PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 725D, 727, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 731, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753G, 753GH, 753GL, 753J, 753JH, 755D, 755K, 757, 759G, 759GH, 759J, 759JH, 762B, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 777, 790, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870D, 870G, 872D, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 925D, 930D, 936D, 944K, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 959J, 959K, 959M, 959MH, 959ML, 1010D, 1010E, 1010G, 1050K, 1050K PL, 1070D, 1070E, 1070G, 1107, 1109, 1110D, 1110E, 1110G, 1111, 1113, 1165, 1170, 1170E, 1170G, 1175, 1185, 1210E, 1210G, 1270D, 1270E, 1270G, 1312C, 1410D, 1420, 1435, 1445, 1450, 1470, 1470D, 1470E, 1470G, 1490D, 1510C, 1510DC, 1510E, 1510G, 1512C, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1620, 1700, 1705, 1710D, 1711D, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725T, 1730, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810C, 1810DC, 1812C, 1812DC, 1814C, 1814DC, 1840, 1842GV, 1842HV, 1848GV, 1848HV, 1850, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 1948GV, 1948HV, 2032R, 2054, 2056, 2058, 2064, 2066, 2112C, 2112DC, 2144G, 2154G, 2156G, 2204, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2400 PRECISIONCUT, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2654G, 2656G, 2700 E-CUT HYBRID, 2704, 2720, 2854, 2904, 2954D, 3004, 3025D, 3028EN, 3029DF128, 3029TF158, 3035D, 3036E, 3036EN, 3043D, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 4039DF008, 4039TF008, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG20, 4045HFG81, 4045HFG85, 4045HFJ85, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFU72, 4045HFU79, 4045HFU81, 4045HG551, 4045HI550, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN056, 4045HSG20, 4045HSG21, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5036C, 5036D, 5038D, 5039D, 5040D, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5075E, 5075M, 5076E, 5076EL, 5078E, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5320, 5320N, 5325, 5400, 5403, 5405, 5410, 5415, 5420, 5420N, 5425, 5430I, 5440, 5460, 5500, 5503, 5510, 5510N, 5520, 5520N, 5525, 5603, 5610, 5615, 5625, 5715, 5720, 5725, 5730, 5820, 5830, 6010, 6020, 6068CI550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HI550, 6068HN075, 6068HN077, 6068HRT81, 6068HSG22, 6068HT087, 6068SFM50, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6076AFN, 6076HF030, 6080A E-CUT, 6081AF001, 6081AFH75, 6081HF001, 6081HF070, 6081HFH70, 6081HFN01, 6081HFN02, 6081HFN03, 6081HFN04, 6081TF001, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6100, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6110, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6115D, 6115E, 6115J, 6115M, 6120, 6120E, 6120EH, 6120L, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135R, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140D, 6140J, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6155J, 6165J, 6180CI510, 6180J, 6200, 6200L, 6205, 6210, 6210L, 6215, 6220, 6220L, 6225, 6230, 6230 Premium, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7195J, 7200, 7200J, 7200R, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 7950, 7980, 8000, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, A420R, A520R, BP15, C2 400, C6R, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C440R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT322, CT332, CTS, CTS II, CX15, CX20, DB37, DB41, DB44, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DF150, DF180G, DF250, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E12, E15, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F441M, F510, F525, F710, F725, F735, F910, F911, F925, F930, F932, F935, F1145, F4365, FC12E, FC15E, FC15M, FC20M, GT242, GT262, GT275, H480, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX15, HX20, L70, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, M-GATOR A1, M15, M20, M4030, M4040, M4040DN, MX15, N530C, N530F, N536C, N540C, N540F, N542C, N543F, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, R10, R40, R230, R450, R4030, R4038, R4044, R4045, R4060, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST18, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, W50, W70, W80, W100, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL56, X9 1000, X9 1100, X300, X304, X310, X320, X324, X500, X520, X530, X534, X540, X570, X580, X590, Y110, Y115, Y210, Y215, Z225, Z245, Z425, Z435, Z445, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
@@ -2415,6 +2885,11 @@
           <t>19M7820</t>
         </is>
       </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 30 Trailer, 42 IN., 48 IN., 54 IN. FRONT BLADE, 60, 102, 105, 115, 120C, 125, 135, 145, 155C, 160C, 190C, 200C, 230C, 270C, 337E, 370E, 410E, 415, 425, 437E, 444J, 445, 455, 460DC, 460E, 500R, 525, 530, 535, 544J, 565, 568, 570, 572, 575, 578, 580, 582, 590, 592, 608C, 620G, 620I, 622G, 624J, 625, 630, 635, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 644K HYBRID, 648G, 648H, 648HT, 648L, 670G, 672G, 678, 724J, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 735FD PERFORMANCE UPGRADES, 740FD, 740FD PERFORMANCE UPGRADES, 744H, 744J, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748G-III, 750A, 750J, 750J-II, 750K, 770G, 772G, 803M, 803MH, 824J, 824K, 844J, 844K, 850J, 850J-II, 850JR, 850K, 853M, 853MH, 859M, 859MH, 870G, 872G, 890, 895, 896, 912, 914, 944K, 946, 956, 990, 994, 997, 1050K, 1450, 1550, 1600 TURBO SERIES II, 1620, 1690, 1700, 1700T, 1705, 1705T, 1720, 1720 CCS, 1725, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1765, 1770, 1775, 1775NT, 1780, 1810, 1830, 1835, 1840, 1860, 1870, 1890, 1895, 1900, 1990, 2020, 2020A, 2030, 2030A, 2054, 2056, 2058, 2064, 2066, 2230FH, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2430, 2430C, 2510H, 2660VT, 2704, 2730, 2854, 2904, 3004, 3025E, 3032E, 3036E, 3038E, 3045B, 3050B, 3204, 3365, 3800, 4710, 4920, 6068CI550, 6068HFC08, 6068HFC09, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFS01, 6068HI550, 6135AFM75, 6135AFM85, 6135HF475, 6135HF485, 6135HFG75, 6135HFG84, 6135HFM85, 6135SFM75, 6135SFM85, 7350, 7380, 7450, 7455, 7460, 7480, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 9009A, 9120, 9220, 9230, 9320, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420, 9420R, 9420RX, 9430, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9630, 9630 SCRAPER, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, A420R, A520R, C450, C500, C650, C670, CP690, CP770, CS690, CS770, CTS, CTS II, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB60, E100, E110, E120, E130, E140, E150, E160, E170, E180, FD55, H540F, H541, H550, H550F, H560F, H561, HD35F, HD40F, HD45F, HD50F, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, N530, N530C, N536, N536C, N540, N540C, N542, N542C, N550, N560, N560F, P576, PLANTER PERFORMANCE UPGRADES, R500, S100, S110, S120, S130, S140, S160, S170, S180, S220, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH12R, STRAIGHT BLADE, T550, T560, T660, T670, TD100, W36R, W48R, W52R, W61R, W540, W550, W650, W660, X9 1000, X9 1100, X105, X106, X107, X110, X115R, X116R, X117R, X120, X125, X126, X127, X130R, X135R, X140, X145, X146R, X147R, X155R, X165, X166, X166R, X167, X167R, X465, X475, X485, X495, X575, X585, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
@@ -2422,6 +2897,16 @@
           <t>19M7837</t>
         </is>
       </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 48 IN., 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 425, 440E, 445, 448, 449, 450M, 455, 458, 459, 460M, 460R, 468, 469, 524 P, 524L, 525, 530, 535, 544 P, 544L, 550M, 558, 559, 560M, 560R, 568, 569, 572, 578, 582, 592, 607C, 608C, 609C, 610C, 611C, 612C, 616, 616R, 618, 620, 622, 624 P, 624L, 625, 625F, 630, 630FD, 635, 635F, 635FD, 640FD, 643H, 644 X, 644J, 644K, 644K HYBRID, 644LH, 645FD, 678, 724K, 730, 730FD, 735, 735FD, 740, 740FD, 744 P, 744L, 745FD, 748, 750A, 824 P, 824L, 830, 835, 835 SHORT CHASSIS, 843H, 844 P, 844J, 844L, 844L AGGREGATE HANDLER, 859M, 859MH, 890, 895, 904 P, 909M, 909MH, 944 X, 944K, 959M, 959MH, 959ML, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1705T, 1725C, 1725T, 1770, 1775NT, 1795, 1820, 1830, 1835, 1870, 1890, 1900, 1910, 2020A, 2030A, 2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 3025D, 3028EN, 3035D, 3036E, 3036EN, 3043D, 3045B, 3050B, 3316, 4700, 4710, 4720, 4730, 4830, 4920, 5036C, 5038D, 5039C, 5041C, 5042C, 5075M, 5085M, 5090M, 5090R, 5100M, 5100MH, 5100R, 5103, 5103E, 5103S, 5104, 5115M, 5115R, 5115RH, 5125M, 5125R, 5203, 5203S, 5204, 5310, 5410, 5610, 6105D, 6115D, 6130D, 6140D, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7460, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8225R, 8245R, 8270R, 8295R, 8300, 8320R, 8320RT, 8335R, 8345R, 8345RT, 8370R, 8370RT, 8400, 8400R, 8500, 8600, 8700, 8800, 9230, 9330, 9370R, 9400, 9410, 9420R, 9420RX, 9430, 9450, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9550, 9560, 9560 STS, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, C1 200, C2 300, C2 400, C100, C110, C120, C230, C240, C440, C670, CP690, CP770, CS690, CS770, CTS, CTS II, DB60, DR8T, H540F, H541, H550, H550F, H560F, H561, HD200, HD300, P540, P556, P576, R2 300, R230, RD30F, RD35F, RD40F, RD45F, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, SST15, SST16, SST18, T550, T560, T660, T670, W70, W200M, W235, W235M, W235R, W260R, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, X710, X730, X734, X738, X739, X750, X754, X758, X950R, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Y210, Y215, Z510A, Z520A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950M, Z950R, Z955M, Z955R, Z960M, Z960R, Z970R, Z994R</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
@@ -2429,6 +2914,11 @@
           <t>19M7838</t>
         </is>
       </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>3-Bag, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 2304, 8R 2704, 8R 3004, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 30R, 46R, 244H, 337E, 350D, 350G, 380G, 410G, 437E, 444E, 450C, 470 P, 470G, 540R, 543M, 543R, 600R, 603M, 603R, 605C, 620R, 623M, 623R, 624J, 624K, 624K-II, 624KR, 625D, 630D, 635D, 640D, 640H, 640R, 643J, 643K, 643L, 643L-II, 643M, 643R, 644J, 644K, 644K HYBRID, 648H, 648HT, 660R, 663R, 680R, 683R, 710 P, 710L, 724J, 724K, 725D, 730D, 735D, 740D, 748, 748H, 748HT, 750J, 755K, 759G, 759GH, 843J, 843K, 843L, 843L-II, 848H, 848HT, 850J, 850J-II, 850JR, 853J, 853JH, 903J, 903JH, 903KH, 909J, 909JH, 909KH, 946, 953J, 956, 959J, 1720, 1720 CCS, 1725, 1725 CCS, 1740, 1745, 1750, 1755, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1820, 1830, 1835, 1870, 1890, 1895, 1900, 1910, 2020A, 2030A, 2204, 2510H, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2704, 2854, 2904, 3004, 3029DF128, 3029DF129, 3029DFG20, 3029DFU20, 3029DFU29, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFU20, 3029TFU29, 3029TFU89, 3204, 3754D, 4039DF008, 4039TF008, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF158, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HF120, 4045HF120R02, 4045HF150, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF287, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFS72, 4045HFS73, 4045HI440, 4045HI550, 4045HI551, 4045TF120, 4045TF150, 4045TF151, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4239TF001, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 6068DF150, 6068HF158, 6068HF258, 6068HFS72, 6068HFS77, 6068TF158, 6068TF258, 6080A E-CUT, 6080A PRECISIONCUT, 6103, 6105AF001, 6105HF001, 6125AF001, 6125AFM01, 6125HF001, 6125HF070, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135HFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6500A E-CUT, 6500A PRECISIONCUT, 6700A PRECISIONCUT, 7180, 7185J, 7195J, 7200A, 7200J, 7205J, 7210J, 7215J, 7225J, 7230J, 7250, 7280, 7350, 7380, 7400A, 7450, 7460, 7480, 7500A E-CUT, 7500A PRECISIONCUT, 7550, 7580, 7630, 7660, 7700A PRECISIONCUT, 7715, 7720, 7730, 7750, 7760, 7780, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8360R, 8360RT, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9400, 9410, 9410R, 9420R, 9420RX, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9540, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9640, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, A420R, A520R, C2 400, C300, C350, C400, C440, C450, C500, CP690, CP770, CS690, CS770, CTS, CX15, CX20, DB44, FC10R, FC15M, FC15R, FC20M, FC20R, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HX15, HX20, L330, L340, M15, M20, N530C, N536C, N540C, N542C, N550, N560, N560F, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R400, RSX 850I, RSX860E, RSX860I, RSX860M, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W430, W540, W550, W650, W660, X730, X734, X738, X739, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Z510A, Z520A, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
@@ -2436,6 +2926,11 @@
           <t>19M8737</t>
         </is>
       </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8RT 310, 8RT 340, 8RT 370, 8RX 310, 8RX 340, 8RX 370, 260, 270, 270A, 270B, 280, 325, 328, 332, 444 P, 444J, 444K, 444L, 524 P, 524K, 524K-II, 524L, 544 P, 544J, 544K, 544K-II, 544L, 572, 582, 592, 620 P, 620G, 622 P, 622G, 623, 624 P, 624J, 624K, 624K-II, 624L, 625D, 630D, 635D, 640D, 644, 644 G, 644 P, 644 X, 644J, 644K, 644K HYBRID, 644L, 644LH, 670 P, 670G, 672 P, 672G, 724 P, 724J, 724K, 724L, 725D, 730D, 735D, 740D, 744, 748H, 770 P, 770G, 772 P, 772G, 800R, 848H, 870G, 872G, 1023E, 1026R, 1575, 1585, 1830, 1870, 1890, 2032R, 2036R, 2038R, 2620, 2623, 2625, 3025D, 3025E, 3032E, 3035D, 3036E, 3036EN, 3038E, 3043D, 4710, 4720, 4730, 4830, 6080A E-CUT, 6080A PRECISIONCUT, 6090AFM75, 6090AFM85, 6090SFM75, 6090SFM85, 6105M, 6115M, 6125M, 6500A E-CUT, 6500A PRECISIONCUT, 6700A E-CUT, 6700A PRECISIONCUT, 7200, 7200A, 7200R, 7210R, 7215R, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7400, 7400A, 7500A E-CUT, 7500A PRECISIONCUT, 7660, 7700A E-CUT, 7700A PRECISIONCUT, 7760, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9470 STS, 9500, 9570 STS, 9600, 9660 STS, 9670 STS, 9700, 9760 STS, 9770 STS, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, C650, C650L, C850, C850T, CP690, CS690, F4365, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, N543F, N550, N560, N560F, P556, P576, S7 600, S7 700, S7 800, S7 850, S7 900, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, STRAIGHT BLADE, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, Z510A, Z520A</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
@@ -2443,6 +2938,11 @@
           <t>19M7823</t>
         </is>
       </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 606C, 608C, 608C PRECISION UPGRADES, 612C, 612FC, 616C, 618C, 706C, 708C, 712C, 712FC, 716C, 718C, 1350, 1355, 1360, 1365, 1460, 1465, 1470, 1570, 1745, 5005, 5036D, 5039D, 5040D, 5042D, 5045D, 5050D, 5105, 5205, 5305, 6180CI510, 9370R, 9420R, 9470R, 9500, 9520R, 9570R, 9600, 9620R, 9700, C6R, C6R PRECISION UPGRADES, C8R, C8R PRECISION UPGRADES, C12F, C12F PRECISION UPGRADES, C12R, C12R PRECISION UPGRADES, C16F, C16F PRECISION UPGRADES, C16R, C16R PRECISION UPGRADES, C18F, C18F PRECISION UPGRADES, C18R, C18R PRECISION UPGRADES, CH330, CH530, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, GROUPER, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T560, T660, T670, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
@@ -2450,6 +2950,11 @@
           <t>03M7198</t>
         </is>
       </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6X4, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 110 TLB, 160A, 180A, 203C, 208R, 209F, 209R, 210F, 213F, 215F, 215R, 218F, 218R, 220F, 222F, 222R, 228, 228A, 240, 245, 260, 265, 285, 314R, 320, 324, 328, 331, 335, 375, 381, 385, 388, 435, 440E, 444K, 446, 447, 448, 449, 450, 450E, 450M, 455, 456, 457, 458, 459, 459E, 460, 460M, 460R, 460S, 466, 467, 468, 469, 490, 490 PRO, 493, 494, 500R, 520M, 524K, 524K-II, 525, 530, 535, 540M, 540R, 544K, 544K-II, 545, 546, 547, 550, 550M, 556, 557, 558, 559, 560M, 560R, 566, 567, 568, 569, 570, 572, 580, 582, 590, 592, 594, 600R, 600T, 604C, 605C, 606C, 607C, 608C, 608FC, 609C, 610C, 611C, 612C, 612FC, 613C, 614C, 614R, 615C, 615F, 615R, 616, 616C, 616F, 616R, 617C, 618, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 622X, 623, 624K, 624K-II, 624KR, 625, 625D, 625F, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630PF, 630R, 630X, 635, 635D, 635F, 635FD, 635PF, 635R, 635X, 639, 640C, 640D, 640FD, 640L, 640L-II, 640X, 643L, 643L-II, 644, 644K, 644K HYBRID, 645C, 645FD, 648L, 648L-II, 649, 659, 678, 692, 693, 694, 700M, 708FC, 712FC, 722PF, 722X, 724K, 725D, 725PF, 725X, 730, 730D, 730FD, 730PF, 730X, 735, 735D, 735FD, 735PF, 735X, 737, 740D, 740FD, 740PF, 740X, 744, 744K-II, 745FD, 748L, 748L-II, 757, 768L-II, 772, 777, 778, 780, 785, 797, 803M, 803MH, 824K, 830, 835, 842, 843L, 843L-II, 844K, 848L, 848L-II, 852, 853M, 853MH, 854, 859M, 859MH, 862, 864, 890, 891, 892, 893, 894, 895, 896, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 956, 960, 990, 994, 995, 997, 1010, 1023E, 1025R, 1026R, 1030, 1035, 1092, 1160A, 1175, 1180A, 1290, 1291, 1293, 1295, 1340, 1350, 1355, 1360, 1365, 1424, 1424C, 1460, 1465, 1470, 1530, 1535, 1570, 1690, 1700, 1705, 1715, 1725, 1725C, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1790, 1795, 1870, 1900, 1990, 2025R, 2026R, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2230FH, 2230LL, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2510C, 2510S, 3033R, 3038R, 3039R, 3045R, 3046R, 3120, 3316, 3320, 3510, 3520, 3720, 4710, 5067E, 5075E, 6105M, 6105R, 6110M, 6110R, 6115M, 6115R, 6120M, 6120R, 6125M, 6125R, 6130M, 6130R, 6135M, 6135R, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6175M, 6175R, 6195M, 6195R, 6210M, 6215R, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7480, 7500, 7550, 7580, 7600, 7610, 7700, 7710, 7750, 7760, 7780, 7800, 7810, 7850, 7950, 7980, 8100, 8200, 8300, 8320RT, 8345RT, 8370RT, 8400, 8500, 8570, 8600, 8700, 8770, 8800, 8870, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9400, 9400T, 9410, 9420, 9420T, 9430, 9430T, 9450, 9470 STS, 9500, 9501, 9510, 9520, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9620, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, C1 200, C2 300, C2 400, C8F, C8F PRECISION UPGRADES, C100, C110, C120, C230, C240, C300, C310R, C350, C350R, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, CP20, CP690, CP770, CS690, CS770, CTS, CTS II, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, F310R, F350R, F440M, F440R, F441M, F441R, GROUPER, H240, H260, H310, H340, H360, H380, H480, L60, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, M-GATOR A1, MaxEmerge XP, P576, R2 300, R40, R230, R310R, R350R, R400, R500, R870R, R930R, R950R, R990R, RD30F, RD35F, RD40F, RD45F, ROW-CROP HARVESTING UNITS, S250, S300, S310R, S350, S350R, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, SH12F, SH12R, T550, T560, T660, T670, TE 4X2, TURF TX 4X2, V451G, V451M, V451R, V461M, V461R, W170, W200M, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, X300, X304, X305R, X310, X320, X324, X340, X360, X465, X475, X485, X495, X575, X585, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, Y210, Y215, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
@@ -2457,6 +2962,11 @@
           <t>H160905</t>
         </is>
       </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>500R, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, C500, R500, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, X9 1000, X9 1100</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
@@ -2464,6 +2974,11 @@
           <t>03M7201</t>
         </is>
       </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>54D IN., 60 IN. DECKS, 60D IN., 62 IN., 160, 200CX, 200X, 440E, 446, 448, 449, 456, 459, 466, 525, 530, 535, 546, 556, 565, 566, 568, 570, 572, 575, 578, 580, 582, 590, 592, 604C, 605C, 606C, 607C, 608C, 608C PRECISION UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612FC, 613C, 614C, 614R, 615C, 615P, 615R, 616, 616C, 616R, 617C, 618C, 618PF, 618R, 620PF, 620R, 622PF, 622R, 622X, 625, 625PF, 625R, 625X, 630, 630PF, 630R, 630X, 635, 635PF, 635R, 635X, 640X, 644, 678, 706C, 708C, 708FC, 712C, 712FC, 716C, 718C, 722PF, 722X, 725PF, 725X, 730, 730PF, 730X, 735, 735PF, 735X, 740PF, 740X, 744, 803M, 803MH, 830, 835, 850L, 853M, 853MH, 854, 859M, 859MH, 864, 903M, 946, 950K, 953M, 953MH, 953ML, 956, 959M, 959MH, 959ML, 1010, 1015, 1023E, 1050K, 1050K PL, 1350, 1355, 1360, 1365, 1460, 1465, 1470, 1512FX, 1516FX, 1524FX, 1535, 1640, 1690, 1700, 1705, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1730, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1830, 1835, 1900, 1910, 1990, 2032R, 2036R, 2038R, 2040, 2040S, 2140, 2230FH, 2230LL, 2310, 2330, 2510H, 2520, 3033R, 3038R, 3039R, 3040, 3045R, 3046R, 3140, 3316, 7200, 7200A, 7260, 7400, 7400A, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8800, 8800A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9400, 9400T, 9410, 9420, 9420T, 9430, 9430T, 9450, 9470 STS, 9500, 9501, 9510, 9520, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9620, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, 9986, 9996, A400, A420R, A520R, BP15, C1 200, C2 300, C2 400, C6R, C6R PRECISION UPGRADES, C8F, C8F PRECISION UPGRADES, C8R, C8R PRECISION UPGRADES, C12F, C12F PRECISION UPGRADES, C12R, C12R PRECISION UPGRADES, C16F, C16F PRECISION UPGRADES, C16R, C16R PRECISION UPGRADES, C18F, C18F PRECISION UPGRADES, C18R, C18R PRECISION UPGRADES, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C451R, C461R, C670, C850, CH330, CH530, CH950, CH960, CP690, CP770, CS770, CTS, CTS II, DB37, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, F440M, F441M, F441R, GROUPER, H130, H540F, H541, H550, H550F, H560F, H561, L330, L331, L340, L341, LX277, LX279, LX280, MaxEmerge XP, N530C, N536C, N540C, N542C, Pro-Series XP, R400, R450, REDEKOP SCU, S160, S180, S200, S250, S300, S350, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
@@ -2471,6 +2986,11 @@
           <t>19M8306</t>
         </is>
       </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>3-Bag, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 47 IN., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 110, 120C, 120D, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180G, 200, 200 G, 200C, 200D, 200G, 210 P, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 230C, 240, 240D, 250, 250 P, 250D, 250D-II, 250G, 260 P, 260E, 270, 270C, 270D, 290G, 300 P, 300D-II, 300DW, 300G, 300WW, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 313, 315, 315 P, 315J, 315SE, 315SG, 315SK, 315SL, 317, 318D, 319D, 320, 320 P, 320D, 323D, 324H, 325, 325J, 325SK, 325SL, 326D, 328, 328D, 329D, 330B, 332D, 333D, 335C, 335D, 337E, 344 P, 344H, 344J, 344K, 344L, 350 P, 350D, 350G, 360DC, 370E, 375, 380 P, 380G, 385, 390, 410 P, 410E, 410G, 410J, 410K, 410L, 410TK TMC, 435C, 437C, 437D, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 450 P, 450G, 450H, 450J, 450K, 454, 455G, 460, 460DC, 460E, 460S, 475, 485E, 486E, 488E, 490, 490 PRO, 524 P, 524K, 524K-II, 524L, 540G-II, 540G-III, 540H, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 548G-II, 548G-III, 548H, 550, 550 P, 550G, 550H, 550J, 550K, 555G, 563, 605C, 605K, 606C, 608C, 608L, 608LH, 608SH, 615F, 618F, 618R, 620F, 620G, 620R, 622F, 622G, 622R, 622X, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 640C, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643G, 643H, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 648G, 648H, 648HT, 648L, 648L-II, 649, 650 P, 650G, 650H, 650J, 650K, 653, 653E, 653G, 654, 655K, 659, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 673, 690, 690E, 692, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 710 P, 710D, 710G, 710J, 710K, 710L, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740PF, 740X, 744 P, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755D, 755K, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770D, 770G, 772, 772G, 778, 800R, 803M, 803MH, 810D, 810E, 824 P, 824K, 824L, 830, 835, 843G, 843H, 843J, 843K, 843L, 843L-II, 844K, 848H, 848HT, 848L, 848L-II, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870G, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 944K, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 959J, 959K, 959M, 959MH, 959ML, 1000, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1050K, 1070D, 1070E, 1070G, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1270D, 1270E, 1270G, 1410D, 1450, 1470, 1470D, 1470E, 1470G, 1490D, 1500, 1510E, 1510G, 1550, 1570, 1710D, 1711D, 1775NT, 1850, 1900, 1910, 1910E, 1910G, 2000, 2020A, 2025R, 2026R, 2030A, 2032R, 2036R, 2038R, 2054, 2144G, 2154D, 2154G, 2156G, 2254, 2256, 2258, 2454D, 2654G, 2656G, 2704, 2904, 2954D, 2956G, 3004, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3033R, 3038R, 3039R, 3045R, 3046R, 3154G, 3156G, 3200, 3204, 3215, 3220, 3225C, 3235C, 3245C, 3365, 3400, 3420, 3520, 3522, 3754D, 3754G, 3756G, 3800, 4039DF008, 4039TF008, 4045AFM85, 4045CA550, 4045CB551, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4239TF001, 4510, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5085E, 5085M, 5090E, 5090EL, 5090M, 5090R, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120ML, 5125M, 5125ML, 5125R, 5130ML, 5430I, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105M, 6105R, 6110 MC, 6110 RC, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115M, 6115R, 6120E, 6120EH, 6120M, 6120R, 6125M, 6125R, 6130D, 6130M, 6130R, 6135E, 6135M, 6135R, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6175M, 6175R, 6195M, 6195R, 6210M, 6215R, 6230R, 6250R, 6610, 6650, 6700, 6710, 6750, 6810, 6850, 6910, 6950, 7180, 7195J, 7200, 7200J, 7210J, 7215J, 7225J, 7230J, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7630, 7660, 7700, 7720, 7730, 7750, 7760, 7780, 7800, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9470 STS, 9470R, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9520, 9520R, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9570 STS, 9570R, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, C1 200, C2 300, C2 400, C230, C240, C440, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CTS, CTS II, DB37, DB41, DB44, DB55, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F510, F525, F1145, F4365, GROUPER, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HD300, M4030, M4040, M4040DN, R2 300, R230, R450, R4023, R4038, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, T550, T560, T660, T670, TC44H, TC54H, TC62H, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X465, X475, X485, X495, X575, X585, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
@@ -2478,6 +2998,11 @@
           <t>19M7818</t>
         </is>
       </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>3-Bag, 5-750, 5-754, 5-800, 5-804, 5-900, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 31C, 47 IN., 54D IN., 60, 60 IN. DECKS, 60D IN., 62 IN., 110 TLB, 112R, 120D, 130G, 160D, 160G, 180G, 200D, 200G, 210G, 240, 240D, 250, 250G, 260, 270, 270D, 280, 290G, 317, 320, 325, 328, 332, 335, 375, 385, 435, 440E, 444H, 444J, 446, 447, 448, 449, 450, 450C, 450D, 450E, 450M, 454, 456, 457, 458, 459, 459E, 460M, 460R, 466, 467, 468, 469, 475, 490, 493, 494, 524K, 525, 530, 535, 540G-II, 540M, 543R, 544G, 544H, 544J, 544K, 545, 546, 547, 548G-II, 550, 550M, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 603R, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 614R, 615C, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 623R, 624G, 624H, 624J, 624K, 624KR, 625, 625F, 625I, 625PF, 625R, 625X, 630, 630FD, 630PF, 630R, 630X, 635, 635F, 635FD, 635PF, 635R, 635X, 640FD, 640G, 640X, 644, 644 X, 644G, 644H, 644HMH, 644J, 644K HYBRID, 644LH, 647, 648G, 648L-II, 653, 654, 655, 660, 665, 670, 670D, 670G, 672D, 672G, 673, 678, 680, 681, 690E, 692, 693, 694, 700J, 700J-II, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724J, 725PF, 725X, 730, 730PF, 730X, 735, 735PF, 735X, 740A, 740G, 740PF, 740X, 744, 744H, 744J, 744K, 744K-II, 748, 748G-III, 748L-II, 750A, 750J, 750J-II, 750K, 750L, 755D, 770, 770D, 770G, 772, 772D, 772G, 777, 797, 824J, 824K, 825 LONG CHASSIS, 830, 835, 835 SHORT CHASSIS, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 848L-II, 850J, 850J-II, 850L, 852, 853, 853J, 853JH, 855 LONG CHASSIS, 862, 870D, 870G, 872D, 872G, 892, 893, 894, 900, 903J, 903JH, 903KH, 909J, 909JH, 909K, 909KH, 911, 913, 915F, 918, 918R, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 930D, 930F, 930R, 936D, 944K, 946, 948L-II, 953J, 956, 959J, 959K, 960, 990, 994, 1092, 1107, 1109, 1111, 1113, 1175, 1290, 1291, 1293, 1312C, 1350, 1360, 1420, 1435, 1445, 1450, 1460, 1470, 1510C, 1510DC, 1512C, 1512E, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1690, 1790, 1795, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1820, 1830, 1835, 1910, 1990, 2010DE, 2014DE, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2112C, 2112DC, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2154D, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2412DE, 2454D, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2720, 2730, 2954D, 3025D, 3025E, 3028EN, 3032E, 3035D, 3036E, 3036EN, 3038E, 3043D, 4044M, 4044R, 4045AFM85, 4045DF120, 4045DF150, 4045DF271, 4045DFM50, 4045DFM70, 4045HF120, 4045HF120R02, 4045HF150, 4045HF275, 4045HF475, 4045TF120, 4045TF150, 4045TF220, 4045TF250, 4045TF271, 4045TF275, 4045TFM50, 4045TFM75, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4630, 4700, 4710, 4720, 4730, 4830, 5036C, 5038D, 5039C, 5039D, 5041C, 5042C, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5067E, 5070E, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5100E, 5100M, 5100R, 5101E, 5101EN, 5103, 5103S, 5104, 5105, 5115M, 5115R, 5125M, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5220, 5225, 5300, 5300N, 5303, 5310, 5310N, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5500, 5500N, 5503, 5510, 5510N, 5520, 5520N, 5525, 5525N, 5603, 5605, 5610, 5615, 5625, 5705, 5715, 5725, 6068AFM75, 6068AFM85, 6068DF150, 6068HF120, 6068HF150, 6068HF250, 6068HF275, 6068HF475, 6068HFG05, 6068HFG06, 6068HT087, 6068SFM50, 6068SFM75, 6068SFM85, 6068TF150, 6068TF220, 6068TF250, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6080A E-CUT, 6090HF475, 6090HF485, 6090HFG06, 6090HFL75, 6090HFL85, 6095B, 6105AF001, 6105HF001, 6110B, 6120B, 6125AF001, 6125AFM01, 6125AFM75, 6125HF001, 6125HF070, 6125SFM75, 6135AFM75, 6135AFM85, 6135B, 6135HF475, 6135HF485, 6135HFC48, 6135HFG75, 6135HFG84, 6135HFM85, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6180CI510, 6500A E-CUT, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7200, 7200A, 7210R, 7230R, 7250, 7250R, 7260, 7270R, 7290R, 7300, 7310R, 7350, 7380, 7400, 7400A, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 8000A E-CUT, 8100, 8130, 8200, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8430, 8500, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, A2, BH7, BH8, BH9, BH11, BP15, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C300, C350, C400, C440R, C441R, C450, C451R, C461R, C650, C670, C850, CH570, CH950, CH960, CP690, CP770, CS690, CS770, CT322, CT332, CTS, CTS II, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, F440M, F440R, F441M, F4365, FL100, G110, GROUPER, H260, H310, H340, H360, H380, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, M-GATOR A1, M4025, R230, R400, R4040i, RSX 850I, RSX860E, RSX860I, RSX860M, S250, S300, S350, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, V451R, V461R, W48M, W48R, W52R, W61R, W330, W540, W550, W650, W660, X9 1000, X9 1100, X530, X540, X580, X590, X710, X730, X734, X738, X739, X750, X754, X758, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855M S4, XUV865E, XUV865M, XUV865R, Z510A, Z515E, Z520A, Z530M, Z530R, Z545R, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
@@ -2485,6 +3010,11 @@
           <t>03M7248</t>
         </is>
       </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>3-Bag, 7H17, 240, 260, 270, 493, 494, 531, 533, 540A, 540M, 543M, 551, 562, 563, 583, 594, 603M, 603R, 620R, 623M, 623R, 631, 633, 635FD, 636M, 640, 640FD, 640R, 643M, 643R, 647A, 648M, 651, 652M, 653, 657A, 660R, 661, 663, 663R, 667A, 673, 680R, 683, 683R, 692, 693, 694, 717, 731, 740, 740A, 741, 751, 753, 892, 893, 894, 946, 956, 1092, 1290, 1291, 1293, 1350, 1355, 1360, 1365, 1460, 1465, 1470, 2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 6020, 6105M, 6110M, 6115M, 6120, 6120M, 6125M, 6130, 6130M, 6135M, 6140M, 6145M, 6150M, 6155M, 6170M, 6175M, 6195M, 6220, 6230, 6320, 6330, 6420, 6420S, 6430, 6520, 6530, 6534, 6620, 6630, 6820, 6830, 6920, 6920S, 6930, 7130, 7220, 7230, 7320, 7330, 7420, 7520, 9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9970, C670, CH950, CH960, CP770, CS770, CTS, CTS II, DB37, DB41, DB44, DB50, DB55, DB60, DB62, DB74, DB80, DB83, DB90, GROUPER, H240, H260, H310, H340, H360, H380, M4030, M4040, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660, Z915B, Z915E, Z920M, Z920R, Z925M, Z930M, Z930R, Z945M, Z950M, Z950R, Z955M, Z960M, Z960R, Z970R</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
@@ -2492,6 +3022,11 @@
           <t>19M7819</t>
         </is>
       </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>3-Bag, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 30R, 31C, 46R, 48 IN., 50 in., 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 108, 160, 250D, 250D-II, 300D, 300D-II, 300DW, 300WW, 335C, 335D, 337E, 435C, 437C, 437D, 437E, 440E, 444H, 449, 450, 456, 457, 458, 466, 467, 468, 540M, 543R, 544H, 550, 553, 556, 557, 558, 563, 565, 566, 567, 568, 575, 578, 603R, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 615C, 615F, 615P, 616C, 616C PERFORMANCE UPGRADES, 617C, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620F, 620I, 620R, 622F, 622R, 623, 623R, 624H, 625F, 625I, 625R, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 643J, 643K, 644, 644H, 644HMH, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648L, 655, 660, 665, 670, 673, 678, 680, 681, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 740FD, 744, 744 P, 744H, 744J, 744L, 745FD, 748, 748L, 750A, 824 P, 824J, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 835 SHORT CHASSIS, 843J, 843K, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848L, 853J, 854, 855 LONG CHASSIS, 855 SHORT CHASSIS, 864, 903J, 904 P, 909J, 944 X, 944K, 946, 948L, 953J, 956, 959J, 960, 990, 995, 1023E, 1035, 1107, 1109, 1111, 1113, 1175, 1442, 1512FX, 1516FX, 1524FX, 1642HS, 1700, 1705, 1705T, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1730, 1735, 1742HS, 1745, 1750, 1755, 1760, 1765, 1770, 1775, 1775NT, 1780, 1785, 1790, 1795, 1900, 1910, 2020, 2020A, 2030, 2030A, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2254, 2256, 2258, 2264, 2266, 2266E, 2510H, 3025E, 3032E, 3033R, 3038E, 3038R, 3039R, 3045R, 3046R, 3200, 3215, 3220, 3316, 3325, 3365, 3400, 3420, 3800, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4045TF220, 4045TF250, 4200, 4210, 4300, 4310, 4400, 4410, 4700, 4710, 4720, 4730, 4830, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5076E, 5082E, 5083E, 5090E, 5090EH, 5090M, 5093E, 5095MH, 5100M, 5100MH, 5101E, 5105MH, 5115RH, 5425, 5625, 5725, 6110M, 6120M, 6125M, 6130M, 6135M, 6140M, 6145M, 6155M, 6175M, 6195M, 6610, 6650, 6700, 6710, 6750, 6810, 6850, 6910, 6950, 7180, 7200, 7210R, 7230R, 7250, 7250R, 7270R, 7280, 7290R, 7300, 7310R, 7350, 7380, 7400, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7630, 7660, 7700, 7730, 7750, 7760, 7780, 7800, 7830, 7850, 7930, 7950, 7980, 8100, 8200, 8300, 8320RT, 8345RT, 8370RT, 8400, 8500, 8600, 8700, 8800, 9009A, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, A2, BP15, C1 200, C2 300, C2 400, C8F, C100, C110, C120, C230, C240, C440, C440R, C441R, C451R, C461R, C650, C670, CP20, CP690, CP770, CS690, CS770, CTS, CTS II, DB37, DB41, DB44, DB55, DB58, DB60, DB60T, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, F440M, F440R, F441M, F441R, F510, F525, F620, F680, F687, F735, FR50, FS50, H541, H550, H561, HD35F, HD40F, HD45F, HD50F, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L17.542, L110, L330, L331, L340, L341, L1742, L2048, L2548, M-GATOR A1, M-GATOR A3, M-GATOR A3T, MaxEmerge XP, N530C, N536C, N540C, N542C, P576, PLANTER PERFORMANCE UPGRADES, R2 300, R230, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451R, V461R, W440, W540, W550, W650, W660, X9 1000, X9 1100, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Z515E, Z530M, Z530R, Z545R, Z720E, Z730M, Z735E, Z735M, Z740R, Z760R, Z920M, Z930M, Z930R, Z950M, Z950R, Z960M, Z960R, Z970R, Z994R</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
@@ -2499,6 +3034,11 @@
           <t>H154928</t>
         </is>
       </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>630FD, 630FD PERFORMANCE UPGRADES, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 748H, 848H, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9450, 9470 STS, 9500, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, C670, CTS, CTS II, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1100, Z994R</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
@@ -2506,6 +3046,11 @@
           <t>19M7788</t>
         </is>
       </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>3-Bag, 04, 4X2, 4X2 TRAIL, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1204, 6E-1204P, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 26, 30 Trailer, 40, 42 IN., 44, 47 IN., 48 IN., 50 in., 54, 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 62 IN. DECKS, 70, 72 IN., 80, 80C, 110 TLB, 120D, 130G, 160D, 160G, 180, 180G, 200C, 200D, 200G, 204C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 225D, 230C, 240, 240D, 244J, 245, 246, 250, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270C, 270D, 280, 285, 290G, 300D, 300D-II, 300E, 304J, 305, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 313, 315, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 317, 318D, 318E, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 324J, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 344H, 344J, 345, 350 P, 350D, 350D-II, 350DW, 350G, 355, 359, 360DC, 370E, 370E-II, 375, 380 P, 380G, 385, 400D, 400D-II, 400R, 410, 410 P, 410D, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 419, 420, 425, 430, 435, 435C, 437C, 437D, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450D, 450E, 450G, 450H, 450J, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 485E, 486E, 488E, 493, 494, 500R, 509, 510D, 520, 521, 522, 524 P, 524K, 524K-II, 524L, 530B, 535, 540, 540A, 540E, 540G-II, 540G-III, 540H, 540R, 541, 542, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 555G, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 600R, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 639, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643G, 643J, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 648E, 648G, 648H, 648HT, 648L, 648L-II, 649, 650D, 650G, 650H, 650J, 650K, 653, 653E, 653G, 654, 655K, 659, 660R, 670, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 678, 680R, 690E, 692, 693, 694, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 709, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 720, 722PF, 722X, 724 P, 724J, 724K, 724L, 725, 725D, 725PF, 725X, 730, 730D, 730PF, 730X, 735, 735D, 735PF, 735X, 740, 740A, 740D, 740G, 740PF, 740X, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 830, 835, 835 SHORT CHASSIS, 840, 842, 843, 843G, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 859M, 859MH, 862, 864, 870, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 912, 913, 914, 915F, 916, 918, 918R, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 970, 990, 994, 995, 997, 1010, 1010E, 1015, 1023E, 1025R, 1030, 1050K, 1050K PL, 1070, 1070E, 1092, 1107, 1109, 1110E, 1110G, 1111, 1113, 1165, 1170, 1170E, 1175, 1210E, 1210G, 1270E, 1270G, 1290, 1291, 1293, 1295, 1340, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1445, 1450, 1460, 1465, 1470, 1470E, 1470G, 1490D, 1510E, 1510G, 1517, 1518, 1530, 1535, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1654, 1690, 1700, 1720, 1720 CCS, 1725, 1725 CCS, 1725NT, 1725T, 1740, 1745, 1750, 1770NT, 1775NT, 1795, 1850, 1854, 1854J, 1870, 1900, 1910, 1910G, 1990, 2018, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2104, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2154D, 2154G, 2156G, 2204, 2230FH, 2230LL, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2430, 2430C, 2454D, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2654G, 2656G, 2660VT, 2704, 2720, 2730, 2854, 2904, 2954D, 3004, 3025D, 3025E, 3028EN, 3029DF120, 3029DF128, 3029DF129, 3029DF150, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF158, 3029TF270, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3204, 3210, 3215, 3220, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3520, 3720, 3754D, 3754G, 3756G, 3800, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC28, 4045HFC93, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG93, 4045HFJ85, 4045HFK80, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI551, 4045HMK80, 4045HN055, 4045HRT83, 4045HSG20, 4045HSG21, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4120, 4200, 4210, 4239TF001, 4310, 4320, 4410, 4510, 4520, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5203, 5203S, 5204, 5205, 5210, 5220, 5225, 5303, 5305, 5310, 5320, 5320N, 5325, 5325N, 5403, 5405, 5410, 5415, 5420, 5420N, 5425, 5425N, 5503, 5520, 5520N, 5525, 5525N, 5603, 5605, 5610, 5615, 5625, 5705, 5715, 5725, 6010, 6068AFM75, 6068AFM85, 6068CP550, 6068DF120R01, 6068DF150, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG20, 6068HFG25, 6068HFG82, 6068HFG85, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081HF001, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG94, 6090HFG95, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6101HF010, 6101HF011, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120B, 6120E, 6120EH, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135E, 6135HF475, 6135HF485, 6135M, 6135R, 6135SFM75, 6135SFM85, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170M, 6175M, 6175R, 6180J, 6185J, 6195M, 6195R, 6200, 6200L, 6205J, 6210, 6210J, 6210L, 6210M, 6215R, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6330, 6330 Premium, 6400, 6400L, 6403, 6410, 6410L, 6415, 6425, 6430, 6430 Premium, 6488, 6500A E-CUT, 6500L, 6506, 6510, 6510L, 6530, 6530 Premium, 6534, 6600, 6603, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6700, 6710, 6750, 6810, 6830, 6830 Premium, 6850, 6910, 6920, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7420, 7425, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7515, 7520, 7525, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8820, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, BL6, BL7, BL8, BL9, BL10, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C500, C670, CH330, CH530, CH570, CH670, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, DB40, DB44, DB50, DB60, DB66, DB74, DB80, DB84, DB90, DB96, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F441M, F441R, F510, F525, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F4365, FC10R, FC15R, FC20R, FD55, GROUPER, GS25, GS30, GS45, GS66, GS72, GS75, GS78, GS84, GS88, GT72, GT80, GT242, GT262, GT275, GU60, GU66, GU72, GU78, GX325, GX335, GX345, GX355, H541, H550, H561, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HH30, HH50, HH75, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX15, HX20, L70, L330, L331, L340, L341, LP72, LP78, LP84, LX172, LX173, LX176, LX178, LX186, LX188, M-GATOR A1, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R15, R20, R230, R400, R450, R500, R4023, R4038, R4044, R4045, R4060, RB72, RB84, RB96, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860I, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SST15, SST16, SST18, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V461M, W50, W70, W80, W100, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W440, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X495, X500, X520, X530, X534, X540, X570, X580, X584, X590, X595, X700, X740, X748, X750, X754, X758, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z510A, Z520A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
@@ -2513,6 +3058,11 @@
           <t>19M7790</t>
         </is>
       </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404P, 6E-1504L, 6E-1504PL, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 30 Trailer, 31C, 42 IN., 46, 47, 47 IN., 48, 48 IN., 54 in., 54 IN. FRONT BLADE, 54D IN., 60, 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 110, 110 TLB, 112R, 120C, 120D, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180G, 200, 200 G, 200C, 200D, 200G, 204C, 205C, 210, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 230C, 240, 240D, 250, 250G, 260, 260 P, 260E, 270, 270A, 270B, 270C, 270D, 280, 290G, 300E, 300G, 305, 310 P, 310E, 310L EP, 312GR, 314G, 315, 316GR, 317, 317G, 318D, 318E, 318G, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 337E, 344J, 344K, 344L, 350 P, 350D, 350G, 360DC, 365, 370B, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 410 P, 410E, 410E-II, 435, 435C, 437C, 437E, 440E, 444 G, 444 P, 444H, 444J, 444K, 444L, 446, 447, 448, 449, 450, 450E, 450H, 450K, 450M, 456, 457, 458, 459, 459E, 460, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 482C, 485, 485A, 490, 493, 494, 500R, 520M, 524 P, 524K, 524K-II, 524L, 525, 530, 535, 540A, 540E, 540G-II, 540G-III, 540H, 540M, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550H, 550K, 550M, 553, 556, 557, 558, 559, 560M, 560R, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 615C, 616C, 616C PERFORMANCE UPGRADES, 617C, 618C, 618C PERFORMANCE UPGRADES, 620, 620G, 620I, 622G, 623, 623R, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625D, 625I, 630, 630D, 630FD, 630FD PERFORMANCE UPGRADES, 635, 635D, 635FD, 635FD PERFORMANCE UPGRADES, 636M, 639, 640, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643G, 643J, 643K, 643L, 643L-II, 643R, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648E, 648G, 648H, 648HT, 648L, 648L-II, 648M, 648R, 649, 650H, 650K, 652E, 652M, 652R, 653E, 653G, 655, 655K, 659, 660, 661R, 665, 670, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 676, 680, 681, 690E, 692, 693, 694, 700H, 700K, 700L, 700L PL, 700M, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 730, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 735, 735FD, 735FD PERFORMANCE UPGRADES, 740A, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755K, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772B, 772BH, 772CH, 772CH II, 772D, 772G, 778, 803M, 803MH, 810D, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 842, 843G, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850K, 850L, 850L PL, 852, 853G, 853J, 853JH, 853M, 853MH, 854, 855 LONG CHASSIS, 855 SHORT CHASSIS, 859M, 859MH, 862, 864, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 911, 913, 915F, 916, 918, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 926, 930F, 930R, 936, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 994, 995, 1010, 1023E, 1025, 1025R, 1026R, 1035, 1050K, 1050K PL, 1054, 1092, 1107, 1109, 1111, 1113, 1175, 1185, 1270E, 1270G, 1290, 1291, 1293, 1295, 1354, 1404, 1415D, 1420, 1420D, 1425D, 1430D, 1435, 1435D, 1440D, 1445, 1445D, 1450, 1470, 1470E, 1470G, 1510C, 1510DC, 1512C, 1512FX, 1516FX, 1524FX, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES III, 1640, 1690, 1700, 1700T, 1705, 1705T, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810, 1810C, 1810DC, 1812C, 1812DC, 1814C, 1814DC, 1820, 1830, 1835, 1840, 1850, 1860, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 1950, 1950N, 1990, 2010DE, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2036R, 2038R, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2112C, 2112DC, 2140, 2144G, 2154D, 2154G, 2155, 2156G, 2200, 2204, 2210, 2210LL, 2230FH, 2230LL, 2250, 2254, 2256, 2258, 2264, 2266, 2266E, 2310, 2330, 2350, 2355, 2355N, 2410, 2412DE, 2430, 2430C, 2450, 2454D, 2510C, 2510H, 2510S, 2550, 2555, 2630, 2633, 2633VT, 2635, 2650, 2653B, 2654G, 2656G, 2660VT, 2704, 2730, 2750, 2755, 2850, 2854, 2904, 2950, 2954D, 2955, 3004, 3025D, 3025E, 3029DF128, 3029TF158, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3040, 3043D, 3045B, 3045R, 3046R, 3050, 3050B, 3055, 3110, 3140, 3150, 3154G, 3155, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3255, 3310, 3316, 3320, 3350, 3400, 3410, 3420, 3520, 3640, 3650, 3754D, 3754G, 3756G, 3800, 4010, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CB551, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF271, 4045DFM50, 4045DFM70, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS80, 4045HFS85, 4045HFU72, 4045HFU79, 4045HFU81, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045SFM85, 4045T, 4045TF120, 4045TF150, 4045TF151, 4045TF155, 4045TF158, 4045TF220, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4110, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4990, 4995, 5005, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5500, 5500N, 5503, 5510, 5510N, 5520, 5520N, 5525, 5525N, 5600, 5603, 5605, 5610, 5615, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CI550, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF150, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG20, 6068HFG25, 6068HFG82, 6068HFG85, 6068HFL84, 6068HFN50, 6068HFS01, 6068HFS89, 6068HFU72, 6068HFU74, 6068HFU79, 6068HI550, 6068HT087, 6068SFM75, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF158, 6068TF220, 6068TF250, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6090AFM75, 6090AFM85, 6090CB450, 6090CI550, 6090HF475, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095B, 6100, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105AF001, 6105D, 6105E, 6105EH, 6110, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115D, 6115E, 6115J, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF070, 6125J, 6125M, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135HFM85, 6135M, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140M, 6140R, 6145J, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155J, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170R, 6175M, 6175R, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6210, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420T, 8430, 8430T, 8500, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8820, 8870, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, BH7, BH8, BH9, BH11, BL6, BL7, BL8, BL9, BL10, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C670, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT322, CT332, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB84, DB88, DB90, DB96, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F710, F725, F735, F915, F925, F935, F1145, FL100, FS22B, G15, GROUPER, GS25, GS30, GS45, GS66, GS72, GS75, GS78, GS84, GS88, GT72, GT80, GU60, GU66, GU72, GU78, H240, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HH30, HH50, HH75, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L70, L330, L331, L340, L341, LP72, LP78, LP84, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M4030, M4040, M4040DN, MaxEmerge XP, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R400, R450, R500, RB72, RB84, RB96, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, X485, X530, X540, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV855E, XUV855M, XUV855M S4, Y110, Y115, Y210, Y215, Z510A, Z520A, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915E, Z920A, Z920M, Z925A, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
@@ -2527,6 +3077,11 @@
           <t>19M7817</t>
         </is>
       </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>3-Bag, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 47 IN., 54D IN., 60 IN. DECKS, 60D IN., 62 IN., 62 IN. DECKS, 110 TLB, 200, 210R, 220R, 243, 244, 250D-II, 260, 270, 300D-II, 335, 337E, 343, 344, 344E, 344G, 370E, 370E-II, 375, 385, 410 P, 410E, 410E-II, 437E, 440E, 443, 444, 444G, 444H, 444J, 446, 447, 448, 449, 450E, 450H, 450J, 450M, 454, 456, 457, 458, 459, 459E, 460 P, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 493, 494, 500R, 525, 530, 535, 543, 544H, 544J, 546, 547, 550H, 550J, 550M, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 594, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 615C, 615F, 615P, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620I, 620R, 622, 622F, 622G, 622R, 623, 624H, 624J, 625D, 625F, 625R, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640L, 640L-II, 640X, 643, 643H, 643J, 643L, 643L-II, 644, 644G, 644H, 644HMH, 644J, 644K, 645, 645FD, 645FD PERFORMANCE UPGRADES, 648L, 648L-II, 650H, 650J, 653, 653G, 654, 655K, 670D, 670G, 672D, 672G, 678, 692, 693, 694, 700H, 700J, 700J-II, 700L, 700L PL, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 722PF, 724J, 725D, 725PF, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740PF, 740X, 744, 744 P, 744H, 744J, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748L, 748L-II, 750A, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 755K, 759G, 759GH, 764, 768L-II, 770D, 770G, 772D, 772G, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 843, 843H, 843J, 843L, 843L-II, 844, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848L, 848L-II, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853, 853JH, 855 LONG CHASSIS, 855 SHORT CHASSIS, 859M, 859MH, 870, 870D, 870G, 872D, 872G, 891, 892, 893, 894, 903JH, 903KH, 903M, 904 P, 909JH, 909KH, 909M, 909MH, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950K, 953M, 953MH, 953ML, 956, 959M, 959MH, 959ML, 960, 970, 990, 994, 995, 997, 1023E, 1025R, 1026R, 1050K, 1050K PL, 1070, 1092, 1107, 1109, 1111, 1243, 1290, 1291, 1293, 1295, 1312C, 1350, 1360, 1450, 1460, 1470, 1505, 1510C, 1550, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1700, 1705, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1730, 1735, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1795, 1812C, 1814C, 1820, 1830, 1835, 1900, 1910, 1990, 2000 SERIES, 2020A, 2025R, 2026R, 2030A, 2032R, 2036R, 2038R, 2230FH, 2243, 2264, 2266, 2266E, 2400 PRECISIONCUT, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2904, 3004, 3033R, 3038R, 3039R, 3045R, 3046R, 3120, 3204, 3320, 3520, 3720, 4044M, 4044R, 4045HF275, 4045TF275, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4120, 4210, 4310, 4320, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4895, 4920, 4990, 4995, 5036C, 5038D, 5039C, 5041C, 5042C, 5050E, 5055E, 5058E, 5060E, 5065E, 5067E, 5070E, 5075E, 5076E, 5076EL, 5076EN, 5078E, 5080E, 5082E, 5083E, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5093E, 5100M, 5103, 5103E, 5103S, 5104, 5115M, 5125M, 5203, 5203S, 5204, 5303, 5310, 5403, 5405, 5415, 5425, 5503, 5610, 5615, 5625, 5715, 5725, 6010, 6068HF250, 6068HF275, 6068TF275, 6090HF485, 6090M, 6100M, 6105R, 6110, 6110L, 6110M, 6110R, 6115R, 6120L, 6120M, 6120R, 6125M, 6125R, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135HFM85, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM85, 6136CG440, 6136CG550, 6136CI550, 6136HI440, 6136HI550, 6140M, 6145M, 6150M MONTENEGRO, 6155M, 6155MH, 6170M MONTENEGRO, 6175M, 6180CI510, 6190M, 6195M, 6205, 6210, 6210L, 6210M, 6215, 6220L, 6230 Premium, 6310, 6310L, 6330 Premium, 6400, 6403, 6405, 6410, 6410L, 6415, 6430 Premium, 6505, 6510L, 6510S, 6530 Premium, 6534 Premium, 6603, 6605, 6610, 6630 Premium, 6650, 6710, 6750, 6810, 6820, 6850, 6910, 6920, 6920S, 6950, 7130 Premium, 7180, 7200, 7200R, 7210R, 7215R, 7220, 7230 Premium, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7350, 7380, 7400, 7420, 7450, 7455, 7460, 7480, 7500, 7520, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8245R, 8270R, 8295R, 8295RT, 8300, 8300T, 8310, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8360RT, 8370R, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8600, 8700, 8800, 9009A, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9976, 9986, 9996, A2, BL6, BL7, BL8, BL9, BL10, BP15, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C300, C350, C400, C440R, C441R, C450, C451R, C461R, C500, C670, CH950, CH960, CP690, CP770, CS690, CS770, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB84, DB88, DB90, DB96, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E330, E360, E400, F440M, F440R, F441M, F441R, F620, F680, F687, F910, F911, F912, F915, F925, F930, F932, F935, GROUPER, GS66, GS72, GS78, GS84, GS88, GT72, GT80, GU60, GU66, GU72, GU78, H540F, H541, H550, H550F, H560F, H561, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HD300, HH30, HH50, HH75, HPX615E, HPX815E, L331, L341, LP72, LP78, LP84, M-GATOR A1, M-GATOR A3, M-GATOR A3T, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, N530C, N536C, N540C, N542C, PLANTER PERFORMANCE UPGRADES, R40, R230, R500, RB72, RB84, RB96, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S300, S350, S430, S440, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH12F, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, V451R, V461R, W36M, W36R, W200M, W235, W235M, W235R, W260, W260R, W540, W550, W650, W660, X9 1000, X9 1100, X500, X520, X530, X540, X570, X580, X590, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Z510A, Z520A, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
@@ -2534,6 +3089,11 @@
           <t>19M7828</t>
         </is>
       </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 46, 47, 48, 240, 245, 250, 260, 265, 270, 280, 312GR, 313, 314G, 315, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 349, 359, 370B, 375, 375A, 385A, 447, 448, 459, 485, 485A, 521, 540A, 541, 563, 570, 572, 580, 582, 590, 592, 620, 620I, 622X, 624H, 630X, 631, 635X, 640, 640X, 651, 661, 673, 720, 721, 725, 726, 730, 731, 735, 735X, 740, 740A, 740X, 741, 751, 803M, 803MH, 842, 852, 853M, 853MH, 859M, 859MH, 862, 960, 990, 1690, 1840, 1990, 2032R, 2038R, 2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 2330, 2510C, 2510S, 3025E, 3032E, 3033R, 3038E, 3038R, 3039R, 3045R, 3046R, 3320, 3365, 3520, 3720, 4044R, 4049M, 4049R, 4052R, 4066R, 4075R, 4200, 4300, 4320, 4400, 4500, 4520, 4600, 4700, 4710, 4720, 4730, 4830, 5080R, 5090R, 5100R, 6090CG550, 6090CI550, 6090CP550, 6090HFG06, 6610, 6650, 6710, 6750, 6810, 6820, 6850, 6910, 6920, 6920S, 6950, 7455, 7660, 7700, 7760, 7780, 7800, 7850, 7950, 7980, 8225R, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8310R, 8320R, 8320RT, 8335R, 8345R, 8345RT, 8360R, 8370R, 8370RT, 8400R, 9370R, 9400, 9410, 9420R, 9420RX, 9450, 9470 STS, 9470R, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9520R, 9520RX, 9520RX SCRAPER, 9550, 9560, 9560 STS, 9570 STS, 9570R, 9570RX, 9570RX SCRAPER, 9600, 9610, 9620R, 9620RX, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, 9986, 9996, A2, A400, C451R, C461R, C650, C850, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, H360, H380, L331, L341, M-GATOR A3, R450, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, SH8R, SH12F, SH12R, STRAIGHT BLADE, T550, T560, T660, T670, TC62H, V451R, V461R, W200M, W235, W235M, W235R, W260, W260R, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
@@ -2541,6 +3101,11 @@
           <t>19M8020</t>
         </is>
       </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20, 27 ZTS, 27C ZTS, 35C, 35ZTS, 80, 160 P, 160D, 160G, 180G, 200 G, 200D, 200G, 204K, 204L, 210C, 210G, 210K, 210K EP, 210LJ, 225D, 240D, 245G, 250D, 250D-II, 250G, 260 P, 260E, 300D, 300D-II, 300DW, 300WW, 304H, 304K, 304L, 310 P, 310D, 310E, 315D, 324H, 330B, 335C, 344H, 344J, 350D, 350D-II, 350DW, 370E, 400D, 400D-II, 410E, 435, 435C, 437C, 444E, 450D, 450G, 450H, 450J, 450K, 455G, 460E, 466, 470G, 482C, 535, 540A, 540M, 550G, 550H, 550J, 550K, 555G, 563, 566, 605C, 605K, 620G, 622G, 624H, 640, 643H, 644 X, 644K HYBRID, 644LH, 650, 650G, 650H, 650J, 650K, 655C, 670C, 670CH, 670D, 670G, 672CH, 672D, 672G, 673, 735, 740, 740A, 741, 750, 750A, 755C, 755D, 764, 770G, 772G, 810D, 810E, 843H, 844K, 848G, 870G, 872G, 904, 913, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 944K, 946, 950C, 950J, 956, 970, 1010, 1025, 1035, 1050C, 1050J, 1050K PL, 1054, 1100/1150, 1354, 1404, 1418, 1512FX, 1516FX, 1524FX, 1530, 1535, 1590, 1700, 1700T, 1705, 1705T, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810, 1870, 1890, 1895, 1990, 2032R, 2036R, 2038R, 2230FH, 2230LL, 2330, 2510H, 2660VT, 3100, 3110, 3200, 3210, 3300, 3310, 3400, 3410, 4055, 4250, 4255, 4450, 4455, 4890, 4895, 4990, 4995, 5036C, 5039C, 5041C, 5042C, 5060E, 5070E, 5070M, 5075M, 5078E, 5080E, 5080M, 5080R, 5085M, 5090E, 5090M, 5090R, 5100M, 5100R, 5115M, 5115R, 5125R, 5620, 5720, 5820, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120M, 6120R, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130M, 6130R, 6135B, 6135E, 6135M, 6135R, 6140B, 6140D, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6155M, 6155MH, 6155R, 6170M, 6170R, 6175M, 6175R, 6190R, 6195M, 6195R, 6200, 6210, 6210M, 6210R, 6215R, 6220, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6310, 6320, 6325, 6330, 6330 Premium, 6400, 6403, 6410, 6420, 6420S, 6425, 6430, 6430 Premium, 6506, 6510, 6510S, 6520, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6610, 6620, 6630, 6630 Premium, 6800, 6810, 6820, 6830, 6830 Premium, 6900, 6910, 6910S, 6920, 6920S, 6930, 7200, 7210, 7220, 7320, 7400, 7410, 7420, 7430E, 7455, 7510, 7520, 7530E, 7600, 7610, 7630, 7700, 7710, 7720, 7730, 7800, 7810, 7820, 7830, 7920, 7930, 8100, 8110, 8120, 8130, 8200, 8210, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310, 8310R, 8310RT, 8320, 8320R, 8320RT, 8330, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8400, 8410, 8420, 8430, 8520, 8530, 9360R, 9370R, 9410R, 9420R, 9420RX, 9430, 9460R, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9560R, 9560RT, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9620R, 9620RX, 9630, 9630 SCRAPER, C850, DB37, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E300LC, E330, E360, E400, F310R, F350R, GPD2224, H360, H380, MaxEmerge XP, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R310R, R870R, R950R, R990R, S430, S440, TC62H, X9 1000, X9 1100</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
@@ -2548,6 +3113,16 @@
           <t>19M8610</t>
         </is>
       </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>6B-954, 6E-1004, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 46, 47, 48, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 80, 110, 120D, 160, 313, 315, 317, 318D, 318E, 319D, 319E, 320, 320D, 320E, 323D, 323E, 325, 326D, 326E, 328, 328D, 328E, 329D, 329E, 332, 332D, 332E, 333D, 333E, 370B, 375, 375A, 385A, 447, 448, 457, 467, 485, 485A, 525, 530, 535, 547, 557, 567, 583, 606SH, 608SH, 615F, 616, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 625D, 625F, 625R, 630, 630D, 630F, 630FD, 630R, 631, 633, 635, 635D, 635F, 635FD, 635PF, 635R, 640D, 640FD, 645FD, 651, 653, 655K, 661, 663, 683, 710 P, 710L, 725D, 730D, 730FD, 731, 735D, 735FD, 740D, 740FD, 745FD, 748, 750J, 750J-II, 750K, 750L, 751, 753, 755K, 850J, 850J-II, 850K, 850L, 1050K, 1050K PL, 1175, 1350, 1355, 1360, 1365, 1460, 1465, 1470, 1570, 1780, 2025R, 2027R, 2032R, 2305, 2320, 3025E, 3032E, 3036E, 3038E, 3510, 3520, 3522, 4200, 4210, 4300, 4310, 4400, 4410, 4700, 4710, 5083E, 5093E, 5101E, 5425, 5625, 5725, 6135M, 6135R, 6140M, 6145M, 6650, 6750, 6850, 6950, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7750, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9420RX, 9430T, 9460RT, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530T, 9540, 9560, 9560 STS, 9560RT, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9620RX, 9630T, 9640, 9660, 9660 STS, 9670, 9680, 9700, 9760 STS, 9800, 9860 STS, 9900, 9970, A400, C2 400, C440, CH330, CH530, CT315, CT322, CT332, DB40, DB41, DB50, DB62, DB74, DB83, DB90, GROUPER, H340, H360, H380, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, L330, L331, L340, L341, R450, S430, S440, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W200M, W235M, W235R, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, X940, X948, X949, ZPF635</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
@@ -2555,6 +3130,11 @@
           <t>19M7846</t>
         </is>
       </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 240, 250, 260, 270, 280, 318D, 318E, 319D, 319E, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325G, 326D, 326E, 328D, 328E, 329D, 329E, 330G, 331G, 332D, 332E, 332G, 333D, 333E, 333G, 450M, 460M, 460R, 512, 540A, 560M, 560R, 562, 563, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 615C, 616C, 616C PERFORMANCE UPGRADES, 617C, 618C, 618C PERFORMANCE UPGRADES, 620, 630FD, 635FD, 640, 640FD, 643R, 644 X, 644K HYBRID, 644LH, 663R, 673, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 740A, 750A, 1175, 1470, 1570, 1690, 1770NT, 1775NT, 1990, 2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 3033R, 3036E, 3038R, 3045R, 3200, 3215, 3220, 3320, 3400, 3420, 3520, 3720, 4200, 4300, 4310, 4400, 4410, 4720, 4730, 4830, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7480, 7500, 7550, 7580, 7700, 7750, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9470 STS, 9500, 9560 STS, 9570 STS, 9600, 9650 STS, 9660 STS, 9670 STS, 9700, 9750 STS, 9760 STS, 9770 STS, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, C8F, C8R, C12F, C12R, C16F, C18F, C650, C850, CP770, CS770, H480, L330, L331, L340, L341, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W330, WL53, WL56</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
@@ -2562,6 +3142,11 @@
           <t>H235880</t>
         </is>
       </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
@@ -2569,6 +3154,11 @@
           <t>H227582</t>
         </is>
       </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>540R, 6100D, 6110D, 6115D, 6125D, 6130D, 6140D, 6403, 6603, 7400A, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 8800A, 9009A, 9470 STS, 9500, 9570 STS, 9600, 9670 STS, 9700, 9770 STS, 9800, 9870 STS, 9900, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1100</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
@@ -2576,6 +3166,16 @@
           <t>19M10018</t>
         </is>
       </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>40I, 50I, 4730, 5430I, 9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, M4025, M4030, M4040, R4030, R4038, R4044, R4045, R4060, S7 600, S7 700, S7 800, S7 850, S7 900, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
@@ -2583,6 +3183,11 @@
           <t>19M7882</t>
         </is>
       </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 210C, 210K, 210K EP, 210L, 210L EP, 210LJ, 300D, 310D, 315D, 335, 375, 410 P, 410D, 410L, 450G, 455G, 510D, 545, 550, 550G, 555G, 570, 580, 590, 595D, 650G, 710D, 1354, 1404, 1690, 1990, 2230FH, 2230LL, 2254, 2256, 2258, 2300, 2400, 3200, 3215, 3220, 3400, 3420, 3710, 3800, 4730, 5055E, 5060E, 5060EN, 5065E, 5070E, 5075E, 5075EF, 5078E, 5080E, 5080EN, 5085E, 5090E, 6100J, 6110J, 6115J, 6125E MONTENEGRO, 6125J, 6145J, 6615, 7185J, 7195J, 7205J, 7210J, 7225J, 8245R, 8250R, 9670 STS, 9770 STS, H540F, H541, H550, H550F, H560F, H561, L330, L331, L331R, L340, L341, L341R, L341R HIGH-DENSITY, M4030, M4040, SH8R, SH12F, SH12R</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
@@ -2590,6 +3195,11 @@
           <t>19M8486</t>
         </is>
       </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>6E-1504L, 6E-1504PL, 210L, 210L EP, 250D, 250D-II, 260 P, 260E, 300C, 300D, 300D-II, 300DW, 300WW, 310D, 310E, 315D, 410D, 415, 425, 445, 447, 448, 455, 457, 458, 467, 468, 510D, 547, 557, 558, 567, 568, 595D, 624H, 624J, 630FD, 630FD PERFORMANCE UPGRADES, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 644H, 644HMH, 644J, 645FD, 645FD PERFORMANCE UPGRADES, 710D, 710G, 710J, 710K, 710L, 724J, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 735FD PERFORMANCE UPGRADES, 740FD, 740FD PERFORMANCE UPGRADES, 745FD, 745FD PERFORMANCE UPGRADES, 750C, 824J, 824K, 850C, 950K, 1050K, 1107, 1109, 1111, 1113, 1690, 1820, 1870, 1890, 1895, 1910, 1990, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2230FH, 2230LL, 2254, 2256, 2258, 2264, 2266, 2266E, 2510H, 2620, 2623, 2625, 2630, 2633, 2635, 2730, 5045E, 5055E, 5065E, 5075E, 5075M, 5085E, 5090E, 5090M, 5090R, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 7200R, 7210, 7215R, 7230R, 7260R, 7280R, 7410, 7510, 7610, 7710, 7810, 8120, 8130, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8310R, 8320, 8320R, 8330, 8335R, 8345R, 8360R, 8420, 8430, 8520, 8530, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9120, 9220, 9230, 9320, 9330, 9400, 9410, 9420, 9430, 9450, 9470 STS, 9500, 9501, 9510, 9520, 9530, 9530 SCRAPER, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9620, 9630, 9630 SCRAPER, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, B25C, B30C, C670, CTS, CTS II, DB40, DB50, DB66, DB74, DB80, DB88, DB90, N540F, N543F, N550, N560, N560F, P576, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, TC62H, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
@@ -2597,6 +3207,11 @@
           <t>19M9024</t>
         </is>
       </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>240, 250, 325, 326D, 326E, 328, 328D, 328E, 329D, 329E, 332, 332D, 332E, 333D, 333E, 710G, 710J, 710K, 710L, 1690, 1890, 1990, 5055E, 5060E, 5060EN, 5065E, 5070E, 5075E, 5075EF, 5078E, 5080E, 5080EN, 5085E, 5090E, 6110J, 6125E MONTENEGRO, 6125J, 6130J, 6135J, 6135M MONTENEGRO, 6145J, 6150J, 6150M MONTENEGRO, 6165J, 6170J, 6170M MONTENEGRO, 6180J, 6190J, 6190M, 6205J, 6210J, 6210M, 7195J, 7200J, 7210J, 7215J, 7225J, 7230J, 7515, 8270R, 8295R, 8320R, 8345R, 8370R, 8400R, CT332, N530C, N530F, N536C, N540C, N540F, N542C, N543F, N550, N560, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
@@ -2604,6 +3219,11 @@
           <t>19M7843</t>
         </is>
       </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 52 IN., 60 in., 160 P, 160G, 180G, 200 G, 200G, 210C, 240, 250, 260, 270, 280, 300C, 317, 318, 318E, 319E, 320, 320E, 320G, 323E, 324G, 325, 325G, 326E, 328, 328E, 329E, 332, 332E, 333E, 350 P, 365, 380 P, 403, 413, 420, 430, 450M, 460DC, 460M, 460R, 503, 513, 530, 540E, 540M, 544 G, 544G, 548E, 560M, 560R, 568, 572, 578, 582, 592, 603, 613, 614R, 615F, 615R, 616R, 618F, 618PF, 618R, 620F, 620PF, 620R, 622F, 622PF, 622R, 622X, 624G, 625D, 625F, 625PF, 625R, 625X, 630, 630D, 630F, 630PF, 630R, 630X, 635, 635D, 635F, 635PF, 635R, 635X, 640D, 640E, 640G, 640H, 640X, 643K, 644 G, 644 P, 644 X, 644G, 644K, 644K HYBRID, 644L, 644LH, 648E, 648G, 648H, 655, 678, 700M, 703JH, 710 P, 710L, 722PF, 722X, 724 P, 724K, 724L, 725D, 725PF, 725X, 730D, 730PF, 730X, 735D, 735PF, 735X, 740D, 740PF, 740X, 744, 744K, 748, 748E, 748G-III, 748H, 750K, 750L, 753J, 753JH, 755, 756, 759J, 759JH, 824K, 830, 835, 843K, 844J, 844K, 848H, 850J, 850K, 850L, 853J, 855, 856, 903J, 912, 913, 914, 915F, 918, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930F, 930R, 946, 950K, 955, 956, 960, 990, 1023E, 1026R, 1050K, 1050K PL, 1355, 1365, 1465, 1470, 1570, 1612DE, 1640, 1720, 1725, 1735, 1785, 2010DE, 2014DE, 2032R, 2036R, 2038R, 2040, 2040S, 2140, 2350, 2355, 2412DE, 2510H, 2550, 2555, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2704, 2750, 2854, 2904, 2950, 3004, 3040, 3140, 3150, 3204, 3316, 3325, 3365, 3640, 3800, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4120, 4200, 4210, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4700, 4710, 4720, 4920, 4930, 4940, 5036C, 5038D, 5041C, 5042C, 5050E, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5070M, 5075E, 5075EN, 5075M, 5076EN, 5080M, 5083EN, 5085M, 5090E, 5090EN, 5090M, 5090R, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101EN, 5103, 5103E, 5103S, 5104, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5203, 5203S, 5204, 5220, 5310, 5320, 5325N, 5405, 5415, 5420, 5425, 5425N, 5520, 5525N, 5610, 6081HF070, 6090 MC, 6090 RC, 6090CG550, 6090CI550, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG09, 6090HFG94, 6090HFG95, 6090M, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105HF001, 6105M, 6105R, 6110 MC, 6110 RC, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115M, 6115R, 6120M, 6120R, 6125AF001, 6125HF001, 6125HF070, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG95, 6135M, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140D, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170R, 6175M, 6175R, 6190R, 6195M, 6195R, 6210M, 6210R, 6215R, 6230, 6230 Premium, 6230R, 6250R, 6330, 6330 Premium, 6430, 6430 Premium, 6530, 6530 Premium, 6534, 6534 Premium, 6630, 6630 Premium, 6700, 6830, 6830 Premium, 6930, 7130, 7130 Premium, 7200, 7200R, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7420, 7430E, 7450, 7455, 7460, 7480, 7500, 7520, 7530E, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8225R, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8500, 8600, 8700, 8800, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9976, 9986, 9996, A400, B30C, BL6, BL7, BL8, BL9, BL10, C1 200, C2 300, C2 400, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C451R, C461R, C670, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CTS, CTS II, DB84, DB96, F710, F725, F735, F4365, FS20, FS22B, GROUPER, GS66, GS72, GS78, GS84, GS88, GT72, GT80, GU60, GU66, GU72, GU78, H240, H260, H310, H340, H360, H380, H480, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HH30, HH50, HH75, L331, L341, LP72, LP78, LP84, LX4, LX5, LX6, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, PLANTER PERFORMANCE UPGRADES, R450, R4030, R4038, R4044, R4045, R4060, RB72, RB84, RB96, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SPRAYER PERFORMANCE UPGRADES, T550, T560, T660, T670, V451R, V461R, W260, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X950R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
@@ -2611,6 +3231,11 @@
           <t>19M8035</t>
         </is>
       </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>8RT 310, 8RT 340, 8RT 370, 8RT 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 31C, 50D, 75C, 75D, 75G, 80, 80C, 85D, 85G, 110, 110 TLB, 120C, 120D, 130G, 135C, 135D, 135G, 160, 160 P, 160C, 160D, 160G, 180C W, 180G, 190DW, 190E, 190GW, 200, 200 G, 200C, 200D, 200G, 210C W, 210G, 210K, 210K EP, 210L, 210L EP, 220DW, 225C, 225D, 230C, 230GW, 240D, 244J, 244L, 250D, 250D-II, 250G, 270, 270C, 290D, 300D, 300D-II, 300DW, 300G, 300WW, 304J, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 317G, 324H, 324J, 324L, 325J, 325SK, 325SL, 330C, 337E, 344E, 344G, 344H, 344J, 344K, 350D, 350D-II, 350DW, 350G, 360DC, 370, 370C, 370E, 370E-II, 380G, 400D, 400D-II, 410 P, 410D, 410E, 410E-II, 410G, 410J, 410K, 410L, 410TK TMC, 437E, 444 P, 444E, 444G, 444H, 444J, 444K, 444L, 450, 450C, 450G, 450H, 450J, 450K, 455G, 460 P, 460DC, 460E, 460E-II, 470 P, 470G, 490E, 510D, 540G-II, 540G-III, 544H, 548G-II, 548G-III, 550, 550G, 550H, 550J, 550K, 555G, 590D, 595D, 605K, 608BH, 608L, 608LH, 608SH, 620G, 622G, 624H, 624K, 624K-II, 640G, 640H, 640L, 640L-II, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 647, 648G, 648H, 648HT, 648L, 648L-II, 650D, 650G, 650H, 650J, 650K, 655, 655C, 655K, 660, 665, 670, 670 P, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 673, 680, 681, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 710D, 710G, 710J, 710K, 710L, 724 P, 724J, 724K, 724L, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750, 750C, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755C, 755K, 759G, 759GH, 759J, 759JH, 768L-II, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 790E, 792D, 800C, 803M, 803MH, 824 P, 824J, 824K, 824L, 843K, 843L, 843L-II, 844 P, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870 P, 870D, 870G, 872D, 872G, 892E, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 944K, 948L, 948L-II, 950C, 950J, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 959J, 959K, 959M, 959MH, 959ML, 1050C, 1050J, 1050K, 1050K PL, 1109, 1111, 1113, 1165, 1175, 1470, 1720, 1725, 1725 CCS, 1725C, 1725NT, 1780, 1785, 1790, 1795, 1900, 1910, 2054, 2144G, 2154D, 2154G, 2156G, 2204, 2230FH, 2230LL, 2254, 2256, 2258, 2310, 2330, 2704, 2904, 3004, 3029DF128, 3029DFU20, 3029DFU29, 3029DFU29R, 3029TF158, 3029TFU20, 3029TFU29, 3029TFU89, 3204, 3554, 3710, 3754D, 4039DF008, 4039TF008, 4045DF120, 4045DF150, 4045DF158, 4045DF271, 4045HF120, 4045HF158, 4045TF158, 4045TF250, 4045TF258, 4045TF271, 4045TFU20, 4239TF001, 4250, 4450, 4650, 4850, 4930, 5040D, 5045D, 5045E, 5050D, 5050E, 5055E, 5058E, 5060E, 5065E, 5067E, 5075E, 5076EF, 5080G, 5080R, 5083E, 5085E, 5090E, 5090EL, 5090G, 5090GH, 5090R, 5093E, 5100E, 5100R, 5101E, 5105, 5105GF, 5205, 5215, 5215F, 5215V, 5300, 5300N, 5310, 5310N, 5315, 5315F, 5315V, 5400, 5405, 5410, 5410N, 5415, 5500, 5500N, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5615, 5615V, 5620, 5720, 5820, 6020, 6068CP550, 6068DF150, 6068HF158, 6068HF258, 6068HFU55, 6068HP550, 6068TF158, 6068TF258, 6100J, 6105J, 6105M, 6105R, 6110, 6110J, 6110L, 6115J, 6115M, 6115R, 6120, 6120L, 6125J, 6125M, 6125R, 6130, 6130J, 6140JH, 6145J, 6150J, 6155JH, 6165J, 6170J, 6170M MONTENEGRO, 6180J, 6190J, 6190M, 6200, 6205, 6205J, 6210, 6210J, 6210L, 6215, 6220, 6220L, 6230, 6230 Premium, 6300, 6310, 6310L, 6320, 6320L, 6330, 6330 Premium, 6400, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6430, 6430 Premium, 6500, 6500L, 6505, 6510L, 6520, 6520L, 6530 Premium, 6534 Premium, 6600, 6605, 6615, 6620, 6630 Premium, 6715, 6820, 6830 Premium, 6920, 6920S, 6930, 7185J, 7195J, 7200, 7200J, 7205J, 7210, 7210J, 7215J, 7220, 7225J, 7230J, 7320, 7330 Premium, 7400, 7405, 7410, 7420, 7425, 7500, 7505, 7510, 7515, 7520, 7525, 7600, 7610, 7630, 7700, 7710, 7715, 7720, 7730, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 8100, 8100T, 8110, 8110T, 8200, 8200T, 8210, 8210T, 8225R, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 9100, 9200, 9230, 9300, 9300T, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RX, 9470RX SCRAPER, 9510, 9510R, 9510RT, 9520R, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RX, 9570RX SCRAPER, 9580, 9610, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, B30C, C670, CH330, CH530, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DF180G, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300LC, E330, E360, E400, PLANTER PERFORMANCE UPGRADES, S160, S180, S200, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, TC44H, TC54H, TC62H, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
@@ -2618,6 +3243,11 @@
           <t>03M7306</t>
         </is>
       </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 210, 240, 250, 260, 270A, 270B, 317, 320, 325, 328, 332, 410, 419, 420, 430, 440, 460, 525, 530, 535, 614R, 615F, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 625D, 625F, 625PF, 625R, 630, 630F, 630PF, 630R, 635, 635D, 635F, 635PF, 635R, 640, 700M, 720, 725, 735D, 740, 740A, 840, 843, 900, 911, 960, 2230FH, 2230LL, 2330, 2510H, 2660VT, 9540, 9560, 9560 STS, 9580, 9640, 9660, 9670, 9680, 9780, 9860 STS, 9880 STS, BH7, BH8, BH9, BH11, C670, DB74, H480, R400, R500, S430, S440, S690, T550, T560, T660, T670, W540, W550, W650, W660, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
@@ -2625,6 +3255,11 @@
           <t>19M7793</t>
         </is>
       </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 6J-1704, 6J-1904, 6R 140, 6R 150, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20, 31C, 46, 47, 48, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72, 72 IN., 100, 260, 270, 280, 300, 300CX, 300R, 300X, 318D, 319D, 320D, 320R, 323D, 326D, 328D, 329D, 332D, 333D, 370B, 375, 375A, 385A, 400CX, 400R, 400X, 408R, 410, 410R, 412R, 419, 420, 430, 447, 448, 450, 460, 485, 485A, 525, 530, 531, 533, 535, 540E, 540G-II, 540M, 540R, 543M, 543R, 544 G, 544J, 544K, 544K-II, 548E, 548G-II, 550, 550K, 551, 568, 570, 572, 578, 580, 582, 583, 590, 592, 600R, 603M, 603R, 608BH, 608L, 608LH, 608SH, 612R, 615F, 616, 616F, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 623R, 625, 625D, 625F, 625R, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640L, 640L-II, 643J, 643K, 643L, 643L-II, 643R, 644 G, 644G, 644J, 645FD, 645FD PERFORMANCE UPGRADES, 647, 648E, 648G, 648L, 648L-II, 650K, 651, 653, 655, 660, 661, 663, 663R, 665, 670, 673, 678, 680, 681, 683, 700K, 700M, 703G, 703GH, 703JH, 724J, 725D, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 744, 744 P, 744H, 745FD, 745FD PERFORMANCE UPGRADES, 748E, 748G-II, 748G-III, 748L, 748L-II, 750A, 750K, 753, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 764, 768L-II, 800R, 803M, 803MH, 824 P, 830, 835, 842, 843J, 843K, 843L, 843L-II, 848G, 848L, 848L-II, 850, 850K, 852, 853G, 853J, 853M, 853MH, 859M, 859MH, 862, 900, 903G, 903J, 903K, 903KH, 903M, 903MH, 909J, 909K, 909KH, 909M, 909MH, 925D, 930D, 936D, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 1023E, 1025R, 1026R, 1050K, 1350, 1355, 1360, 1365, 1450, 1460, 1465, 1470, 1550, 1570, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1654, 1700, 1700T, 1705, 1705T, 1745, 1750, 1755, 1770, 1775, 1790, 1795, 1830, 1840, 1854, 1854J, 1870, 1895, 1900, 1910, 2054, 2056, 2058, 2064, 2066, 2104, 2230FH, 2254, 2256, 2258, 2264, 2266, 2266E, 2510H, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2660VT, 2704, 2730, 2854, 2904, 3004, 3028EN, 3033R, 3036E, 3036EN, 3038R, 3039R, 3045R, 3046R, 3120, 3200, 3203, 3204, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3320, 3400, 3420, 3520, 3720, 3800, 4044M, 4044R, 4045AFM85, 4045DFM70, 4045TFM75, 4045TFM85, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4320, 4500, 4520, 4600, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 5045E, 5050E, 5055E, 5058E, 5060E, 5065E, 5067E, 5070E, 5070M, 5075E, 5075M, 5076EN, 5078E, 5080E, 5080M, 5080R, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5100E, 5100M, 5100MH, 5100R, 5101E, 5101EN, 5105, 5105M, 5115M, 5115R, 5125M, 5125R, 5205, 5220, 5225, 5320, 5320N, 5325, 5325N, 5405, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5520, 5520N, 5525, 5525N, 5603, 5615, 5620, 5625, 5715, 5720, 5725, 5820, 6010, 6020, 6068HBM01, 6068HBM04, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068TBM01, 6068TBM02, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6090 MC, 6090 RC, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6105 MC, 6105 RC, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125J, 6125M, 6125R, 6130, 6130J, 6130M, 6130R, 6135R, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145R, 6150M, 6150R, 6150RH, 6155J, 6155JH, 6155R, 6155RH, 6165J, 6170M, 6170R, 6175M, 6175R, 6180J, 6185J, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7200, 7210, 7220, 7230, 7230 Premium, 7250, 7260, 7280, 7300, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7410, 7420, 7430E, 7450, 7480, 7500, 7505, 7510, 7515, 7520, 7530E, 7550, 7580, 7660, 7700, 7720, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8130, 8200, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8430, 8500, 8530, 8600, 8700, 8800, 8820, 9009A, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, A420R, A520R, BP15, C300, C350, C400, C440R, C441R, C450, C500, C650, C670, C850, CP20, CP690, CP770, CS690, CS770, CTS, CTS II, F910, F911, F912, F915, F925, F930, F932, F935, F1145, FD22B, FD45, FD55, FR21B, FR22B, FR24B, FR50, FS20, FS22B, FS50, GROUPER, H160, H165, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, L330, L331, L340, L341, M-GATOR A1, N530, N530C, N536C, N540C, N542C, N550, N560, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, R40, R230, R400, R4040i, R4050i, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, STRAIGHT BLADE, T550, T560, T660, T670, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V461M, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X950R, Y110, Y115, Y210, Y215, Z915B, Z915E, Z920M, Z920R, Z925M, Z930M, Z930R, Z945M, Z950M, Z950R, Z955M, Z955R, Z960M, Z960R, Z970R, Z994R</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
@@ -2632,6 +3267,11 @@
           <t>19M7794</t>
         </is>
       </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 46, 47, 48, 54 in., 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72 IN., 80, 100, 210L, 210L EP, 240, 245, 260, 260E, 270A, 270B, 300, 300CX, 300R, 300X, 310E, 310K, 310K EP, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 312GR, 313, 314G, 315, 315 P, 315SK, 315SL, 316GR, 317G, 318D, 318E, 318G, 319D, 319E, 320 P, 320D, 320E, 320G, 320R, 323D, 323E, 324E, 324G, 325G, 325J, 325SK, 325SL, 326D, 326E, 328D, 328E, 329D, 329E, 330G, 331G, 332D, 332E, 332G, 333D, 333E, 333G, 370B, 370E, 370E-II, 375, 375A, 385A, 400CX, 400X, 410 P, 410E, 410E-II, 410K, 410L, 410TK TMC, 435, 435C, 437C, 437D, 437E, 440E, 444 P, 444K, 444L, 447, 448, 449, 450E, 450M, 456, 457, 458, 459, 459E, 460 P, 460E, 460E-II, 460M, 460R, 467, 468, 469, 485, 485A, 500R, 509, 512, 520M, 522, 524 P, 524K, 524K-II, 524L, 525, 530, 531, 535, 540A, 540M, 542, 544 G, 544 P, 544K, 544K-II, 544L, 547, 550M, 551, 553, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 595, 600R, 603M, 603R, 609, 614R, 615F, 615R, 616R, 618F, 618R, 620, 620F, 620G, 620R, 622F, 622G, 622R, 623, 623M, 623R, 624 P, 624J, 624K, 624K-II, 624KR, 624L, 625, 625F, 625R, 630, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 631, 633, 635, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 640, 640FD, 640FD PERFORMANCE UPGRADES, 640H, 640L, 640L-II, 640R, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644J, 644K, 644K HYBRID, 644L, 644LH, 648H, 648HT, 648L, 648L-II, 651, 653, 660R, 661, 663, 663R, 670G, 672G, 673, 678, 680R, 683, 683R, 700M, 703JH, 709, 710 P, 710K, 710L, 720, 721, 724 P, 724J, 724K, 724L, 725, 726, 730, 731, 735, 740, 740A, 741, 744, 744K-II, 744L, 748, 748H, 748HT, 748L, 748L-II, 750A, 751, 753, 753J, 753JH, 759J, 759JH, 768L-II, 770G, 772G, 803M, 803MH, 824K, 824L, 830, 835, 840, 842, 843, 843K, 843L, 843L-II, 844 P, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848L, 848L-II, 852, 853J, 853JH, 853M, 853MH, 854, 859M, 859MH, 862, 864, 870G, 872G, 890, 895, 896, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 913, 915F, 916, 918, 918R, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930D, 930F, 930R, 936, 936D, 946, 948L, 948L-II, 950K, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 990, 994, 995, 1008, 1018, 1023E, 1026R, 1050K, 1050K PL, 1170, 1185, 1350, 1355, 1360, 1365, 1418, 1460, 1465, 1470, 1508, 1510DC, 1512FX, 1516FX, 1517, 1518, 1524FX, 1570, 1690, 1705, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725T, 1745, 1765, 1770NT, 1775, 1775NT, 1785, 1790, 1795, 1810DC, 1812DC, 1814DC, 1870, 1890, 1895, 1900, 1910, 1990, 2018, 2054, 2056, 2058, 2064, 2066, 2112DC, 2254, 2256, 2258, 2264, 2266, 2266E, 2412DE, 2510C, 2510H, 2510S, 2730, 3025E, 3032E, 3033R, 3038E, 3039R, 3046R, 3215, 3220, 3365, 3420, 3520, 3522, 3800, 4052M, 4210, 4310, 4410, 4510, 4610, 4700, 4710, 4890, 4895, 4990, 4995, 5065M, 5070M, 5075M, 5076EL, 5076EN, 5080M, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5125R, 5203, 5225, 5303, 5310N, 5325, 5325N, 5403, 5415, 5425, 5425N, 5500N, 5510N, 5525, 5525N, 5603, 5615, 5625, 5715, 5725, 6090 MC, 6090 RC, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6103, 6105 MC, 6105 RC, 6105E, 6105M, 6105R, 6110 MC, 6110 RC, 6110M, 6110R, 6115 MC, 6115 RC, 6115M, 6115R, 6120E, 6120EH, 6120M, 6120R, 6125M, 6125R, 6130M, 6130R, 6135CI550, 6135E, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135M, 6135M MONTENEGRO, 6135R, 6140M, 6140R, 6145M, 6145R, 6150M, 6150M MONTENEGRO, 6150R, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6190M, 6190R, 6195M, 6195R, 6210M, 6210R, 6215R, 6230R, 6250R, 6300, 6488, 6500, 6600, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7180, 7200, 7210, 7250, 7280, 7300, 7350, 7380, 7400, 7410, 7450, 7455, 7460, 7480, 7500, 7510, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8245R, 8270R, 8295R, 8300, 8320R, 8320RT, 8335R, 8345R, 8345RT, 8370R, 8370RT, 8400, 8400R, 8500, 8600, 8700, 8800, 9400, 9410, 9410R, 9420R, 9420RX, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A400, BL6, BL7, BL8, BL9, BL10, C300, C350, C400, C440R, C441R, C450, C451R, C461R, C500, C670, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CTS, CTS II, DB84, DB90, DB96, DR12, DR12T, DR16, DR18, DR24, F440M, F440R, F441M, F441R, FD22B, FD45, FL100, FR22B, FR24B, FS22B, FS50, GROUPER, GS66, GS72, GS78, GS84, GS88, GT72, GT80, GU60, GU66, GU72, GU78, H160, H165, H240, H260, H310, H340, H360, H380, H480, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HH30, HH50, HH75, L331, L341, LP72, LP78, LP84, M4040, M4040DN, MaxEmerge XP, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, MX5, MX6, MX7, N530C, N530F, N536C, N540C, N540F, N542C, N543F, N560F, P540, P556, P576, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R400, R450, R500, RB72, RB84, RB96, RC5M, RC6M, ROW-CROP HARVESTING UNITS, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, V451G, V451M, V451R, V461M, V461R, W200M, W235, W235M, W235R, W260, W260R, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, Y110, Y115, Y210, Y215</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
@@ -2639,6 +3279,11 @@
           <t>19M7824</t>
         </is>
       </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 2304, 8R 2704, 8R 3004, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 175, 210L, 210L EP, 260, 265, 270A, 270B, 280, 310K, 310K EP, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 315 P, 315SK, 315SL, 316GR, 317G, 318G, 320 P, 320G, 324G, 325G, 325J, 325SK, 325SL, 330G, 331G, 332G, 333G, 370E, 370E-II, 410 P, 410E, 410E-II, 410K, 410L, 410TK TMC, 440E, 440R, 449, 450C, 450E, 450M, 459, 459E, 460 P, 460E, 460E-II, 460M, 460R, 469, 470 P, 470G, 500R, 520, 521, 522, 531, 533, 535, 540, 540A, 541, 542, 543R, 550M, 551, 559, 560M, 560R, 568, 569, 578, 583, 603R, 608BH, 608L, 608LH, 608SH, 614R, 615F, 615R, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 622X, 623R, 625F, 625PF, 625R, 625X, 630, 630F, 630FD, 630PF, 630R, 630X, 631, 633, 635, 635F, 635FD, 635PF, 635R, 635X, 640, 640FD, 640L, 640L-II, 640X, 643J, 643L, 643L-II, 643R, 644 P, 644 X, 644K, 644L, 644LH, 645FD, 648L, 648L-II, 651, 653, 661, 663, 663R, 678, 683, 700M, 703JH, 710K, 720, 721, 722PF, 722X, 724 P, 724K, 724L, 725, 725PF, 725X, 726, 730, 730FD, 730PF, 730X, 731, 735, 735FD, 735PF, 735X, 740, 740A, 740FD, 740PF, 740X, 744, 744K, 745FD, 748, 748L, 748L-II, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 759J, 759JH, 768L-II, 803M, 803MH, 824K, 830, 835, 840, 843, 843J, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848L, 848L-II, 850, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 913, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944 X, 944K, 948L, 948L-II, 953G, 953J, 953K, 953M, 953MH, 953ML, 959J, 959K, 959M, 959MH, 959ML, 1050K, 1050K PL, 1450, 1470, 1510DC, 1550, 1570, 1745, 1775NT, 1790, 1795, 1810DC, 1812DC, 1814DC, 2032R, 2038R, 2054, 2056, 2058, 2064, 2066, 2112DC, 2254, 2256, 2258, 2264, 2266, 2266E, 2412DE, 2510C, 2510S, 2730, 2854, 3033R, 3036E, 3038R, 3045R, 3110, 3210, 3215, 3220, 3310, 3320, 3410, 3420, 3520, 3720, 3800, 4044M, 4044R, 4045CC550, 4045HRT90, 4049R, 4052M, 4052R, 4066M, 4066R, 4200, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4920, 5036C, 5039C, 5041C, 5042C, 5075M, 5090M, 5100M, 5100MH, 5115M, 6068HC550, 6068HRT81, 6090CP550, 6090HFU84, 6105AF001, 6105HF001, 6125AF001, 6125AFM01, 6125AFM75, 6125HF001, 6125HF070, 6125SFM75, 6135AFM75, 6135AFM85, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG09, 6135HFM85, 6135M MONTENEGRO, 6135SFM75, 6135SFM85, 6140J, 6140JH, 6145J, 6150J, 6150M, 6150M MONTENEGRO, 6155J, 6155JH, 6403, 6488, 6610, 6650, 6710, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7180, 7200, 7210, 7250, 7260, 7280, 7300, 7330, 7330 Premium, 7350, 7380, 7400, 7405, 7410, 7420, 7425, 7450, 7455, 7460, 7480, 7500, 7505, 7510, 7515, 7520, 7525, 7550, 7580, 7600, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8225R, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310R, 8310RT, 8320RT, 8335R, 8335RT, 8345RT, 8360R, 8360RT, 8370RT, 8400, 8500, 8600, 8700, 8800, 9320T, 9400, 9410, 9410R, 9420T, 9450, 9460R, 9460RT, 9470 STS, 9500, 9501, 9510, 9510R, 9510RT, 9520T, 9520T SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9580, 9600, 9610, 9620T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, C300, C350, C400, C440R, C441R, C450, C451R, C461R, C500, C670, CH570, CH670, CP20, CP690, CP770, CS690, CS770, CTS, CTS II, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, FD45, FS20, GROUPER, H180, H240, H260, H310, H340, H360, H380, H480, HD35F, HD40F, HD45F, HD50F, N530, N530C, N536, N536C, N540, N540C, N542, N542C, N543F, R500, RD30F, RD35F, RD40F, RD45F, REDEKOP SCU, S300, S350, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, Y210, Y215, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
@@ -2646,6 +3291,11 @@
           <t>19M10822</t>
         </is>
       </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>600 - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 625R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 635F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 622R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 625F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 630R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 620R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 630F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 622F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 620F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 618R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 618F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 615F - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 635R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 615R - Combine, Platform (Cutting), 600 R and F Cutting Platforms (Worldwide Edition) - PC9242, , 6136NW301 - Harvester, CH950 Sugarcane Harvester (South America Edition) - PC13659, , CH950 - Harvester, CH950 Sugarcane Harvester (South America Edition) - PC13659, , 6136NW301 - Harvester, CH960 Sugarcane Harvester (Worldwide Edition) - PC13660, , 6136NW401 - Harvester, CH960 Sugarcane Harvester (Worldwide Edition) - PC13660, , CH960 - Harvester, CH960 Sugarcane Harvester (Worldwide Edition) - PC13660, , CP690 - Picker, Cotton, CP690 Cotton Picker - PC12380, , 6135HN004 - Picker, Cotton, CP690 Cotton Picker - PC12380, , 6135HN005 - Picker, Cotton, CP690 Cotton Picker - PC12380, , 6135HN007 - Picker, Cotton, CP690 Cotton Picker - PC12380, , 6135HN008 - Picker, Cotton, CP690 Cotton Picker - PC12380, , 6135HN006 - Picker, Cotton, CP690 Cotton Picker - PC12380, , 6136NX401 - Picker, Cotton, CP770 Cotton Picker - PC13734, , CP770 - Picker, Cotton, CP770 Cotton Picker - PC13734, , CS690 - Stripper, Cotton, CS690 Cotton Stripper - PC12381, , 6135HN005 - Stripper, Cotton, CS690 Cotton Stripper - PC12381, , 606SH - Stripper, Cotton, CS690 Cotton Stripper - PC12381, , 608SH - Stripper, Cotton, CS690 Cotton Stripper - PC12381, , 6135HN007 - Stripper, Cotton, CS690 Cotton Stripper - PC12381, , 6135HN008 - Stripper, Cotton, CS690 Cotton Stripper - PC12381, , CS770 - Stripper, Cotton, CS770 Cotton Stripper - PC13735, , 6136NX401 - Stripper, Cotton, CS770 Cotton Stripper - PC13735, , 6068HCQ09 - Combine, S430 Combine (South America Edition) - PC13017, , S430 - Combine, S430 Combine (South America Edition) - PC13017, , S440 - Combine, S440 Combine (China Edition) - PC13305, , 6068HYC02 - Combine, S440 Combine (China Edition) - PC13305, , 6068HCQ10 - Combine, S440 Combine (South America Edition) - PC13018, , 6068HCQ11 - Combine, S440 Combine (South America Edition) - PC13018, , S440 - Combine, S440 Combine (South America Edition) - PC13018</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
@@ -2653,6 +3303,11 @@
           <t>03M7209</t>
         </is>
       </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>260, 265, 270A, 270B, 280, 314R, 335, 375, 385, 435, 446, 447, 456, 457, 466, 467, 500R, 525, 530, 535, 540A, 546, 547, 556, 557, 566, 567, 622X, 625X, 630, 630C, 630X, 635, 635X, 639, 640, 640C, 640X, 645C, 649, 659, 680, 722X, 725X, 730X, 735X, 740, 740A, 740X, 835, 840, 843, 913, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925F, 925R, 926, 930, 930F, 930R, 936, 994, 995, 1770NT, 1775NT, 2230FH, 2230LL, 2730, 5090R, 5100R, 5115R, 5125R, 6488, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 9009A, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, C300, C350, C400, C441R, C500, DB40, DB50, DB74, DB90, F441R, L50, L60, L70, L331, L341, R400, R500, S300, S350, S560, S690, W50, W70, W210, W230, W430, Y110, Y115, Y210, Y215</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
@@ -2660,6 +3315,11 @@
           <t>03M7210</t>
         </is>
       </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>112R, 210R, 212R, 215F, 215R, 218F, 218R, 220F, 222F, 222R, 240, 245, 260, 265, 450M, 460M, 460R, 506, 509, 516, 540A, 560M, 560R, 606, 609, 616, 631, 640, 651, 661, 709, 717, 731, 740, 740A, 751, 1008, 1018, 1418, 1508, 1517, 1518, 1830, 1835, 2018, 6488, 8100T, 8110T, 8120T, 8200T, 8210T, 8220T, 8230T, 8300T, 8310T, 8320T, 8330T, 8400T, 8410T, 8420T, 8430T, 8520T, 9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, C110, C120, H540F, H541, H550, H550F, H560F, H561, L50, L60, L70, R40, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W50, W70, W80, W100, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, Y110, Y115, Y210, Y215</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
@@ -2667,6 +3327,11 @@
           <t>03M7388</t>
         </is>
       </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>30R, 46R, 748H, 848H, 1450, 1550, 9470 STS, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, C670, S540, S550, S560, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
@@ -2674,6 +3339,11 @@
           <t>19M7827</t>
         </is>
       </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 46, 47, 48, 260, 270A, 270B, 300, 300CX, 300X, 325, 335, 345, 355, 370B, 375, 375A, 385A, 410, 419, 420, 430, 447, 448, 449, 450M, 459, 460, 460M, 460R, 469, 470 P, 470G, 485, 485A, 520M, 540M, 540R, 543M, 543R, 550M, 553, 559, 560M, 560R, 563, 565, 568, 569, 570, 572, 575, 578, 580, 582, 590, 592, 600R, 603M, 603R, 615F, 618F, 618R, 620F, 620R, 622F, 622R, 625D, 625F, 625R, 630D, 630F, 630R, 635D, 635F, 640D, 640L, 640L-II, 648L, 648L-II, 673, 722PF, 725D, 725PF, 730, 730D, 730PF, 735, 735D, 735PF, 740D, 740PF, 748, 748L, 748L-II, 764, 803M, 803MH, 848G, 848L, 848L-II, 853M, 853MH, 859M, 859MH, 890, 895, 896, 903M, 903MH, 909M, 909MH, 948L, 948L-II, 953M, 953MH, 953ML, 959M, 959MH, 959ML, 1107, 1109, 1111, 1113, 1450, 1470, 1550, 1570, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1780, 2025R, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2510H, 2660VT, 3025E, 3032E, 3038E, 3200, 3215, 3220, 3400, 3420, 3800, 4044M, 4052M, 4710, 4720, 4730, 4830, 4890, 4895, 5036C, 5039C, 5041C, 5042C, 5075M, 5076EL, 5076EN, 5083EN, 5085E, 5085M, 5090E, 5090EL, 5090EN, 5090M, 5090R, 5093EN, 5095M, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101EN, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5215F, 5215V, 5225, 5300N, 5310N, 5315F, 5315V, 5320N, 5325, 5325N, 5400, 5410N, 5420N, 5500N, 5510N, 5515F, 5515V, 5520N, 5615, 5615V, 6020, 6105D, 6105E, 6105M, 6115D, 6115M, 6120, 6120E, 6120L, 6125M, 6130, 6130D, 6130M, 6135E, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140D, 6140M, 6150M, 6170M, 6170R, 6190R, 6210J, 6210R, 6215, 6220, 6220L, 6225, 6230, 6320, 6320L, 6325, 6330, 6415, 6420, 6420L, 6420S, 6425, 6430, 6488, 6515, 6520, 6520L, 6525, 6530, 6534, 6610, 6615, 6620, 6630, 6650, 6710, 6715, 6750, 6810, 6850, 6910, 6950, 7130, 7180, 7200, 7200A, 7230, 7250, 7280, 7300, 7330, 7350, 7380, 7400, 7400A, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, C440R, C441R, C670, CH950, CH960, CP20, CP770, CS690, CS770, CTS, CTS II, DB90, F440M, F440R, F441M, F441R, GROUPER, H240, H260, H310, H480, HD35F, HD35R, HD40F, HD40R, HD40X, HD45F, HD45R, HD50F, HD50R, L331, L341, R230, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W330, W540, W550, W650, W660, X9 1000, X9 1100, Y210, Y215</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
@@ -2681,6 +3351,11 @@
           <t>19M7720</t>
         </is>
       </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>5-750, 5-754, 5-800, 5-804, 5-900, 5E-704, 5E-850H, 5E-854, 5E-904, 5E-1200, 5E-1204, 6B-1204/6120B, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 7, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8, 8A, 8B, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 10, 10A, 17D, 17G, 20 Trailer, 30 Trailer, 46, 47, 48, 49, 160 P, 160D, 160G, 180G, 200 G, 200D, 200G, 210G, 220DW, 225D, 230GW, 240D, 244E, 244H, 244J, 250D-II, 250G, 260 P, 260E, 270D, 290G, 300D-II, 300G, 304J, 310 P, 310E, 324, 324A, 324J, 328, 328A, 331, 335, 344T, 346T, 350 P, 350D, 350G, 370B, 370E, 375, 375A, 380 P, 380G, 385, 385A, 410D, 410E, 435, 440E, 444H, 444J, 446, 447, 448, 449, 450D, 450E, 450G, 450M, 455G, 456, 457, 458, 459, 459E, 460 P, 460E, 460M, 460R, 466, 467, 468, 469, 470G, 485, 485A, 490E, 493, 494, 510D, 521, 522, 535, 540E, 540G-II, 541, 542, 544H, 544J, 546, 547, 548E, 548G-II, 550G, 550M, 555G, 556, 557, 558, 559, 560M, 560R, 566, 567, 568, 569, 590D, 594, 605C, 620I, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625I, 640E, 640G, 644K, 648E, 648G, 650G, 655C, 692, 693, 694, 724 P, 724K, 724L, 740G, 744 P, 744J, 744K, 744K-II, 744L, 748E, 748G-III, 750A, 750C, 750J-II, 750K, 750L, 755C, 755D, 764, 824 P, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 848G, 850, 850C, 850J-II, 850K, 850L, 850L PL, 855 LONG CHASSIS, 855 SHORT CHASSIS, 870, 890, 892, 893, 894, 895, 896, 903K, 903KH, 903M, 903MH, 904, 909J, 909JH, 909K, 909KH, 909M, 909MH, 913, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 946, 950, 950C, 950J, 950K, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 970, 1010, 1015, 1025, 1030, 1035, 1050, 1050C, 1050E, 1054, 1070, 1092, 1100/1150, 1107, 1109, 1111, 1113, 1165, 1175, 1290, 1291, 1293, 1320, 1326, 1327, 1354, 1404, 1450, 1470, 1512FX, 1516FX, 1524FX, 1530, 1535, 1550, 1570, 1590, 1700, 1705, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1730, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1775, 1775NT, 1780, 1785, 1790, 1795, 1820, 1830, 1835, 1890, 1895, 1990, 2025R, 2026R, 2144G, 2154D, 2154G, 2156G, 2204, 2230FH, 2230LL, 2330, 2454D, 2510H, 2654G, 2656G, 2660VT, 2704, 2810, 2904, 2954D, 3004, 3040, 3050, 3100, 3110, 3140, 3154G, 3156G, 3200, 3204, 3210, 3300, 3310, 3350, 3400, 3410, 3640, 3650, 3710, 3754D, 3754G, 3756G, 4044R, 4052R, 4066R, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 5090R, 5100R, 5115R, 5125R, 5215, 5215F, 5215V, 5315, 5315F, 5315V, 5415, 5515, 5515 HIGH CROP, 5515F, 5515V, 5615, 5615V, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100J, 6100M, 6105 MC, 6105 RC, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115J, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125J, 6125M, 6125R, 6130, 6130D, 6130J, 6130M, 6130R, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145M, 6145R, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6210, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6715, 6820, 6830 Premium, 6920, 6920S, 6930, 7130, 7130 Premium, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7320, 7330 Premium, 7400, 7405, 7410, 7420, 7425, 7430E, 7455, 7505, 7510, 7520, 7525, 7530E, 7600, 7610, 7630, 7700, 7710, 7715, 7720, 7730, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 8100, 8200, 8225R, 8245R, 8270R, 8295R, 8300, 8320R, 8335R, 8345R, 8370R, 8400, 8400R, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9370R, 9400, 9400T, 9420, 9420R, 9420RX, 9420T, 9430T, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530T, 9560 STS, 9560RT, 9570 STS, 9570RT, 9570RX, 9570RX SCRAPER, 9620, 9620RX, 9620T, 9630T, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, A2, C310R, C350R, CH570, CH670, CH950, CH960, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E210, E210LC, E230, E240, E240LC, E260, E300LC, E330, E360, E380, E400, F310R, F350R, H260, H310, H360, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, M-GATOR A3, MaxEmerge XP, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R310R, R870R, R950R, R990R, S310R, S350R, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, V451G, V451M, V461M, W200M, W235, W235M, W235R, W260, W260R, W540, W550, W650, W660, WL56, XUV825E, XUV825M, XUV825M S4, XUV855E, XUV855M, XUV855M S4</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
@@ -2688,6 +3363,11 @@
           <t>A50325</t>
         </is>
       </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>912, 914, 1700, 1740, 1750, 1760, 1760/1765 PRECISION UPGRADES, 1775NT, 1790, 1795, 1910, 7760, 9009A, 9450, 9550, 9560, 9650, 9660, CP690, CP770, CS690, CS770, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
@@ -2695,6 +3375,11 @@
           <t>19M7845</t>
         </is>
       </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>6B-1204/6120B, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 54D IN., 60 IN. DECKS, 60D IN., 62 IN., 500R, 525, 530, 535, 540A, 565, 568, 575, 578, 603R, 606C, 608C, 608C PRECISION UPGRADES, 612C, 612FC, 616C, 618C, 623, 623R, 625D, 630, 630D, 631, 635, 635D, 640, 640D, 644, 651, 661, 678, 706C, 708C, 712C, 712FC, 716C, 718C, 725D, 730, 730D, 731, 735, 735D, 740A, 740D, 744, 748, 750A, 751, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 855 LONG CHASSIS, 855 SHORT CHASSIS, 890, 895, 896, 904, 960, 990, 1054, 1354, 1355, 1365, 1404, 1465, 1720, 1725, 1725C, 1854, 1854J, 1860, 1870, 1890, 1900, 1910, 2025R, 2026R, 2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 3025E, 3032E, 3036E, 3038E, 4500, 4600, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4940, 4990, 4995, 5070M, 5075M, 5080M, 5085M, 5090M, 5095M, 5100M, 5105M, 5105MH, 5115M, 5130M, 6080A E-CUT, 6080A PRECISIONCUT, 6081HF070, 6090AFM75, 6090AFM85, 6090CG550, 6090CI550, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG09, 6090HFG94, 6090HFG95, 6090M, 6090SFM75, 6090SFM85, 6100B, 6100M, 6105AF001, 6105HF001, 6105J, 6110B, 6110M, 6110R, 6120M, 6120R, 6125AF001, 6125HF001, 6125HF070, 6125M, 6130M, 6130R, 6135CI550, 6135HF485, 6135HFC09, 6135HFC95, 6135HFG95, 6135M, 6135M MONTENEGRO, 6135R, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205J, 6210J, 6210M, 6210R, 6215R, 6230R, 6250R, 6300, 6300L, 6400, 6400L, 6403, 6405, 6415, 6500, 6500A E-CUT, 6500A PRECISIONCUT, 6500L, 6600, 6603, 6605, 6610, 6615, 6650, 6700A E-CUT, 6700A PRECISIONCUT, 6710, 6750, 6810, 6820, 6830, 6830 Premium, 6850, 6910, 6910S, 6920, 6920S, 6930, 6950, 7180, 7200, 7200A, 7250, 7260, 7300, 7330, 7330 Premium, 7350, 7400, 7400A, 7420, 7425, 7430E, 7450, 7455, 7460, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7515, 7520, 7525, 7530E, 7550, 7700, 7700A E-CUT, 7700A PRECISIONCUT, 7750, 7760, 7800, 7850, 7950, 8000A E-CUT, 8100, 8200, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310R, 8320R, 8320RT, 8335R, 8345R, 8345RT, 8360R, 8370R, 8370RT, 8400, 8400R, 8500, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9360R, 9370R, 9400, 9410, 9420R, 9450, 9460RT, 9470 STS, 9470R, 9470RT, 9500, 9501, 9510, 9510RT, 9520R, 9520RT, 9540, 9550, 9560, 9560 STS, 9560RT, 9570 STS, 9570RT, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, A2, C6R, C6R PRECISION UPGRADES, C8R, C8R PRECISION UPGRADES, C12F, C12F PRECISION UPGRADES, C12R, C12R PRECISION UPGRADES, C16F, C16F PRECISION UPGRADES, C16R, C16R PRECISION UPGRADES, C18F, C18F PRECISION UPGRADES, C18R, C18R PRECISION UPGRADES, C300, C350, C400, C441R, C451R, C461R, C500, C650, C670, C850, CH950, CH960, CP690, CP770, CS690, CS770, CTS, CTS II, DB40, DB50, DB74, DR12, DR12T, DR16, DR18, DR24, F441M, F441R, GROUPER, GX335, GX345, GX355, L341, M-GATOR A3, M-GATOR A3T, P576, R500, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, STRAIGHT BLADE, T550, T560, T660, T670, V451R, V461R, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
@@ -2702,6 +3387,11 @@
           <t>19M8486</t>
         </is>
       </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>6E-1504L, 6E-1504PL, 210L, 210L EP, 250D, 250D-II, 260 P, 260E, 300C, 300D, 300D-II, 300DW, 300WW, 310D, 310E, 315D, 410D, 415, 425, 445, 447, 448, 455, 457, 458, 467, 468, 510D, 547, 557, 558, 567, 568, 595D, 624H, 624J, 630FD, 630FD PERFORMANCE UPGRADES, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 644H, 644HMH, 644J, 645FD, 645FD PERFORMANCE UPGRADES, 710D, 710G, 710J, 710K, 710L, 724J, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 735FD PERFORMANCE UPGRADES, 740FD, 740FD PERFORMANCE UPGRADES, 745FD, 745FD PERFORMANCE UPGRADES, 750C, 824J, 824K, 850C, 950K, 1050K, 1107, 1109, 1111, 1113, 1690, 1820, 1870, 1890, 1895, 1910, 1990, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2230FH, 2230LL, 2254, 2256, 2258, 2264, 2266, 2266E, 2510H, 2620, 2623, 2625, 2630, 2633, 2635, 2730, 5045E, 5055E, 5065E, 5075E, 5075M, 5085E, 5090E, 5090M, 5090R, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 7200R, 7210, 7215R, 7230R, 7260R, 7280R, 7410, 7510, 7610, 7710, 7810, 8120, 8130, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8310R, 8320, 8320R, 8330, 8335R, 8345R, 8360R, 8420, 8430, 8520, 8530, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9120, 9220, 9230, 9320, 9330, 9400, 9410, 9420, 9430, 9450, 9470 STS, 9500, 9501, 9510, 9520, 9530, 9530 SCRAPER, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9620, 9630, 9630 SCRAPER, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, B25C, B30C, C670, CTS, CTS II, DB40, DB50, DB66, DB74, DB80, DB88, DB90, N540F, N543F, N550, N560, N560F, P576, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, TC62H, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
@@ -2709,6 +3399,11 @@
           <t>19M7969</t>
         </is>
       </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>3B-404, 3B-454, 3B-504, 3B-554, 3B-604, 5-750, 5-754, 5-800, 5-804, 5-900, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-954, 5E-1004, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 204K, 204L, 210K, 210K EP, 210L, 210L EP, 210LJ, 220DW, 225D, 244E, 244H, 245G, 250D, 250D-II, 260E, 300D, 300D-II, 300DW, 300WW, 304K, 304L, 310E, 350C, 350D, 350D-II, 350DW, 370E, 370E-II, 400C, 400D, 400D-II, 410D, 410E, 444 G, 444 P, 444H, 444J, 444K, 444L, 450D, 450G, 450H, 450J, 450K, 455G, 460E, 470G, 510D, 540A, 540E, 540G-II, 544E, 544G, 544H, 544J, 548E, 548G-II, 550G, 550H, 550J, 550K, 555G, 608BH, 608L, 608LH, 608SH, 620G, 622G, 622X, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625X, 630X, 635X, 640, 640E, 640G, 640X, 643J, 644 P, 644H, 644HMH, 644J, 644K, 644L, 648E, 648G, 650D, 650G, 650H, 650J, 650K, 653E, 653G, 670 P, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 680, 690E, 700K, 702, 703G, 703GH, 703JH, 710D, 720, 722X, 724 P, 724J, 724K, 724L, 725, 725X, 730X, 731, 735X, 740, 740A, 740G, 740X, 741, 744K, 748E, 748G-III, 750J, 750J-II, 750K, 750L, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 764, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 803M, 803MH, 824K, 840, 843J, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 850, 850D, 850J, 850J-II, 850K, 850L, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870 P, 870D, 870G, 872D, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 904, 904 P, 909J, 909JH, 909K, 909KH, 950K, 953G, 953J, 953K, 959J, 959K, 1050C, 1050J, 1050K, 1050K PL, 1054, 1354, 1404, 1450, 1470, 1550, 1570, 1654, 1854, 1854J, 2054, 2104, 2154D, 2204, 2410, 2430, 2430C, 2454D, 2704, 2854, 2904, 2954D, 3045B, 3050B, 3510, 3520, 3522, 3554, 3754D, 4555, 4560, 4650, 4755, 4760, 4850, 4955, 4960, 5065M, 5075M, 5076E, 5076EF, 5076EL, 5082E, 5085M, 5090E, 5090EH, 5090R, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100R, 5105M, 5115M, 5115R, 5125R, 5425, 5625, 5725, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6105 MC, 6105 RC, 6105EH, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115M, 6115R, 6120, 6120B, 6120EH, 6120M, 6120R, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130M, 6130R, 6135B, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6205J, 6210, 6210J, 6210M, 6210R, 6215, 6215R, 6220, 6230, 6230 Premium, 6230R, 6250R, 6300, 6310, 6310L, 6320, 6320L, 6330, 6330 Premium, 6400, 6403, 6405, 6410, 6415, 6420, 6420L, 6420S, 6430, 6430 Premium, 6500L, 6506, 6510, 6510S, 6520, 6520L, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6715, 6800, 6810, 6820, 6830, 6830 Premium, 6900, 6910, 6910S, 6920, 6920S, 6930, 7130, 7130 Premium, 7200, 7200R, 7210, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7320, 7330, 7330 Premium, 7400, 7410, 7420, 7425, 7430E, 7500, 7505, 7510, 7515, 7520, 7525, 7530E, 7600, 7610, 7630, 7700, 7710, 7720, 7730, 7800, 7810, 7820, 7830, 7920, 7930, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8520, 8520T, 8530, 8630, 9300T, 9320T, 9400T, 9420T, 9460RT, 9470RT, 9470RX, 9470RX SCRAPER, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9560RT, 9570RT, 9570RX, 9570RX SCRAPER, 9620RX, 9620T, 9670 STS, 9770 STS, 9870 STS, 9880 STS, B35C, B40C, CH570, CH670, DB40, DB50, DB74, DB90, E300, E300LC, E330, E360, FD22B, FD55, FR21B, FR22B, FR24B, FR50, FS20, FS22B, FS50, L331, L341, L1524, S670, S680, S690, S770, S780, S790, TC44H, TC54H, TC62H, W200M, W235, W235M, W235R, W260, W260R</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
@@ -2716,6 +3411,11 @@
           <t>19M8138</t>
         </is>
       </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>625D, 630D, 635D, 640D, 700M, 725D, 730D, 735D, 740D, 926, 936, DB37, DB40, DB41, DB44, DB50, DB55, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, H480, S430, S440, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
@@ -2723,6 +3423,11 @@
           <t>19M7968</t>
         </is>
       </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>5-750, 5-754, 5-800, 5-804, 5-900, 5E-850, 5E-850H, 5E-854, 6M-2104, 6R 175, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 50D, 50G, 60D, 130G, 200, 225D, 250D-II, 260 P, 260E, 300D, 300D-II, 304H, 310 P, 310D, 310E, 310SE, 315D, 315SE, 330C, 350 P, 350D, 350G, 360DC, 370, 370C, 370E, 370E-II, 380 P, 380G, 410 P, 410D, 410E, 410E-II, 437D, 444 G, 444 P, 444H, 444K, 444L, 450D, 450G, 450M, 455G, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 470 P, 470G, 510D, 524 P, 524K, 524K-II, 524L, 540E, 540G-II, 540G-III, 540H, 544 P, 544E, 544G, 544J, 544K, 544K-II, 544L, 548E, 548G-II, 548G-III, 548H, 550, 550G, 555G, 560M, 560R, 600C, 608BH, 608L, 608LH, 608SH, 620G, 622G, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 640E, 640G, 640H, 644E, 644G, 644H, 644HMH, 644J, 644K, 648E, 648G, 648H, 648HT, 650D, 650G, 655K, 670 P, 670G, 672G, 690E, 700H, 700L, 700L PL, 703G, 703GH, 703JH, 710D, 724J, 724K, 740G, 741, 744H, 744J, 748E, 748G-II, 748G-III, 748H, 748HT, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755K, 759G, 759GH, 759J, 759JH, 764, 770G, 772G, 792D, 803M, 803MH, 824J, 848G, 848H, 848HT, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853G, 853M, 853MH, 859M, 859MH, 870G, 872G, 892E, 900, 903G, 903K, 903KH, 909J, 909K, 909KH, 913, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 950K, 953G, 953K, 959J, 959K, 1050C, 1050K, 1050K PL, 1418, 1854, 1910, 2054, 2104, 2156G, 2410, 2430, 2430C, 2454D, 2510C, 2510H, 2510S, 2854, 2954D, 3154G, 3156G, 3554, 3754D, 3754G, 3756G, 5076E, 5076EF, 5076EL, 5082E, 5090E, 5090EH, 5090EL, 5210, 5310, 5310N, 5320N, 5410, 5415, 5420, 5420N, 5425, 5510, 5510N, 5520, 5520N, 5600, 5603, 5615, 5625, 5700, 5715, 5725, 6090AFM75, 6090AFM85, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG94, 6090HFG95, 6090HFU84, 6090SFM75, 6090SFM85, 6100, 6110, 6175R, 6190J, 6190R, 6195R, 6200, 6205J, 6210, 6210J, 6210R, 6215R, 6230R, 6250R, 6300, 6310, 6310L, 6400, 6410, 6500L, 6506, 6510, 6510S, 6600, 6610, 7200, 7210, 7400, 7405, 7410, 7500, 7510, 7600, 7610, 7700, 7710, 7800, 7810, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8400, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8520, 8520T, 8530, 8850, 9300T, 9320T, 9400T, 9420T, 9430T, 9460RT, 9470RT, 9510RT, 9520R, 9520RT, 9520T, 9520T SCRAPER, 9530T, 9560RT, 9570RT, 9620T, 9630T, 9670 STS, 9770 STS, 9970, 9976, 9986, CH330, CH530, E240, E260, HX10, HX14, MX5, MX6, MX7, MX8, MX10, PC7, RC5M, RC6M, RC8M, RC10M, RC10R, RC14R, S540, S650, S660, S670, S670H, S760, S770, T550, T560, T660, T670, TC44H, TC62H, W540, W550, W650, W660, WL56</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
@@ -2730,6 +3435,11 @@
           <t>19M7921</t>
         </is>
       </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>6B-1204/6120B, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 185, 6R 230, 6R 250, 6R 2304, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 20 Trailer, 30 Trailer, 200, 250D-II, 300D-II, 318D, 319D, 320D, 323D, 324H, 344H, 370E, 410E, 444 P, 444J, 444K, 444L, 450G, 450J, 455G, 460E, 524 P, 524K, 524K-II, 524L, 540M, 544 G, 544 P, 544J, 544K, 544K-II, 544L, 550G, 550J, 555G, 563, 620, 624 P, 624K, 624K-II, 624L, 640, 644 G, 644 P, 644 X, 644G, 644K, 644L, 644LH, 650G, 650J, 655K, 673, 690E, 721, 724 P, 724K, 724L, 726, 740, 741, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748G-II, 750J, 755C, 755D, 755K, 824 P, 824J, 824K, 824L, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 850J, 850J-II, 850K, 850L, 903K, 903KH, 903M, 903MH, 904 P, 909K, 909KH, 909M, 909MH, 950C, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1050K, 1050K PL, 1354, 1404, 1450, 1470, 1550, 1570, 1654, 1830, 1835, 1854, 1854J, 1870, 2054, 2104, 2310, 2410, 2430, 2430C, 2510H, 2510S, 3554, 4895, 4995, 5075M, 5090M, 5090R, 5100M, 5100MH, 5100R, 5115M, 5115R, 5115RH, 5125M, 5125R, 6010, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135B, 6135E, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140J, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6715, 6800, 6810, 6820, 6830, 6830 Premium, 6900, 6910, 6910S, 6920, 6920S, 6930, 7130, 7130 Premium, 7200, 7210, 7220, 7230, 7230 Premium, 7320, 7330, 7330 Premium, 7400, 7405, 7410, 7420, 7425, 7500, 7505, 7510, 7515, 7520, 7525, 7600, 7610, 7630, 7700, 7710, 7720, 7730, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 8100, 8100T, 8110T, 8120T, 8200, 8200T, 8210T, 8220T, 8300, 8300T, 8310T, 8320T, 8400, 8400T, 8410T, 8420T, 8520T, 8850, 9230, 9300T, 9320T, 9330, 9370R, 9400, 9400T, 9410, 9420R, 9420T, 9430, 9430T, 9450, 9470 STS, 9470R, 9470RT, 9500, 9510, 9520R, 9520RT, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9570 STS, 9570R, 9570RT, 9580, 9600, 9610, 9620R, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9970, C670, CTS, CTS II, DB40, DB50, DB74, DB90, E300, E330, E360, E380, H360, H380, H540F, H541, H550, H550F, H560F, H561, P540, P556, R4038, R4044, R4045, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W330, W440, W540, W550, W650, W660, WL53, WL56</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
@@ -2737,6 +3447,11 @@
           <t>H121472</t>
         </is>
       </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
@@ -2744,6 +3459,11 @@
           <t>19M8002</t>
         </is>
       </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 6B-1204/6120B, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 6R 175, 6R 195, 6R 215, 6R 230, 6R 250, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 20 Trailer, 26, 30 Trailer, 47 IN., 54 IN. FRONT BLADE, 59 IN., 135 P, 160 P, 160C, 160D, 160G, 180C W, 180G, 190DW, 200, 200 G, 200C, 200D, 200G, 210C, 210C W, 210G, 220DW, 225C, 225D, 230C, 240D, 245 P, 245G, 246, 250G, 270D, 290G, 300D, 310D, 310E, 310G, 310K, 310L, 310SE, 310SG, 310SJ, 315D, 315J, 315SE, 315SG, 335C, 335D, 337E, 350 P, 350D, 350G, 360DC, 380 P, 380G, 435C, 437C, 437D, 437E, 445, 450G, 450H, 450J, 450K, 455G, 460DC, 520M, 540E, 540G-II, 540G-III, 540H, 540M, 548E, 548G-II, 548G-III, 548H, 550G, 550H, 550J, 550K, 555G, 563, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 615C, 616C, 616C PERFORMANCE UPGRADES, 617C, 618C, 618C PERFORMANCE UPGRADES, 640E, 640G, 640H, 640L, 640L-II, 643L, 643L-II, 644 X, 644K HYBRID, 644LH, 648E, 648G, 648H, 648HT, 650D, 650G, 650H, 650J, 650K, 655K, 670 P, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 673, 676, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 721, 726, 740G, 748E, 748G-II, 748G-III, 748H, 748HT, 750C, 750J, 750J-II, 750K, 753J, 753JH, 755K, 759J, 759JH, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 790E, 803M, 803MH, 843L, 843L-II, 848G, 848H, 848HT, 850C, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853M, 853MH, 859M, 859MH, 870 P, 870D, 870G, 872D, 872G, 903K, 903KH, 903M, 903MH, 904, 909K, 909KH, 909M, 909MH, 950J, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1050K, 1050K PL, 1054, 1270D, 1270E, 1270G, 1354, 1404, 1450, 1470, 1470D, 1470E, 1470G, 1510C, 1510DC, 1512C, 1512E, 1550, 1570, 1612DE, 1710D, 1711D, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1910E, 1910G, 2010DE, 2014DE, 2054, 2112C, 2112DC, 2112E, 2144G, 2154D, 2154G, 2156G, 2412DE, 2704, 2854, 2904, 3004, 3154G, 3156G, 3204, 3215, 3220, 3420, 3520, 3522, 3554, 3754D, 3754G, 3756G, 3800, 5060EN, 5070M, 5075M, 5076EL, 5076EN, 5080EN, 5080M, 5080R, 5083EN, 5085M, 5090EL, 5090EN, 5090M, 5090R, 5093EN, 5100M, 5100R, 5101EN, 5115M, 5115R, 5125R, 5620, 5720, 5820, 6010, 6020, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100B, 6100M, 6105 MC, 6105 RC, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110M, 6110R, 6115 MC, 6115 RC, 6115M, 6115R, 6120, 6120M, 6120R, 6125M, 6125R, 6130, 6130M, 6130R, 6135M, 6135R, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6155M, 6155MH, 6155R, 6170M, 6170R, 6175M, 6175R, 6190R, 6195M, 6195R, 6200, 6205, 6210, 6210M, 6210R, 6215, 6215R, 6220, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6310, 6320, 6325, 6330, 6330 Premium, 6400, 6410, 6420, 6420S, 6425, 6430, 6430 Premium, 6505, 6506, 6510, 6510S, 6515, 6520, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6610, 6620, 6630, 6630 Premium, 6800, 6810, 6820, 6830, 6830 Premium, 6900, 6910, 6910S, 6920, 6920S, 6930, 7130, 7200, 7200R, 7210R, 7215R, 7230, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7400, 7430E, 7530E, 7630, 7720, 7730, 7820, 7830, 7920, 7930, 8100, 8110, 8120, 8130, 8200, 8210, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310, 8310R, 8310RT, 8320, 8320R, 8330, 8335R, 8335RT, 8345R, 8360R, 8360RT, 8370R, 8400, 8400R, 8410, 8420, 8430, 8520, 8530, 9450, 9460RT, 9470 STS, 9470RT, 9510RT, 9520R, 9520RT, 9540, 9550, 9560, 9560 STS, 9560RT, 9570 STS, 9570RT, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9996, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C670, CH570, CH670, CP770, CS770, DB37, DB41, DB50, DB55, DB60, DB62, DB74, DB80, DB83, DB88, DB90, DB120, E330, E360, E380, E400, H240, H260, H480, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
@@ -2751,6 +3471,11 @@
           <t>19M8224</t>
         </is>
       </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>6R 145, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 30 Trailer, 110, 110 TLB, 120C, 120D, 130 P, 130G, 135 P, 135C, 135D, 135G, 160, 160 P, 160C, 160D, 160G, 180C W, 180G, 190DW, 190GW, 200, 200 G, 200C, 200G, 210C W, 210G, 220DW, 225C, 225D, 245G, 250D, 250D-II, 260 P, 260E, 270, 270C, 270D, 290G, 300D, 300D-II, 300DW, 300G, 300WW, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 315D, 315SE, 315SG, 330, 330C, 344E, 345, 350G, 360DC, 370, 370C, 370E, 380G, 410D, 410E, 410G, 410J, 410K, 410L, 444 G, 444E, 444H, 444J, 445, 450, 450C, 450G, 450H, 450J, 450K, 455G, 460, 460 P, 460DC, 460E, 470 P, 470G, 475, 490, 490E, 509, 510D, 512, 524 P, 524K, 524K-II, 524L, 540A, 540E, 540G-II, 540G-III, 540H, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 548E, 548G-II, 548G-III, 548H, 550G, 550H, 550J, 550K, 555G, 605C, 605K, 609, 620G, 622G, 624 P, 624H, 624J, 624K, 624K-II, 624L, 631, 640, 640E, 640G, 640H, 640L, 640L-II, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650G, 650H, 650J, 650K, 651, 653, 653E, 653G, 661, 663, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 676, 683, 684, 686, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 709, 710G, 710J, 710K, 710L, 720, 724 P, 724J, 724K, 724L, 725, 731, 740, 740A, 740G, 744 P, 744H, 744K, 744K-II, 744L, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 751, 753, 753J, 753JH, 755C, 755D, 755K, 759J, 759JH, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 778, 792D, 824 P, 824K, 824L, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850L, 850L PL, 853G, 853J, 853JH, 859M, 859MH, 870D, 870G, 872D, 872G, 892E, 900, 903G, 903J, 903JH, 903K, 903KH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 944K, 946, 948L, 948L-II, 950C, 950J, 950K, 953G, 953J, 953K, 956, 959J, 959K, 959M, 959MH, 959ML, 1050C, 1050J, 1050K, 1050K PL, 1107, 1109, 1111, 1113, 1165, 1175, 1424, 1424C, 1433, 1433C, 1434, 1434C, 1450, 1517, 1518, 1535, 1550, 1720 CCS, 1725T, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1790, 1795, 1830, 1835, 1870, 2018, 2054, 2154D, 2154G, 2156G, 2204, 2230FH, 2330, 2454D, 2510C, 2510H, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2654G, 2656G, 2704, 2720, 2854, 2904, 2954D, 3004, 3154G, 3156G, 3204, 3510, 3520, 3554, 3754D, 3754G, 3756G, 4555, 4560, 4730, 4755, 4760, 4830, 4920, 4955, 4960, 6010, 6020, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFM85, 6090HFU84, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6105 MC, 6105 RC, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6115 MC, 6115 RC, 6115M, 6115R, 6120, 6125M, 6125R, 6130, 6130M, 6130R, 6135M, 6135R, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6190J, 6190M, 6190R, 6195M, 6195R, 6205, 6205J, 6210, 6210J, 6210M, 6210R, 6215, 6215R, 6220, 6225, 6230, 6310, 6320, 6325, 6330, 6410, 6420, 6420S, 6425, 6430, 6505, 6510, 6515, 6520, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6810, 6820, 6830, 6830 Premium, 6850, 6910, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7410, 7420, 7430E, 7450, 7480, 7500, 7510, 7520, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8520, 8520T, 8530, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9460R, 9460RT, 9470R, 9470RX, 9470RX SCRAPER, 9500, 9510, 9510R, 9510RT, 9520, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9560R, 9560RT, 9570RX, 9570RX SCRAPER, 9600, 9610, 9620, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9670, 9670 STS, 9770 STS, C670, CH330, CH530, CTS, CTS II, CX15, CX20, DB37, DB41, DB44, DB55, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, E12, E15, E300, E300LC, E330, E360, E380, E400, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, FS22B, H540F, H541, H550, H550F, H560F, H561, HX6, HX7, HX10, HX14, HX15, HX20, L624, L633, L634, L1533, L1534, M15, M20, MX5, MX6, MX7, MX8, MX10, MX15, P540, P556, PLANTER PERFORMANCE UPGRADES, R10, R15, R20, RC5M, RC6M, RC6R, RC7M, RC7R, RC8M, RC10M, RC10R, RC14R, S540, S650, S660, S670, S670H, S760, S770, T550, T560, T660, T670, TC44H, TC54H, TC62H, W170, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
@@ -2758,6 +3483,11 @@
           <t>19M8639</t>
         </is>
       </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 17D, 210K, 210K EP, 210L, 210L EP, 210LJ, 250D, 250D-II, 260 P, 260E, 300D, 300D-II, 300DW, 300WW, 310 P, 310E, 335C, 350D, 350D-II, 350DW, 360DC, 370E, 370E-II, 390, 400D, 400D-II, 408R, 410 P, 410E, 410E-II, 435C, 437C, 444 G, 444 P, 444H, 444J, 444K, 444L, 450J, 450K, 460, 460 P, 460DC, 460E, 460E-II, 460S, 475, 490, 520M, 524 P, 524K, 524K-II, 524L, 530B, 535, 540E, 540G-II, 540G-III, 540H, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 548E, 548G-II, 548G-III, 550, 550J, 550K, 554, 600L HIGH DUMP, 600R, 605K, 606SH, 608L, 608LH, 608SH, 620G, 620R, 622G, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 640E, 640G, 640H, 640L, 640L-II, 640R, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650, 650J, 650K, 653E, 653G, 654, 655K, 670D, 670G, 672D, 672G, 690E, 692, 700H, 700J, 700M, 724 P, 724J, 724K, 724L, 740G, 744H, 744J, 744K, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753GL, 753J, 753JH, 755K, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770D, 770G, 772, 772D, 772G, 778, 803M, 803MH, 824J, 824K, 843L, 843L-II, 844K, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870D, 870G, 872D, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904, 909J, 909JH, 909K, 909KH, 909M, 909MH, 944K, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 959J, 959K, 959M, 959MH, 959ML, 1050J, 1050K, 1054, 1354, 1404, 1690, 1700, 1705, 1730, 1770NT, 1775NT, 1790, 1835, 1840, 1860, 1890, 1895, 1900, 1910, 1990, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653A, 2704, 2720, 2904, 3204, 3510, 3520, 3522, 5076E, 5076EF, 5076EL, 5076EN, 5082E, 5083E, 5083EN, 5085E, 5090E, 5090EH, 5090EL, 5090EN, 5093E, 5093EN, 5100E, 5101E, 5101EN, 5215, 5215F, 5215V, 5300N, 5310, 5310N, 5315, 5315F, 5315V, 5320N, 5325N, 5400, 5410, 5410N, 5415, 5420N, 5425, 5425N, 5500N, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520N, 5525, 5525N, 5603, 5615, 5615V, 5625, 5715, 5725, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6095B, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105M, 6105R, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120M, 6120R, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130M, 6130R, 6135B, 6135E, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145M, 6145R, 6150M, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170R, 6190R, 6220, 6230, 6230 Premium, 6320, 6330, 6330 Premium, 6403, 6415, 6420, 6420S, 6430, 6430 Premium, 6520, 6530 Premium, 6534 Premium, 6603, 6615, 6620, 6630 Premium, 7130 Premium, 7200, 7200R, 7210, 7210R, 7215R, 7220, 7230 Premium, 7230R, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7310R, 7320, 7330, 7330 Premium, 7380, 7400, 7410, 7420, 7455, 7460, 7480, 7510, 7515, 7520, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7720, 7730, 7780, 7800, 7810, 7820, 7830, 7920, 7930, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430T, 8520, 8520T, 8530, 8850, 9300T, 9320T, 9400T, 9420T, 9430T, 9460RT, 9470 STS, 9510RT, 9520T, 9520T SCRAPER, 9530T, 9550, 9560RT, 9570 STS, 9620T, 9630T, 9650, 9650 STS, 9750 STS, 9935, 9970, 9976, 9986, 9996, C100, C110, C120, C650, C850, CH570, CH670, CH950, CH960, DB37, DB40, DB41, DB44, DB50, DB55, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, H240, H480, H540F, H550F, H560F, L70, L330, L331, L340, L341, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, PLANTER PERFORMANCE UPGRADES, R4030, R4045, S430, S440, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, TC44H, TC54H, TC62H, W80, W100, W170, W210, Y110, Y115, Y210, Y215</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
@@ -2765,6 +3495,11 @@
           <t>H210201</t>
         </is>
       </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>1900, 1910, 2254, 7250, 7350, 7450, 7550, 7750, 7780, 7850, 7950, 7980, 9450, 9470 STS, 9550, 9560, 9560 STS, 9570 STS, 9610, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, CH330, S430, S440, S560, S690</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
@@ -2772,6 +3507,11 @@
           <t>R111437</t>
         </is>
       </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 1654, 1854, 1854J, 2054, 2104, 2204, 2704, 2854, 2904, 3004, 3204, 4055, 4255, 4455, 4555, 4560, 4755, 4760, 4955, 4960, 6090M, 6100J, 6100M, 6110J, 6110M, 6115J, 6120M, 6125J, 6125M, 6130J, 6130M, 6130R, 6135J, 6135M MONTENEGRO, 6140M, 6145J, 6145M, 6145R, 6150J, 6150M MONTENEGRO, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6205J, 6210J, 6210M, 6210R, 6215R, 6230R, 6250R, 6415, 7130 Premium, 7185J, 7195J, 7200, 7200J, 7205J, 7210, 7210J, 7210R, 7215J, 7220, 7225J, 7230 Premium, 7230J, 7230R, 7250R, 7260R, 7270R, 7290R, 7310R, 7320, 7330, 7330 Premium, 7400, 7410, 7510, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7760, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 8100, 8110, 8120, 8130, 8200, 8210, 8220, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310, 8310R, 8320, 8320R, 8330, 8335R, 8345R, 8360R, 8370R, 8400, 8400R, 8410, 8420, 8430, 8520, 8530, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9320, 9330, 9360R, 9370R, 9400, 9410R, 9420, 9420R, 9430, 9470R, 9520, 9530, 9530 SCRAPER, 9570R, 9620, 9620R, 9630, 9630 SCRAPER, 9670, 9970, C650, C850, CP690, CP770, CS690, CS770, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
@@ -2779,6 +3519,11 @@
           <t>19M8006</t>
         </is>
       </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 60, 120C, 160 P, 160C, 160G, 175, 180G, 200 G, 200G, 210 P, 210K, 210K EP, 210L, 210L EP, 240, 245, 310 P, 310K, 310K EP, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 315 P, 315SK, 315SL, 318E, 319E, 320 P, 320E, 323E, 325SK, 325SL, 332, 335C, 335D, 337E, 350D, 350D-II, 350DW, 370E, 370E-II, 400D, 400D-II, 410 P, 410E, 410E-II, 410K, 410L, 410TK TMC, 435C, 437C, 437D, 437E, 444H, 450C, 460 P, 460E, 460E-II, 470 P, 470G, 540G-II, 540M, 544G, 544H, 548G-II, 605C, 606C, 607C, 608BH, 608C, 608C PRECISION UPGRADES, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612FC, 613C, 614C, 615C, 616C, 617C, 618C, 620G, 622G, 624G, 624K, 624K-II, 635FD, 640FD, 640G, 640R, 644G, 644K, 647A, 648G, 652R, 657A, 667A, 670D, 670G, 672D, 672G, 700J, 700J-II, 703G, 703GH, 703JH, 706C, 708C, 710 P, 710K, 710L, 712C, 712FC, 716C, 717, 717A, 718C, 724K, 727A, 737, 744H, 744J, 748, 748G-II, 750J, 750J-II, 753G, 753GH, 753GL, 753J, 753JH, 757, 759G, 759GH, 759J, 759JH, 764, 770D, 770G, 772D, 772G, 777, 797, 824J, 824K, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 870D, 870G, 872D, 872G, 904 P, 944 X, 944K, 950K, 997, 1050K, 1050K PL, 1420, 1435, 1445, 1545, 1565, 1900, 1910, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2204, 2254, 2256, 2258, 2264, 2266, 2266E, 2510C, 2510S, 2653B, 3025D, 3029HFC03, 3029HFG03, 3029HFG80, 3029HG530, 3029HI530, 3032E, 3033R, 3035D, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3756G, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4044M, 4044R, 4045HI551, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4075R, 4720, 4730, 4830, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5045E, 5050E, 5055E, 5060E, 5065E, 5065M, 5067E, 5075E, 5075M, 5085M, 5090M, 5090R, 5100M, 5100R, 5115M, 5115R, 5125R, 5220, 5225, 5320, 5325, 5325N, 5405, 5420, 5520, 6068HFN50, 6068HFN51, 6080A E-CUT, 6080A PRECISIONCUT, 6081AF001, 6081HF001, 6081HF070, 6081HFN02, 6081HFN04, 6081TF001, 6125HF070, 6135CI550, 6135HF475, 6135HFC09, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6500A E-CUT, 6500A PRECISIONCUT, 6700A E-CUT, 6700A PRECISIONCUT, 7185J, 7195J, 7200, 7200A, 7200J, 7205J, 7210J, 7210R, 7215J, 7225J, 7230J, 7230R, 7250, 7250R, 7270R, 7280, 7290R, 7300, 7310R, 7350, 7380, 7400, 7400A, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7550, 7580, 7630, 7660, 7700, 7700A E-CUT, 7700A PRECISIONCUT, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7815, 7820, 7830, 7850, 7920, 7930, 8000, 8000A E-CUT, 8100, 8200, 8300, 8310RT, 8320RT, 8335RT, 8345RT, 8360RT, 8370RT, 8400, 8500, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9120, 9220, 9320, 9320T, 9330, 9370R, 9400, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9650, 9660 STS, 9670, 9670 STS, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, A400, C6R, C6R PRECISION UPGRADES, C8R, C8R PRECISION UPGRADES, C12R, C12R PRECISION UPGRADES, C16R, C16R PRECISION UPGRADES, C18R, C18R PRECISION UPGRADES, C650, C670, CP690, CS690, CTS, CTS II, E210, E210LC, E230, E230-II, FR21B, FR22B, FR24B, FR50, GX85, H260, H360, H380, HD35F, HD40F, HD45F, HD50F, HPX 4X2, HPX 4X4, HPX 4X4 TRAIL, S430, S440, S540, S550, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, STRAIGHT BLADE, SX85, T550, T560, T660, T670, TC44H, TC54H, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, Z510A, Z520A, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930R, Z950A, Z960A, Z970A</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
@@ -2786,6 +3531,11 @@
           <t>19M8125</t>
         </is>
       </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 370E, 410E, 450D, 460E, 625D, 630D, 635D, 650D, 703JH, 725D, 730D, 735D, 737, 753J, 753JH, 757, 759J, 759JH, 777, 797, 803M, 803MH, 824K, 844K, 850D, 853M, 853MH, 859M, 859MH, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 950J, 953K, 953M, 953MH, 959K, 959M, 959MH, 959ML, 1050J, 1050K, 1270D, 1270E, 1270G, 1470D, 1470E, 1470G, 1710D, 1711D, 1775NT, 1795, 1900, 1910E, 2230FH, 2230LL, 2330, 2660VT, 2704, 2854, 2904, 3004, 3204, 3520, 3522, 4024HF285, 4024TF220, 4024TF270, 4024TF280, 4024TF281, 4930, 4940, 5030HF220, 5030HF270, 5030TF220, 5030TF270, 6068HFS89, 6090HF475, 6090HF485, 6090HFG84, 6090HFL75, 6090HFL85, 6135HF485, 6135HFC48, 7180, 7200R, 7210R, 7215R, 7230R, 7250, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7350, 7380, 7450, 7480, 7550, 7580, 7660, 7750, 7760, 7780, 8100, 8110, 8130, 8200, 8210, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8410, 8430, 8430T, 8500, 8530, 8600, 8700, 8800, 9330, 9360R, 9370R, 9410R, 9420R, 9420RX, 9430, 9430T, 9460R, 9460RT, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9560, 9560 STS, 9560R, 9560RT, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9620R, 9630, 9630 SCRAPER, 9630T, 9640, 9660, 9660 STS, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, 9870 STS, C670, CH570, CH670, CP48, CP690, CP770, CS690, DB44, DB60, DB66, E330, E360, E400, GX85, HPX615E, R944I, R952I, R962I, R975I, R4040i, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, SX85, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, X394</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
@@ -2793,6 +3543,11 @@
           <t>19M7865</t>
         </is>
       </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>2C-280, 2C-284, 2C-300, 2C-304, 2C-324, 2C-350, 2C-354, 3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12 PC, 12SB, 13HP, 14PB, 14PZ, 14SB, 14SBS, 14SC, 14SE, 14SX, 14SZ, 15HP, 16HP, 17D, 17G, 20 Trailer, 22B, 26G, 27D, 30 Trailer, 30G, 35D, 35G, 38 IN., 42 IN., 46, 47, 47 IN., 48, 50D, 50G, 54, 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D, 60D IN., 60G, 62 IN., 62 IN. DECKS, 75D, 75G, 80, 85D, 85G, 102, 105, 107, 110, 110 TLB, 115, 120C, 120D, 125, 130 P, 130G, 135, 143, 145, 146, 148, 155C, 158, 160, 160 P, 160C, 160G, 168, 170, 175, 180, 180A, 180B, 180C, 180E, 180G, 180SL, 184 G, 185, 190C, 200, 200 G, 200G, 203C, 204 G, 204C, 204L, 205C, 206C, 207C, 208C, 210C, 210F, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 215F, 215R, 218F, 218R, 220, 220A, 220B, 220C, 220F, 220SL, 222F, 222R, 230C, 240, 240D, 244E, 244H, 244J, 244K, 244K-II, 244L, 245, 245 P, 245G, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260B, 260C, 260E, 260SL, 265, 270, 270D, 280, 285, 290D, 290G, 300, 300D, 300D-II, 300DW, 300G, 300WW, 304, 304H, 304J, 304L, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324E, 324G, 324H, 324J, 324K, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335D, 337E, 344E, 344G, 344H, 344J, 344K, 344L, 345, 345 P, 345G LC, 349, 350, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 354, 355, 359, 360DC, 370B, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400, 400C, 400D, 400D-II, 400R, 404, 408R, 410 P, 410D, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 420, 425, 430, 435, 437D, 437E, 440E, 444 G, 444 P, 444E, 444G, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450, 450C, 450D, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 480, 482C, 484, 485, 485A, 485E, 486E, 488E, 493, 494, 500, 500R, 504, 509, 510D, 520, 520M, 521, 522, 524 P, 524K, 524K-II, 524L, 525, 530, 531, 533, 535, 540, 540A, 540E, 540G-II, 540G-III, 540H, 540M, 540R, 541, 542, 543M, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 554, 555G, 556, 557, 558, 559, 560M, 560R, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 590D, 592, 594, 595D, 600, 600R, 603M, 603R, 604, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608L, 608LH, 608SH, 609, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 615C, 615F, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620G, 620I, 620R, 622, 622F, 622G, 622R, 622X, 623, 623M, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625D, 625F, 625I, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 636M, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 647A, 648E, 648G, 648H, 648HT, 648L, 648L-II, 648M, 648R, 650, 650D, 650G, 650H, 650J, 650K, 651, 652B, 652E, 652M, 652R, 653, 653E, 653G, 654, 655, 655K, 657, 657A, 660R, 661, 661R, 663, 663R, 667, 667A, 670, 670 P, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 673, 676, 678, 680R, 683, 683R, 690E, 692, 693, 694, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 709, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 720, 721, 722PF, 722X, 724 P, 724J, 724K, 724L, 725, 725D, 725PF, 725X, 726, 727, 727A, 730, 730D, 730LL, 730PF, 730X, 731, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770C II, 770CH II, 770D, 770G, 772CH II, 772D, 772G, 777, 790, 792D, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 840, 842, 843, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 862, 864, 870, 870 P, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 913, 915F, 915R, 916, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 940, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 994, 995, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1030, 1040, 1050K, 1050K PL, 1054, 1070, 1070D, 1070E, 1070G, 1092, 1107, 1109, 1110D, 1110E, 1110G, 1111, 1113, 1140, 1165, 1170, 1170E, 1170G, 1175, 1200A, 1210E, 1210G, 1270E, 1270G, 1290, 1291, 1293, 1295, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1465, 1470, 1470E, 1470G, 1490D, 1505, 1510E, 1510G, 1515, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1560, 1565, 1570, 1575, 1580, 1585, 1590, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1640, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1700, 1700T, 1705, 1705T, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1742GS, 1742HS, 1742PR, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1800, 1810, 1820, 1830, 1835, 1840, 1846, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1905, 1910, 1910E, 1910G, 1950, 1950N, 1990, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2040, 2040S, 2046HV, 2054, 2056, 2058, 2064, 2066, 2104, 2140, 2144G, 2150, 2154G, 2155, 2156G, 2204, 2210, 2243, 2250, 2254, 2255, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2350, 2355, 2355N, 2400 PRECISIONCUT, 2450, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2520, 2550, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2555, 2650, 2653, 2653A, 2653B, 2654G, 2656G, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2750, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2755, 2850, 2854, 2904, 2950, 2954D, 2955, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF120, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG80, 3029HFG89, 3029HFU20, 3029HFU80, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF158, 3029TF270, 3029TFG20, 3029TFG80, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU80, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3040, 3043D, 3045B, 3045R, 3046R, 3050, 3050B, 3055, 3110, 3120, 3140, 3150, 3154G, 3155, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3255, 3310, 3320, 3325, 3350, 3365, 3375, 3400, 3410, 3420, 3510, 3520, 3522, 3640, 3650, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4010, 4020DF101, 4020TF006, 4020TF105, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4035B, 4039D, 4039DF001, 4039DF008, 4039DF092, 4039T, 4039TF001, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045D, 4045DF001, 4045DF120, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF287, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF001, 4045TF120, 4045TF150, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4239TF001, 4250, 4300, 4310, 4320, 4400, 4410, 4450, 4475, 4500, 4510, 4520, 4600, 4610, 4650, 4700, 4710, 4720, 4730, 4830, 4850, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055B, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075GL, 5075GN, 5075GV, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085GL, 5085GN, 5085GV, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GL, 5090GN, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GL, 5100GN, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105GF, 5105GN, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5575, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF150, 6068DFM01, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF250, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM01, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081AFM01, 6081AFM75, 6081HF070, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6675, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7775, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8820, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, A420R, A520R, B25C, B35C, B40C, B350, B550, B554, BP15, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E12, E15, E100, E110, E120, E130, E140, E150, E160, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, FC20M, FC20R, G15, G110, GROUPER, GS25, GS30, GS45, GS75, GT242, GT245, GT262, GT275, GX85, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX10, HX14, HX15, HX20, JS61, JS63, JS63C, L60, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX277, LX279, LX280, LX288, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M15, M20, M4030, M4040, M4040DN, MaxEmerge XP, MCS, MX8, MX10, MX15, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PC4, PC7, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R15, R20, R40, R230, R400, R450, R500, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S140, S160, S170, S180, S220, S240, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2546, SPRAYER PERFORMANCE UPGRADES, SST16, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TE 4X2, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W36M, W36R, W48M, W48R, W50, W52R, W61R, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WG32A, WG36A, WG48A, WH36A, WH48A, WH52A, WH61A, WHP36A, WHP48A, WHP52A, WHP61A, WL53, WL56, X9 1000, X9 1100, X110, X120, X125, X135R, X140, X145, X155R, X165, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z425, Z435, Z445, Z465, Z510A, Z520A, Z540M, Z540R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
@@ -2800,6 +3555,11 @@
           <t>03M7184</t>
         </is>
       </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17HP, 20 Trailer, 22 in., 26, 30 IN., 30 Trailer, 30R, 31C, 38 IN., 42 IN., 46R, 47 IN., 48 IN., 50 in., 52 IN., 54, 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 62 IN., 62 IN. DECKS, 72, 72 IN., 100, 102, 105, 107, 108, 110 TLB, 111, 112L, 115, 120C, 125, 135, 145, 155C, 160C, 170, 175, 180, 180A, 180B, 180C, 180E, 180SL, 185, 190C, 200, 203C, 204C, 205C, 206C, 207C, 208C, 209F, 210F, 210K, 210K EP, 210L, 210L EP, 210LJ, 213F, 215F, 215R, 218F, 218R, 220, 220A, 220B, 220C, 220F, 220SL, 222F, 222R, 228, 228A, 240, 243, 244, 245, 246, 250, 260, 260B, 260C, 260SL, 265, 270, 280, 285, 310L, 310L EP, 310SL, 312GR, 313, 314G, 315, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 325, 325G, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 343, 344, 345, 349, 355, 359, 360, 375, 381, 385, 388, 390, 410L, 415, 420, 425, 430, 435, 440E, 443, 444, 444 P, 444K, 444L, 445, 446, 447, 448, 449, 450, 450E, 450M, 454, 455, 456, 457, 458, 459, 459E, 460, 460M, 460R, 460S, 466, 467, 468, 469, 475, 490, 493, 494, 500R, 520M, 524 P, 524K, 524K-II, 524L, 525, 530, 531, 533, 535, 540M, 540R, 543, 543R, 544 P, 544K, 544K-II, 544L, 545, 546, 547, 550, 550M, 551, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 600L HIGH DUMP, 600R, 600T, 603R, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620I, 620PF, 620R, 622, 622F, 622PF, 622R, 622X, 623, 623R, 624 P, 624K, 624K-II, 624KR, 624L, 625, 625D, 625F, 625I, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 639, 640C, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640R, 640X, 643, 643R, 644, 644 P, 644 X, 644K, 644K HYBRID, 644L, 644LH, 645, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 647A, 648R, 649, 651, 652B, 652E, 652R, 653, 654, 655, 657, 657A, 659, 660, 660R, 661, 661R, 663, 663R, 665, 667, 667A, 670, 670D, 670G, 672D, 672G, 673, 676, 678, 680, 680R, 681, 683, 683R, 686, 690, 692, 693, 694, 696, 698, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724 P, 724K, 724L, 725D, 725PF, 725X, 727, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 731, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740PF, 740X, 741, 744, 744 P, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 750A, 751, 753, 755, 756, 757, 764, 770, 770D, 770G, 772, 772D, 772G, 777, 778, 780, 785, 797, 800, 824 P, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 840, 842, 843, 844, 844 P, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 852, 853, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 862, 864, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 903M, 904 P, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 953M, 953MH, 953ML, 955, 956, 959M, 959MH, 959ML, 960, 990, 994, 995, 997, 1010, 1015, 1023E, 1025R, 1026R, 1030, 1035, 1092, 1107, 1109, 1111, 1113, 1165, 1175, 1243, 1290, 1291, 1293, 1295, 1340, 1350, 1354, 1355, 1360, 1365, 1404, 1420D, 1424, 1424C, 1425D, 1430D, 1434, 1434C, 1435D, 1438GS, 1438HS, 1440D, 1442, 1445D, 1450, 1460, 1465, 1470, 1504, 1505, 1512FX, 1516FX, 1524FX, 1535, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1550, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1690, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1900, 1910, 1948GV, 1948HV, 1990, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2148HV, 2155, 2230FH, 2230LL, 2250, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2330, 2354, 2355, 2355N, 2400 PRECISIONCUT, 2450, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510C, 2510H, 2510S, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2555, 2650, 2653, 2653A, 2653B, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2755, 2850, 2955, 3025E, 3032E, 3033R, 3036E, 3038E, 3038R, 3039R, 3040, 3045R, 3046R, 3050, 3055, 3120, 3140, 3150, 3155, 3203, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3255, 3316, 3320, 3325, 3350, 3365, 3420, 3520, 3522, 3640, 3650, 3720, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4200, 4300, 4320, 4400, 4520, 4600, 4700, 4720, 4730, 4830, 4890, 4895, 4920, 4990, 4995, 5050E, 5055E, 5058E, 5060E, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080M, 5080R, 5082E, 5083E, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100R, 5101E, 5105M, 5105ML, 5115M, 5115R, 5115RH, 5125M, 5125R, 5210, 5215, 5220, 5225, 5300N, 5310, 5315, 5320, 5325, 5400, 5405, 5410, 5415, 5420, 5425, 5500N, 5510, 5515, 5515 HIGH CROP, 5520, 5525, 5603, 5615, 5620, 5625, 5715, 5720, 5725, 5820, 6010, 6020, 6080A E-CUT, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6095B, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6103, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130M, 6130R, 6135B, 6135E, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140J, 6140M, 6140R, 6145M, 6145R, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6190M, 6190R, 6195M, 6195R, 6200L, 6210, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500A E-CUT, 6500L, 6510, 6510L, 6510S, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6710, 6715, 6750, 6810, 6820, 6830, 6830 Premium, 6850, 6910, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7200, 7200A, 7200R, 7210, 7210R, 7215R, 7220, 7230, 7230 Premium, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7410, 7420, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7510, 7520, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8600, 8700, 8760, 8800, 8800A, 8900A, 8960, 9009A, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, A420R, A520R, AMT600, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C310R, C350, C350R, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C670, CH570, CH670, CH950, CH960, CP20, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E100, E110, E120, E130, E140, E150, E160, E170, E180, F310R, F350R, F440M, F440R, F441M, F441R, F510, F525, F620, F680, F687, F710, F725, F735, F910, F911, F915, F925, F930, F932, F935, F1145, G15, G100, G110, GROUPER, GS25, GS30, GS45, GS75, GT225, GT242, GT245, GT262, GT275, GX85, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L17.542, L50, L60, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, L1742, L2048, L2548, L2554, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M-GATOR A3, M-GATOR A3T, M653, M655, M665, MaxEmerge XP, MCS, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R310R, R400, R450, R500, R962I, R4040i, R4050i, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S140, S160, S170, S180, S200, S220, S240, S250, S300, S310R, S350, S350R, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2048, S2348, S2546, S2554, SH8R, SH12F, SH12R, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TE 4X2, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W36R, W48M, W48R, W50, W52R, W61R, W70, W80, W100, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, X9 1000, X9 1100, X105, X106, X107, X110, X120, X125, X126, X127, X135R, X140, X145, X155R, X165, X166, X167, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z425, Z435, Z445, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
@@ -2807,6 +3567,11 @@
           <t>19M7866</t>
         </is>
       </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>2C-280, 2C-284, 2C-300, 2C-304, 2C-324, 2C-350, 2C-354, 3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 04, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17 ZTS, 17D, 17G, 17HP, 20 Trailer, 26, 26G, 27 ZTS, 27C ZTS, 27D, 30 Trailer, 30G, 35C, 35D, 35G, 35ZTS, 42 IN., 46, 47, 47 IN., 48, 48 IN., 50C, 50D, 50G, 50ZTS, 52 IN., 54, 54 in., 54 IN. FRONT BLADE, 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 60G, 62 IN., 62 IN. DECKS, 72 IN., 75C, 75D, 75G, 80, 80C, 85D, 85G, 102, 105, 107, 110, 110 TLB, 112R, 115, 120C, 120D, 125, 130 P, 130G, 135, 135 P, 135C, 135D, 135G, 145, 146, 155C, 160, 160 P, 160C, 160D, 160G, 170, 175, 180, 180A, 180B, 180C, 180C W, 180E, 180G, 180SL, 185, 190C, 190DW, 190GW, 200, 200 G, 200C, 200D, 200G, 203C, 204 G, 204C, 204K, 204L, 205C, 206C, 207C, 208C, 210C, 210C W, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 215F, 215R, 218F, 218R, 220, 220A, 220B, 220C, 220DW, 220F, 220SL, 222F, 222R, 225C, 225D, 230C, 230GW, 240, 240D, 243, 244, 244E, 244H, 244J, 244K, 244K-II, 244L, 245, 245 P, 245G, 246, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260B, 260C, 260E, 260SL, 265, 270, 270A, 270B, 270C, 270D, 280, 285, 290G, 300, 300C, 300D, 300D-II, 300DW, 300E, 300G, 300WW, 304, 304H, 304J, 304K, 304L, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 314R, 315, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324E, 324G, 324H, 324J, 324K, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330C, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 343, 344, 344G, 344H, 344J, 344K, 344L, 345, 345 P, 345G LC, 350, 350 P, 350C, 350D, 350D-II, 350DW, 350G, 354, 355, 360DC, 370, 370B, 370C, 370E, 370E-II, 375, 375A, 380 P, 380G, 385, 385A, 400, 400C, 400D, 400D-II, 400E, 400R, 404, 408R, 410 P, 410D, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 420, 425, 430, 435, 435C, 437C, 437D, 437E, 440E, 443, 444, 444 G, 444 P, 444G, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450, 450C, 450D, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 480, 484, 485, 485A, 485E, 486E, 488E, 490, 490E, 493, 494, 500, 500R, 504, 510D, 512, 521, 522, 524 P, 524K, 524K-II, 524L, 525, 530, 531, 533, 535, 540A, 540G-II, 540G-III, 540H, 540M, 540R, 541, 542, 543, 543M, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 600, 600C, 600R, 603M, 603R, 604, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 623M, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625D, 625F, 625I, 625PF, 625R, 625X, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 636M, 639, 640, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645, 645FD, 645FD PERFORMANCE UPGRADES, 647A, 648G, 648H, 648HT, 648L, 648L-II, 648M, 648R, 649, 650, 650D, 650G, 650H, 650J, 650K, 651, 652E, 652M, 652R, 653, 653E, 653G, 654, 655, 655K, 657A, 659, 660R, 661, 661R, 663, 663R, 667A, 670, 670 P, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 673, 678, 680R, 683, 683R, 690E, 692, 693, 694, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 700M, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 720, 721, 722PF, 722X, 724 P, 724J, 724K, 724L, 725, 725D, 725PF, 725X, 726, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 730PF, 730X, 731, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753, 753J, 753JH, 755, 755D, 755K, 756, 757, 759J, 759JH, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772, 772CH, 772CH II, 772D, 772G, 777, 790, 790E, 792D, 797, 800C, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 840, 842, 843, 843G, 843H, 843J, 843K, 843L, 843L-II, 844, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850, 850C, 850D, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 862, 864, 870, 870 P, 870D, 870G, 872D, 872G, 890, 891, 892, 892E, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920D, 920F, 920R, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 994, 995, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1030, 1035, 1050, 1050E, 1050K, 1050K PL, 1054, 1070, 1070D, 1070E, 1070G, 1092, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1200A, 1210E, 1210G, 1243, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1295, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1505, 1510DC, 1510E, 1510G, 1512FX, 1515, 1516FX, 1524FX, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1700, 1705, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810DC, 1812DC, 1814DC, 1820, 1830, 1835, 1840, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1850, 1854, 1854J, 1870, 1890, 1895, 1900, 1903, 1905, 1910, 1910E, 1910G, 1948GV, 1948HV, 1990, 2010DE, 2014DE, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2104, 2112DC, 2144G, 2148HV, 2154D, 2154G, 2155, 2156G, 2204, 2210, 2230FH, 2230LL, 2243, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2330, 2354, 2355N, 2400 PRECISIONCUT, 2412DE, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2510S, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653, 2653A, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3120, 3154G, 3156G, 3200, 3203, 3204, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3316, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 3950, 3955, 3970, 3975, 4005, 4010, 4020DF101, 4020TF006, 4020TF105, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4035B, 4039D, 4039DF001, 4039DF004, 4039DF005, 4039DF006, 4039DF008, 4039DF031, 4039DF032, 4039DF092, 4039T, 4039TF001, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045D, 4045DF001, 4045DF120, 4045DF150, 4045DF154, 4045DF158, 4045DF271, 4045DFM50, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF287, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS73, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045T, 4045TF001, 4045TF120, 4045TF150, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF250, 4045TF253, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFU20, 4045TFU70, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4475, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055B, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5575, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6059TF, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF150, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HT087, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081AFH75, 6081AFM75, 6081HF070, 6081HFH70, 6081HFN02, 6081HFN03, 6081HFN04, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6675, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7775, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8560, 8570, 8600, 8700, 8760, 8770, 8800, 8800A, 8870, 8875, 8900A, 8960, 8970, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, B25C, B30C, B35C, B40C, B350, B550, B554, BP15, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E100, E110, E120, E130, E140, E150, E160, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F620, F680, F687, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FL100, G15, G100, G110, GROUPER, GS25, GS30, GS45, GS75, GT225, GT242, GT245, GT262, GT275, GX85, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, H480, H541, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX15, HX20, L60, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L624, L633, L634, L1524, L1533, L1534, L2554, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MCS, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, P540, P556, P576, PC4, PC7, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R400, R450, R500, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S140, S160, S170, S180, S220, S240, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2048, S2348, S2546, S2554, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W50, W61R, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W440, W540, W550, W650, W660, WG32A, WG36A, WG48A, WL53, WL56, X9 1000, X9 1100, X105, X106, X110, X115R, X116R, X117R, X120, X125, X130R, X135R, X140, X145, X146R, X147R, X155R, X165, X166R, X167R, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z425, Z435, Z445, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
@@ -2814,6 +3579,11 @@
           <t>19M7867</t>
         </is>
       </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17HP, 20 Trailer, 27D, 30 IN., 30 Trailer, 30G, 30R, 31C, 35G, 38 IN., 42 IN., 46R, 47 IN., 48 IN., 50 in., 50D, 50G, 52 IN., 54, 54 in., 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 60G, 62 IN., 62 IN. DECKS, 72 IN., 74 IN., 84 IN., 102, 105, 107, 108, 110, 110 TLB, 111, 112L, 112R, 115, 120C, 120D, 120R, 125, 130 P, 130G, 135, 145, 155C, 160, 160 P, 160C, 160D, 160G, 180, 180A, 180B, 180C, 180E, 180G, 180SL, 185, 190C, 200, 200 G, 200C, 200D, 200G, 203C, 204C, 204L, 205C, 206C, 207C, 208C, 210C, 210F, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 220, 220A, 220B, 220C, 220R, 220SL, 230C, 240, 240D, 243, 244, 244E, 244J, 244L, 245, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260B, 260C, 260E, 260SL, 265, 270, 270C, 270D, 280, 285, 290G, 300D, 300D-II, 300DW, 300E, 300G, 300WW, 304J, 304L, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 324J, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335, 335C, 335D, 337E, 343, 344, 344G, 344H, 344J, 344K, 344L, 345, 350 P, 350D, 350D-II, 350DW, 350G, 355, 360DC, 365, 366, 370E, 370E-II, 375, 380, 380 P, 380A, 380G, 385, 390, 400D, 400D-II, 400E, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 420, 425, 430, 435, 435C, 437C, 437D, 437E, 440E, 440R, 443, 444, 444 G, 444 P, 444G, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 460S, 466, 467, 468, 469, 470 P, 470G, 475, 482C, 485E, 486E, 488E, 493, 494, 500R, 520M, 524 P, 524K, 524K-II, 524L, 525, 530, 530B, 531, 533, 535, 540A, 540E, 540G-II, 540G-III, 540H, 540M, 540R, 543, 543M, 543R, 544 G, 544 P, 544E, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 553, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 600R, 603M, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 606SH, 607C, 608BH, 608C, 608C PERFORMANCE UPGRADES, 608FC, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 623M, 623R, 624 P, 624E, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625D, 625F, 625I, 625PF, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 636M, 639, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640R, 640X, 643, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643M, 643R, 644, 644 G, 644 P, 644 X, 644E, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 647A, 648E, 648G, 648H, 648HT, 648L, 648L-II, 648M, 648R, 649, 650, 650G, 650H, 650J, 650K, 651, 652B, 652E, 652M, 652R, 653, 653E, 653G, 654, 655, 655K, 657A, 659, 660, 660R, 661, 661R, 663, 663R, 665, 667A, 670, 670B, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672B, 672CH, 672D, 672G, 673, 678, 680, 680R, 681, 683, 683R, 690E, 692, 693, 694, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 700M, 703G, 703GH, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724 P, 724J, 724K, 724L, 725D, 725PF, 725X, 727, 727A, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730LL, 730PF, 730X, 731, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740PF, 740X, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 746, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753, 753G, 753GH, 753GL, 753J, 753JH, 755, 755D, 755K, 756, 757, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 777, 790, 797, 800, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843, 843G, 843H, 843J, 843K, 843L, 843L-II, 844, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853G, 853J, 853JH, 853M, 853MH, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 862, 864, 870, 870D, 870G, 872D, 872G, 890, 891, 892, 893, 894, 895, 896, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 944K, 946, 948L, 948L-II, 950, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 994, 995, 997, 1010, 1010D, 1010E, 1010G, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050, 1050K, 1050K PL, 1054, 1070, 1070D, 1070E, 1070G, 1092, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1200, 1200A, 1200H, 1210E, 1210G, 1243, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1295, 1312C, 1350, 1354, 1360, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1470, 1470D, 1470E, 1470G, 1490D, 1505, 1510C, 1510DC, 1510E, 1510G, 1512C, 1512E, 1512FX, 1515, 1516FX, 1524FX, 1530, 1535, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1560, 1565, 1570, 1575, 1580, 1585, 1590, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1612DE, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1700, 1700T, 1705, 1705T, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1800, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1830, 1835, 1840, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1905, 1910, 1910E, 1910G, 1948GV, 1948HV, 1990, 2010DE, 2014DE, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2104, 2109, 2111, 2112C, 2112DC, 2112E, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2148HV, 2154D, 2154G, 2156G, 2204, 2210, 2230FH, 2230LL, 2243, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2330, 2354, 2400 PRECISIONCUT, 2410C, 2412DE, 2430, 2430C, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653, 2653A, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2730, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF120, 3029DF124, 3029DF128, 3029DF129, 3029DF150, 3029DF151, 3029DF160, 3029DF180, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HF270, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG80, 3029HFG89, 3029HFU20, 3029HFU80, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF152, 3029TF158, 3029TF160, 3029TF180, 3029TF270, 3029TFG20, 3029TFG80, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU80, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4010, 4020DF101, 4020TF006, 4020TF105, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4475, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5575, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6081AF001, 6081AFH75, 6081AFM75, 6081HF001, 6081HF070, 6081HFH70, 6081HFN02, 6081HFN04, 6081TF001, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6675, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7775, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, A420R, A520R, B25C, BA72C, BA84C, BA96C, BL6, BL7, BL8, BL9, BL10, BP15, BP72C, BP84C, BR60C, BR72C, BR84C, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C400, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB84, DB88, DB90, DB96, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, E130, E140, E150, E160, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F620, F680, F687, F710, F725, F735, F912, F925, F932, F935, F1145, F4365, G15, G100, G110, GR66B, GR72B, GR78B, GR84B, GROUPER, GS25, GS30, GS45, GS66, GS66B, GS72, GS72B, GS75, GS78, GS78B, GS84, GS84B, GS88, GT72, GT80, GT225, GT242, GT245, GT262, GT275, GU60, GU66, GU72, GU78, GX85, GX255, GX325, GX335, GX345, GX355, H180, H240, H260, H310, H340, H360, H380, H480, H540F, H541, H550, H550F, H560F, H561, HB15, HB30, HB50, HB60, HB75, HB85, HB100, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HH30, HH50, HH75, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L17.542, L60, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L624, L634, L1524, L1533, L1534, L2554, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LP72, LP78, LP84, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX280, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M653, M655, M665, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MCS, MP66, MP66B, MP72, MP72B, MP78, MP78B, MP84, MP84B, MS60, MS72, MS84, MS96, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, P540, P556, P576, PC4, PC7, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R40, R230, R400, R450, R500, R944I, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RB72, RB84, RB96, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, ROW-CROP HARVESTING UNITS, RSX 850I, RSX860E, RSX860I, RSX860M, S130, S140, S160, S170, S180, S240, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2048, S2348, S2546, S2554, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W36M, W36R, W48M, W48R, W50, W52R, W61R, W70, W80, W100, W150, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W440, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X110, X115R, X116R, X117R, X120, X125, X130R, X135R, X140, X145, X146R, X147R, X155R, X165, X166, X166R, X167, X167R, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z375R, Z425, Z435, Z445, Z465, Z515E, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
@@ -2821,6 +3591,11 @@
           <t>19M7868</t>
         </is>
       </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>2C-280, 2C-284, 2C-300, 2C-304, 2C-324, 2C-350, 2C-354, 3-Bag, 3B-554, 3B-604, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6A-1104, 6A/1204, 6A/1354, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17HP, 20 Trailer, 26, 26G, 27D, 30 Trailer, 30G, 35D, 35G, 38 IN., 40, 42, 46, 47, 47 IN., 48, 48 IN., 50D, 50G, 52 IN., 54, 54 in., 54 IN. FRONT BLADE, 54 IN. HEAVY DUTY SNOWBLOWER, 54D IN., 59 IN., 60, 60 in., 60 IN. DECKS, 60 IN. HEAVY DUTY SNOWBLOWER, 60D IN., 60G, 62 IN., 62 IN. DECKS, 72 IN., 75G, 80, 85G, 107, 108, 110, 110 TLB, 111, 112L, 120C, 120D, 120R, 130 P, 130G, 135D, 160, 160 P, 160C, 160D, 160G, 170, 175, 180, 180B, 180C, 180E, 180G, 180SL, 184 G, 185, 200, 200 G, 200C, 200D, 200G, 203C, 204 G, 204K, 204L, 206C, 207C, 208C, 210G, 210K, 210K EP, 210L, 210L EP, 210LJ, 215F, 215R, 218F, 218R, 220, 220B, 220C, 220F, 220R, 220SL, 222F, 222R, 230C, 240, 240D, 243, 244, 244H, 244J, 244K-II, 244L, 245, 246, 250, 250C, 250D, 250D-II, 250G, 260, 260 P, 260B, 260C, 260E, 260SL, 265, 270, 270A, 270B, 270C, 270D, 280, 285, 290G, 300, 300C, 300D, 300D-II, 300DW, 300E, 300G, 300WW, 304, 304H, 304J, 304K, 304L, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324, 324E, 324G, 324H, 324J, 324K, 324L, 325, 325G, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330C, 330G, 331G, 332, 332D, 332E, 332G, 332T, 333D, 333E, 333G, 335, 335C, 335D, 337E, 338, 339, 343, 344, 344H, 344J, 344K, 344L, 345, 348, 349, 350 P, 350D, 350D-II, 350DW, 350G, 355, 359, 360DC, 370B, 370C, 370E, 370E-II, 375, 375A, 380 P, 380G, 385A, 400D, 400D-II, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 425, 435, 435C, 437C, 437D, 437E, 440E, 443, 444, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450C, 450E, 450G, 450H, 450J, 450K, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 485, 485A, 493, 494, 500R, 524 P, 524K, 524K-II, 524L, 530, 530B, 531, 535, 540A, 540E, 540G-II, 540G-III, 540H, 543, 543R, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 545, 546, 547, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 551, 554, 555G, 556, 557, 558, 559, 560M, 560R, 562, 563, 566, 567, 568, 569, 570, 572, 578, 580, 582, 590, 592, 594, 600R, 603R, 604C, 605C, 605K, 606C, 607C, 608C, 608FC, 609C, 610C, 611C, 612C, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 615C, 615F, 616C, 616R, 617C, 618F, 618R, 620F, 620G, 620I, 620R, 622F, 622G, 622R, 623, 623R, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625R, 630C, 630D, 630F, 630R, 630X, 631, 635D, 635F, 635FD, 636M, 640, 640C, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643, 643D, 643G, 643H, 643J, 643K, 643L, 643L-II, 643R, 644, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645, 645C, 647, 647A, 648E, 648G, 648H, 648HT, 648L, 648L-II, 648M, 648R, 650, 650G, 650H, 650J, 650K, 651, 652B, 652E, 652M, 652R, 653, 653E, 653G, 654, 655, 655K, 657, 657A, 661, 661R, 663R, 667, 667A, 670, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 673, 678, 683R, 690E, 692, 693, 694, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 708FC, 710D, 710G, 710J, 710K, 710L, 712FC, 712FC PERFORMANCE UPGRADES, 717, 717A, 724 P, 724J, 724K, 724L, 727, 727A, 730, 731, 735, 737, 740, 740A, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748, 748E, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 751, 753J, 753JH, 755, 755D, 755K, 756, 757, 759J, 759JH, 764, 768L-II, 770, 770C, 770C II, 770CH, 770CH II, 770D, 770G, 772CH, 772CH II, 772D, 772G, 777, 790, 797, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 830, 835, 835 SHORT CHASSIS, 842, 843, 843G, 843H, 843J, 843K, 843L, 843L-II, 844, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853, 853J, 853JH, 853M, 853MH, 854, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 862, 864, 870, 870D, 870G, 872D, 872G, 890, 892, 893, 894, 895, 896, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 912, 913, 914, 915F, 918, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930D, 930F, 930R, 936D, 944K, 946, 948L, 948L-II, 950, 950K, 953J, 953K, 953M, 953MH, 953ML, 955, 956, 959J, 959K, 959M, 959MH, 959ML, 960, 970, 990, 997, 1010, 1010D, 1010E, 1010G, 1023E, 1025, 1025R, 1026R, 1030, 1035, 1050, 1050K, 1050K PL, 1070, 1070D, 1070E, 1070G, 1092, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1200A, 1200H, 1210E, 1210G, 1243, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1504, 1505, 1510E, 1510G, 1512FX, 1515, 1516FX, 1524FX, 1530, 1535, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1560, 1565, 1570, 1575, 1580, 1585, 1590, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1700, 1700T, 1705, 1710D, 1711D, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1800, 1830, 1835, 1846, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1903, 1905, 1910, 1910E, 1910G, 1990, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2054, 2056, 2058, 2064, 2066, 2104, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2144G, 2154D, 2154G, 2156G, 2204, 2210, 2243, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2400 PRECISIONCUT, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2510H, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2653, 2653B, 2654G, 2656G, 2660VT, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF120, 3029DF128, 3029DF129, 3029DF150, 3029DF160, 3029DF180, 3029DFG20, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF120, 3029TF129, 3029TF150, 3029TF158, 3029TF160, 3029TF180, 3029TFG89, 3029TFU20, 3029TFU29, 3029TFU89, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3554, 3720, 3754D, 3754G, 3756G, 3800, 3950, 3955, 3970, 3975, 4005, 4020DF101, 4020TF006, 4020TF105, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF004, 4039DF005, 4039DF006, 4039DF008, 4039DF031, 4039DF032, 4039DF092, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4239A, 4239D, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4475, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5300N, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5575, 5600, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5700, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6059TF, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6076AFM00, 6076AFM30, 6080A E-CUT, 6081AF001, 6081AFM75, 6081HF001, 6081HF070, 6081TF001, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6103, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500, 6500A E-CUT, 6500L, 6506, 6510, 6510L, 6510S, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6675, 6700, 6710, 6715, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7775, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, B25C, B30C, B350, BUCK 500, BUCK 650, BUCK EX, BUCK EXT, C2 400, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C300, C350, C440, C440R, C441R, C450, C451R, C461R, C500, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, CX15, CX20, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, E18ZS, E60, E68, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F440M, F440R, F441M, F441R, F510, F525, F710, F725, F735, F910, F911, F912, F915, F925, F930, F932, F935, F1145, F4365, FL100, GROUPER, GS25, GS30, GS45, GS75, GT242, GT262, GT275, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, H480, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45, HD45F, HD45R, HD45X, HD50F, HD50R, HD75, HD200, HD300, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, HX15, HX20, L60, L70, L331, L341, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX277, LX279, LX280, LX289, M-GATOR A1, M-GATOR A3, M-GATOR A3T, M655, M665, M4025, M4030, M4040, M4040DN, MaxEmerge XP, MX15, N530C, N536C, N540C, N540F, N542C, N543F, N550, N560, P540, P556, P576, PC4, PC7, PLANTER PERFORMANCE UPGRADES, Pro-Series XP, R10, R40, R230, R400, R450, R500, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, RSX 850I, RSX860E, RSX860I, RSX860M, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2546, SH8R, SH12F, SH12R, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, STX46, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TRAIL BUCK 500, TRAIL BUCK 650, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W36M, W36R, W48M, W48R, W50, W52R, W61R, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WG32A, WG36A, WG48A, WH36A, WHP36A, WHP48A, WHP52A, WL53, WL56, X9 1000, X9 1100, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X384, X390, X394, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z425, Z435, Z445, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
@@ -2828,6 +3603,11 @@
           <t>03M7188</t>
         </is>
       </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>3-Bag, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7H17, 7M 200, 7M 215, 7M 230, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12 PC, 12.5HP, 12SB, 13HP, 14HP, 14PB, 14PZ, 14SB, 14SBS, 14SC, 14SE, 14SX, 14SZ, 15HP, 16HP, 17HP, 42 IN., 47 IN., 48 IN., 54, 54 IN. FRONT BLADE, 54D IN., 60, 60 IN. DECKS, 60D IN., 62 IN., 180, 180A, 180B, 180C, 220A, 220B, 220C, 240, 245, 260, 260B, 260C, 265, 270, 280, 285, 310 P, 310K, 310L, 312GR, 313, 314G, 315, 316GR, 317G, 318G, 319E, 320, 320G, 323E, 324G, 325, 325G, 326E, 328, 328E, 329E, 330G, 331G, 332, 332E, 332G, 333E, 333G, 335, 345, 440E, 449, 450, 450E, 450M, 455, 459, 459E, 460M, 460R, 469, 550M, 559, 560M, 560R, 569, 615F, 616, 616F, 616R, 618, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 625D, 625F, 625R, 630, 630D, 630F, 630R, 635, 635D, 635F, 717, 730, 730LL, 737, 750A, 757, 777, 780, 785, 797, 997, 1023E, 1025R, 1026R, 1420, 1435, 1445, 1520, 1538HR, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1590, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1740, 1770NT, 1775NT, 1835, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1890, 1895, 1948GV, 1948HV, 1990, 2026R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2148HV, 2243, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2354, 2400 PRECISIONCUT, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2704, 2854, 2904, 3004, 3025E, 3032E, 3033R, 3036E, 3038E, 3038R, 3039R, 3045R, 3046R, 3204, 3215B, 3225B, 3225C, 3235B, 3235C, 4044M, 4044R, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4075R, 5050E, 5055E, 5058E, 5065E, 5067E, 5075E, 5075EN, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5083EN, 5085M, 5090E, 5090EL, 5090EN, 5090M, 5090R, 5093EN, 5100M, 5100MH, 5100ML, 5100R, 5101EN, 5105ML, 5115M, 5115ML, 5115R, 5125ML, 5125R, 5310N, 5320N, 5325N, 5420N, 5425, 5425N, 5500N, 5510N, 5520N, 5525N, 6110R, 6120R, 6130R, 6135R, 6145R, 6155R, 6155RH, 6175R, 6195R, 6215R, 6230R, 6250R, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7200, 7200R, 7210R, 7215R, 7230R, 7250, 7250R, 7260R, 7270R, 7280R, 7290R, 7300, 7310R, 7350, 7400, 7400A, 7450, 7500, 7550, 7700, 7750, 7800, 7850, 7950, 8100, 8200, 8225R, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8500, 8600, 8700, 8800, 9009A, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, A400, AMT600, C230, C440, C441R, C650, C670, C850, CP770, CS770, CT315, CT332, CTS, CTS II, F441R, F510, F525, F4365, G15, G100, GS25, GS30, GS45, GS75, GT225, GT242, GT245, GT262, GT275, GX85, GX255, GX325, GX335, GX345, GX355, H540F, H550F, H560F, HD45, HD75, JX85, L330, L331, L340, L341, L2554, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M-GATOR A3, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, N560F, R2 300, R230, R450, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, S1642, S2046, S2048, S2348, S2546, S2554, SST15, SST16, SST18, SX85, T550, T560, T660, T670, W200M, W235, W235M, W235R, W260, W260R, W540, W550, W650, W660, X300, X304, X305R, X310, X320, X324, X340, X360, X500, X520, X530, X534, X540, X584, X590, X710, X730, X734, X738, X739, X750, X754, X758, Z235, Z255, Z355E, Z355R, Z375R, Z425, Z435, Z445, Z465, Z510A, Z520A, Z625, Z645, Z655, Z665, Z710A, Z720A, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z910A, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
@@ -2835,6 +3615,12 @@
           <t>19M7800</t>
         </is>
       </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 20 Trailer, 26G, 27D, 30 Trailer, 35D, 50D, 62 IN. DECKS, 110 TLB, 120D, 130 P, 130G, 148, 158, 160 P, 160D, 160G, 168, 180G, 200 G, 200D, 200G, 210 P, 210G, 210K, 210K EP, 210L, 210L EP, 210LJ, 240, 240D, 244E, 244H, 244J, 245, 250, 250 P, 250D, 250D-II, 250G, 260, 260 P, 260E, 270, 270D, 280, 290G, 300 P, 300C, 300D, 300D-II, 300DW, 300G, 300WW, 304J, 310 P, 310E, 310J, 310K, 310K EP, 310L, 310L EP, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315 P, 315J, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320 P, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 324J, 325, 325G, 326D, 326E, 328, 328D, 329D, 330G, 331G, 332, 332D, 332G, 333D, 333G, 335D, 337E, 344 P, 344H, 344J, 344K, 344L, 350C, 350D, 350D-II, 350DW, 355, 360DC, 370E, 400C, 400D, 400D-II, 408R, 410 P, 410E, 410J, 410K, 410L, 410TK TMC, 415, 425, 437D, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 450 P, 450J, 450K, 455, 460 P, 460DC, 460E, 520M, 524 P, 524K, 524K-II, 524L, 525, 530, 535, 540G-II, 540G-III, 540H, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 548G-II, 548G-III, 548H, 550, 550 P, 550J, 550K, 554, 605K, 615F, 618F, 618R, 620F, 620G, 620I, 620R, 622F, 622G, 622R, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625, 625F, 625R, 630, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 648G, 648H, 648HT, 648L, 648L-II, 650, 650 P, 650J, 650K, 654, 655, 655K, 670, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 710 P, 710J, 710K, 710L, 724 P, 724J, 724K, 724L, 730, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 735FD PERFORMANCE UPGRADES, 740FD, 740FD PERFORMANCE UPGRADES, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748G-III, 748H, 748HT, 748L, 748L-II, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755, 755D, 755K, 756, 759J, 759JH, 764, 768L-II, 770, 770D, 770G, 772D, 772G, 790, 803M, 803MH, 810D, 810E, 824J, 824K, 824L, 840, 843J, 843K, 843L, 843L-II, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 848H, 848HT, 848L, 848L-II, 850, 850J, 850J-II, 850JR, 850K, 852, 853JH, 853M, 853MH, 854, 855, 856, 859M, 859MH, 862, 864, 870, 870D, 870G, 872D, 872G, 903JH, 903M, 903MH, 909JH, 909M, 909MH, 910G, 913, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 940, 944 X, 944K, 948L, 948L-II, 950, 950J, 950K, 953M, 953MH, 953ML, 955, 959M, 959MH, 959ML, 970, 990, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1040, 1050, 1050J, 1050K, 1070, 1070D, 1070E, 1070G, 1110D, 1110E, 1110G, 1140, 1170, 1170E, 1170G, 1210E, 1210G, 1350, 1354, 1404, 1410D, 1435, 1445, 1450, 1470, 1490D, 1505, 1510E, 1510G, 1515, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1620, 1640, 1690, 1725C, 1750, 1770, 1770NT, 1775NT, 1840, 1850, 1854, 1854J, 1900, 1905, 1910, 1990, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2038R, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2140, 2144G, 2150, 2154D, 2154G, 2155, 2156G, 2204, 2254, 2255, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2350, 2355N, 2454D, 2500B, 2500E, 2520, 2550, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2653, 2653A, 2653B, 2654G, 2656G, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2750, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2950, 2954D, 2956G, 3004, 3005, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025D, 3025E, 3028EN, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3029WG401, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3040, 3043D, 3045R, 3046R, 3110, 3120, 3140, 3150, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3520, 3522, 3640, 3720, 3754G, 3756G, 3800, 4005, 4020DF101, 4020TF006, 4020TF105, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF271, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF150, 4045HF152, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS73, 4045HFS82, 4045HFS83, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF150, 4045TF151, 4045TF155, 4045TF158, 4045TF220, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFM50, 4045TFM85, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4475, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4930, 4940, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075EN, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5203, 5203S, 5204, 5205, 5210, 5225, 5303, 5305, 5310, 5310N, 5325, 5325N, 5403, 5405, 5410, 5415, 5420, 5425, 5425N, 5430I, 5503, 5510, 5510N, 5520, 5525, 5525N, 5575, 5603, 5605, 5610, 5615, 5620, 5625, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF150, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HT087, 6068HYF01, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF158, 6068TF220, 6068TF250, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM75, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6081AF001, 6081HF001, 6081HF070, 6081TF001, 6090 MC, 6090 RC, 6090HF485, 6090HFC95, 6090M, 6095 MC, 6095 RC, 6095B, 6100, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135B, 6135E, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6400L, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500, 6500L, 6505, 6506, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6675, 6710, 6715, 6750, 6810, 6820, 6830, 6830 Premium, 6850, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7505, 7510, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7730, 7750, 7760, 7775, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8120, 8120T, 8130, 8200, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9986, 9996, A2, A400, B25C, B30C, B35C, B40C, C1 200, C2 300, C2 400, C12F, C16F, C18F, C100, C110, C120, C230, C240, C440, C650, C670, C850, CH330, CH530, CP12C, CP12D, CP18C, CP18D, CP20, CP24C, CP24D, CP30C, CP30D, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, F510, F525, F735, F912, F915, F925, F932, F935, F1145, GROUPER, GX355, H240, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX815E, L60, L331, L341, M-GATOR A1, M4025, M4030, M4040, M4040DN, MH60, MH60C, N530C, N536C, N540C, N542C, PC4, R2 300, R40, R230, R450, R4023, R4030, R4040i, R4050i, R4140i, R4150i, RC60B, RC60L, RC72, RC72B, RC72L, RC78, RC78B, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, RS72, RT52, RT66, S250, S300, S350, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SA60, SA72, SB60, SB60B, SB72, SB72B, SB72H, SB78, SB78B, SB78H, SB84, SB84B, SB84H, SD72, SD84, SPRAYER PERFORMANCE UPGRADES, STRAIGHT BLADE, STX30, STX38, T550, T560, T660, T670, TC44H, TC54H, TC62H, TH 6X4, TH 6X4 D, TS 4X2, TURF TX 4X2, TX 4X2, V451M, V461M, VR66C, VR73C, VR84C, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X465, X475, X485, X495, X575, X585, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, Y110, Y115, Y210, Y215, Z720E, Z730M, Z735E, Z735M, Z740R, Z760R, Z910A, Z915B, Z915E, Z920A, Z920M, Z920R, Z925A, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
@@ -2842,6 +3628,12 @@
           <t>19M7801</t>
         </is>
       </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>3-Bag, 5B-700, 5B-704, 5B-750, 5B-754, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12 PC, 12SB, 13HP, 14PB, 14PZ, 14SB, 14SBS, 14SC, 14SE, 14SX, 14SZ, 15HP, 16HP, 20 Trailer, 27D, 30 IN., 30 Trailer, 35D, 47 IN., 50D, 50G, 54, 60D, 60G, 62 IN. DECKS, 75G, 80, 85G, 105, 107, 108, 110, 110 TLB, 115, 120C, 120D, 125, 130 P, 130G, 135, 145, 155C, 160, 160 P, 160C, 160D, 160G, 180G, 190C, 200, 200 G, 200C, 200D, 200G, 204 G, 204C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 210R, 212R, 222F, 222R, 230C, 240, 240D, 244E, 244H, 244J, 244K, 244K-II, 244L, 250, 250D, 250D-II, 250G, 260, 260 P, 260E, 270, 270C, 270D, 280, 290G, 300D-II, 300DW, 300G, 300WW, 304J, 304L, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324H, 324J, 324K, 324L, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335C, 335D, 337E, 344H, 344J, 344K, 344L, 350D, 350D-II, 350DW, 350G, 355, 360DC, 370E, 370E-II, 380G, 400D, 400D-II, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 420, 435, 435C, 437C, 437D, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 450E, 450G, 450H, 450J, 450K, 450M, 455G, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 469, 470 P, 470G, 485E, 486E, 488E, 524 P, 524K, 524K-II, 524L, 530, 535, 540A, 540G-II, 540G-III, 540H, 540M, 540R, 543R, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 545, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 550M, 554, 555G, 560M, 560R, 565, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 600R, 603R, 604C, 605C, 605K, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 622X, 623, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625PF, 625R, 625X, 630, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630PF, 630R, 630X, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635PF, 635R, 635X, 640, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643G, 643H, 643J, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644G, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 648G, 648H, 648HT, 648L, 648L-II, 650, 650G, 650H, 650J, 650K, 653, 653E, 653G, 654, 655, 655K, 670, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 678, 683, 690E, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 708FC, 710D, 710G, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 724 P, 724K, 724L, 725D, 725PF, 725X, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 740, 740A, 740D, 740FD, 740G, 740PF, 740X, 744, 744 P, 744H, 744K, 744K-II, 746, 748, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750A, 750C, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755, 755D, 755K, 756, 759J, 759JH, 764, 768L-II, 770, 770D, 770G, 772D, 772G, 790, 800R, 803M, 803MH, 810D, 810E, 824 P, 824K, 825 LONG CHASSIS, 825 SHORT CHASSIS, 835 SHORT CHASSIS, 842, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 852, 853M, 853MH, 855, 855 LONG CHASSIS, 856, 859M, 859MH, 862, 870, 870D, 870G, 872D, 872G, 903K, 903KH, 903M, 903MH, 904 P, 909K, 909KH, 909M, 909MH, 910G, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 948L, 948L-II, 950, 950K, 953K, 953M, 953MH, 953ML, 955, 959K, 959M, 959MH, 959ML, 960, 970, 990, 995, 997, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1050, 1050K, 1050K PL, 1070, 1070D, 1070E, 1070G, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1270D, 1270E, 1270G, 1350, 1354, 1355, 1360, 1365, 1404, 1410D, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1460, 1465, 1470, 1470D, 1470E, 1470G, 1490D, 1505, 1510E, 1510G, 1515, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1654, 1690, 1710D, 1711D, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1795, 1820, 1830, 1835, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1850, 1854, 1854J, 1860, 1890, 1895, 1900, 1905, 1910, 1910E, 1948GV, 1948HV, 1990, 2020, 2020A, 2025R, 2026R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2104, 2144G, 2148HV, 2154D, 2154G, 2156G, 2204, 2230FH, 2230LL, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2354, 2400 PRECISIONCUT, 2454D, 2500 DIESEL, 2500 GAS, 2500B, 2500E, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2653B, 2654G, 2656G, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2720, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 2954D, 3004, 3013DF270, 3013DF271, 3016DF270, 3016DF271, 3025E, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4005, 4020DF101, 4020TF006, 4020TF105, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4115, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4475, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4990, 4995, 5005, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5225, 5300, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5575, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HRT81, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090HF475, 6090HF484, 6090HF485, 6090HFC47, 6090HFC48, 6090HFG84, 6090HFG86, 6090HFL75, 6090HFL85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135E, 6135HF475, 6135HF485, 6135HFC95, 6135HFG95, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140B, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145J, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6210R, 6215, 6215R, 6220, 6220L, 6225, 6230, 6230 Premium, 6230R, 6250R, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6488, 6500A E-CUT, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6650, 6675, 6700, 6710, 6715, 6750, 6810, 6820, 6830, 6830 Premium, 6850, 6910, 6910S, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7775, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8800, 8800A, 8900A, 9009A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A2, A400, BP15, C2 400, C6R, C8F, C8R, C12F, C12R, C16F, C16R, C18F, C18R, C100, C110, C120, C230, C240, C440, C441R, C451R, C461R, C650, C670, C850, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, D110, D120, D125, D130, D160, D170, DB80, DB88, DB90, E110, E120, E130, E140, E170, E180, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F441M, F441R, F510, F525, F910, F911, F912, F915, F925, F930, F932, F935, F1145, G100, G110, GROUPER, GT225, GT245, GX85, GX255, GX325, GX335, GX345, GX355, H260, H310, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HD200, HD300, HPX615E, HPX815E, L17.542, L60, L70, L105, L107, L108, L110, L111, L118, L120, L130, L2048, L2548, L2554, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX255, LX266, LX277, LX279, LX280, LX288, LX289, M-GATOR A3, M4025, M4030, M4040, M4040DN, MCS, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, N550, N560, PC7, PLANTER PERFORMANCE UPGRADES, R40, R230, R450, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, RSX 850I, RSX860E, RSX860I, RSX860M, S100, S110, S120, S130, S170, S180, S220, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S2046, S2048, S2348, S2546, S2554, SH12R, SPRAYER PERFORMANCE UPGRADES, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TE 4X2, TH 6X4, TH 6X4 D, TURF TX 4X2, TX 4X2, V451R, V461R, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X107, X110, X115R, X116R, X117R, X120, X125, X126, X127, X130R, X135R, X140, X145, X146R, X147R, X155R, X165, X166, X166R, X167, X167R, X300, X304, X310, X320, X324, X370, X500, X520, X530, X540, X570, X580, X590, X710, X730, X734, X738, X739, X950R, XUV 550, XUV 550 S4, XUV560E, XUV560E S4, XUV590E, XUV590E S4, XUV590I, XUV590I S4, XUV590M, XUV590M S4, XUV825E, XUV825M, XUV825M S4, XUV835E, XUV835M, XUV835R, XUV855E, XUV855M S4, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z425, Z435, Z445, Z465, Z510A, Z515E, Z520A, Z525E, Z530M, Z530R, Z535M, Z535R, Z540M, Z540R, Z545R, Z625, Z645, Z655, Z665, Z810A, Z820A, Z830A, Z840A, Z850A, Z860A, Z915B, Z915E, Z920M, Z925M, Z930A, Z930M, Z930R, Z945M, Z950A, Z950M, Z950R, Z955M, Z955R, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
@@ -2849,6 +3641,12 @@
           <t>19M7802</t>
         </is>
       </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>3-Bag, 3B-400, 3B-404, 3B-450, 3B-454, 3B-480, 3B-484, 3B-504, 3B-554, 3B-604, 5B-700, 5B-704, 5B-750, 5B-754, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6B-1404, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7H17, 7H19, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 30 Trailer, 42 IN., 47 IN., 48 IN., 102, 110, 110 TLB, 120C, 120D, 130 P, 130G, 160, 160 P, 160C, 160D, 160G, 180G, 200, 200 G, 200C, 200D, 200G, 210 P, 210C, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 230C, 240, 240D, 243, 244, 250, 250 P, 250D, 250D-II, 250G, 260, 260 P, 260E, 270, 270C, 270D, 280, 290G, 300 P, 300D, 300D-II, 300DW, 300E, 300G, 300WW, 310 G, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315 P, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318E, 318G, 319E, 320, 320 P, 320E, 320G, 323E, 324E, 324G, 324H, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330B, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335C, 335D, 337E, 343, 344, 344 P, 344H, 344J, 344K, 344L, 350 P, 350D, 350G, 360DC, 370E-II, 380 P, 380G, 400R, 408R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 435C, 437C, 437D, 437E, 443, 444, 444 G, 444 P, 444H, 444J, 444K, 444L, 450 P, 450G, 450H, 450J, 450K, 455G, 460 P, 460DC, 460E-II, 485E, 486E, 488E, 493, 494, 524 P, 524K, 524K-II, 524L, 540G-II, 540G-III, 540H, 540R, 543, 544 G, 544 P, 544H, 544J, 544K, 544K-II, 544L, 546, 548G-II, 548G-III, 548H, 550, 550 P, 550G, 550H, 550J, 550K, 554, 555G, 594, 600R, 604C, 605C, 605K, 606C, 607C, 608C, 609C, 610C, 611C, 612C, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 615C, 615F, 616C, 616R, 617C, 618F, 618R, 620F, 620G, 620R, 622F, 622G, 622R, 624 P, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625R, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 643, 643G, 643H, 643J, 643K, 643L, 643L-II, 644, 644 G, 644 P, 644 X, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645, 645FD, 645FD PERFORMANCE UPGRADES, 648G, 648H, 648HT, 648L, 648L-II, 650, 650 P, 650G, 650H, 650J, 650K, 653E, 653G, 654, 655, 655K, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 690E, 692, 693, 694, 700H, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 710 P, 710D, 710G, 710J, 710K, 710L, 712FC, 712FC PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 730FD, 730FD PERFORMANCE UPGRADES, 735FD, 735FD PERFORMANCE UPGRADES, 740, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 744 P, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755, 755D, 755K, 756, 759J, 759JH, 764, 768L-II, 770D, 770G, 772G, 800R, 803M, 803MH, 810D, 810E, 824 P, 824L, 825 LONG CHASSIS, 825 SHORT CHASSIS, 843, 843G, 843H, 843J, 843K, 843L, 843L-II, 844, 844 P, 844L, 848H, 848HT, 848L, 848L-II, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853M, 853MH, 855, 855 LONG CHASSIS, 855 SHORT CHASSIS, 856, 859M, 859MH, 870G, 872G, 892, 893, 894, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 910G, 913, 914, 915F, 915R, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 944 X, 944K, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 955, 959K, 959M, 959MH, 959ML, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1070D, 1070E, 1070G, 1092, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1243, 1270D, 1270E, 1270G, 1290, 1291, 1293, 1354, 1404, 1410D, 1420, 1435, 1445, 1450, 1470, 1470D, 1470E, 1470G, 1490D, 1510E, 1510G, 1545, 1550, 1565, 1570, 1690, 1700, 1705, 1710D, 1711D, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1800, 1820, 1830, 1835, 1840, 1842GV, 1842HV, 1848GV, 1848HV, 1850, 1854, 1854J, 1860, 1870, 1890, 1895, 1900, 1910, 1910E, 1910G, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2054, 2144G, 2154D, 2154G, 2156G, 2204, 2210, 2254, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2454D, 2500 DIESEL, 2500 GAS, 2500A, 2500E, 2510S, 2520, 2653A, 2653B, 2654G, 2656G, 2704, 2720, 2730, 2854, 2904, 2954D, 2956G, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029HFC03, 3029HFG03, 3029HG530, 3029HI530, 3029TF158, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045B, 3045R, 3046R, 3050B, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3215B, 3220, 3225B, 3225C, 3235, 3235B, 3235C, 3245C, 3310, 3320, 3400, 3410, 3420, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4039DF008, 4039TF008, 4044M, 4044R, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF154, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF152, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HMK80, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HSG20, 4045HSG21, 4045HYF01, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF155, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF253, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF281, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFG20, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4045TT851, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4105, 4120, 4239TF001, 4320, 4510, 4520, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5005, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5060E, 5060EN, 5065E, 5067E, 5070E, 5070M, 5075E, 5075EF, 5075EN, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5080G, 5080GF, 5080GV, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090G, 5090GH, 5090GV, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100GV, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130M, 5130ML, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320N, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5610, 5615, 5615V, 5620, 5625, 5705, 5715, 5720, 5725, 5820, 6010, 6020, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068DF120R01, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG20, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFN51, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HSG22, 6068HT087, 6068HYF01, 6068SFM50, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM75, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6080A E-CUT, 6080A PRECISIONCUT, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6095B, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135B, 6135E, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140J, 6140JH, 6140M, 6145J, 6145M, 6150J, 6150M, 6150M MONTENEGRO, 6155J, 6155JH, 6155M, 6155MH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6175M, 6180J, 6185J, 6190J, 6190M, 6195M, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6215, 6220, 6220L, 6225, 6230, 6230 Premium, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500A E-CUT, 6500A PRECISIONCUT, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6700, 6700A PRECISIONCUT, 6715, 6810, 6820, 6830, 6830 Premium, 6910, 6910S, 6920, 6920S, 6930, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7400A, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7500A PRECISIONCUT, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000A E-CUT, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8430, 8430T, 8500, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9009A, 9230, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9760 STS, 9770 STS, 9780, 9800, 9870 STS, 9900, 9935, 9970, 9986, 9996, A2, A400, B30C, B35C, B40C, C1 200, C2 300, C2 400, C12F, C16F, C100, C110, C120, C230, C240, C440, C670, CH330, CH530, CH570, CH670, CP690, CS690, CT315, CT322, CT332, CTS, D100, DB37, DB44, DB55, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F510, F525, F910, F925, F930, F935, F1145, F4365, G15, GS25, GS30, GS45, GS75, GT245, GX85, GX255, H540F, H541, H550, H550F, H560F, H561, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HH75, HH100, HPX815E, L60, L70, LA100, LA105, LT133, LT150, LT160, LT170, LT180, LX172, LX173, LX176, LX178, LX186, LX188, LX280, LX289, M4025, M4030, M4040, M4040DN, N530F, N540F, N543F, N550, N560, PA40, PLANTER PERFORMANCE UPGRADES, R2 300, R40, R230, R450, R4023, R4038, R4044, R4045, R4060, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, SP10B, SP12B, STRAIGHT BLADE, SX85, T550, T560, T660, T670, TC44H, TC54H, TC62H, W50, W70, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X300, X300R, X304, X305R, X310, X320, X324, X340, X360, X500, X520, X530, X534, X540, X590, X710, X730, X734, X738, X739, X750, X754, X950R, XUV825E, XUV825M, XUV825M S4, XUV855E, XUV855M, XUV855M S4, Y110, Y115, Y210, Y215, Z425, Z435, Z445, Z465, Z510A, Z520A, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z760R, Z910A, Z915B, Z920A, Z920M, Z925A, Z930A, Z930M, Z945M, Z950A, Z950M, Z950R, Z955M, Z960A, Z960M, Z960R, Z970A, Z970R, Z994R</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
@@ -2856,6 +3654,12 @@
           <t>19M7803</t>
         </is>
       </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 6E-1404L, 6E-1404PL, 6E-1504L, 6E-1504PL, 6M-1654, 6M-1854, 6M-2104, 6R 145, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7G18, 7H17, 7H19, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12 PC, 12SB, 13HP, 14PB, 14PZ, 14SB, 14SBS, 14SC, 14SE, 14SX, 14SZ, 15HP, 16HP, 20 Trailer, 30 Trailer, 47 IN., 54, 54D IN., 60 IN. DECKS, 60D IN., 60G, 62 IN., 62 IN. DECKS, 75G, 80, 85G, 107, 110 TLB, 112R, 190C, 200C, 210G, 210K, 210K EP, 210L, 210L EP, 210LJ, 230C, 240, 244E, 244H, 244L, 245, 250D, 250D-II, 250G, 260, 260 P, 260E, 265, 270, 270A, 270B, 270C, 285, 290G, 300D-II, 300DW, 300E, 300G, 300WW, 304H, 310 P, 310E, 310J, 310L EP, 310SJ, 310TJ, 312GR, 313, 314G, 316GR, 317G, 318G, 319D, 319E, 320, 323D, 323E, 324L, 325, 329D, 329E, 330G, 331G, 332G, 333D, 333E, 333G, 335, 335D, 337E, 344J, 345, 350 P, 350D, 350D-II, 350DW, 350G, 370E, 370E-II, 380 P, 380G, 400D, 400D-II, 400E, 400R, 408R, 410 P, 410E, 410E-II, 410J, 410R, 412R, 425, 430, 437D, 437E, 444H, 444K, 445, 450, 450C, 455, 460 P, 460E, 460E-II, 470 P, 470G, 520M, 524 P, 524K, 524K-II, 524L, 540E, 540M, 544 G, 544 P, 544G, 544K, 544K-II, 544L, 548E, 550, 550K, 554, 600L HIGH DUMP, 600R, 604C, 605C, 606C, 606C PERFORMANCE UPGRADES, 607C, 608C, 608C PERFORMANCE UPGRADES, 609C, 610C, 611C, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 612R, 613C, 614C, 614R, 615C, 615F, 615P, 615R, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 617C, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618PF, 618R, 620, 620F, 620G, 620I, 620PF, 620R, 622, 622F, 622G, 622PF, 622R, 624 P, 624G, 624K, 624K-II, 624KR, 624L, 625D, 625F, 625I, 625PF, 625R, 630, 630D, 630F, 630PF, 630R, 635, 635D, 635F, 635PF, 635R, 636M, 640E, 640L, 640L-II, 643D, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644J, 644K, 644K HYBRID, 644L, 644LH, 647A, 648E, 648L, 648L-II, 650, 650K, 654, 655K, 657A, 667A, 670, 670G, 672G, 700K, 700L, 700L PL, 700M, 703JH, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 710J, 710K, 710L, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 717, 717A, 718C, 718C PERFORMANCE UPGRADES, 724 P, 724J, 724K, 724L, 725D, 727A, 730D, 735D, 737, 740A, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748, 748E, 748L, 748L-II, 750A, 750K, 750L, 753J, 753JH, 755K, 757, 759J, 759JH, 764, 768L-II, 770, 770G, 772G, 777, 790, 797, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 835 SHORT CHASSIS, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848L, 848L-II, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870G, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 913, 915F, 915R, 918, 918F, 918R, 920, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 930, 930D, 930F, 930R, 936D, 944K, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 959J, 959K, 959M, 959MH, 959ML, 990, 997, 1023E, 1025R, 1026R, 1050K, 1050K PL, 1070E, 1070G, 1110E, 1110G, 1170E, 1170G, 1175, 1210E, 1210G, 1270E, 1270G, 1420, 1435, 1438GS, 1438HS, 1445, 1450, 1470, 1470E, 1470G, 1504, 1505, 1510C, 1510DC, 1510E, 1510G, 1512C, 1512E, 1515, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1545, 1550, 1565, 1570, 1575, 1580, 1585, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1690, 1705, 1725, 1725 CCS, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1765, 1770NT, 1775NT, 1780, 1785, 1790, 1795, 1800, 1810C, 1810DC, 1810E, 1812C, 1812DC, 1814C, 1814DC, 1814E, 1820, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1860, 1870, 1890, 1895, 1900, 1910, 1910G, 1948GV, 1948HV, 1990, 2020, 2020A, 2025R, 2026R, 2027R, 2030, 2030A, 2032R, 2036R, 2038R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2112C, 2112DC, 2112E, 2148HV, 2154G, 2156G, 2204, 2210, 2230FH, 2243, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2354, 2400 PRECISIONCUT, 2430, 2430C, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2520, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2630, 2633, 2633VT, 2635, 2653, 2653B, 2654G, 2656G, 2660VT, 2704, 2720, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2904, 3004, 3005, 3025E, 3028EN, 3029DF129, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFU20, 3029HFU89, 3032E, 3033R, 3036E, 3036EN, 3038E, 3038R, 3039R, 3045R, 3046R, 3120, 3154G, 3156G, 3203, 3204, 3225C, 3235C, 3245C, 3320, 3520, 3720, 3754G, 3756G, 4005, 4010, 4020DF101, 4020TF006, 4020TF105, 4024TF270, 4044M, 4044R, 4045DF159, 4045HF285, 4045HF286, 4045HF288, 4045HFC28, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFU72, 4045HFU79, 4045T, 4045TF252, 4045TF254, 4045TF285, 4045TFG20, 4045TFU20, 4045TFU70, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4100, 4105, 4110, 4115, 4120, 4200, 4210, 4300, 4310, 4320, 4400, 4410, 4500, 4510, 4520, 4600, 4610, 4630, 4700, 4710, 4720, 4730, 4830, 4920, 4930, 4940, 5005, 5030HF285, 5036C, 5036D, 5038D, 5039C, 5039D, 5040D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070E, 5075E, 5075EF, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5078E, 5080E, 5080EN, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5103, 5103E, 5103S, 5104, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125R, 5200, 5203, 5203S, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5303, 5305, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5500, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5610, 5615, 5615V, 5625, 5705, 5715, 5725, 6068CG550, 6068CI550, 6068CP550, 6068HB551, 6068HC550, 6068HF252, 6068HF254, 6068HF279, 6068HF285, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG82, 6068HFG94, 6068HFG95, 6068HFS01, 6068HFS89, 6068HFU72, 6068HFU74, 6068HFU79, 6068HG550, 6068HI550, 6068HN075, 6068HP550, 6068TF252, 6068TF254, 6080A E-CUT, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFS85, 6090HFS86, 6090HFU84, 6090SFM75, 6090SFM85, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6105D, 6105E, 6105EH, 6105J, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6115D, 6115E, 6120E, 6120EH, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125HF070, 6125SFM75, 6130D, 6130E SALTILLO, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135SFM75, 6140D, 6140J, 6140R, 6145R, 6150M, 6150R, 6150RH, 6155J, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170R, 6175M, 6175R, 6180CI510, 6190R, 6195M, 6195R, 6210R, 6215R, 6230R, 6250R, 6403, 6415, 6425, 6488, 6500A E-CUT, 6603, 6610, 6650, 6710, 6750, 6800, 6810, 6850, 6900, 6910, 6910S, 6950, 7180, 7185J, 7195J, 7200, 7200A, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7350, 7380, 7400, 7400A, 7410, 7420, 7425, 7450, 7455, 7460, 7480, 7500, 7500A E-CUT, 7510, 7520, 7525, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7830, 7850, 7930, 7950, 7980, 8000, 8000A E-CUT, 8100, 8130, 8200, 8225R, 8230, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8300, 8310R, 8310RT, 8320R, 8320RT, 8330, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8430, 8500, 8530, 8600, 8700, 8800, 8800A, 8900A, 9100, 9120, 9200, 9220, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9996, 15538, A400, BP15, C2 400, C12F, C16F, C18F, C230, C440, C441R, C650, C670, C850, CH330, CH530, CH570, CH670, CP690, CP770, CS690, CS770, CT315, CT332, CTS, CTS II, D170, DB37, DB41, DB44, DB55, DB58, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, E12, E15, F441R, F710, F725, F735, F911, F912, F915, F925, F932, F935, F1145, F4365, FC10R, FC12E, FC15E, FC15M, FC15R, G15, G100, G110, GS25, GS30, GS45, GS75, GX345, GX355, H240, H260, H310, H340, H360, H380, H480, HD35F, HD40F, HD45, HD45F, HD50F, HD75, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L17.542, L60, L110, L130, L330, L331, L340, L341, L2554, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX288, M15, MaxEmerge XP, N530F, N536C, N540C, N540F, N542C, N543F, N550, N560, P540, P556, PLANTER PERFORMANCE UPGRADES, R10, R15, R40, R230, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, S240, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S2046, S2048, S2348, S2546, S2554, SPRAYER PERFORMANCE UPGRADES, SST15, SST16, STRAIGHT BLADE, STX30, STX38, STX46, T550, T560, T660, T670, TC44H, TD100, W36M, W36R, W48M, W48R, W50, W52R, W70, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WG32A, WG36A, WG48A, WH36A, WH48A, WH52A, WHP36A, WHP48A, WHP52A, X9 1000, X9 1100, X300, X300R, X304, X305R, X310, X320, X324, X330, X340, X350, X350R, X354, X360, X370, X380, X390, X500, X520, X534, X540, X710, X730, X734, X738, X739, X750, X754, X758, X950R, XUV 550, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV560E S4, XUV835E, XUV835M, XUV835R, XUV865E, XUV865M, XUV865R, Y110, Y115, Y210, Y215, Z225, Z235, Z245, Z255, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z335E, Z335M, Z345M, Z345R, Z355E, Z355R, Z365R, Z375R, Z425, Z445, Z465, Z720E, Z730M, Z735E, Z735M, Z740R, Z840A, Z915E, Z920M, Z925M, Z930M, Z930R, Z945M, Z950M, Z950R, Z955M, Z955R, Z960M, Z970R, Z994R, Z997R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
@@ -2863,6 +3667,12 @@
           <t>19M8039</t>
         </is>
       </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>3-Bag, 4X2, 4X2 TRAIL, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 6X4, 6X4 D, 6X4 D TRAIL, 6X4 D Worksite, 6X4 TRAIL, 6X4 Trail Camo, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12 PC, 12.5HP, 12SB, 14HP, 14PB, 14PS, 14PT, 14PZ, 14SB, 14SBS, 14SC, 14SE, 14ST, 14SX, 14SZ, 17HP, 40I, 48 IN., 50 in., 50I, 54, 54D IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 108, 110 TLB, 111, 112L, 130G, 180, 185 E-CUT, 210 G, 210 P, 210K, 210K EP, 210L, 210L EP, 210LJ, 225 E-CUT, 240, 245, 250D-II, 260, 260 P, 260E, 265, 270, 270A, 270B, 285, 300D-II, 300E, 305, 310 G, 310 P, 310E, 310K, 310L, 310L EP, 310SK, 310SL, 310SL HL, 310TK TMC, 312GR, 314G, 315 P, 315SK, 315SL, 316GR, 317G, 318E, 318G, 319E, 320, 320 P, 320E, 320G, 323E, 324E, 324G, 325G, 325SK, 325SL, 326E, 330G, 331G, 332G, 333G, 350 P, 350G, 370E, 370E-II, 380 P, 380G, 400R, 408R, 410 P, 410E, 410E-II, 410K, 410L, 410R, 410TK TMC, 412R, 425, 435, 437E, 440E, 444 P, 444J, 444K, 444L, 445, 446, 447, 448, 449, 450 P, 450C, 450E, 450M, 455, 456, 457, 458, 459, 459E, 460 P, 460DC, 460E, 460E-II, 460M, 460R, 466, 467, 468, 469, 470 P, 470G, 493, 494, 524 P, 524K, 524L, 531, 533, 535, 540H, 540M, 543M, 543R, 544 P, 544J, 544K, 544L, 545, 546, 547, 548H, 550, 550 P, 550K, 550M, 551, 556, 557, 558, 559, 560M, 560R, 563, 566, 567, 568, 569, 570, 572, 580, 582, 583, 590, 592, 594, 600R, 603M, 603R, 606C, 606SH, 608C, 608C PRECISION UPGRADES, 608SH, 612C, 612FC, 612R, 616C, 616R, 618C, 620G, 620R, 622G, 623, 623R, 624 P, 624J, 624K, 624L, 625D, 630D, 631, 633, 635D, 640D, 640G, 640H, 640L, 640R, 643R, 644J, 644K, 648G, 648H, 648HT, 648L, 650 P, 650K, 651, 652R, 653, 655K, 660R, 661, 661R, 663, 663R, 670G, 672G, 673, 678, 680R, 683, 683R, 692, 693, 694, 706C, 708C, 710 P, 710L, 712C, 712FC, 716C, 718C, 724 P, 724J, 724K, 724L, 725D, 730D, 731, 735D, 740, 740A, 740D, 741, 744, 744 P, 744H, 744J, 744K, 744K-II, 744L, 748H, 748HT, 748L, 748L-II, 750A, 750K, 751, 753, 753J, 753JH, 759J, 759JH, 768L-II, 770G, 772G, 777, 797, 800, 800R, 803M, 803MH, 824 P, 824J, 824K, 824L, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848H, 848HT, 848L, 848L-II, 850K, 850L, 850L PL, 852, 853M, 853MH, 854, 856, 859M, 859MH, 862, 864, 870G, 872G, 892, 893, 894, 903M, 903MH, 904 P, 909M, 909MH, 925D, 930D, 936D, 944 X, 944K, 948L, 948L-II, 950K, 953M, 953MH, 953ML, 959M, 959MH, 959ML, 960, 990, 1010, 1015, 1023E, 1025, 1025R, 1026R, 1035, 1050K, 1050K PL, 1092, 1110E, 1110G, 1165, 1175, 1210E, 1210G, 1270E, 1270G, 1290, 1291, 1293, 1420, 1435, 1445, 1450, 1470, 1470E, 1470G, 1510E, 1510G, 1545, 1550, 1565, 1570, 1600 TURBO SERIES II, 1600 TURBO SERIES III, 1620, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725T, 1745, 1750, 1755, 1770NT, 1775NT, 1790, 1795, 1850, 1890, 1895, 1910, 1910G, 1948GV, 1948HV, 1990, 2020A, 2025R, 2026R, 2027R, 2030A, 2032R, 2036R, 2038R, 2048HV, 2054, 2056, 2058, 2064, 2066, 2100, 2148HV, 2204, 2254, 2256, 2258, 2264, 2266, 2266E, 2354, 2400 PRECISIONCUT, 2500A, 2500E, 2510H, 2520, 2554HV, 2554ST, 2653A, 2653B, 2700 E-CUT HYBRID, 2700 PRECISIONCUT, 2704, 2750 E-CUT HYBRID, 2750 PRECISIONCUT, 2854, 2904, 3004, 3025D, 3025E, 3028EN, 3029DF128, 3029DF129, 3029HFC03, 3029HFG03, 3029TF129, 3029TF158, 3032E, 3033R, 3035D, 3036E, 3036EN, 3038E, 3038R, 3039R, 3043D, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3203, 3204, 3210, 3215, 3220, 3310, 3320, 3325, 3365, 3400, 3410, 3420, 3510, 3520, 3522, 3720, 3754G, 3756G, 4039DF008, 4039TF008, 4044M, 4044R, 4045DF120, 4045DF120R02, 4045DF150, 4045DF158, 4045DF270, 4045DF271, 4045HF120, 4045HF120R02, 4045HF150, 4045HF157, 4045HF158, 4045HF275, 4045HF475, 4045HFG20, 4045HFG81, 4045HFG82, 4045HFS72, 4045HFS73, 4045HFS80, 4045HFS82, 4045HFS83, 4045HFS85, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU81, 4045HFU82, 4045HSG20, 4045HSG21, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF157, 4045TF158, 4045TF220, 4045TF250, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TFG20, 4045TFS70, 4045TFU20, 4045TFU70, 4045TSG20, 4049M, 4049R, 4052M, 4052R, 4066M, 4066R, 4075R, 4105, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4510, 4520, 4610, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5065M, 5075M, 5076EN, 5080R, 5085M, 5090EN, 5090R, 5095M, 5095MH, 5100M, 5100MH, 5100ML, 5100R, 5105, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125R, 5205, 5220, 5310, 5320, 5420, 5425, 5520, 5525, 5620, 5625, 5720, 5820, 6068DF150, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HFC08, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG20, 6068HFG55, 6068HFG82, 6068HFS01, 6068HFS72, 6068HFS73, 6068HFS77, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFS89, 6068HFU20, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HI550, 6068HN075, 6068HRT81, 6068HSG22, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF258, 6068TF275, 6090 MC, 6090 RC, 6090CB450, 6090CB451, 6090CG550, 6090CI550, 6090CP550, 6090HFC09, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG94, 6090HFG95, 6090M, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6100D, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105HF001, 6105J, 6105M, 6105R, 6110 MC, 6110 RC, 6110D, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115J, 6115M, 6115R, 6120M, 6120R, 6125AF001, 6125AFM01, 6125AFM75, 6125D, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6125SFM75, 6130D, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135CI550, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG75, 6135HFG84, 6135HFG95, 6135HFM85, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM75, 6135SFM85, 6140D, 6140J, 6140M, 6140R, 6145M, 6145R, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155M, 6155MH, 6155R, 6155RH, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6190M, 6190R, 6195M, 6195R, 6210M, 6210R, 6215R, 6230 Premium, 6230R, 6250R, 6330 Premium, 6430 Premium, 6530 Premium, 6534 Premium, 6610, 6630 Premium, 6650, 6710, 6750, 6810, 6830 Premium, 6850, 6910, 6930, 6950, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210J, 7210R, 7215J, 7215R, 7225J, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7330 Premium, 7350, 7380, 7400, 7430E, 7450, 7480, 7500, 7530E, 7550, 7580, 7630, 7660, 7700, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8000, 8100, 8120, 8120T, 8130, 8200, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8420, 8420T, 8430, 8430T, 8500, 8520, 8520T, 8530, 8600, 8700, 8700A PRECISIONCUT, 8800, 8800A, 8900A, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9970, 9976, 9986, 9996, C1 200, C2 300, C2 400, C6R, C6R PRECISION UPGRADES, C8R, C8R PRECISION UPGRADES, C12F, C12F PRECISION UPGRADES, C12R, C12R PRECISION UPGRADES, C16F, C16F PRECISION UPGRADES, C16R, C16R PRECISION UPGRADES, C18F, C18F PRECISION UPGRADES, C18R, C18R PRECISION UPGRADES, C230, C240, C440, C440R, C441R, C451R, C461R, C670, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CTS, CTS II, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DR12, DR12T, DR16, DR18, DR24, E210, E230, E230-II, F441R, F510, F525, F620, F680, F687, F710, F725, F735, F915, F925, F935, F1145, F4365, G100, G110, GS25, GS30, GS45, GS75, GT225, GT242, GT262, GT275, GX325, GX335, GX345, GX355, H260, H310, H340, H360, H380, HD45, HD75, HD200, HD300, HPX 4X2 D, HPX 4X4 D, HPX815E, JA60, JA62, JA65, JE75, JX75, JX85, L2554, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX280, LX289, M-GATOR A1, M653, M655, M665, M4030, M4040, M4040DN, N530, N530C, N530F, N536, N536C, N540, N540C, N540F, N542, N542C, N543F, R2 300, R230, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, S80, S82, S92, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, S2348, S2554, SST16, STRAIGHT BLADE, STX30, STX38, STX46, T550, T560, T660, T670, TH 6X4 D, TURF TX 4X2, V451R, V461R, W50, W61R, W70, W200M, W230, W235, W235M, W235R, W330, W430, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES, X115R, X116R, X117R, X475, X485, X575, X585, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, Z225, Z235, Z245, Z425, Z435, Z445, Z465, Z510A, Z520A, Z625, Z645, Z655, Z665, Z710A, Z720A, Z720E, Z730M, Z735E, Z735M, Z740R, Z760R, Z915B, Z915E, Z925A, Z925M, Z930M, Z945M</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
@@ -2870,6 +3680,12 @@
           <t>19M7913</t>
         </is>
       </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>3-Bag, 5B-700, 5B-704, 5B-750, 5B-754, 6J-1704, 6J-1904, 6R 110, 6R 120, 6R 130, 6R 140, 6R 150, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 12.5HP, 14HP, 17HP, 20 Trailer, 30 Trailer, 48 IN., 60G, 75G, 80, 85G, 100, 110, 120D, 130 P, 130G, 160, 160 P, 160D, 160G, 180G, 200, 200 G, 200D, 200G, 210G, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 215, 216, 218, 220, 222R, 224, 230, 240D, 244E, 244J, 250D, 250D-II, 250G, 260, 260 P, 260E, 270A, 270B, 270D, 290G, 300D-II, 300DW, 300E, 300G, 300WW, 304J, 305, 310 P, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 312GR, 313, 314G, 315, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 320G, 323D, 323E, 324E, 324G, 324J, 325, 325G, 325J, 325SK, 325SL, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330G, 331G, 332, 332D, 332E, 332G, 333D, 333E, 333G, 335C, 335D, 337E, 344K, 344L, 350D, 350G, 360DC, 370E, 370E-II, 380G, 400R, 410 P, 410E, 410E-II, 410G, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 415, 425, 435C, 437C, 437D, 437E, 444 G, 444 P, 444H, 444J, 444K, 444L, 445, 449, 450G, 450H, 450J, 450K, 455, 455G, 460 P, 460DC, 460E, 460E-II, 470 P, 470G, 524 P, 524K, 524K-II, 524L, 540E, 540G-II, 540G-III, 540H, 544 G, 544 P, 544G, 544H, 544J, 544K, 544K-II, 544L, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 550K, 554, 555G, 600R, 605C, 605K, 608BH, 608L, 608LH, 608SH, 612R, 616R, 620G, 620I, 622G, 622X, 624 P, 624G, 624H, 624J, 624K, 624K-II, 624KR, 624L, 625D, 625I, 625X, 630D, 630X, 635D, 635X, 640D, 640E, 640FD, 640FD PERFORMANCE UPGRADES, 640G, 640H, 640L, 640L-II, 640X, 643G, 643H, 643J, 643K, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644H, 644HMH, 644J, 644K, 644K HYBRID, 644L, 644LH, 645FD, 645FD PERFORMANCE UPGRADES, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650, 650G, 650H, 650J, 650K, 653E, 653G, 654, 655K, 670C, 670C II, 670CH, 670CH II, 670D, 670G, 672CH, 672D, 672G, 700H, 700J, 700K, 700L, 700L PL, 703G, 703GH, 703JH, 710G, 710J, 710K, 710L, 722X, 724 P, 724J, 724K, 724L, 725D, 725X, 730D, 730X, 735D, 735X, 740, 740A, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740G, 740X, 744 P, 744H, 744J, 744K, 744K-II, 744L, 745FD, 745FD PERFORMANCE UPGRADES, 748, 748E, 748G-II, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750K, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755D, 755K, 759G, 759GH, 759J, 759JH, 764, 768L-II, 770D, 770G, 772D, 772G, 800R, 803M, 803MH, 810D, 810E, 824 P, 824J, 824K, 824L, 835 SHORT CHASSIS, 843G, 843H, 843J, 843K, 843L, 843L-II, 844 P, 844J, 844K, 844K-III, 844K-III AGGREGATE HANDLER, 844L, 844L AGGREGATE HANDLER, 848G, 848H, 848HT, 848L, 848L-II, 850C, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853G, 853J, 853JH, 853M, 853MH, 859M, 859MH, 870D, 870G, 872D, 872G, 900, 903G, 903J, 903JH, 903K, 903KH, 903M, 903MH, 904 P, 909J, 909JH, 909K, 909KH, 909M, 909MH, 910G, 913, 915F, 915R, 918, 918F, 918R, 920F, 920R, 922F, 922R, 924, 925, 925F, 925R, 930, 930F, 930R, 944K, 946, 948L, 948L-II, 950K, 953G, 953J, 953K, 953M, 953MH, 953ML, 956, 959J, 959K, 959M, 959MH, 959ML, 1010D, 1010E, 1010G, 1023E, 1025R, 1026R, 1050J, 1050K, 1050K PL, 1070D, 1070E, 1070G, 1110D, 1110E, 1110G, 1165, 1170, 1170E, 1170G, 1175, 1210E, 1210G, 1270D, 1270E, 1270G, 1312C, 1410D, 1450, 1470, 1470D, 1470E, 1470G, 1490D, 1510C, 1510E, 1510G, 1512E, 1550, 1565, 1570, 1580, 1600 TURBO SERIES III, 1612DE, 1654, 1710D, 1711D, 1720 CCS, 1725 CCS, 1725T, 1770, 1770NT, 1775NT, 1790, 1795, 1810E, 1812C, 1814C, 1814E, 1854, 1854J, 1870, 1910E, 1910G, 2010DE, 2014DE, 2025R, 2026R, 2032R, 2036R, 2038R, 2054, 2056, 2058, 2064, 2066, 2104, 2112E, 2144G, 2154D, 2154G, 2156G, 2204, 2254, 2256, 2258, 2264, 2266, 2266E, 2412DE, 2454D, 2654G, 2656G, 2660VT, 2704, 2854, 2904, 2954D, 3004, 3025E, 3029DF128, 3029DF129, 3029DFG20, 3029DFS29, 3029DFU20, 3029DFU29, 3029DFU29R, 3029DSG20, 3029HFC03, 3029HFG03, 3029HFG20, 3029HFG89, 3029HFU20, 3029HFU89, 3029HG530, 3029HI530, 3029TF129, 3029TF158, 3029TFG20, 3029TFG89, 3029TFH79, 3029TFS29, 3029TFU20, 3029TFU29, 3029TFU89, 3029TSG20, 3032E, 3033R, 3038E, 3038R, 3039R, 3045R, 3046R, 3110, 3120, 3154G, 3156G, 3200, 3204, 3210, 3215, 3220, 3310, 3320, 3400, 3410, 3420, 3510, 3520, 3522, 3720, 3754D, 3754G, 3756G, 3800, 4024DFN70, 4024HF285, 4024HF295, 4024TF220, 4024TF270, 4024TF271, 4024TF272, 4024TF280, 4024TF281, 4039DF008, 4039TF008, 4045CA550, 4045CB551, 4045CI550, 4045CI551, 4045DF120, 4045DF120R02, 4045DF150, 4045DF158, 4045DF159, 4045DF270, 4045DF271, 4045DFM50, 4045DFM70, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF120, 4045HF120R02, 4045HF150, 4045HF157, 4045HF158, 4045HF275, 4045HF280, 4045HF285, 4045HF286, 4045HF287, 4045HF289, 4045HF475, 4045HF485, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG81, 4045HFG82, 4045HFG85, 4045HFG92, 4045HFG93, 4045HFJ85, 4045HFK04, 4045HFK80, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS72, 4045HFS80, 4045HFU72, 4045HFU79, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045SFM85, 4045T, 4045TF120, 4045TF120R02, 4045TF150, 4045TF150R02, 4045TF151, 4045TF157, 4045TF158, 4045TF220, 4045TF220R02, 4045TF250, 4045TF252, 4045TF254, 4045TF258, 4045TF270, 4045TF271, 4045TF275, 4045TF276, 4045TF277, 4045TF280, 4045TF285, 4045TF290, 4045TFC03, 4045TFG03, 4045TFM50, 4045TFM75, 4045TFM85, 4045TFS70, 4045TFU20, 4045TFU70, 4120, 4200, 4210, 4239TF001, 4300, 4310, 4320, 4400, 4410, 4500, 4520, 4600, 4630, 4700, 4710, 4720, 4730, 4830, 4890, 4895, 4920, 4930, 4940, 4990, 4995, 5030HF220, 5030HF270, 5030HF285, 5030TF220, 5030TF270, 5030TF271, 5030TF272, 5045E, 5050E, 5055E, 5060E, 5065E, 5065M, 5070E, 5070M, 5075E, 5075M, 5076E, 5076EF, 5076EN, 5078E, 5080E, 5080M, 5080R, 5082E, 5083E, 5083EN, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5093EN, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5101EN, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5200, 5210, 5215, 5215F, 5215V, 5220, 5225, 5300, 5303, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5325, 5325N, 5400, 5403, 5405, 5410, 5410N, 5415, 5420, 5420N, 5425, 5425N, 5430I, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520, 5520N, 5525, 5525N, 5603, 5605, 5615, 5615V, 5620, 5625, 5705, 5720, 5725, 5820, 6010, 6020, 6068CG550, 6068CI550, 6068CP550, 6068DF150, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF120, 6068HF120R02, 6068HF150, 6068HF150R02, 6068HF157, 6068HF158, 6068HF250, 6068HF252, 6068HF254, 6068HF258, 6068HF275, 6068HF279, 6068HF285, 6068HF475, 6068HF485, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG25, 6068HFG55, 6068HFG82, 6068HFG85, 6068HFG94, 6068HFG95, 6068HFL84, 6068HFN50, 6068HFS01, 6068HFS55, 6068HFS72, 6068HFS73, 6068HFS82, 6068HFS83, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HSG22, 6068HT087, 6068TBM01, 6068TBM02, 6068TF120, 6068TF150, 6068TF151, 6068TF157, 6068TF158, 6068TF220, 6068TF220R02, 6068TF250, 6068TF250R02, 6068TF252, 6068TF254, 6068TF258, 6068TF275, 6068TFM50, 6068TFM76, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6081AF001, 6081AFM75, 6081HF001, 6081HF070, 6081HFN02, 6081TF001, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CI550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG84, 6090HFG86, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100J, 6105 MC, 6105 RC, 6105AF001, 6105D, 6105E, 6105EH, 6105HF001, 6105J, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110J, 6110L, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120, 6120B, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125AF001, 6125D, 6125E MONTENEGRO, 6125E ROSARIO, 6125E SALTILLO, 6125HF001, 6125HF070, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130J, 6130M, 6130R, 6135AFM75, 6135AFM85, 6135B, 6135CI550, 6135E, 6135HF475, 6135HF485, 6135HFC09, 6135HFC48, 6135HFC95, 6135HFG06, 6135HFG09, 6135HFG95, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6135SFM85, 6136CG440, 6136CG550, 6136CI440, 6136CI550, 6136HI440, 6136HI550, 6140D, 6140J, 6140JH, 6140M, 6145J, 6145M, 6150J, 6150M, 6150M MONTENEGRO, 6155J, 6155JH, 6155M, 6155MH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6175M, 6180CI510, 6180J, 6185J, 6190J, 6190M, 6195M, 6205, 6205J, 6210, 6210J, 6210L, 6210M, 6215, 6220, 6220L, 6225, 6230, 6230 Premium, 6310, 6310L, 6320, 6320L, 6325, 6330, 6330 Premium, 6400, 6403, 6405, 6410, 6410L, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6505, 6510, 6510L, 6510S, 6515, 6520, 6520L, 6525, 6530, 6530 Premium, 6534, 6534 Premium, 6603, 6605, 6610, 6615, 6620, 6630, 6630 Premium, 6700, 6715, 6810, 6820, 6830, 6830 Premium, 6910, 6910S, 6920, 6920S, 6930, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7260R, 7270R, 7280, 7280R, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7505, 7510, 7515, 7520, 7525, 7530E, 7550, 7580, 7610, 7630, 7660, 7700, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8100, 8120, 8130, 8200, 8220, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8310R, 8310RT, 8320, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8420, 8430, 8430T, 8500, 8520, 8530, 8600, 8700, 8800, 9100, 9200, 9230, 9300, 9330, 9360R, 9370R, 9400, 9410, 9410R, 9420R, 9420RX, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9510, 9510R, 9510RT, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9530, 9530 SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9630, 9630 SCRAPER, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, A2, A400, C2 400, C230, C440, C450, C500, C670, CH330, CH530, CH570, CH670, CH950, CH960, CP690, CP770, CS690, CS770, CT315, CT322, CT332, CTS, CTS II, D105, D140, D150, D155, DB44, E100, E130, E140, E210, E210-II, E210LC, E230, E230-II, E240, E240LC, E260, E300, E300LC, E330, E360, E380, E400, F510, F525, F925, F935, F4365, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HPX 4X2, HPX 4X2 D, HPX 4X4, HPX 4X4 D, HPX 4X4 TRAIL, HPX615E, HPX815E, L60, LA145, LX277, LX279, LX280, M-GATOR A3, M724, M732, M732i, M740, M740i, M944, M944I, M952, M952I, M962, M962I, M4025, P540, P556, PLANTER PERFORMANCE UPGRADES, R230, R450, R4023, R4038, R4040i, R4044, R4045, R4060, R4140i, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, STRAIGHT BLADE, T550, T560, T660, T670, TC44H, TC54H, TC62H, TD100, TX 4X2, W50, W70, W100, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W540, W550, W650, W660, WL53, WL56, X9 1000, X9 1100, X105, X106, X330, X350, X354, X370, X380, X384, X390, X394, X465, X475, X485, X495, X570, X575, X580, X584, X585, X590, X595, XUV835M, XUV835R, XUV865M, XUV865R, Z315E, Z320M, Z320R, Z325E, Z330M, Z330R, Z720E, Z730M, Z735E, Z735M, Z740R, Z915B, Z915E, Z920M, Z920R, Z925M, Z930M, Z930R, Z945M, Z950M, Z950R, Z955M, Z955R, Z960M, Z960R, Z970R, Z994R, Z997R</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
@@ -2877,6 +3693,12 @@
           <t>19H3267</t>
         </is>
       </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>47 IN., 146, 148, 158, 168, 210C, 313, 315, 317, 318D, 319D, 320, 320D, 323D, 330C, 344E, 370, 370C, 444E, 450, 530B, 535, 540E, 540G-II, 544E, 548E, 548G-II, 570B, 608BH, 608L, 608LH, 608SH, 624E, 640E, 640G, 643D, 644E, 644G, 644H, 644HMH, 648E, 648G, 653E, 670B, 670C, 670C II, 670CH, 670CH II, 672B, 672CH, 703G, 703GH, 703JH, 740G, 748E, 748G-II, 748G-III, 750C, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 762B, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 772B, 772BH, 772CH, 772CH II, 772D, 792D, 840, 850C, 853G, 853J, 853JH, 862B, 870D, 872D, 892E, 900, 903G, 903J, 903JH, 909J, 909JH, 940, 953G, 953J, 959J, 1040, 1140, 1185, 1350, 1550, 1640, 1750, 1840, 1850, 1950, 1950N, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2140, 2150, 2155, 2250, 2254, 2255, 2256, 2258, 2264, 2266, 2266E, 2350, 2355, 2355N, 2450, 2550, 2555, 2650, 2750, 2755, 2850, 2950, 2955, 3029D, 3029DF120, 3029DF128, 3029DF150, 3029DF180, 3029HF270, 3029T, 3029TF120, 3029TF150, 3029TF152, 3029TF158, 3029TF180, 3029TF270, 3040, 3050, 3055, 3140, 3150, 3155, 3179DF, 3179T, 3255, 3350, 3510, 3554, 3640, 3650, 4039D, 4039DF001, 4039DF004, 4039DF005, 4039DF006, 4039DF008, 4039DF031, 4039DF032, 4039DF092, 4039T, 4039TF001, 4039TF007, 4039TF008, 4045D, 4045DF001, 4045DF158, 4045HF158, 4045TF001, 4045TF092, 4045TF158, 4045TF258, 4055, 4219DF01, 4239A, 4239D, 4239DF001, 4239DT004, 4239TF001, 4250, 4255, 4276DF01, 4276T, 4276TF01, 4450, 4455, 4555, 4560, 4650, 4755, 4760, 4850, 4955, 4960, 5200, 5400, 5440, 5460, 5720, 5730, 5820, 5830, 6059DF001, 6059DF092, 6059T, 6059TF, 6059TF001, 6059TF002, 6059TF003, 6059TF004, 6068D, 6068DF, 6068DF001, 6068HF158, 6068HF258, 6068TF092, 6068TF158, 6068TF258, 6076AFM00, 6076AFM30, 6076AFN, 6076HF030, 6076TF, 6081AF001, 6081AFH75, 6081AFM01, 6081AFM75, 6081HF001, 6081HF070, 6081HFH70, 6081HFN01, 6081HFN02, 6081HFN03, 6081TF001, 6095 MC, 6095 RC, 6101HF010, 6101HF011, 6105 MC, 6105 RC, 6110M, 6115 MC, 6115 RC, 6120M, 6125M, 6130M, 6135M, 6140M, 6145M, 6155M, 6175M, 6195M, 6359A, 6359DF001, 6359T, 6359TF001, 6414D, 6414T, 6414TDW14, 6414TDW16, 6466A, 6466D, 6466T, 6610, 6619A, 6619A Engine SE500219, 6619A Engine SE500493, 6619A Engine SE500087, 6619A Engine SE500089, 6619A Engine SE500090, 6619A Engine SE500091, 6619TF-01, 6620, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7020, 7600, 7610, 7700, 7710, 7720, 7800, 7810, 8120, 8220, 8320, 8420, 8430, 8440, 8450, 8520, 8560, 8570, 8630, 8640, 8650, 8760, 8770, 8820, 8870, 8960, 8970, 9100, 9200, 9300, 9400, 9410, 9450, 9500, 9510, 9550, 9560 STS, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9680, 9750 STS, 9760 STS, 9780, 9970, 9976, CT315, CT322, CTS, CTS II</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
@@ -2884,6 +3706,12 @@
           <t>19H3031</t>
         </is>
       </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>20 Trailer, 25A, 30 Trailer, 47 IN., 59 IN., 190E, 210 G, 210 P, 210C, 210K, 210K EP, 210L, 210L EP, 210LE, 210LJ, 240, 250, 260, 270, 290D, 300D, 310D, 315D, 318E, 319E, 320E, 320G, 323E, 324E, 324G, 326E, 328, 330C, 335, 338, 344E, 344G, 348, 350, 359, 370, 370C, 375, 385, 410D, 415D, 420D, 425D, 430D, 435, 435D, 440D, 444E, 444G, 446, 447, 448, 450, 450G, 455G, 456, 457, 458, 466, 467, 468, 482C, 485E, 486E, 488E, 490E, 510D, 530B, 535, 540E, 540G-II, 544E, 544G, 546, 547, 548E, 548G-II, 550G, 555G, 556, 557, 558, 566, 567, 568, 570B, 590D, 595D, 608BH, 608L, 608LH, 608SH, 624E, 624G, 640E, 640G, 643D, 643G, 644G, 644H, 644HMH, 644J, 647, 648E, 648G, 650, 650G, 653E, 653G, 657, 667, 670B, 670C, 670CH, 672B, 672CH, 690E, 703G, 703GH, 703JH, 710D, 717, 724J, 727, 740G, 748E, 748G-III, 750C, 753G, 753GH, 753GL, 753J, 753JH, 759G, 759GH, 759J, 759JH, 762B, 770B, 770BH, 770C, 770C II, 770CH, 770CH II, 770D, 772B, 772BH, 772CH, 772CH II, 772D, 790E, 840, 843G, 850C, 853G, 853J, 853JH, 862B, 870D, 872D, 892E, 900, 903G, 903J, 903JH, 909J, 909JH, 911, 940, 953G, 953J, 959J, 960, 1000, 1040, 1140, 1200, 1200A, 1350, 1415D, 1420D, 1425D, 1430D, 1435D, 1440D, 1445D, 1450, 1470, 1500, 1550, 1640, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1750, 1800, 1840, 1850, 1870, 1950, 1950N, 2000, 2040, 2040S, 2054, 2056, 2058, 2064, 2066, 2140, 2150, 2155, 2250, 2254, 2255, 2256, 2258, 2264, 2266, 2266E, 2350, 2355, 2355N, 2450, 2550, 2555, 2650, 2750, 2755, 2850, 2950, 2955, 3029D, 3029DF120, 3029DF124, 3029DF128, 3029DF150, 3029DF151, 3029DF160, 3029DF180, 3029HF270, 3029HFG80, 3029HFU80, 3029T, 3029TF120, 3029TF150, 3029TF152, 3029TF158, 3029TF160, 3029TF180, 3029TF270, 3029TFG80, 3029TFU80, 3040, 3050, 3055, 3100, 3110, 3140, 3150, 3155, 3179DF, 3179T, 3200, 3210, 3255, 3300, 3310, 3350, 3375, 3400, 3410, 3510, 3520, 3522, 3554, 3640, 3650, 3950, 3955, 3970, 3975, 4039D, 4039DF001, 4039DF004, 4039DF005, 4039DF006, 4039DF007, 4039DF008, 4039DF031, 4039DF032, 4039DF092, 4039T, 4039TF001, 4039TF007, 4039TF008, 4045D, 4045DF001, 4045DF092, 4045DF158, 4045HF158, 4045HFU72, 4045HFU79, 4045T, 4045TF001, 4045TF092, 4045TF158, 4045TF258, 4045TFU70, 4219DF01, 4239A, 4239D, 4239DF001, 4239DT004, 4239TF001, 4250, 4276DF01, 4276T, 4276TF01, 4450, 4475, 4890, 4895, 4990, 4995, 5038D, 5039C, 5039D, 5041C, 5042C, 5042D, 5045D, 5045E, 5047D, 5050D, 5050E, 5055D, 5055E, 5065E, 5075E, 5075EF, 5103, 5103E, 5103S, 5104, 5105, 5200, 5203, 5204, 5205, 5210, 5215, 5215F, 5215V, 5220, 5300, 5300N, 5303, 5310, 5310N, 5315, 5315F, 5315V, 5320, 5320N, 5400, 5403, 5410, 5410N, 5415, 5420N, 5440, 5460, 5500, 5500N, 5503, 5510, 5510N, 5515, 5515 HIGH CROP, 5515F, 5515V, 5520N, 5575, 5600, 5615, 5615V, 5700, 5720, 5730, 5820, 5830, 6059DF001, 6059DF092, 6059T, 6059TF, 6059TF001, 6059TF002, 6059TF003, 6059TF004, 6068D, 6068DF, 6068DF001, 6068DFM01, 6068HF158, 6068HF258, 6068HF279, 6068HFU72, 6068HFU74, 6068HFU79, 6068TF001, 6068TF092, 6068TF158, 6068TF258, 6068TFM01, 6076AFM00, 6081AF001, 6081HF001, 6081HF070, 6081HFN02, 6081HFN04, 6081TF001, 6100, 6200, 6200L, 6300, 6300L, 6329DF01, 6359A, 6359DF001, 6359T, 6359TF001, 6400, 6400L, 6414D, 6414T, 6414TDW14, 6414TDW16, 6500, 6500L, 6506, 6600, 6610, 6620, 6650, 6675, 6700, 6710, 6750, 6800, 6810, 6850, 6900, 6910, 6950, 7200, 7400, 7500, 7600, 7700, 7720, 7721, 7722, 7775, 7800, 8100, 8100T, 8110, 8110T, 8200, 8200T, 8210, 8210T, 8300, 8300T, 8310, 8310T, 8400, 8400T, 8410, 8410T, 8820, 8875, 9100, 9200, 9300, 9400, 9410, 9450, 9500, 9510, 9550, 9560, 9560 STS, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9680, 9750 STS, 9760 STS, 9780, 9976, 9986, 9996, BH7, BH8, BH9, BH11, CH570, CH670, CTS, CTS II, LT150, LT160, LT170, LT180, LT190, M653, M655, M665, MCS, P540, R40, ROW-CROP HARVESTING UNITS, ST12 DRAWN, ST12 INTEGRAL, ST16 DRAWN, ST16 INTEGRAL, ST18 DRAWN, W110, W150, W155</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
@@ -2891,6 +3719,12 @@
           <t>H158387</t>
         </is>
       </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S430, S440, S560, S690</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
@@ -2898,6 +3732,12 @@
           <t>N282052</t>
         </is>
       </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>1520 - Drill, Grain, 1520 Integral Grain Drill - PC2513, , 450 - Drill, Grain, 450 Series End-Wheel and Folding Grain Drills (North American Edition) - PC2250, , 455 - Drill, Grain, 455 Series Folding Grain Drills (North American Edition) - PC2333, , 730 - Drill, Air, 730 Air Disk Drill - PC2392, , 730 LL - Drill, Air, 730 LL Air Disk Drill - PC9901, , 740A - Drill, Grain, 740A Mulch Grain Drill (Worldwide Edition) - PC4293, , 9400 - Drill, Grain, 9400 Series Grain Drills and Multiple Hitches (North American Edition) - PC2222, , 9450 - Drill, Grain, 9400 Series Grain Drills and Multiple Hitches (North American Edition) - PC2222</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
@@ -2905,6 +3745,12 @@
           <t>H131088</t>
         </is>
       </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>20 Trailer, 30 Trailer, 630C, 640C, 645C, 678, 744, 946, 956, 1175, 1450, 1470, 1550, 1570, 9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S540, S550, S560, S690, T550, T560, T660, T670, W330, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
@@ -2912,6 +3758,12 @@
           <t>19M8166</t>
         </is>
       </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>6J-1704, 6J-1904, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RT 470, 9RT 470 SCRAPER, 9RT 520, 9RT 520 SCRAPER, 9RT 570, 9RT 570 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 40I, 50I, 200C, 225C, 230C, 250D, 250D-II, 270, 270C, 300D, 300D-II, 300DW, 300WW, 304H, 310 G, 310 P, 310D, 310E, 310G, 310J, 310K, 310K EP, 310L, 310L EP, 310SE, 310SG, 310SJ, 310SK, 310SL, 310SL HL, 312GR, 314G, 315 P, 315D, 315J, 315SE, 315SG, 315SK, 315SL, 316GR, 317G, 318G, 320 P, 324H, 325J, 325SK, 325SL, 326D, 326E, 328D, 328E, 329D, 329E, 330C, 330G, 331G, 332D, 332E, 332G, 333D, 333E, 333G, 344H, 344J, 344K, 344L, 350D, 350DW, 360DC, 370, 370C, 400D, 410 P, 410D, 410E, 410G, 410J, 410K, 410L, 450C, 450G, 450H, 450J, 455G, 460DC, 510D, 540E, 540G-II, 540G-III, 540H, 548E, 548G-II, 548G-III, 548H, 550, 550G, 550H, 550J, 555G, 600C, 604C, 605C, 606C, 607C, 608C, 608L, 608LH, 608SH, 609C, 610C, 611C, 612C, 613C, 614C, 615C, 616C, 617C, 620G, 622G, 640E, 640G, 640H, 640L, 640L-II, 644G, 644H, 644HMH, 648E, 648G, 648H, 648HT, 648L, 648L-II, 650D, 650G, 650H, 650J, 655C, 670C, 670CH, 670G, 672CH, 672G, 700H, 700J, 710 P, 710D, 710G, 710J, 710K, 710L, 740G, 744H, 748E, 748G-III, 748H, 748HT, 748L, 748L-II, 750C, 750J, 750J-II, 750L, 753G, 753GH, 753GL, 753J, 753JH, 755C, 759J, 759JH, 764, 770C, 770CH, 770G, 772CH, 772G, 800C, 848H, 848HT, 850, 850C, 850D, 850J, 850J-II, 850JR, 853G, 870G, 872G, 950C, 953G, 1050C, 1100/1150, 1512E, 1810E, 1814E, 1854, 1854J, 2010DE, 2014DE, 2054, 2112E, 2154D, 2154G, 2156G, 2412DE, 2454D, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2654G, 2656G, 2954D, 3154G, 3156G, 3554, 3754D, 3754G, 3756G, 3800, 5060E, 5070E, 5078E, 5080E, 5090E, 5215, 5215F, 5215V, 5300, 5310, 5315, 5315F, 5315V, 5400, 5410, 5415, 5500, 5510, 5515, 5515 HIGH CROP, 5515F, 5515V, 5615, 5615V, 6010, 6020, 6076AFN, 6076HF030, 6081AF001, 6081AFM01, 6081HF001, 6081HF070, 6081HFN02, 6081HFN03, 6081HFN04, 6081TF001, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100J, 6100M, 6105 MC, 6105 RC, 6105AF001, 6105HF001, 6105M, 6105R, 6110, 6110 MC, 6110 RC, 6110M, 6110R, 6115 MC, 6115 RC, 6115J, 6115M, 6115R, 6120, 6120L, 6120M, 6120R, 6125AF001, 6125HF001, 6125J, 6125M, 6125R, 6130, 6130M, 6130R, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140M, 6140R, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6200L, 6205J, 6210, 6210J, 6210M, 6210R, 6215R, 6220, 6220L, 6230, 6230 Premium, 6230R, 6250R, 6300, 6300L, 6310, 6320, 6320L, 6330, 6330 Premium, 6400, 6400L, 6410, 6420, 6420L, 6420S, 6430, 6430 Premium, 6500L, 6506, 6510, 6510S, 6520, 6520L, 6530, 6530 Premium, 6534, 6534 Premium, 6600, 6610, 6620, 6630, 6630 Premium, 6800, 6810, 6820, 6830, 6830 Premium, 6900, 6910, 6910S, 6920, 6920S, 6930, 7130, 7130 Premium, 7200, 7210, 7220, 7230, 7230 Premium, 7320, 7330, 7330 Premium, 7400, 7410, 7430E, 7510, 7530E, 7600, 7610, 7660, 7700, 7710, 7760, 7800, 7810, 8560, 8570, 8760, 8770, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9230, 9300, 9300T, 9320, 9320T, 9330, 9360R, 9370R, 9400, 9400T, 9410, 9410R, 9420, 9420R, 9420RX, 9420T, 9430, 9430T, 9450, 9460R, 9460RT, 9470 STS, 9470R, 9470RT, 9470RX, 9470RX SCRAPER, 9500, 9501, 9510, 9510R, 9510RT, 9520, 9520R, 9520RT, 9520RX, 9520RX SCRAPER, 9520T, 9520T SCRAPER, 9530T, 9540, 9550, 9560, 9560 STS, 9560R, 9560RT, 9570 STS, 9570R, 9570RT, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620, 9620R, 9620RX, 9620T, 9630T, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, 9986, 9996, BUCK 500, BUCK 650, C670, CP690, CP770, CTS, CTS II, E130, E140, F710, F725, F735, R4040i, R4050i, R4140i, R4150i, S160, S180, S200, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, TRAIL BUCK 500, TRAIL BUCK 650, W110, W150, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
@@ -2926,6 +3778,12 @@
           <t>JD16</t>
         </is>
       </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>112, 115, 118, 120, 200, 210C, 220, 225, 350, 370, 425, 450, 455, 512, 520, 550, 570, 610, 620, 627, 637, 650, 670, 680, 714, 726, 730, 730D, 730LL, 735, 735D, 740D, 856, 886, 913V, 915V, 925D, 930D, 936D, 955, 960, 965, 970, 980, 985, 995, 1065A, 1560, 1590, 1690, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1740, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1810, 1820, 1830, 1835, 1840, 1870, 1990, 2200, 2210LL, 2230FH, 2230LL, 2310, 2330, 2400, 2410C, 2430, 2430C, 2510C, 2510S, 2620, 2623, 2623VT, 2625, 2630, 2633, 2633VT, 2635, 2660VT, 2700, 2720, 2810, 3710, 4250, 4450, 5055E, 5065E, 5075E, 5078E, 5085E, 5105, 5200, 5205, 5210, 5220, 5300, 5303, 5310, 5310N, 5320, 5320N, 5400, 5403, 5410, 5420, 5420N, 5500, 5500N, 5510, 5510N, 5520, 5520N, 5600, 5603, 5605, 5700, 5705, 6300, 6405, 6500, 6600, 6605, 6620, 6700, 7720, DB44, DB58, DB60, DB66, DB80, DB88, DB90, DB120, DR8T, DR12, DR12T, DR16, DR18, DR24, HD35F, HD35R, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, MX225, MX425, P540, P556, PLANTER PERFORMANCE UPGRADES</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
@@ -2933,6 +3791,12 @@
           <t>RE528096</t>
         </is>
       </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>5E-850, 5E-850H, 5E-854, 5E-904, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 5E-1204, 6B-954, 6B-1104/6110B, 6B-1204/6120B, 6E-1004, 6E-1204, 6E-1204P, 6E-1404, 6E-1404L, 6E-1404P, 6E-1404PL, 6E-1504L, 6E-1504PL, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 120D, 130 P, 130G, 160 P, 160D, 160G, 180G, 200 G, 200D, 200G, 210G, 210K, 210K EP, 210L, 210L EP, 210LJ, 250D, 250D-II, 250G, 260 P, 260E, 290G, 300D-II, 300DW, 300G, 300WW, 310 P, 310E, 310J, 310K, 310K EP, 310L, 310L EP, 310SJ, 310SK, 310SL, 310SL HL, 310TJ, 310TK TMC, 315J, 315SK, 315SL, 335D, 337E, 344J, 344K, 344L, 350 P, 350D, 350G, 380 P, 380G, 400R, 408R, 410J, 410K, 410L, 410R, 410TK TMC, 412R, 437D, 437E, 444 G, 444 P, 444J, 444K, 444L, 450J, 450K, 460DC, 524 P, 524K, 524K-II, 524L, 540H, 544 G, 544 P, 544J, 544K, 544K-II, 544L, 548H, 550J, 550K, 600R, 605K, 612R, 616R, 620G, 622G, 624 P, 624J, 624K, 624K-II, 624KR, 624L, 640G, 640H, 640L, 640L-II, 643L, 643L-II, 644 G, 644 P, 644 X, 644G, 644J, 644K, 644K HYBRID, 644L, 644LH, 648G, 648H, 648HT, 648L, 648L-II, 650J, 650K, 655K, 670G, 672G, 700J, 700J-II, 700K, 700L, 700L PL, 703JH, 710J, 710K, 710L, 724 P, 724K, 724L, 744 P, 744K, 744K-II, 744L, 748, 748H, 748HT, 748L, 748L-II, 750J, 750J-II, 750K, 750L, 753J, 753JH, 755K, 759J, 759JH, 764, 768L-II, 770G, 772G, 800R, 803M, 803MH, 824 P, 824L, 843L, 843L-II, 848H, 848HT, 848L, 848L-II, 850J, 850J-II, 850JR, 850K, 850L, 850L PL, 853M, 853MH, 859M, 859MH, 870G, 872G, 903K, 903KH, 903M, 903MH, 909K, 909KH, 909M, 909MH, 910G, 948L, 948L-II, 950K, 953K, 953M, 953MH, 953ML, 959K, 959M, 959MH, 959ML, 1010E, 1010G, 1070E, 1070G, 1110E, 1110G, 1170E, 1170G, 1210E, 1210G, 1270E, 1270G, 1354, 1404, 1450, 1470, 1470D, 1470E, 1470G, 1510E, 1510G, 1550, 1570, 1654, 1854, 1854J, 1910E, 1910G, 2054, 2104, 2144G, 2154D, 2154G, 2156G, 2204, 2654G, 2656G, 2704, 2854, 2904, 3004, 3029HFC03, 3029HFG03, 3029HG530, 3029HI530, 3154G, 3156G, 3204, 3520, 3522, 3754D, 3754G, 3756G, 4045AFM85, 4045CA550, 4045CB551, 4045CC550, 4045CI550, 4045CI551, 4045DF159, 4045HAC04, 4045HAC05, 4045HAC07, 4045HAC09, 4045HB551, 4045HF285, 4045HF286, 4045HF287, 4045HF288, 4045HF289, 4045HFC04, 4045HFC06, 4045HFC07, 4045HFC09, 4045HFC28, 4045HFC92, 4045HFC93, 4045HFC95, 4045HFG04, 4045HFG06, 4045HFG09, 4045HFG82, 4045HFG92, 4045HFG93, 4045HFK04, 4045HFL07, 4045HFL09, 4045HFL92, 4045HFL93, 4045HFS73, 4045HFS82, 4045HFS83, 4045HFS86, 4045HFS87, 4045HFS88, 4045HFU72, 4045HFU79, 4045HFU82, 4045HG551, 4045HI440, 4045HI550, 4045HI551, 4045HLC07, 4045HLC09, 4045HMC04, 4045HMC05, 4045HMC85, 4045HMC92, 4045HN055, 4045HN056, 4045HRT83, 4045HRT90, 4045HYF01, 4045SFM85, 4045T, 4045TF252, 4045TF254, 4045TF276, 4045TF277, 4045TF285, 4045TFC03, 4045TFG03, 4045TFM85, 4045TFU70, 4630, 4730, 4830, 4930, 4940, 5045E, 5050E, 5055E, 5058E, 5060E, 5060EN, 5065E, 5067E, 5070E, 5075E, 5075M, 5080E, 5080EN, 5080R, 5085E, 5085M, 5090E, 5090EL, 5090M, 5090R, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5105M, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5125M, 5125ML, 5125R, 5210, 5305, 5310, 5405, 6068AFM75, 6068AFM85, 6068CG550, 6068CI550, 6068CP550, 6068HB551, 6068HBM01, 6068HBM04, 6068HC550, 6068HCQ01, 6068HCQ05, 6068HCQ06, 6068HCQ07, 6068HF252, 6068HF254, 6068HF279, 6068HF285, 6068HFC08, 6068HFC09, 6068HFC28, 6068HFC48, 6068HFC93, 6068HFC94, 6068HFC95, 6068HFG05, 6068HFG06, 6068HFG08, 6068HFG09, 6068HFG55, 6068HFG82, 6068HFG94, 6068HFG95, 6068HFS01, 6068HFS55, 6068HFS73, 6068HFS82, 6068HFS83, 6068HFS85, 6068HFS86, 6068HFU55, 6068HFU72, 6068HFU74, 6068HFU79, 6068HFU82, 6068HG550, 6068HI550, 6068HN075, 6068HN077, 6068HN078, 6068HP550, 6068HT087, 6068HYF01, 6068SFM75, 6068SFM85, 6068TBM01, 6068TBM02, 6068TF252, 6068TF254, 6068TJ04, 6068TJ12, 6068TJ14, 6068TJ15, 6068TYC50, 6081HF001, 6090 MC, 6090 RC, 6090AFM75, 6090AFM85, 6090CB450, 6090CG550, 6090CI550, 6090CP550, 6090HF475, 6090HF484, 6090HF485, 6090HFC09, 6090HFC47, 6090HFC48, 6090HFC94, 6090HFC95, 6090HFG06, 6090HFG09, 6090HFG84, 6090HFG86, 6090HFG94, 6090HFG95, 6090HFL75, 6090HFL85, 6090HFM85, 6090HFS85, 6090HFS86, 6090HFU84, 6090M, 6090SFM75, 6090SFM85, 6095 MC, 6095 RC, 6100 MC, 6100 RC, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105M, 6105R, 6110 MC, 6110 RC, 6110B, 6110D, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115E, 6115J, 6115M, 6115R, 6120B, 6120E, 6120EH, 6120M, 6120R, 6125D, 6125E MONTENEGRO, 6125J, 6125M, 6125R, 6130, 6130D, 6130E SALTILLO, 6130M, 6130R, 6135B, 6135E, 6135J, 6135M, 6135M MONTENEGRO, 6135R, 6140B, 6140D, 6140M, 6140R, 6145M, 6145R, 6150J, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6205J, 6210J, 6210M, 6210R, 6215R, 6225, 6230, 6230 Premium, 6230R, 6250R, 6325, 6330, 6330 Premium, 6425, 6430, 6430 Premium, 6525, 6530, 6534, 6630, 6830, 6930, 7130, 7130 Premium, 7180, 7195J, 7200, 7200J, 7200R, 7210J, 7210R, 7215J, 7215R, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7330, 7330 Premium, 7460, 7630, 7660, 7730, 7830, 7930, 8100, 8130, 8200, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8310R, 8310RT, 8320R, 8320RT, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400R, 8430, 8430T, 8530, 9230, 9360R, 9370R, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9660, 9660 STS, 9670, 9670 STS, 9680, 9760 STS, 9770 STS, 9780, A400, C2 400, C100, C110, C120, C230, C240, C440, C670, CH330, CH530, CH570, CH670, E130, E140, E240, E240LC, E260, E300LC, E330, E360, E380, E400, F4365, M4025, M4030, M4040, M4040DN, R230, R450, R4023, R4030, R4038, R4040i, R4044, R4045, R4050i, R4060, R4140i, R4150i, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S760, S770, SPRAYER PERFORMANCE UPGRADES, T550, T560, T660, T670, W80, W100, W155, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W540, W550, W650, W660, WL53, WL56, Y110, Y115, Y210, Y215</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
@@ -2940,6 +3804,12 @@
           <t>19M7830</t>
         </is>
       </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>440E, 447, 448, 449, 450E, 450M, 454, 457, 458, 459, 459E, 460M, 460R, 467, 468, 469, 547, 550M, 557, 558, 559, 560M, 560R, 567, 568, 569, 630FD, 630FD PERFORMANCE UPGRADES, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 653, 654, 853, 853J, 853JH, 903J, 903JH, 909J, 909JH, 925D, 930D, 936D, 950K, 953J, 959J, 1745, 1790, 1795, 1870, 2510H, 2510S, 2620, 2623, 2625, 2630, 2633, 2635, 4710, 4720, 6488, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7455, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8000, 8400, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, 9970, CP690, CS690, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, L330, L331, L340, L341, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1100, Y210, Y215</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
@@ -2947,6 +3817,12 @@
           <t>19M7830</t>
         </is>
       </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>440E, 447, 448, 449, 450E, 450M, 454, 457, 458, 459, 459E, 460M, 460R, 467, 468, 469, 547, 550M, 557, 558, 559, 560M, 560R, 567, 568, 569, 630FD, 630FD PERFORMANCE UPGRADES, 635FD, 635FD PERFORMANCE UPGRADES, 640FD, 640FD PERFORMANCE UPGRADES, 653, 654, 853, 853J, 853JH, 903J, 903JH, 909J, 909JH, 925D, 930D, 936D, 950K, 953J, 959J, 1745, 1790, 1795, 1870, 2510H, 2510S, 2620, 2623, 2625, 2630, 2633, 2635, 4710, 4720, 6488, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7455, 7480, 7500, 7550, 7580, 7660, 7700, 7750, 7760, 7780, 7800, 7850, 7950, 7980, 8000, 8400, 9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, 9970, CP690, CS690, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, L330, L331, L340, L341, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1100, Y210, Y215</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
@@ -2954,6 +3830,12 @@
           <t>03M7183</t>
         </is>
       </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>5-750, 5-754, 5-800, 5-804, 5-900, 5B-700, 5B-704, 5B-750, 5B-754, 5E-704, 5E-850, 5E-854, 5E-950, 5E-954, 5E-1000, 5E-1004, 5E-1200, 6A-1104, 6A/1204, 6A/1354, 6B-1204/6120B, 6J-1704, 6J-1904, 6M-1654, 6M-1854, 6M-2104, 6R 110, 6R 120, 6R 130, 6R 140, 6R 145, 6R 150, 6R 155, 6R 165, 6R 175, 6R 185, 6R 195, 6R 215, 6R 230, 6R 250, 6R 2304, 7G18, 7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 12.5HP, 13HP, 14HP, 15HP, 16HP, 17HP, 20 Trailer, 26, 30 Trailer, 31C, 40, 42, 47 IN., 48 IN., 50 in., 54, 54 in., 54D IN., 59 IN., 60 in., 60 IN. DECKS, 60D IN., 62 IN., 72, 72 IN., 100, 102, 105, 107, 108, 110, 110 TLB, 111, 112L, 115, 120D, 125, 135, 145, 155C, 160, 170, 175, 180, 180A, 180B, 180C, 180E, 180SL, 185, 190C, 205C, 206C, 210 G, 210 P, 210C, 210K, 210K EP, 210L, 210L EP, 210LJ, 220, 220A, 220B, 220C, 220SL, 222R, 240, 243, 244, 245, 246, 260, 260B, 260C, 260SL, 265, 270A, 270B, 285, 300D, 310D, 312GR, 313, 314G, 315, 315D, 316GR, 317G, 318D, 318E, 318G, 319D, 319E, 320, 320D, 320E, 323D, 323E, 324E, 325, 326D, 326E, 328, 328D, 328E, 329D, 329E, 330G, 331G, 332D, 332E, 332G, 333D, 333E, 333G, 335, 338, 339, 343, 344, 345, 348, 349, 355, 359, 360, 375, 385, 390, 410D, 415, 425, 430D, 435, 435D, 440D, 440E, 443, 444, 445, 446, 447, 448, 449, 450, 450E, 450G, 450M, 454, 455, 455G, 456, 457, 458, 459, 459E, 460M, 460R, 460S, 466, 467, 468, 469, 493, 494, 500R, 510D, 525, 530, 531, 533, 535, 540R, 543, 543M, 543R, 545, 546, 547, 550, 550G, 550M, 551, 554, 555G, 556, 557, 558, 559, 560M, 560R, 565, 566, 567, 568, 569, 570, 572, 575, 578, 580, 582, 583, 590, 592, 594, 600R, 603M, 603R, 606C, 606C PERFORMANCE UPGRADES, 608C, 608C PERFORMANCE UPGRADES, 612C, 612C PERFORMANCE UPGRADES, 612FC, 612FC PERFORMANCE UPGRADES, 615F, 615P, 616, 616C, 616C PERFORMANCE UPGRADES, 616F, 616R, 618, 618C, 618C PERFORMANCE UPGRADES, 618F, 618R, 620, 620F, 620R, 622, 622F, 622R, 622X, 623, 623M, 623R, 625, 625D, 625F, 625R, 625X, 630, 630C, 630D, 630F, 630FD, 630FD PERFORMANCE UPGRADES, 630R, 630X, 631, 633, 635, 635D, 635F, 635FD, 635FD PERFORMANCE UPGRADES, 635R, 635X, 640C, 640D, 640FD, 640FD PERFORMANCE UPGRADES, 640R, 640X, 643, 643M, 643R, 644, 645, 645C, 645FD, 645FD PERFORMANCE UPGRADES, 647, 650, 650G, 651, 653, 654, 655, 660, 660R, 661, 663, 663R, 665, 670, 673, 676, 678, 680, 680R, 681, 683, 683R, 690, 692, 693, 694, 696, 698, 706C, 706C PERFORMANCE UPGRADES, 708C, 708C PERFORMANCE UPGRADES, 710D, 712C, 712C PERFORMANCE UPGRADES, 712FC, 712FC PERFORMANCE UPGRADES, 716C, 716C PERFORMANCE UPGRADES, 718C, 718C PERFORMANCE UPGRADES, 722PF, 722X, 725D, 725PF, 725X, 730, 730D, 730FD, 730FD PERFORMANCE UPGRADES, 730PF, 730X, 731, 735, 735D, 735FD, 735FD PERFORMANCE UPGRADES, 735PF, 735X, 737, 740D, 740FD, 740FD PERFORMANCE UPGRADES, 740PF, 740X, 744, 745FD, 745FD PERFORMANCE UPGRADES, 748, 750C, 750K, 751, 753, 755, 756, 757, 777, 797, 805, 830, 835, 842, 843, 844, 850C, 850K, 852, 853, 854, 855, 856, 862, 864, 892, 893, 894, 896, 904, 912, 913, 914, 915F, 915R, 916, 918, 918F, 918R, 920, 920D, 920F, 920R, 922, 922F, 922R, 924, 925, 925D, 925F, 925R, 926, 930, 930D, 930F, 930R, 936, 936D, 946, 955, 956, 960, 990, 994, 995, 997, 1015, 1023E, 1025R, 1026R, 1030, 1035, 1054, 1092, 1107, 1109, 1111, 1113, 1165, 1170, 1175, 1243, 1290, 1291, 1293, 1354, 1404, 1430D, 1435D, 1438GS, 1438HS, 1440D, 1445D, 1450, 1470, 1512FX, 1516FX, 1524FX, 1535, 1538GS, 1538HR, 1538HS, 1542, 1542GS, 1542HS, 1550, 1570, 1590, 1642HS, 1642HV, 1646, 1646HS, 1646HV, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725T, 1730, 1735, 1740, 1742GS, 1742HS, 1742PR, 1745, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1842GV, 1842HV, 1846, 1848GV, 1848HV, 1854, 1854J, 1948GV, 1948HV, 2025R, 2026R, 2027R, 2032R, 2036R, 2046HV, 2048HV, 2054, 2056, 2058, 2064, 2066, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, 2148HV, 2204, 2243, 2250, 2254, 2254HV, 2256, 2258, 2264, 2266, 2266E, 2305, 2320, 2354, 2355, 2400 PRECISIONCUT, 2450, 2500 DIESEL, 2500 GAS, 2500A, 2500B, 2500E, 2550 E-CUT HYBRID TRIPLEX MOWER, 2550 PRECISIONCUT TRIPLEX MOWER, 2554HV, 2554ST, 2555, 2650, 2653, 2653A, 2653B, 2704, 2755, 2850, 2904, 2955, 3004, 3025E, 3033R, 3038E, 3038R, 3039R, 3045R, 3046R, 3050, 3055, 3155, 3204, 3255, 3320, 3325, 3350, 3365, 3520, 3522, 3650, 3720, 3950, 3955, 3970, 3975, 4044R, 4049M, 4049R, 4052R, 4066R, 4200, 4210, 4300, 4310, 4320, 4400, 4410, 4520, 4630, 4720, 4730, 4830, 4890, 4895, 4990, 4995, 5045E, 5050E, 5055E, 5058E, 5060E, 5060EN, 5065E, 5065M, 5067E, 5070M, 5075E, 5075EF, 5075EN, 5075M, 5076E, 5076EF, 5076EL, 5076EN, 5080EN, 5080M, 5080R, 5082E, 5083E, 5085E, 5085M, 5090E, 5090EH, 5090EL, 5090EN, 5090M, 5090R, 5093E, 5095M, 5095MH, 5100E, 5100M, 5100MH, 5100ML, 5100R, 5101E, 5105M, 5105MH, 5105ML, 5115M, 5115ML, 5115R, 5115RH, 5120M, 5120ML, 5125M, 5125ML, 5125R, 5130ML, 5200, 5210, 5220, 5225, 5300, 5310, 5310N, 5320, 5320N, 5325, 5400, 5405, 5410, 5415, 5420, 5420N, 5425, 5500, 5500N, 5510, 5510N, 5520, 5520N, 5525, 5603, 5615, 5620, 5625, 5715, 5720, 5725, 5820, 6020, 6090 MC, 6090 RC, 6090M, 6095 MC, 6095 RC, 6100, 6100 MC, 6100 RC, 6100B, 6100D, 6100E ROSARIO, 6100E SALTILLO, 6100M, 6105 MC, 6105 RC, 6105D, 6105E, 6105EH, 6105J, 6105M, 6105R, 6110 MC, 6110 RC, 6110B, 6110D, 6110E ROSARIO, 6110E SALTILLO, 6110M, 6110R, 6115 MC, 6115 RC, 6115D, 6115M, 6115R, 6120, 6120E, 6120EH, 6120L, 6120M, 6120R, 6125D, 6125E ROSARIO, 6125E SALTILLO, 6125M, 6125R, 6130, 6130D, 6130M, 6130R, 6135E, 6135M, 6135M MONTENEGRO, 6135R, 6140D, 6140J, 6140JH, 6140M, 6140R, 6145M, 6145R, 6150M, 6150M MONTENEGRO, 6150R, 6150RH, 6155J, 6155JH, 6155M, 6155MH, 6155R, 6155RH, 6165J, 6170J, 6170M, 6170M MONTENEGRO, 6170R, 6175M, 6175R, 6180J, 6185J, 6190J, 6190M, 6190R, 6195M, 6195R, 6200, 6205J, 6210J, 6210M, 6210R, 6215R, 6220, 6220L, 6230, 6230 Premium, 6230R, 6250R, 6300, 6320, 6320L, 6330, 6330 Premium, 6400, 6403, 6415, 6420, 6420L, 6420S, 6425, 6430, 6430 Premium, 6500L, 6520, 6520L, 6530, 6530 Premium, 6534 Premium, 6603, 6610, 6620, 6630, 6630 Premium, 6650, 6700A PRECISIONCUT, 6710, 6750, 6800, 6810, 6820, 6830, 6830 Premium, 6850, 6900, 6910, 6920, 6920S, 6930, 6950, 7130, 7130 Premium, 7180, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7220, 7225J, 7230, 7230 Premium, 7230J, 7230R, 7250, 7250R, 7260, 7270R, 7280, 7290R, 7300, 7310R, 7320, 7330, 7330 Premium, 7350, 7380, 7400, 7405, 7410, 7420, 7425, 7430E, 7450, 7455, 7460, 7480, 7500, 7510, 7520, 7525, 7530E, 7550, 7580, 7600, 7610, 7630, 7660, 7700, 7700A PRECISIONCUT, 7710, 7715, 7720, 7730, 7750, 7760, 7780, 7800, 7810, 7815, 7820, 7830, 7850, 7920, 7930, 7950, 7980, 8100, 8200, 8225R, 8245R, 8270R, 8295R, 8300, 8310RT, 8320R, 8320RT, 8335R, 8335RT, 8345R, 8345RT, 8360RT, 8370R, 8370RT, 8400, 8400R, 8500, 8560, 8570, 8600, 8700, 8700A PRECISIONCUT, 8760, 8770, 8800, 8870, 8960, 8970, 9100, 9120, 9200, 9220, 9300, 9320, 9400, 9410, 9420, 9450, 9470 STS, 9500, 9501, 9510, 9520, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9620, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9700, 9750 STS, 9760 STS, 9770 STS, 9780, 9800, 9860 STS, 9870 STS, 9880 STS, 9900, 9935, 9970, 9976, 9986, 9996, 15538, A420R, A520R, AMT600, BP15, C1 200, C2 300, C100, C110, C120, C300, C310R, C350, C350R, C400, C440R, C441R, C450, C451R, C461R, C500, C670, CP20, CP690, CP770, CS690, CS770, CT315, CTS, CTS II, D100, D105, D110, D120, D125, D130, D140, D150, D155, D160, D170, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR12, DR12T, DR16, DR18, DR24, E180, F440M, F440R, F441M, F441R, F510, F525, F710, F725, F735, G100, G110, GROUPER, GT225, GT242, GT245, GT262, GT275, GX85, GX255, GX325, GX335, GX345, GX355, H240, H260, H310, H340, H360, H380, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, HX10, HX14, L70, L100, L105, L107, L108, L110, L111, L118, L120, L130, L330, L331, L340, L341, L624, L633, L634, L2554, LA100, LA105, LA110, LA115, LA120, LA125, LA130, LA135, LA140, LA145, LA150, LA155, LA165, LA175, LT133, LT150, LT155, LT160, LT166, LT170, LT180, LT190, LTR155, LTR166, LTR180, LX172, LX173, LX176, LX178, LX186, LX188, LX255, LX266, LX277, LX279, LX280, LX288, LX289, MaxEmerge XP, MCS, MX8, MX10, PLANTER PERFORMANCE UPGRADES, R40, R310R, R350R, R400, R500, R870R, R930R, R950R, R990R, RD30F, RD30F PERFORMANCE UPGRADES, RD35F, RD35F PERFORMANCE UPGRADES, RD40F, RD40F PERFORMANCE UPGRADES, RD45F, RD45F PERFORMANCE UPGRADES, REDEKOP SCU, ROW-CROP HARVESTING UNITS, S180, S240, S250, S300, S310R, S350, S350R, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, S1642, S1742, S2046, S2048, S2348, S2546, S2554, SH8R, SH12F, SH12R, SST15, SST16, SST18, STRAIGHT BLADE, STX30, STX38, STX46, SX85, T550, T560, T660, T670, TH 6X4, TS 4X2, TURF TX 4X2, TX 4X2, V451G, V451M, V451R, V461M, V461R, W70, W100, W170, W200M, W210, W230, W235, W235M, W235R, W260, W260R, W330, W430, W440, W540, W550, W650, W660, X9 1000, X9 1100, X110, X120, X125, X135R, X140, X145, X155R, X165, X300, X304, X310, X320, X324, X340, X360, X465, X475, X485, X495, X500, X520, X530, X534, X540, X570, X575, X580, X584, X585, X590, X595, X700, X710, X720, X724, X728, X729, X730, X734, X738, X739, X740, X744, X748, X749, X750, X754, X758, X940, X948, X949, X950R, XUV 550 S4, XUV560, XUV560 S4, XUV560E, XUV590I, XUV590I S4, XUV590M, XUV590M S4, Z225, Z235, Z245, Z255, Z345R, Z355R, Z375R, Z425, Z435, Z445, Z465, Z535M, Z540M, Z625, Z645, Z655, Z665, Z997R</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
@@ -2961,6 +3843,12 @@
           <t>N331364</t>
         </is>
       </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>1890 - Drill, Air, 1890 No-Till Air Drill (3-Section) - PC9227, , 1890 - Drill, Air, 1890 No-Till Air Drill (5-Section) - PC11647, , 1895 - Drill, Air, 1895 No-Till Air Drill (3-Section) - PC9228, , CCS - Cart, Commodity, 1990 CCS Air Drill - PC9494, , CCS - Drill, Air, 1990 CCS Air Drill - PC9494, , 1990 - Drill, Air, 1990 CCS Air Drill - PC9494, , 1990 - Cart, Commodity, 1990 CCS Air Drill - PC9494, , 2510C - Applicator, 2510C Conventional Applicator - PC9779, , 2510H - Applicator, 2510H High Speed Low Disturbance Applicator - PC9780, , 2510S - Applicator, 2510S Strip Tillage Applicator - PC9647</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
@@ -2968,6 +3856,12 @@
           <t>N167577</t>
         </is>
       </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>1060 - Tool, Seeding, 1060 Seeding Tool - PC2273, , 2200 - Cultivator, Field, 2200 Field Cultivator - PC2764, , 2210 - Cultivator, Field, 2210 Field Cultivator - PC9379, , 2210 - Cultivator, Field, 2210 Level Lift Field Cultivator - PC9380, , 410A - Tiller, Mulch, 410A Mulch Tiller (European Edition) - PC4291, , 515 - Drill, Soybean and Grain, 515 Series Integral Soybean and Grain Drills - PC1912, , 520 - Drill, Soybean and Grain, 520 Series Integral Soybean and Grain Drills - PC1893, , 722 - Tiller, Mulch, 722 Finisher Mulch Tiller - PC1954, , 724 - Tiller, Mulch, 724 Finisher Mulch Tiller - PC2244, , 726 - Tiller, Mulch, 726 Mulch Finisher - PC2379, , 770 - Drill, Air, 770 Air Drill - PC2017, , 780 - Drill, Air, 780 Air Drill - PC2019, , 8350 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8500 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8000 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8250 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8100 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8200 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8300 - HITCH, GRAIN DRILL, 8000 Series Grain Drills and Grain Drill Hitches - PC1446, , 8500 - Drill, Grain, 8500 Series 3-Section Folding Grain Drill - PC2136, , 9000 - Drill, Grain, 9000 Series Grain Drills and Two-Drill and Three-Drill and Grain Drill Hitches - PC1593, , 960 - Cultivator, Field, 960 Series Field Cultivators - PC2161, , 980 - Cultivator, Field, 980 Field Cultivator - PC2390, , 985 - Cultivator, Field, 985 Field Cultivator - PC2378, , 420A - Mulch Finisher, Mulch Finisher 420A (European Edition) - PC4292</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
@@ -2975,6 +3869,16 @@
           <t>N133705</t>
         </is>
       </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>1520 - Drill, Grain, 1520 Integral Grain Drill - PC2513, , 1530 - Drill, Tru-Vee, 1530 Tru-Vee Drill - PC2659, , 1535 - Drill, Grain, 1535 Tru-Vee Integral Grain Drill (North American Edition) - PC2806, , 200 - THINNER, SYNCHRONOUS, 200 Crop Thinner - PC1447, , 400 - HOE, Rotary, 400 Series Folding Universal Rotary Hoes - PC1710, , 440 - HOE, Rotary, 400 Series Folding Universal Rotary Hoes - PC1710, , 430 - HOE, Rotary, 400 Series Folding Universal Rotary Hoes - PC1710, , 428 - HOE, Rotary, 400 Series Folding Universal Rotary Hoes - PC1710, , 430 - HOE, Rotary, 415, 420, 428 and 430 Universal Rotary Hoes - PC1319, , 428 - HOE, Rotary, 415, 420, 428 and 430 Universal Rotary Hoes - PC1319, , 415 - HOE, Rotary, 415, 420, 428 and 430 Universal Rotary Hoes - PC1319, , 420 - HOE, Rotary, 415, 420, 428 and 430 Universal Rotary Hoes - PC1319, , 530 - HITCH, GRAIN DRILL, 530 Transport Hitch Grain Drill - PC1913, , 665 - Seeder, CENTRAL METERING, 665 Central Metering Seeder - PC1840, , 780 - Drill, Air, 780 Air Drill - PC2019, , 785 - Drill, Air, 785 Air Drill - PC2020, , 845 - Cultivator, Row-Crop, 845 Series Folding Row-Crop Cultivator - PC1867, , 85 - Cultivator, Row-Crop, 85 Series Folding Row-Crop Cultivator - PC1709, , 856 - ROW CROP Cultivator, 856 Row Crop Cultivator - PC2554, , RM - Cultivator, Row-Crop, RM Series Row-Crop Cultivators - PC1273</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
@@ -2982,6 +3886,12 @@
           <t>A23249</t>
         </is>
       </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>1035 - Planter, 1035 Planter (Mexico Edition) - PC6134, , 7000 - Planter, Attachment, 7000 and 7100 MAXEMERGE Planting Units and Attachments - PC2604, , 7100 - Planter, Attachment, 7000 and 7100 MAXEMERGE Planting Units and Attachments - PC2604, , 7000 - Planter, Unit, 7000 and 7100 MAXEMERGE Planting Units and Attachments - PC2604, , 7000 - Planter, 7000 and 7100 MAXEMERGE Planting Units and Attachments - PC2604, , 7100 - Planter, Unit, 7000 and 7100 MAXEMERGE Planting Units and Attachments - PC2604, , 7100 - Planter, 7000 and 7100 MAXEMERGE Planting Units and Attachments - PC2604, , 7000 - Planter, 7000 Drawn Cotton and Corn Planter - PC1467</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
@@ -2989,6 +3899,16 @@
           <t>A46533</t>
         </is>
       </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>1035, 1512FX, 1516FX, 1524FX, 1700, 1700T, 1705, 1705T, 1710, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1750, 1755, 1760, 1760NT, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, 1900, 1910, 2109, 2111, 2113, 2115, 2117, 2122, 2126, 2130, 2134, DB37, DB40, DB41, DB44, DB50, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, MaxEmerge XP, PLANTER PERFORMANCE UPGRADES, Pro-Series XP</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
@@ -2996,6 +3916,12 @@
           <t>H171040</t>
         </is>
       </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
@@ -3003,6 +3929,12 @@
           <t>AH165012</t>
         </is>
       </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
@@ -3010,6 +3942,12 @@
           <t>H131088</t>
         </is>
       </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>20 Trailer, 30 Trailer, 630C, 640C, 645C, 678, 744, 946, 956, 1175, 1450, 1470, 1550, 1570, 9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S540, S550, S560, S690, T550, T560, T660, T670, W330, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
@@ -3017,6 +3955,12 @@
           <t>R121195</t>
         </is>
       </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>250D, 300D, 300DW, 370, 415D, 420D, 425D, 430D, 435D, 440D, 530B, 535, 540G-II, 548G-II, 640G, 644G, 644H, 644HMH, 648G, 653E, 740G, 748G-II, 748G-III, 750C, 762B, 770C, 770C II, 770CH, 770CH II, 772CH, 772CH II, 848G, 850C, 1185, 1415D, 1420D, 1425D, 1430D, 1435D, 1440D, 1445D, 1450, 1550, 1570, 2254, 2256, 2258, 2264, 2266, 2266E, 3510, 6076AFM30, 6076AFN, 6076HF030, 6081AF001, 6081AFM01, 6081HF001, 6081TF001, 6650, 6750, 6850, 6950, 7610, 7710, 7810, 8100, 8100T, 8110, 8110T, 8200, 8200T, 8210, 8210T, 8300, 8300T, 8310, 8310T, 8400, 8400T, 8410, 8410T, 9100, 9200, 9300, 9400, 9500, 9510, 9550, 9600, 9610, 9650, 9650 STS, 9750 STS, 9780, 9970, 9976, 9986, CTS, CTS II</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
@@ -3045,6 +3989,8 @@
           <t>DE31283</t>
         </is>
       </c>
+      <c r="B316" t="inlineStr"/>
+      <c r="C316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
@@ -3052,6 +3998,12 @@
           <t>DE3138</t>
         </is>
       </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>CP770, CS770, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T560, T660, T670, W650, W660</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
@@ -3080,6 +4032,8 @@
           <t>DE31282</t>
         </is>
       </c>
+      <c r="B321" t="inlineStr"/>
+      <c r="C321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
@@ -3101,6 +4055,12 @@
           <t>DE31746</t>
         </is>
       </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>9470 STS, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9870 STS, 9880 STS, 9970, C670, S560, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
@@ -3108,6 +4068,12 @@
           <t>DE31747</t>
         </is>
       </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>9470 STS, 9540, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9870 STS, 9880 STS, 9970, C670, S560, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
@@ -3122,6 +4088,16 @@
           <t>AH224518</t>
         </is>
       </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9970 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 6068HN052 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 6076AN031 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 6081AN001 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 9970 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723, , 6076AN031 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723, , 6068HN052 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723, , 6081AN001 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
@@ -3164,6 +4140,16 @@
           <t>AH224518</t>
         </is>
       </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9970 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 6068HN052 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 6076AN031 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 6081AN001 - Picker, Cotton, 9970 Cotton Picker - PC2602, , 9970 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723, , 6076AN031 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723, , 6068HN052 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723, , 6081AN001 - Picker, Cotton, 9970 Cotton Picker (S.N. -1YC9970XXX0020000)(China Edition) - PC11723</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="inlineStr">
@@ -3171,6 +4157,12 @@
           <t>AH222366</t>
         </is>
       </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" s="1" t="inlineStr">
@@ -3178,6 +4170,12 @@
           <t>AH219846</t>
         </is>
       </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" s="1" t="inlineStr">
@@ -3185,6 +4183,12 @@
           <t>A52062</t>
         </is>
       </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>7200 - Planter, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 1760 - Planter, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 1780 - Planter, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 7200 - Planter, Unit, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 7300 - Planter, Unit, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 7300 - Planter, Attachment, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 7200 - Planter, Attachment, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 7300 - Planter, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 1760 - Planter, Unit, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 1780 - Planter, Unit, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 1760 - Planter, Attachment, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290, , 1780 - Planter, Attachment, 7200 and 7300 MAXEMERGE 2, 1760 and 1780 Planting Units and Attachments - PC2290</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" s="1" t="inlineStr">
@@ -3192,6 +4196,12 @@
           <t>A92817</t>
         </is>
       </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>1025, 1035, 1512FX, 1516FX, 1524FX, 1535, 1700, 1705, 1705T, 1715, 1720, 1720 CCS, 1725, 1725 CCS, 1725C, 1725NT, 1725T, 1730, 1735, 1745, 1750, 1755, 1760, 1765, 1770, 1770NT, 1775, 1775NT, 1780, 1785, 1790, 1795, DB37, DB41, DB44, DB55, DB58, DB60, DB60T, DB62, DB66, DB74, DB80, DB83, DB88, DB90, DB120, DL12, DL16, DR8T, DR12, DR12T, DR16, DR18, DR24, MaxEmerge XP, PLANTER PERFORMANCE UPGRADES, Pro-Series XP</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" s="1" t="inlineStr">
@@ -3199,6 +4209,12 @@
           <t>AH113139</t>
         </is>
       </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9500, 9501, 9510, 9540, 9550, 9560, 9580, 9600, 9610, 9640, 9650, 9660, 9670, 9680, 9780, C670, CTS, CTS II, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" s="1" t="inlineStr">
@@ -3206,6 +4222,12 @@
           <t>AH219844</t>
         </is>
       </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" s="1" t="inlineStr">
@@ -3213,6 +4235,12 @@
           <t>H227696</t>
         </is>
       </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>2730, 9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, DB80, DB88, DB90, DB120, S560, S690, ST12 DRAWN, ST16 DRAWN, ST18 DRAWN</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" s="1" t="inlineStr">
@@ -3220,6 +4248,16 @@
           <t>HXE10455</t>
         </is>
       </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>1775NT, DB37, DB40, DB44, DB50, DB55, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, S430, S440, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="inlineStr">
@@ -3234,6 +4272,16 @@
           <t>AH202772</t>
         </is>
       </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="inlineStr">
@@ -3241,6 +4289,12 @@
           <t>H227696</t>
         </is>
       </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>2730, 9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, DB80, DB88, DB90, DB120, S560, S690, ST12 DRAWN, ST16 DRAWN, ST18 DRAWN</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" s="1" t="inlineStr">
@@ -3248,6 +4302,16 @@
           <t>HXE10455</t>
         </is>
       </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>1775NT, DB37, DB40, DB44, DB50, DB55, DB60, DB62, DB66, DB74, DB80, DB83, DB88, DB90, HD35F, HD35R, HD35X, HD40F, HD40R, HD40X, HD45F, HD45R, HD45X, HD50F, HD50R, S430, S440, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="inlineStr">
@@ -3255,6 +4319,12 @@
           <t>AH222366</t>
         </is>
       </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" s="1" t="inlineStr">
@@ -3262,6 +4332,16 @@
           <t>AH202772</t>
         </is>
       </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="inlineStr">
@@ -3269,6 +4349,16 @@
           <t>AH202631</t>
         </is>
       </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="inlineStr">
@@ -3276,6 +4366,12 @@
           <t>AXE16294</t>
         </is>
       </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" s="1" t="inlineStr">
@@ -3290,6 +4386,12 @@
           <t>AH220452</t>
         </is>
       </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>9560STS - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH028 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH019 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6068HH058 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 9560 - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 9560i - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 6090HH005 - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , i-Series - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" s="1" t="inlineStr">
@@ -3297,6 +4399,16 @@
           <t>AH159247</t>
         </is>
       </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>9560STS - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH028 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH019 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6068HH058 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="inlineStr">
@@ -3311,6 +4423,16 @@
           <t>H166313</t>
         </is>
       </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>30R, 46R, 493, 494, 594, 604C, 605C, 606C, 607C, 608C, 608C PRECISION UPGRADES, 608FC, 609C, 610C, 611C, 612C, 612FC, 613C, 614C, 615C, 616C, 617C, 618C, 639, 649, 659, 692, 693, 694, 706C, 708C, 708FC, 712C, 712FC, 716C, 718C, 891, 892, 893, 894, 995, 1092, 1290, 1291, 1293, 1295, 9450, 9470 STS, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C6R, C6R PRECISION UPGRADES, C8F, C8F PRECISION UPGRADES, C8R, C8R PRECISION UPGRADES, C12F, C12F PRECISION UPGRADES, C12R, C12R PRECISION UPGRADES, C16F, C16F PRECISION UPGRADES, C16R, C16R PRECISION UPGRADES, C18F, C18F PRECISION UPGRADES, C18R, C18R PRECISION UPGRADES, C670, CTS, S540, S550, S560, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="inlineStr">
@@ -3318,6 +4440,12 @@
           <t>AH155256</t>
         </is>
       </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>9560STS - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH028 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH019 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6068HH058 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" s="1" t="inlineStr">
@@ -3346,6 +4474,12 @@
           <t>H161342</t>
         </is>
       </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>20 Trailer, 30 Trailer, 1450, 1470, 1550, 1570, 1910, 9450, 9470 STS, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, C850, CTS, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1100</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" s="1" t="inlineStr">
@@ -3360,6 +4494,12 @@
           <t>H207095</t>
         </is>
       </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" s="1" t="inlineStr">
@@ -3367,6 +4507,12 @@
           <t>AH93110</t>
         </is>
       </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>2054, 2056, 2058, 2064, 2066, 6620, 7720, 7722, 8820, 9400, 9410, 9450, 9500, 9501, 9510, 9550, 9560, 9600, 9610, 9650, 9650 STS, 9750 STS, CTS, CTS II, S430, S440</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" s="1" t="inlineStr">
@@ -3374,6 +4520,12 @@
           <t>R40915</t>
         </is>
       </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>7R 210, 7R 230, 7R 250, 7R 270, 7R 290, 7R 310, 7R 330, 7R 350, 8R 230, 8R 250, 8R 280, 8R 310, 8R 340, 8R 370, 8R 410, 8R 2304, 8R 2704, 8R 3004, 8RT 310, 8RT 340, 8RT 370, 8RT 410, 8RX 310, 8RX 340, 8RX 370, 8RX 410, 9R 390, 9R 440, 9R 490, 9R 490 SCRAPER, 9R 540, 9R 540 SCRAPER, 9R 590, 9R 590 SCRAPER, 9R 640, 9R 640 SCRAPER, 9RX 490, 9RX 490 SCRAPER, 9RX 540, 9RX 540 SCRAPER, 9RX 590, 9RX 590 SCRAPER, 9RX 640, 2204, 2704, 2854, 2904, 3004, 3204, 4650, 4850, 5225, 5325, 5325N, 5425, 5425N, 5525, 5525N, 5625, 6103, 6800, 6810, 6900, 6910, 6910S, 7185J, 7195J, 7200, 7200J, 7200R, 7205J, 7210, 7210J, 7210R, 7215J, 7215R, 7225J, 7230J, 7230R, 7250R, 7260R, 7270R, 7280R, 7290R, 7310R, 7400, 7405, 7410, 7500, 7505, 7510, 7600, 7610, 7630, 7700, 7710, 7715, 7720, 7730, 7800, 7810, 7815, 7820, 7830, 7920, 7930, 8100, 8100T, 8110, 8110T, 8120, 8120T, 8130, 8200, 8200T, 8210, 8210T, 8220, 8220T, 8225R, 8230, 8230T, 8235R, 8245R, 8260R, 8270R, 8285R, 8295R, 8295RT, 8300, 8300T, 8310, 8310R, 8310RT, 8310T, 8320, 8320R, 8320RT, 8320T, 8330, 8330T, 8335R, 8335RT, 8345R, 8345RT, 8360R, 8360RT, 8370R, 8370RT, 8400, 8400R, 8400T, 8410, 8410T, 8420, 8420T, 8430, 8430T, 8440, 8450, 8520, 8520T, 8530, 8630, 8640, 8650, 8850, 9410, 9420R, 9420RX, 9450, 9470R, 9470RX, 9470RX SCRAPER, 9510, 9520R, 9520RX, 9520RX SCRAPER, 9540, 9550, 9560, 9570R, 9570RX, 9570RX SCRAPER, 9580, 9600, 9610, 9620R, 9620RX, 9640, 9650, 9650 STS, 9660, 9670, 9680, 9750 STS, 9780, 9880 STS, C670, CTS, CTS II, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" s="1" t="inlineStr">
@@ -3388,6 +4540,12 @@
           <t>AH223015</t>
         </is>
       </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" s="1" t="inlineStr">
@@ -3395,6 +4553,12 @@
           <t>AH223014</t>
         </is>
       </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" s="1" t="inlineStr">
@@ -3402,6 +4566,12 @@
           <t>HXE104073</t>
         </is>
       </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>S7 600, S7 700, S7 800, S7 850, S7 900, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" s="1" t="inlineStr">
@@ -3409,6 +4579,12 @@
           <t>AH201433</t>
         </is>
       </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>614R, 615F, 615R, 616, 616F, 616R, 618, 618F, 618PF, 618R, 620, 620F, 620PF, 620R, 622, 622F, 622PF, 622R, 625F, 625PF, 625R, 630, 630F, 630PF, 630R, 635, 635F, 635PF, 635R, ZPF618, ZPF620, ZPF622, ZPF625, ZPF630, ZPF635</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" s="1" t="inlineStr">
@@ -3423,6 +4599,12 @@
           <t>AH223014</t>
         </is>
       </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" s="1" t="inlineStr">
@@ -3430,6 +4612,12 @@
           <t>AH223015</t>
         </is>
       </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" s="1" t="inlineStr">
@@ -3444,6 +4632,12 @@
           <t>H202347</t>
         </is>
       </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>9470STS - Combine, 9470 STS Combine (South American Edition) - PC8626, , 6068HCQ04 - Combine, 9470 STS Combine (South American Edition) - PC8626, , 9560STS - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH028 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH019 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6068HH058 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 9560 - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 9560i - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 6090HH005 - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , i-Series - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 9570STS - Combine, 9570 STS Self-Propelled Combine (North American Edition) - PC9659, , 6068HH059 - Combine, 9570 STS Self-Propelled Combine (North American Edition) - PC9659, , 6068HH062 - Combine, 9570 STS Self-Propelled Combine (North American Edition) - PC9659, , 6068HH061 - Combine, 9570 STS Self-Propelled Combine (North American Edition) - PC9659, , 6068HH060 - Combine, 9570 STS Self-Propelled Combine (North American Edition) - PC9659, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9670 STS - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH006 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH008 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 9770 STS - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH006 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH008 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9870STS - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH002 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH001 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , S560 - Combine, S560 Combine (Europe Edition) - PC9677, , 6090HH008 - Combine, S560 Combine (Europe Edition) - PC9677, , S690 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH002 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , S690HM - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , Hillmaster - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" s="1" t="inlineStr">
@@ -3458,6 +4652,12 @@
           <t>AH138231</t>
         </is>
       </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9500, 9510, 9540, 9550, 9560, 9580, 9600, 9610, 9640, 9650, 9660, 9670, 9680, 9780, C670, CTS, CTS II, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" s="1" t="inlineStr">
@@ -3514,6 +4714,16 @@
           <t>H177930</t>
         </is>
       </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>748, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7460, 7480, 7500, 7550, 7580, 7700, 7750, 7780, 7800, 7850, 7980, 9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9986, 9996, C670, CTS, CTS II, S7 600, S7 700, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S690, S760, S760 PRECISION UPGRADES, S770, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="inlineStr">
@@ -3521,6 +4731,12 @@
           <t>AXE57243</t>
         </is>
       </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr"/>
     </row>
     <row r="385">
       <c r="A385" s="1" t="inlineStr">
@@ -3528,6 +4744,12 @@
           <t>H216336</t>
         </is>
       </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>1450, 1470, 1550, 1570, 9470 STS, 9560 STS, 9570 STS, 9660 STS, 9670 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W330, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" s="1" t="inlineStr">
@@ -3542,6 +4764,12 @@
           <t>HXE11023</t>
         </is>
       </c>
+      <c r="B387" t="inlineStr"/>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" s="1" t="inlineStr">
@@ -3549,6 +4777,12 @@
           <t>AH211438</t>
         </is>
       </c>
+      <c r="B388" t="inlineStr"/>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="389">
       <c r="A389" s="1" t="inlineStr">
@@ -3577,6 +4811,12 @@
           <t>AH204440</t>
         </is>
       </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>9450 - Combine, 9450 Self-Propelled Combine - PC2800, , 6068HH052 - Combine, 9450 Self-Propelled Combine - PC2800, , TRACK - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550SH - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH054 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH055 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH020 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH009 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH021 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH008 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9560SH - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9560 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH054 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH055 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , TRACK - Combine, 9650 Self-Propelled Combine - PC2802, , 9650 - Combine, 9650 Self-Propelled Combine - PC2802, , 6081HH017 - Combine, 9650 Self-Propelled Combine - PC2802, , 6081HH010 - Combine, 9650 Self-Propelled Combine - PC2802, , 9660 - Combine, 9660 Self-Propelled Combine (North American Edition) - PC9206, , 6081HH017 - Combine, 9660 Self-Propelled Combine (North American Edition) - PC9206</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" s="1" t="inlineStr">
@@ -3591,6 +4831,12 @@
           <t>AXE16895</t>
         </is>
       </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>S7 800, S7 850, S7 900, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" s="1" t="inlineStr">
@@ -3605,6 +4851,12 @@
           <t>H233203</t>
         </is>
       </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr"/>
     </row>
     <row r="397">
       <c r="A397" s="1" t="inlineStr">
@@ -3612,6 +4864,16 @@
           <t>AH206788</t>
         </is>
       </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>748, 7460, 9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9986, 9996, C670, CTS, CTS II, S7 600, S7 700, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S690, S760, S760 PRECISION UPGRADES, S770, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="398">
       <c r="A398" s="1" t="inlineStr">
@@ -3626,6 +4888,12 @@
           <t>DE19870</t>
         </is>
       </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>1165, 1175, 1450, 1470, 1550, 1570, 9400, 9410, 9450, 9470 STS, 9500, 9510, 9550, 9560, 9560 STS, 9570 STS, 9600, 9610, 9650, 9650 STS, 9660, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, CTS, CTS II, S7 600, S7 700, S430, S440, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S690, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T550, T660, W330, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" s="1" t="inlineStr">
@@ -3640,6 +4908,12 @@
           <t>CE21251</t>
         </is>
       </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>8100, 8200, 8300, 8400, 8500, 8600, 9500, 9600, 9700, S7 600, S7 700, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr"/>
     </row>
     <row r="402">
       <c r="A402" s="1" t="inlineStr">
@@ -3647,6 +4921,12 @@
           <t>AH122575</t>
         </is>
       </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>1170, 2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 6610, 6650, 6710, 6750, 6810, 6850, 6910, 6950, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7455, 7480, 7500, 7550, 7580, 7700, 7750, 7780, 7800, 7850, 9400, 9410, 9450, 9500, 9510, 9540, 9550, 9560, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9680, 9750 STS, 9780, 9880 STS, 9935, 9970, 9976, 9986, CTS, CTS II</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr"/>
     </row>
     <row r="403">
       <c r="A403" s="1" t="inlineStr">
@@ -3654,6 +4934,12 @@
           <t>AH138230</t>
         </is>
       </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 9400, 9410, 9450, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9680, 9750 STS, 9760 STS, 9780, 9860 STS, 9880 STS, C670, CTS, CTS II, S560, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr"/>
     </row>
     <row r="404">
       <c r="A404" s="1" t="inlineStr">
@@ -3661,6 +4947,12 @@
           <t>AH138230</t>
         </is>
       </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>2054, 2056, 2058, 2064, 2066, 2254, 2256, 2258, 2264, 2266, 2266E, 9400, 9410, 9450, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9680, 9750 STS, 9760 STS, 9780, 9860 STS, 9880 STS, C670, CTS, CTS II, S560, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr"/>
     </row>
     <row r="405">
       <c r="A405" s="1" t="inlineStr">
@@ -3682,6 +4974,12 @@
           <t>AH219844</t>
         </is>
       </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr"/>
     </row>
     <row r="408">
       <c r="A408" s="1" t="inlineStr">
@@ -3689,6 +4987,12 @@
           <t>AH219846</t>
         </is>
       </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr"/>
     </row>
     <row r="409">
       <c r="A409" s="1" t="inlineStr">
@@ -3703,6 +5007,12 @@
           <t>AL211142</t>
         </is>
       </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>8100, 8200, 8300, 8400, 8500, 8600, 8700, 8800, 9500, 9600, 9700, 9800, 9900, CH570, CH670, CH950, CH960, CP770, CS770, S430, S440, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W235, W235R, W260, W260R, W540, W550, W650, W660, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr"/>
     </row>
     <row r="411">
       <c r="A411" s="1" t="inlineStr">
@@ -3710,6 +5020,12 @@
           <t>AH220398</t>
         </is>
       </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9670 STS, 9770 STS, 9870 STS, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790, T550, T560, T660, T670, W540, W550, W650, W660, X9 1000, X9 1100</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr"/>
     </row>
     <row r="412">
       <c r="A412" s="1" t="inlineStr">
@@ -3717,6 +5033,12 @@
           <t>AH220452</t>
         </is>
       </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>9560STS - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH028 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6081HH019 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 6068HH058 - Combine, 9560 STS Self-Propelled Combine (North American Edition) - PC9562, , 9560 - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 9560i - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 6090HH005 - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , i-Series - Combine, 9560i STS Self-Propelled Combine (European Edition) - PC9563, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr"/>
     </row>
     <row r="413">
       <c r="A413" s="1" t="inlineStr">
@@ -3724,6 +5046,12 @@
           <t>AXE15601</t>
         </is>
       </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>S430, S440, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr"/>
     </row>
     <row r="414">
       <c r="A414" s="1" t="inlineStr">
@@ -3731,6 +5059,12 @@
           <t>AXE15601</t>
         </is>
       </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>S430, S440, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, X9 1000, X9 1000 PRECISION UPGRADES, X9 1100, X9 1100 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr"/>
     </row>
     <row r="415">
       <c r="A415" s="1" t="inlineStr">
@@ -3738,6 +5072,16 @@
           <t>AH209275</t>
         </is>
       </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>1450, 1550, 9540, 9560, 9560 STS, 9580, 9640, 9650 STS, 9660, 9660 STS, 9670, 9680, 9750 STS, 9760 STS, 9780, 9860 STS, 9880 STS, C670, T550, T560, T660, T670, W440, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="416">
       <c r="A416" s="1" t="inlineStr">
@@ -3745,6 +5089,12 @@
           <t>H224510</t>
         </is>
       </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>9670 STS, 9770 STS, 9870 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr"/>
     </row>
     <row r="417">
       <c r="A417" s="1" t="inlineStr">
@@ -3752,6 +5102,12 @@
           <t>AH156738</t>
         </is>
       </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>9640, 9650, 9660, 9670, 9680, T660, T670, W650, W660</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr"/>
     </row>
     <row r="418">
       <c r="A418" s="1" t="inlineStr">
@@ -3759,6 +5115,12 @@
           <t>H171186</t>
         </is>
       </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr"/>
     </row>
     <row r="419">
       <c r="A419" s="1" t="inlineStr">
@@ -3766,6 +5128,12 @@
           <t>CE18452</t>
         </is>
       </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>9540, 9560, 9560 STS, 9580, 9640, 9660, 9670, 9680, 9780, 9880 STS, C670, S560, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr"/>
     </row>
     <row r="420">
       <c r="A420" s="1" t="inlineStr">
@@ -3773,6 +5141,12 @@
           <t>H161055</t>
         </is>
       </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr"/>
     </row>
     <row r="421">
       <c r="A421" s="1" t="inlineStr">
@@ -3780,6 +5154,12 @@
           <t>H156576</t>
         </is>
       </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>9410 - Combine, 9410 Maximizer Combine - PC2700, , 6068HH051 - Combine, 9410 Maximizer Combine - PC2700, , 9450 - Combine, 9450 Self-Propelled Combine - PC2800, , 6068HH052 - Combine, 9450 Self-Propelled Combine - PC2800, , 9510 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , SH9510 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , 6081HH001 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , 6081HH002 - Combine, 9510 and SH9510 Maximizer Combines - PC2701, , TRACK - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550SH - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH054 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH055 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH020 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH009 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH021 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH008 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9560SH - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9560 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH054 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH055 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , TRACK - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 9650CTS - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH017 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH010 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9660CTS - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 6081HH017 - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9780 - Combine, 9780 CTS Combine (S.N. 071443-072697)(Europe Edition) - PC4373, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , CTS - Combine, CTS Combine (S.N. 070231-071384) (Europe Edition) - PC4318, , CTS - Combine, CTS Combines (S.N. 068887-070122) (Europe Edition) - PC4304, , CTSII - Combine, CTSII Combine (North American Edition) - PC2752, , 6081HH003 - Combine, CTSII Combine (North American Edition) - PC2752, , CTSII - Combine, CTSII Combine (S.N. 675000- ) (European Edition) - PC2753</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr"/>
     </row>
     <row r="422">
       <c r="A422" s="1" t="inlineStr">
@@ -3801,6 +5181,12 @@
           <t>H171186</t>
         </is>
       </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr"/>
     </row>
     <row r="425">
       <c r="A425" s="1" t="inlineStr">
@@ -3808,6 +5194,12 @@
           <t>AH210762</t>
         </is>
       </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>6103, 9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C2 400, C440, C670, CTS, CTS II, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W430, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr"/>
     </row>
     <row r="426">
       <c r="A426" s="1" t="inlineStr">
@@ -3815,6 +5207,12 @@
           <t>H201111</t>
         </is>
       </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>9450, 9470 STS, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9996, C670, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S760, S770, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr"/>
     </row>
     <row r="427">
       <c r="A427" s="1" t="inlineStr">
@@ -3822,6 +5220,12 @@
           <t>H157043</t>
         </is>
       </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>9450, 9470 STS, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9880 STS, C670, CTS, S540, S550, S560, S650, S660, S670, S690, S760, S770, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr"/>
     </row>
     <row r="428">
       <c r="A428" s="1" t="inlineStr">
@@ -3829,6 +5233,12 @@
           <t>AH210762</t>
         </is>
       </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>6103, 9400, 9410, 9450, 9470 STS, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C2 400, C440, C670, CTS, CTS II, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, T550, T560, T660, T670, W430, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr"/>
     </row>
     <row r="429">
       <c r="A429" s="1" t="inlineStr">
@@ -3836,6 +5246,12 @@
           <t>H201111</t>
         </is>
       </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>9450, 9470 STS, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9996, C670, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S760, S770, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr"/>
     </row>
     <row r="430">
       <c r="A430" s="1" t="inlineStr">
@@ -3843,6 +5259,12 @@
           <t>H231268</t>
         </is>
       </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>9670 STS, 9770 STS, 9870 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr"/>
     </row>
     <row r="431">
       <c r="A431" s="1" t="inlineStr">
@@ -3850,6 +5272,12 @@
           <t>H173375</t>
         </is>
       </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr"/>
     </row>
     <row r="432">
       <c r="A432" s="1" t="inlineStr">
@@ -3857,6 +5285,12 @@
           <t>AH139118</t>
         </is>
       </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S540, S550, S560, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S690, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr"/>
     </row>
     <row r="433">
       <c r="A433" s="1" t="inlineStr">
@@ -3864,6 +5298,12 @@
           <t>H129934</t>
         </is>
       </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, C670, CTS, CTS II, S560, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr"/>
     </row>
     <row r="434">
       <c r="A434" s="1" t="inlineStr">
@@ -3871,6 +5311,12 @@
           <t>AH218464</t>
         </is>
       </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>9470 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr"/>
     </row>
     <row r="435">
       <c r="A435" s="1" t="inlineStr">
@@ -3878,6 +5324,12 @@
           <t>H158386</t>
         </is>
       </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S7 600, S7 700, S7 800, S7 850, S7 900, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr"/>
     </row>
     <row r="436">
       <c r="A436" s="1" t="inlineStr">
@@ -3885,6 +5337,12 @@
           <t>HXE134521</t>
         </is>
       </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>9650 STS, 9670 STS, 9750 STS, 9770 STS, S650, S660, S670, S670H, S680, S680H, S685, S685H, S690, S690H, S760, S770, S780, S785, S790</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr"/>
     </row>
     <row r="437">
       <c r="A437" s="1" t="inlineStr">
@@ -3892,6 +5350,12 @@
           <t>CE21376</t>
         </is>
       </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>S670, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S770, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr"/>
     </row>
     <row r="438">
       <c r="A438" s="1" t="inlineStr">
@@ -3906,6 +5370,12 @@
           <t>H133598</t>
         </is>
       </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>9400, 9410, 9450, 9500, 9501, 9510, 9540, 9550, 9560, 9560 STS, 9580, 9650, 9650 STS, 9660, 9750 STS, 9780, 9880 STS, C670, CTS, CTS II, T550, T560, W540, W550</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr"/>
     </row>
     <row r="440">
       <c r="A440" s="1" t="inlineStr">
@@ -3913,6 +5383,12 @@
           <t>H165508</t>
         </is>
       </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>20 Trailer, 30 Trailer, 748, 1450, 1550, 2254, 2256, 2258, 2264, 2266, 2266E, 6650, 6750, 6850, 6950, 7180, 7200, 7250, 7280, 7300, 7350, 7380, 7400, 7450, 7455, 7460, 7480, 7500, 7550, 7580, 7700, 7750, 7780, 7800, 7850, 9400, 9410, 9450, 9470 STS, 9500, 9510, 9540, 9550, 9560, 9560 STS, 9570 STS, 9580, 9600, 9610, 9640, 9650, 9650 STS, 9660, 9660 STS, 9670, 9670 STS, 9680, 9750 STS, 9760 STS, 9770 STS, 9780, 9860 STS, 9870 STS, 9880 STS, 9935, 9970, 9976, 9986, C670, CTS, CTS II, S430, S440, S540, S550, S560, S650, S660, S670, S670H, S690, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr"/>
     </row>
     <row r="441">
       <c r="A441" s="1" t="inlineStr">
@@ -3920,6 +5396,12 @@
           <t>AH228557</t>
         </is>
       </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>9570STS - Combine, 9570 STS Combine (South American Edition) - PC9752, , 6068HCQ05 - Combine, 9570 STS Combine (South American Edition) - PC9752, , 6068HCQ07 - Combine, 9570 STS Combine (South American Edition) - PC9752, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HCQ03 - Combine, 9670 STS Combine (South American Edition) - PC11564, , 6090HCQ01 - Combine, 9670 STS Combine (South American Edition) - PC11564, , 9670 STS - Combine, 9670 STS Combine (South American Edition) - PC11564, , 9670 STS - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH006 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH008 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HCQ01 - Combine, 9770 STS Combine (South American Edition) - PC11565, , 9770 STS - Combine, 9770 STS Combine (South American Edition) - PC11565, , 9770 STS - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH006 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH008 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr"/>
     </row>
     <row r="442">
       <c r="A442" s="1" t="inlineStr">
@@ -3927,6 +5409,12 @@
           <t>H161010</t>
         </is>
       </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , TRACK - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH005 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH013 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH012 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 6081HH006 - Combine, 9650STS and 9750STS Self-Propelled Combines - PC2900, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HCQ03 - Combine, 9670 STS Combine (South American Edition) - PC11564, , 6090HCQ01 - Combine, 9670 STS Combine (South American Edition) - PC11564, , 9670 STS - Combine, 9670 STS Combine (South American Edition) - PC11564, , 9670 STS - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH006 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH008 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6090HCQ01 - Combine, 9770 STS Combine (South American Edition) - PC11565, , 9770 STS - Combine, 9770 STS Combine (South American Edition) - PC11565, , 9770 STS - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH006 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH008 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9870STS - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH002 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH001 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , S690 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH002 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , S690HM - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , Hillmaster - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr"/>
     </row>
     <row r="443">
       <c r="A443" s="1" t="inlineStr">
@@ -3934,6 +5422,12 @@
           <t>CE20120</t>
         </is>
       </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>S7 600, S7 700, S7 800, S7 850, S7 900, S540, S550, S650, S660, S660 PRECISION UPGRADES, S670, S670 PRECISION UPGRADES, S670H, S680, S680 PRECISION UPGRADES, S680H, S685, S685H, S690, S690 PRECISION UPGRADES, S690H, S760, S760 PRECISION UPGRADES, S770, S770 PRECISION UPGRADES, S780, S780 PRECISION UPGRADES, S785, S790, S790 PRECISION UPGRADES, T550, T560, T660, T670, W540, W550, W650, W660</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr"/>
     </row>
     <row r="444">
       <c r="A444" s="1" t="inlineStr">
@@ -3941,6 +5435,12 @@
           <t>H156938</t>
         </is>
       </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>9470 STS, 9560 STS, 9570 STS, 9650 STS, 9660 STS, 9670 STS, 9750 STS, 9760 STS, 9770 STS, 9860 STS, 9870 STS, 9880 STS, S540, S550, S560, S650, S660, S670, S670H, S690, S760, S770</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr"/>
     </row>
     <row r="445">
       <c r="A445" s="1" t="inlineStr">
@@ -3948,6 +5448,12 @@
           <t>H168256</t>
         </is>
       </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>9450 - Combine, 9450 Self-Propelled Combine - PC2800, , 6068HH052 - Combine, 9450 Self-Propelled Combine - PC2800, , TRACK - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550SH - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 9550 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH054 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH055 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH020 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH009 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH021 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , 6081HH008 - Combine, 9550 and 9550SH Self-Propelled Combines - PC2801, , TRACK - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 9650CTS - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH017 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , 6081HH010 - Combine, 9650 CTS Self-Propelled Combine - PC2803, , TRACK - Combine, 9650 Self-Propelled Combine - PC2802, , 9650 - Combine, 9650 Self-Propelled Combine - PC2802, , 6081HH017 - Combine, 9650 Self-Propelled Combine - PC2802, , 6081HH010 - Combine, 9650 Self-Propelled Combine - PC2802, , 9780 - Combine, 9780 CTS Combine (S.N. 071443-072697)(Europe Edition) - PC4373, , CTS - Combine, CTS Combine (S.N. 070231-071384) (Europe Edition) - PC4318, , CTS - Combine, CTS Combines (S.N. 068887-070122) (Europe Edition) - PC4304</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr"/>
     </row>
     <row r="446">
       <c r="A446" s="1" t="inlineStr">
@@ -3955,6 +5461,12 @@
           <t>H203850</t>
         </is>
       </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9670 STS - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH006 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH008 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 9750STS - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 6125HH003 - Combine, 9750STS Canadian Combine (S.N. 700602 - 700631) - PC9234, , 9770 STS - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH006 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH008 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9870STS - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH002 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH001 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , S690 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH002 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , S690HM - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , Hillmaster - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr"/>
     </row>
     <row r="447">
       <c r="A447" s="1" t="inlineStr">
@@ -3962,6 +5474,12 @@
           <t>H218671</t>
         </is>
       </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>9580WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9540WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9560WTS - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ017 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6068HZ060 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ008 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6068HZ470 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 6081HZ009 - Combine, 9540WTS, 9560WTS, 9580WTS Combines (S.N. -080015) Europe Edition - PC4376, , 9560SH - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9560 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH054 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 6068HH055 - Combine, 9560 and 9560SH Self-Propelled Combines (North American Edition) - PC9205, , 9750STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9650STS - Combine, 9650STS and 9750STS Self-Propelled Combines (South American Edition) - PC9241, , 9660CTS - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 6081HH017 - Combine, 9660CTS Self-Propelled Combine (North American Edition) - PC9207, , 9760STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9660STS - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH013 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6081HH012 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 6090HH005 - Combine, 9660STS and 9760STS Self-Propelled Combines (North American Edition) - PC9208, , 9670 STS - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH006 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 6090HH008 - Combine, 9670 STS Self-Propelled Combine (Worldwide Edition) - PC10554, , 9770 STS - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH006 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 6090HH008 - Combine, 9770 STS Self-Propelled Combine (Worldwide Edition) - PC10555, , 9860STS - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH006 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 6125HH003 - Combine, 9860 STS Self-Propelled Combine (North American Edition) - PC2901, , 9870STS - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH002 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 6135HH001 - Combine, 9870 STS Self-Propelled Combine (Worldwide Edition) - PC9661, , 9880STS - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HH006 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 6125HZ004 - Combine, 9880 STS Combine (S.N. -715700) Europe Edition - PC4378, , 9880i STS - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 6125HH006 - Combine, 9880i STS Combine (S.N.715701- ) European Edition - PC9529, , 9880i STS HILLMASTER - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , 6125HH006 - Combine, 9880i STS Hillmaster Combine (S.N.715801- ) European Edition - PC9564, , S690 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH002 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690 Combine (Europe Edition, S.N. -745100) - PC9662, , 6135HH001 - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , S690HM - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663, , Hillmaster - Combine, S690HM Combine (Europe Edition, S.N. -745100) - PC9663</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr"/>
     </row>
     <row r="448">
       <c r="A448" s="1" t="inlineStr">

</xml_diff>